<commit_message>
04.07.2020 MC Sales details
</commit_message>
<xml_diff>
--- a/2020/Others/Cash A.xlsx
+++ b/2020/Others/Cash A.xlsx
@@ -515,47 +515,71 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -576,21 +600,9 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -600,17 +612,8 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -624,15 +627,12 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -640,6 +640,12 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -661,12 +667,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -706,7 +706,7 @@
         <xdr:cNvPr id="2" name="Straight Connector 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -756,7 +756,7 @@
         <xdr:cNvPr id="3" name="Straight Connector 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -806,7 +806,7 @@
         <xdr:cNvPr id="4" name="Straight Connector 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -856,7 +856,7 @@
         <xdr:cNvPr id="5" name="Straight Connector 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -911,7 +911,7 @@
         <xdr:cNvPr id="12" name="Straight Connector 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000C000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00000C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -961,7 +961,7 @@
         <xdr:cNvPr id="6" name="Straight Connector 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3F693EA6-49EB-42D1-B3CA-F15B26A03B41}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3F693EA6-49EB-42D1-B3CA-F15B26A03B41}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1011,7 +1011,7 @@
         <xdr:cNvPr id="8" name="Straight Connector 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{334CB43E-1331-4297-A64C-0895C28A3BBB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{334CB43E-1331-4297-A64C-0895C28A3BBB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1061,7 +1061,7 @@
         <xdr:cNvPr id="9" name="Straight Connector 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0D774EF-0DA8-4AF5-A477-477DFA29C2B2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A0D774EF-0DA8-4AF5-A477-477DFA29C2B2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1111,7 +1111,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0F2A810E-B364-491B-AB34-AE585B8D27E3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0F2A810E-B364-491B-AB34-AE585B8D27E3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1123,7 +1123,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1161,7 +1161,7 @@
         <xdr:cNvPr id="13" name="Picture 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BBEAD3A6-FB1B-45D2-BDBE-713A9FCBE3DE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{BBEAD3A6-FB1B-45D2-BDBE-713A9FCBE3DE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1173,7 +1173,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1216,7 +1216,7 @@
         <xdr:cNvPr id="2" name="Straight Connector 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1266,7 +1266,7 @@
         <xdr:cNvPr id="3" name="Straight Connector 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1316,7 +1316,7 @@
         <xdr:cNvPr id="4" name="Straight Connector 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1366,7 +1366,7 @@
         <xdr:cNvPr id="5" name="Straight Connector 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1416,7 +1416,7 @@
         <xdr:cNvPr id="6" name="Straight Connector 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000006000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1471,7 +1471,7 @@
         <xdr:cNvPr id="7" name="Straight Connector 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000007000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1521,7 +1521,7 @@
         <xdr:cNvPr id="8" name="Straight Connector 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000008000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1571,7 +1571,7 @@
         <xdr:cNvPr id="9" name="Straight Connector 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000009000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000009000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1621,7 +1621,7 @@
         <xdr:cNvPr id="10" name="Straight Connector 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000A000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-00000A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1671,7 +1671,7 @@
         <xdr:cNvPr id="11" name="Straight Connector 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000B000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-00000B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1721,7 +1721,7 @@
         <xdr:cNvPr id="12" name="Straight Connector 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000C000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-00000C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1771,7 +1771,7 @@
         <xdr:cNvPr id="13" name="Straight Connector 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000D000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-00000D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1826,7 +1826,7 @@
         <xdr:cNvPr id="2" name="Straight Connector 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1876,7 +1876,7 @@
         <xdr:cNvPr id="3" name="Straight Connector 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1926,7 +1926,7 @@
         <xdr:cNvPr id="4" name="Straight Connector 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1976,7 +1976,7 @@
         <xdr:cNvPr id="5" name="Straight Connector 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2031,7 +2031,7 @@
         <xdr:cNvPr id="4" name="Straight Connector 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2081,7 +2081,7 @@
         <xdr:cNvPr id="5" name="Straight Connector 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2371,7 +2371,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2393,60 +2393,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
-      <c r="J1" s="38"/>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="39"/>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="39"/>
+      <c r="B2" s="45"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="45"/>
+      <c r="I2" s="45"/>
+      <c r="J2" s="45"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="39"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
-      <c r="I3" s="39"/>
-      <c r="J3" s="39"/>
+      <c r="B3" s="45"/>
+      <c r="C3" s="45"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="45"/>
+      <c r="G3" s="45"/>
+      <c r="H3" s="45"/>
+      <c r="I3" s="45"/>
+      <c r="J3" s="45"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="47" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="40"/>
-      <c r="I4" s="40"/>
-      <c r="J4" s="40"/>
+      <c r="B4" s="47"/>
+      <c r="C4" s="47"/>
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="47"/>
+      <c r="G4" s="47"/>
+      <c r="H4" s="47"/>
+      <c r="I4" s="47"/>
+      <c r="J4" s="47"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
@@ -2455,10 +2455,10 @@
       <c r="D5" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="37" t="s">
+      <c r="E5" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="37"/>
+      <c r="F5" s="48"/>
       <c r="G5" s="14" t="s">
         <v>5</v>
       </c>
@@ -2473,10 +2473,10 @@
       <c r="D6" s="13">
         <v>1000</v>
       </c>
-      <c r="E6" s="41">
+      <c r="E6" s="43">
         <v>50</v>
       </c>
-      <c r="F6" s="41"/>
+      <c r="F6" s="43"/>
       <c r="G6" s="13">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>50000</v>
@@ -2492,10 +2492,10 @@
       <c r="D7" s="13">
         <v>500</v>
       </c>
-      <c r="E7" s="41">
+      <c r="E7" s="43">
         <v>16</v>
       </c>
-      <c r="F7" s="41"/>
+      <c r="F7" s="43"/>
       <c r="G7" s="13">
         <f t="shared" si="0"/>
         <v>8000</v>
@@ -2511,10 +2511,10 @@
       <c r="D8" s="13">
         <v>100</v>
       </c>
-      <c r="E8" s="41">
+      <c r="E8" s="43">
         <v>151</v>
       </c>
-      <c r="F8" s="41"/>
+      <c r="F8" s="43"/>
       <c r="G8" s="13">
         <f t="shared" si="0"/>
         <v>15100</v>
@@ -2530,10 +2530,10 @@
       <c r="D9" s="13">
         <v>50</v>
       </c>
-      <c r="E9" s="41">
+      <c r="E9" s="43">
         <v>58</v>
       </c>
-      <c r="F9" s="41"/>
+      <c r="F9" s="43"/>
       <c r="G9" s="13">
         <f t="shared" si="0"/>
         <v>2900</v>
@@ -2549,8 +2549,8 @@
       <c r="D10" s="13">
         <v>20</v>
       </c>
-      <c r="E10" s="41"/>
-      <c r="F10" s="41"/>
+      <c r="E10" s="43"/>
+      <c r="F10" s="43"/>
       <c r="G10" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2566,8 +2566,8 @@
       <c r="D11" s="13">
         <v>10</v>
       </c>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
+      <c r="E11" s="43"/>
+      <c r="F11" s="43"/>
       <c r="G11" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2580,10 +2580,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="37" t="s">
+      <c r="D12" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="37"/>
+      <c r="E12" s="48"/>
       <c r="F12" s="14"/>
       <c r="G12" s="14">
         <f>SUM(G6:G11)</f>
@@ -2630,58 +2630,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="42" t="s">
+      <c r="A16" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="42"/>
+      <c r="B16" s="49"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="42" t="s">
+      <c r="H16" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="42"/>
-      <c r="J16" s="42"/>
+      <c r="I16" s="49"/>
+      <c r="J16" s="49"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="42"/>
-      <c r="B17" s="42"/>
+      <c r="A17" s="49"/>
+      <c r="B17" s="49"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="42"/>
-      <c r="I17" s="42"/>
-      <c r="J17" s="42"/>
+      <c r="H17" s="49"/>
+      <c r="I17" s="49"/>
+      <c r="J17" s="49"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="42"/>
-      <c r="B18" s="42"/>
+      <c r="A18" s="49"/>
+      <c r="B18" s="49"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="42"/>
-      <c r="I18" s="42"/>
-      <c r="J18" s="42"/>
+      <c r="H18" s="49"/>
+      <c r="I18" s="49"/>
+      <c r="J18" s="49"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="43"/>
-      <c r="B19" s="43"/>
+      <c r="A19" s="42"/>
+      <c r="B19" s="42"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="44" t="s">
+      <c r="H19" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="44"/>
-      <c r="J19" s="44"/>
+      <c r="I19" s="50"/>
+      <c r="J19" s="50"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -2691,11 +2691,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="45" t="s">
+      <c r="H20" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="46"/>
-      <c r="J20" s="46"/>
+      <c r="I20" s="38"/>
+      <c r="J20" s="38"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -2770,60 +2770,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="38" t="s">
+      <c r="A27" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="38"/>
-      <c r="C27" s="38"/>
-      <c r="D27" s="38"/>
-      <c r="E27" s="38"/>
-      <c r="F27" s="38"/>
-      <c r="G27" s="38"/>
-      <c r="H27" s="38"/>
-      <c r="I27" s="38"/>
-      <c r="J27" s="38"/>
+      <c r="B27" s="44"/>
+      <c r="C27" s="44"/>
+      <c r="D27" s="44"/>
+      <c r="E27" s="44"/>
+      <c r="F27" s="44"/>
+      <c r="G27" s="44"/>
+      <c r="H27" s="44"/>
+      <c r="I27" s="44"/>
+      <c r="J27" s="44"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="39" t="s">
+      <c r="A28" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="39"/>
-      <c r="C28" s="39"/>
-      <c r="D28" s="39"/>
-      <c r="E28" s="39"/>
-      <c r="F28" s="39"/>
-      <c r="G28" s="39"/>
-      <c r="H28" s="39"/>
-      <c r="I28" s="39"/>
-      <c r="J28" s="39"/>
+      <c r="B28" s="45"/>
+      <c r="C28" s="45"/>
+      <c r="D28" s="45"/>
+      <c r="E28" s="45"/>
+      <c r="F28" s="45"/>
+      <c r="G28" s="45"/>
+      <c r="H28" s="45"/>
+      <c r="I28" s="45"/>
+      <c r="J28" s="45"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="47" t="s">
+      <c r="A29" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="47"/>
-      <c r="C29" s="47"/>
-      <c r="D29" s="47"/>
-      <c r="E29" s="47"/>
-      <c r="F29" s="47"/>
-      <c r="G29" s="47"/>
-      <c r="H29" s="47"/>
-      <c r="I29" s="47"/>
-      <c r="J29" s="47"/>
+      <c r="B29" s="46"/>
+      <c r="C29" s="46"/>
+      <c r="D29" s="46"/>
+      <c r="E29" s="46"/>
+      <c r="F29" s="46"/>
+      <c r="G29" s="46"/>
+      <c r="H29" s="46"/>
+      <c r="I29" s="46"/>
+      <c r="J29" s="46"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="40" t="s">
+      <c r="A30" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="40"/>
-      <c r="C30" s="40"/>
-      <c r="D30" s="40"/>
-      <c r="E30" s="40"/>
-      <c r="F30" s="40"/>
-      <c r="G30" s="40"/>
-      <c r="H30" s="40"/>
-      <c r="I30" s="40"/>
-      <c r="J30" s="40"/>
+      <c r="B30" s="47"/>
+      <c r="C30" s="47"/>
+      <c r="D30" s="47"/>
+      <c r="E30" s="47"/>
+      <c r="F30" s="47"/>
+      <c r="G30" s="47"/>
+      <c r="H30" s="47"/>
+      <c r="I30" s="47"/>
+      <c r="J30" s="47"/>
     </row>
     <row r="31" spans="1:10" ht="24.95" customHeight="1">
       <c r="A31" s="6"/>
@@ -2832,10 +2832,10 @@
       <c r="D31" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="37" t="s">
+      <c r="E31" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="37"/>
+      <c r="F31" s="48"/>
       <c r="G31" s="15" t="s">
         <v>5</v>
       </c>
@@ -2850,10 +2850,10 @@
       <c r="D32" s="16">
         <v>1000</v>
       </c>
-      <c r="E32" s="41">
+      <c r="E32" s="43">
         <v>50</v>
       </c>
-      <c r="F32" s="41"/>
+      <c r="F32" s="43"/>
       <c r="G32" s="16">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>50000</v>
@@ -2869,10 +2869,10 @@
       <c r="D33" s="16">
         <v>500</v>
       </c>
-      <c r="E33" s="41">
+      <c r="E33" s="43">
         <v>116</v>
       </c>
-      <c r="F33" s="41"/>
+      <c r="F33" s="43"/>
       <c r="G33" s="16">
         <f t="shared" si="1"/>
         <v>58000</v>
@@ -2888,10 +2888,10 @@
       <c r="D34" s="16">
         <v>100</v>
       </c>
-      <c r="E34" s="41">
+      <c r="E34" s="43">
         <v>151</v>
       </c>
-      <c r="F34" s="41"/>
+      <c r="F34" s="43"/>
       <c r="G34" s="16">
         <f t="shared" si="1"/>
         <v>15100</v>
@@ -2907,10 +2907,10 @@
       <c r="D35" s="16">
         <v>50</v>
       </c>
-      <c r="E35" s="41">
+      <c r="E35" s="43">
         <v>58</v>
       </c>
-      <c r="F35" s="41"/>
+      <c r="F35" s="43"/>
       <c r="G35" s="16">
         <f t="shared" si="1"/>
         <v>2900</v>
@@ -2926,8 +2926,8 @@
       <c r="D36" s="16">
         <v>20</v>
       </c>
-      <c r="E36" s="41"/>
-      <c r="F36" s="41"/>
+      <c r="E36" s="43"/>
+      <c r="F36" s="43"/>
       <c r="G36" s="16">
         <f>SUM(D36*E36)</f>
         <v>0</v>
@@ -2943,8 +2943,8 @@
       <c r="D37" s="16">
         <v>10</v>
       </c>
-      <c r="E37" s="41"/>
-      <c r="F37" s="41"/>
+      <c r="E37" s="43"/>
+      <c r="F37" s="43"/>
       <c r="G37" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2957,10 +2957,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="48" t="s">
+      <c r="D38" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="49"/>
+      <c r="E38" s="40"/>
       <c r="F38" s="15"/>
       <c r="G38" s="15">
         <f>SUM(G32:G37)</f>
@@ -3007,58 +3007,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" ht="15.75">
-      <c r="A42" s="50" t="s">
+      <c r="A42" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="50"/>
+      <c r="B42" s="41"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="50" t="s">
+      <c r="H42" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="50"/>
-      <c r="J42" s="50"/>
+      <c r="I42" s="41"/>
+      <c r="J42" s="41"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="43"/>
-      <c r="B43" s="43"/>
+      <c r="A43" s="42"/>
+      <c r="B43" s="42"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="43"/>
-      <c r="I43" s="43"/>
-      <c r="J43" s="43"/>
+      <c r="H43" s="42"/>
+      <c r="I43" s="42"/>
+      <c r="J43" s="42"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="43"/>
-      <c r="B44" s="43"/>
+      <c r="A44" s="42"/>
+      <c r="B44" s="42"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="43"/>
-      <c r="I44" s="43"/>
-      <c r="J44" s="43"/>
+      <c r="H44" s="42"/>
+      <c r="I44" s="42"/>
+      <c r="J44" s="42"/>
     </row>
     <row r="45" spans="1:10" ht="15.75">
-      <c r="A45" s="43"/>
-      <c r="B45" s="43"/>
+      <c r="A45" s="42"/>
+      <c r="B45" s="42"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="43" t="s">
+      <c r="H45" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="50"/>
-      <c r="J45" s="50"/>
+      <c r="I45" s="41"/>
+      <c r="J45" s="41"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="6"/>
@@ -3068,11 +3068,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="45" t="s">
+      <c r="H46" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="46"/>
-      <c r="J46" s="46"/>
+      <c r="I46" s="38"/>
+      <c r="J46" s="38"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -3100,14 +3100,24 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="E37:F37"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A27:J27"/>
@@ -3120,24 +3130,14 @@
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.25" footer="0"/>
   <pageSetup scale="85" orientation="portrait" r:id="rId1"/>
@@ -3149,8 +3149,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection sqref="A1:J46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3169,64 +3169,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="51" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
-      <c r="F1" s="58"/>
-      <c r="G1" s="58"/>
-      <c r="H1" s="58"/>
-      <c r="I1" s="58"/>
-      <c r="J1" s="58"/>
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
+      <c r="G1" s="51"/>
+      <c r="H1" s="51"/>
+      <c r="I1" s="51"/>
+      <c r="J1" s="51"/>
       <c r="K1" s="24"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="59" t="s">
+      <c r="A2" s="52" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="59"/>
-      <c r="C2" s="59"/>
-      <c r="D2" s="59"/>
-      <c r="E2" s="59"/>
-      <c r="F2" s="59"/>
-      <c r="G2" s="59"/>
-      <c r="H2" s="59"/>
-      <c r="I2" s="59"/>
-      <c r="J2" s="59"/>
+      <c r="B2" s="52"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="52"/>
+      <c r="I2" s="52"/>
+      <c r="J2" s="52"/>
       <c r="K2" s="24"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="59" t="s">
+      <c r="A3" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="59"/>
-      <c r="C3" s="59"/>
-      <c r="D3" s="59"/>
-      <c r="E3" s="59"/>
-      <c r="F3" s="59"/>
-      <c r="G3" s="59"/>
-      <c r="H3" s="59"/>
-      <c r="I3" s="59"/>
-      <c r="J3" s="59"/>
+      <c r="B3" s="52"/>
+      <c r="C3" s="52"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="52"/>
+      <c r="F3" s="52"/>
+      <c r="G3" s="52"/>
+      <c r="H3" s="52"/>
+      <c r="I3" s="52"/>
+      <c r="J3" s="52"/>
       <c r="K3" s="24"/>
     </row>
     <row r="4" spans="1:11" ht="26.25">
-      <c r="A4" s="66">
+      <c r="A4" s="55">
         <f ca="1">TODAY()</f>
-        <v>43974</v>
-      </c>
-      <c r="B4" s="66"/>
-      <c r="C4" s="66"/>
-      <c r="D4" s="66"/>
-      <c r="E4" s="66"/>
-      <c r="F4" s="66"/>
-      <c r="G4" s="66"/>
-      <c r="H4" s="66"/>
-      <c r="I4" s="66"/>
-      <c r="J4" s="66"/>
+        <v>44014</v>
+      </c>
+      <c r="B4" s="55"/>
+      <c r="C4" s="55"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="55"/>
+      <c r="F4" s="55"/>
+      <c r="G4" s="55"/>
+      <c r="H4" s="55"/>
+      <c r="I4" s="55"/>
+      <c r="J4" s="55"/>
       <c r="K4" s="24"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -3236,10 +3236,10 @@
       <c r="D5" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="61" t="s">
+      <c r="E5" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="61"/>
+      <c r="F5" s="53"/>
       <c r="G5" s="26" t="s">
         <v>5</v>
       </c>
@@ -3254,13 +3254,13 @@
       <c r="D6" s="27">
         <v>1000</v>
       </c>
-      <c r="E6" s="62">
-        <v>70</v>
-      </c>
-      <c r="F6" s="62"/>
+      <c r="E6" s="54">
+        <v>100</v>
+      </c>
+      <c r="F6" s="54"/>
       <c r="G6" s="27">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
-        <v>70000</v>
+        <v>100000</v>
       </c>
       <c r="H6" s="25"/>
       <c r="I6" s="25"/>
@@ -3273,13 +3273,13 @@
       <c r="D7" s="27">
         <v>500</v>
       </c>
-      <c r="E7" s="62">
-        <v>600</v>
-      </c>
-      <c r="F7" s="62"/>
+      <c r="E7" s="54">
+        <v>500</v>
+      </c>
+      <c r="F7" s="54"/>
       <c r="G7" s="27">
         <f t="shared" si="0"/>
-        <v>300000</v>
+        <v>250000</v>
       </c>
       <c r="H7" s="25"/>
       <c r="I7" s="25"/>
@@ -3292,13 +3292,13 @@
       <c r="D8" s="27">
         <v>100</v>
       </c>
-      <c r="E8" s="62">
-        <v>300</v>
-      </c>
-      <c r="F8" s="62"/>
+      <c r="E8" s="54">
+        <v>500</v>
+      </c>
+      <c r="F8" s="54"/>
       <c r="G8" s="27">
         <f t="shared" si="0"/>
-        <v>30000</v>
+        <v>50000</v>
       </c>
       <c r="H8" s="25"/>
       <c r="I8" s="25"/>
@@ -3311,8 +3311,8 @@
       <c r="D9" s="27">
         <v>50</v>
       </c>
-      <c r="E9" s="62"/>
-      <c r="F9" s="62"/>
+      <c r="E9" s="54"/>
+      <c r="F9" s="54"/>
       <c r="G9" s="27">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3328,8 +3328,8 @@
       <c r="D10" s="27">
         <v>20</v>
       </c>
-      <c r="E10" s="62"/>
-      <c r="F10" s="62"/>
+      <c r="E10" s="54"/>
+      <c r="F10" s="54"/>
       <c r="G10" s="27">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3345,8 +3345,8 @@
       <c r="D11" s="27">
         <v>10</v>
       </c>
-      <c r="E11" s="62"/>
-      <c r="F11" s="62"/>
+      <c r="E11" s="54"/>
+      <c r="F11" s="54"/>
       <c r="G11" s="27">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3359,10 +3359,10 @@
       <c r="A12" s="25"/>
       <c r="B12" s="25"/>
       <c r="C12" s="25"/>
-      <c r="D12" s="62" t="s">
+      <c r="D12" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="62"/>
+      <c r="E12" s="54"/>
       <c r="F12" s="27"/>
       <c r="G12" s="22">
         <f>SUM(G6:G11)</f>
@@ -3410,59 +3410,59 @@
     </row>
     <row r="16" spans="1:11">
       <c r="A16" s="28"/>
-      <c r="B16" s="69" t="s">
+      <c r="B16" s="57" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="69"/>
-      <c r="D16" s="69"/>
+      <c r="C16" s="57"/>
+      <c r="D16" s="57"/>
       <c r="E16" s="28"/>
       <c r="F16" s="29"/>
       <c r="G16" s="29"/>
-      <c r="H16" s="68" t="s">
+      <c r="H16" s="56" t="s">
         <v>7</v>
       </c>
-      <c r="I16" s="68"/>
-      <c r="J16" s="68"/>
+      <c r="I16" s="56"/>
+      <c r="J16" s="56"/>
     </row>
     <row r="17" spans="1:11">
-      <c r="A17" s="68"/>
-      <c r="B17" s="68"/>
-      <c r="C17" s="68"/>
-      <c r="D17" s="68"/>
+      <c r="A17" s="56"/>
+      <c r="B17" s="56"/>
+      <c r="C17" s="56"/>
+      <c r="D17" s="56"/>
       <c r="E17" s="29"/>
       <c r="F17" s="29"/>
       <c r="G17" s="29"/>
-      <c r="H17" s="68"/>
-      <c r="I17" s="68"/>
-      <c r="J17" s="68"/>
+      <c r="H17" s="56"/>
+      <c r="I17" s="56"/>
+      <c r="J17" s="56"/>
     </row>
     <row r="18" spans="1:11">
-      <c r="A18" s="68"/>
-      <c r="B18" s="68"/>
-      <c r="C18" s="68"/>
-      <c r="D18" s="68"/>
+      <c r="A18" s="56"/>
+      <c r="B18" s="56"/>
+      <c r="C18" s="56"/>
+      <c r="D18" s="56"/>
       <c r="E18" s="29"/>
       <c r="F18" s="29"/>
       <c r="G18" s="29"/>
-      <c r="H18" s="68"/>
-      <c r="I18" s="68"/>
-      <c r="J18" s="68"/>
+      <c r="H18" s="56"/>
+      <c r="I18" s="56"/>
+      <c r="J18" s="56"/>
     </row>
     <row r="19" spans="1:11" ht="17.25" customHeight="1">
       <c r="A19" s="33"/>
-      <c r="B19" s="67" t="s">
+      <c r="B19" s="58" t="s">
         <v>28</v>
       </c>
-      <c r="C19" s="67"/>
-      <c r="D19" s="67"/>
+      <c r="C19" s="58"/>
+      <c r="D19" s="58"/>
       <c r="E19" s="29"/>
       <c r="F19" s="29"/>
       <c r="G19" s="29"/>
-      <c r="H19" s="42" t="s">
+      <c r="H19" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="I19" s="42"/>
-      <c r="J19" s="42"/>
+      <c r="I19" s="49"/>
+      <c r="J19" s="49"/>
     </row>
     <row r="20" spans="1:11">
       <c r="A20" s="25"/>
@@ -3472,9 +3472,9 @@
       <c r="E20" s="25"/>
       <c r="F20" s="25"/>
       <c r="G20" s="25"/>
-      <c r="H20" s="53"/>
-      <c r="I20" s="54"/>
-      <c r="J20" s="54"/>
+      <c r="H20" s="61"/>
+      <c r="I20" s="62"/>
+      <c r="J20" s="62"/>
     </row>
     <row r="21" spans="1:11">
       <c r="A21" s="25"/>
@@ -3561,66 +3561,66 @@
       <c r="J27" s="25"/>
     </row>
     <row r="28" spans="1:11" ht="31.5">
-      <c r="A28" s="58" t="s">
+      <c r="A28" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="B28" s="58"/>
-      <c r="C28" s="58"/>
-      <c r="D28" s="58"/>
-      <c r="E28" s="58"/>
-      <c r="F28" s="58"/>
-      <c r="G28" s="58"/>
-      <c r="H28" s="58"/>
-      <c r="I28" s="58"/>
-      <c r="J28" s="58"/>
+      <c r="B28" s="51"/>
+      <c r="C28" s="51"/>
+      <c r="D28" s="51"/>
+      <c r="E28" s="51"/>
+      <c r="F28" s="51"/>
+      <c r="G28" s="51"/>
+      <c r="H28" s="51"/>
+      <c r="I28" s="51"/>
+      <c r="J28" s="51"/>
     </row>
     <row r="29" spans="1:11" ht="18">
-      <c r="A29" s="59" t="str">
+      <c r="A29" s="52" t="str">
         <f>A2</f>
         <v>Komola Super Market, Alaipur, Natore</v>
       </c>
-      <c r="B29" s="59"/>
-      <c r="C29" s="59"/>
-      <c r="D29" s="59"/>
-      <c r="E29" s="59"/>
-      <c r="F29" s="59"/>
-      <c r="G29" s="59"/>
-      <c r="H29" s="59"/>
-      <c r="I29" s="59"/>
-      <c r="J29" s="59"/>
+      <c r="B29" s="52"/>
+      <c r="C29" s="52"/>
+      <c r="D29" s="52"/>
+      <c r="E29" s="52"/>
+      <c r="F29" s="52"/>
+      <c r="G29" s="52"/>
+      <c r="H29" s="52"/>
+      <c r="I29" s="52"/>
+      <c r="J29" s="52"/>
     </row>
     <row r="30" spans="1:11" ht="18.75">
-      <c r="A30" s="60" t="str">
+      <c r="A30" s="66" t="str">
         <f>A3</f>
         <v>Cash Details As Per Below</v>
       </c>
-      <c r="B30" s="60"/>
-      <c r="C30" s="60"/>
-      <c r="D30" s="60"/>
-      <c r="E30" s="60"/>
-      <c r="F30" s="60"/>
-      <c r="G30" s="60"/>
-      <c r="H30" s="60"/>
-      <c r="I30" s="60"/>
-      <c r="J30" s="60"/>
+      <c r="B30" s="66"/>
+      <c r="C30" s="66"/>
+      <c r="D30" s="66"/>
+      <c r="E30" s="66"/>
+      <c r="F30" s="66"/>
+      <c r="G30" s="66"/>
+      <c r="H30" s="66"/>
+      <c r="I30" s="66"/>
+      <c r="J30" s="66"/>
       <c r="K30" s="6" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="26.25">
-      <c r="A31" s="66">
+      <c r="A31" s="55">
         <f ca="1">TODAY()</f>
-        <v>43974</v>
-      </c>
-      <c r="B31" s="66"/>
-      <c r="C31" s="66"/>
-      <c r="D31" s="66"/>
-      <c r="E31" s="66"/>
-      <c r="F31" s="66"/>
-      <c r="G31" s="66"/>
-      <c r="H31" s="66"/>
-      <c r="I31" s="66"/>
-      <c r="J31" s="66"/>
+        <v>44014</v>
+      </c>
+      <c r="B31" s="55"/>
+      <c r="C31" s="55"/>
+      <c r="D31" s="55"/>
+      <c r="E31" s="55"/>
+      <c r="F31" s="55"/>
+      <c r="G31" s="55"/>
+      <c r="H31" s="55"/>
+      <c r="I31" s="55"/>
+      <c r="J31" s="55"/>
     </row>
     <row r="32" spans="1:11" ht="27.95" customHeight="1">
       <c r="A32" s="25"/>
@@ -3629,10 +3629,10 @@
       <c r="D32" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="61" t="s">
+      <c r="E32" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="61"/>
+      <c r="F32" s="53"/>
       <c r="G32" s="26" t="s">
         <v>5</v>
       </c>
@@ -3647,14 +3647,14 @@
       <c r="D33" s="30">
         <v>1000</v>
       </c>
-      <c r="E33" s="62">
+      <c r="E33" s="54">
         <f>E6</f>
-        <v>70</v>
-      </c>
-      <c r="F33" s="62"/>
+        <v>100</v>
+      </c>
+      <c r="F33" s="54"/>
       <c r="G33" s="30">
         <f t="shared" ref="G33:G38" si="1">SUM(D33*E33)</f>
-        <v>70000</v>
+        <v>100000</v>
       </c>
       <c r="H33" s="25"/>
       <c r="I33" s="25"/>
@@ -3667,14 +3667,14 @@
       <c r="D34" s="30">
         <v>500</v>
       </c>
-      <c r="E34" s="62">
+      <c r="E34" s="54">
         <f>E7</f>
-        <v>600</v>
-      </c>
-      <c r="F34" s="62"/>
+        <v>500</v>
+      </c>
+      <c r="F34" s="54"/>
       <c r="G34" s="30">
         <f t="shared" si="1"/>
-        <v>300000</v>
+        <v>250000</v>
       </c>
       <c r="H34" s="25"/>
       <c r="I34" s="25"/>
@@ -3687,14 +3687,14 @@
       <c r="D35" s="30">
         <v>100</v>
       </c>
-      <c r="E35" s="62">
+      <c r="E35" s="54">
         <f>E8</f>
-        <v>300</v>
-      </c>
-      <c r="F35" s="62"/>
+        <v>500</v>
+      </c>
+      <c r="F35" s="54"/>
       <c r="G35" s="30">
         <f t="shared" si="1"/>
-        <v>30000</v>
+        <v>50000</v>
       </c>
       <c r="H35" s="25"/>
       <c r="I35" s="25"/>
@@ -3707,8 +3707,8 @@
       <c r="D36" s="30">
         <v>50</v>
       </c>
-      <c r="E36" s="62"/>
-      <c r="F36" s="62"/>
+      <c r="E36" s="54"/>
+      <c r="F36" s="54"/>
       <c r="G36" s="30">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -3724,8 +3724,8 @@
       <c r="D37" s="30">
         <v>20</v>
       </c>
-      <c r="E37" s="62"/>
-      <c r="F37" s="62"/>
+      <c r="E37" s="54"/>
+      <c r="F37" s="54"/>
       <c r="G37" s="30">
         <f>SUM(D37*E37)</f>
         <v>0</v>
@@ -3741,8 +3741,8 @@
       <c r="D38" s="30">
         <v>10</v>
       </c>
-      <c r="E38" s="62"/>
-      <c r="F38" s="62"/>
+      <c r="E38" s="54"/>
+      <c r="F38" s="54"/>
       <c r="G38" s="30">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -3755,10 +3755,10 @@
       <c r="A39" s="25"/>
       <c r="B39" s="25"/>
       <c r="C39" s="25"/>
-      <c r="D39" s="63" t="s">
+      <c r="D39" s="67" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="64"/>
+      <c r="E39" s="68"/>
       <c r="F39" s="30"/>
       <c r="G39" s="23">
         <f>SUM(G33:G38)</f>
@@ -3814,53 +3814,53 @@
       <c r="E43" s="29"/>
       <c r="F43" s="29"/>
       <c r="G43" s="29"/>
-      <c r="H43" s="55" t="s">
+      <c r="H43" s="63" t="s">
         <v>7</v>
       </c>
-      <c r="I43" s="55"/>
-      <c r="J43" s="55"/>
+      <c r="I43" s="63"/>
+      <c r="J43" s="63"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="56"/>
-      <c r="B44" s="56"/>
-      <c r="C44" s="56"/>
-      <c r="D44" s="56"/>
+      <c r="A44" s="64"/>
+      <c r="B44" s="64"/>
+      <c r="C44" s="64"/>
+      <c r="D44" s="64"/>
       <c r="E44" s="25"/>
       <c r="F44" s="25"/>
       <c r="G44" s="25"/>
-      <c r="H44" s="56"/>
-      <c r="I44" s="56"/>
-      <c r="J44" s="56"/>
+      <c r="H44" s="64"/>
+      <c r="I44" s="64"/>
+      <c r="J44" s="64"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="56"/>
-      <c r="B45" s="56"/>
-      <c r="C45" s="56"/>
-      <c r="D45" s="56"/>
+      <c r="A45" s="64"/>
+      <c r="B45" s="64"/>
+      <c r="C45" s="64"/>
+      <c r="D45" s="64"/>
       <c r="E45" s="25"/>
       <c r="F45" s="25"/>
       <c r="G45" s="25"/>
-      <c r="H45" s="56"/>
-      <c r="I45" s="56"/>
-      <c r="J45" s="56"/>
+      <c r="H45" s="64"/>
+      <c r="I45" s="64"/>
+      <c r="J45" s="64"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="31"/>
-      <c r="B46" s="65" t="str">
+      <c r="B46" s="69" t="str">
         <f>B19</f>
         <v>Rahinul Kabir</v>
       </c>
-      <c r="C46" s="65"/>
-      <c r="D46" s="65"/>
+      <c r="C46" s="69"/>
+      <c r="D46" s="69"/>
       <c r="E46" s="32"/>
       <c r="F46" s="32"/>
       <c r="G46" s="32"/>
-      <c r="H46" s="57" t="str">
+      <c r="H46" s="65" t="str">
         <f>H19</f>
         <v>Jafor Iqbal</v>
       </c>
-      <c r="I46" s="57"/>
-      <c r="J46" s="57"/>
+      <c r="I46" s="65"/>
+      <c r="J46" s="65"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="21"/>
@@ -3870,35 +3870,12 @@
       <c r="E47" s="21"/>
       <c r="F47" s="21"/>
       <c r="G47" s="21"/>
-      <c r="H47" s="51"/>
-      <c r="I47" s="52"/>
-      <c r="J47" s="52"/>
+      <c r="H47" s="59"/>
+      <c r="I47" s="60"/>
+      <c r="J47" s="60"/>
     </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="A17:D18"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="A31:J31"/>
-    <mergeCell ref="B19:D19"/>
     <mergeCell ref="H47:J47"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="H43:J43"/>
@@ -3913,6 +3890,29 @@
     <mergeCell ref="D39:E39"/>
     <mergeCell ref="B46:D46"/>
     <mergeCell ref="A44:D45"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="A31:J31"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="A17:D18"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="A4:J4"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -3944,63 +3944,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
-      <c r="J1" s="38"/>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="39"/>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="39"/>
+      <c r="B2" s="45"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="45"/>
+      <c r="I2" s="45"/>
+      <c r="J2" s="45"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="39"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
-      <c r="I3" s="39"/>
-      <c r="J3" s="39"/>
+      <c r="B3" s="45"/>
+      <c r="C3" s="45"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="45"/>
+      <c r="G3" s="45"/>
+      <c r="H3" s="45"/>
+      <c r="I3" s="45"/>
+      <c r="J3" s="45"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="40"/>
-      <c r="I4" s="40"/>
-      <c r="J4" s="40"/>
+      <c r="B4" s="47"/>
+      <c r="C4" s="47"/>
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="47"/>
+      <c r="G4" s="47"/>
+      <c r="H4" s="47"/>
+      <c r="I4" s="47"/>
+      <c r="J4" s="47"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -4010,10 +4010,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="37" t="s">
+      <c r="E5" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="37"/>
+      <c r="F5" s="48"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -4028,10 +4028,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="41">
+      <c r="E6" s="43">
         <v>68</v>
       </c>
-      <c r="F6" s="41"/>
+      <c r="F6" s="43"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>68000</v>
@@ -4047,10 +4047,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="41">
+      <c r="E7" s="43">
         <v>135</v>
       </c>
-      <c r="F7" s="41"/>
+      <c r="F7" s="43"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>67500</v>
@@ -4066,10 +4066,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="41">
+      <c r="E8" s="43">
         <v>53</v>
       </c>
-      <c r="F8" s="41"/>
+      <c r="F8" s="43"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>5300</v>
@@ -4085,10 +4085,10 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="41">
+      <c r="E9" s="43">
         <v>2</v>
       </c>
-      <c r="F9" s="41"/>
+      <c r="F9" s="43"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -4104,10 +4104,10 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="41">
+      <c r="E10" s="43">
         <v>5</v>
       </c>
-      <c r="F10" s="41"/>
+      <c r="F10" s="43"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -4123,8 +4123,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
+      <c r="E11" s="43"/>
+      <c r="F11" s="43"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4137,10 +4137,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="37" t="s">
+      <c r="D12" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="37"/>
+      <c r="E12" s="48"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -4187,76 +4187,76 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="42" t="s">
+      <c r="A16" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="42"/>
+      <c r="B16" s="49"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="42" t="s">
+      <c r="H16" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="42"/>
-      <c r="J16" s="42"/>
+      <c r="I16" s="49"/>
+      <c r="J16" s="49"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="42"/>
-      <c r="B17" s="42"/>
+      <c r="A17" s="49"/>
+      <c r="B17" s="49"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="42"/>
-      <c r="I17" s="42"/>
-      <c r="J17" s="42"/>
+      <c r="H17" s="49"/>
+      <c r="I17" s="49"/>
+      <c r="J17" s="49"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="42"/>
-      <c r="B18" s="42"/>
+      <c r="A18" s="49"/>
+      <c r="B18" s="49"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="42"/>
-      <c r="I18" s="42"/>
-      <c r="J18" s="42"/>
+      <c r="H18" s="49"/>
+      <c r="I18" s="49"/>
+      <c r="J18" s="49"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="43" t="s">
+      <c r="A19" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="43"/>
+      <c r="B19" s="42"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="44" t="s">
+      <c r="H19" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="44"/>
-      <c r="J19" s="44"/>
+      <c r="I19" s="50"/>
+      <c r="J19" s="50"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="70" t="s">
+      <c r="A20" s="71" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="70"/>
+      <c r="B20" s="71"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="45" t="s">
+      <c r="H20" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="46"/>
-      <c r="J20" s="46"/>
+      <c r="I20" s="38"/>
+      <c r="J20" s="38"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4331,60 +4331,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="38" t="s">
+      <c r="A27" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="38"/>
-      <c r="C27" s="38"/>
-      <c r="D27" s="38"/>
-      <c r="E27" s="38"/>
-      <c r="F27" s="38"/>
-      <c r="G27" s="38"/>
-      <c r="H27" s="38"/>
-      <c r="I27" s="38"/>
-      <c r="J27" s="38"/>
+      <c r="B27" s="44"/>
+      <c r="C27" s="44"/>
+      <c r="D27" s="44"/>
+      <c r="E27" s="44"/>
+      <c r="F27" s="44"/>
+      <c r="G27" s="44"/>
+      <c r="H27" s="44"/>
+      <c r="I27" s="44"/>
+      <c r="J27" s="44"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="39" t="s">
+      <c r="A28" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="39"/>
-      <c r="C28" s="39"/>
-      <c r="D28" s="39"/>
-      <c r="E28" s="39"/>
-      <c r="F28" s="39"/>
-      <c r="G28" s="39"/>
-      <c r="H28" s="39"/>
-      <c r="I28" s="39"/>
-      <c r="J28" s="39"/>
+      <c r="B28" s="45"/>
+      <c r="C28" s="45"/>
+      <c r="D28" s="45"/>
+      <c r="E28" s="45"/>
+      <c r="F28" s="45"/>
+      <c r="G28" s="45"/>
+      <c r="H28" s="45"/>
+      <c r="I28" s="45"/>
+      <c r="J28" s="45"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="47" t="s">
+      <c r="A29" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="47"/>
-      <c r="C29" s="47"/>
-      <c r="D29" s="47"/>
-      <c r="E29" s="47"/>
-      <c r="F29" s="47"/>
-      <c r="G29" s="47"/>
-      <c r="H29" s="47"/>
-      <c r="I29" s="47"/>
-      <c r="J29" s="47"/>
+      <c r="B29" s="46"/>
+      <c r="C29" s="46"/>
+      <c r="D29" s="46"/>
+      <c r="E29" s="46"/>
+      <c r="F29" s="46"/>
+      <c r="G29" s="46"/>
+      <c r="H29" s="46"/>
+      <c r="I29" s="46"/>
+      <c r="J29" s="46"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="40" t="s">
+      <c r="A30" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="40"/>
-      <c r="C30" s="40"/>
-      <c r="D30" s="40"/>
-      <c r="E30" s="40"/>
-      <c r="F30" s="40"/>
-      <c r="G30" s="40"/>
-      <c r="H30" s="40"/>
-      <c r="I30" s="40"/>
-      <c r="J30" s="40"/>
+      <c r="B30" s="47"/>
+      <c r="C30" s="47"/>
+      <c r="D30" s="47"/>
+      <c r="E30" s="47"/>
+      <c r="F30" s="47"/>
+      <c r="G30" s="47"/>
+      <c r="H30" s="47"/>
+      <c r="I30" s="47"/>
+      <c r="J30" s="47"/>
     </row>
     <row r="31" spans="1:10" ht="20.25">
       <c r="A31" s="6"/>
@@ -4393,10 +4393,10 @@
       <c r="D31" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="74" t="s">
+      <c r="E31" s="70" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="74"/>
+      <c r="F31" s="70"/>
       <c r="G31" s="9" t="s">
         <v>5</v>
       </c>
@@ -4411,10 +4411,10 @@
       <c r="D32" s="2">
         <v>1000</v>
       </c>
-      <c r="E32" s="73">
+      <c r="E32" s="74">
         <v>68</v>
       </c>
-      <c r="F32" s="73"/>
+      <c r="F32" s="74"/>
       <c r="G32" s="2">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>68000</v>
@@ -4430,10 +4430,10 @@
       <c r="D33" s="2">
         <v>500</v>
       </c>
-      <c r="E33" s="73">
+      <c r="E33" s="74">
         <v>135</v>
       </c>
-      <c r="F33" s="73"/>
+      <c r="F33" s="74"/>
       <c r="G33" s="2">
         <f t="shared" si="1"/>
         <v>67500</v>
@@ -4449,10 +4449,10 @@
       <c r="D34" s="2">
         <v>100</v>
       </c>
-      <c r="E34" s="73">
+      <c r="E34" s="74">
         <v>53</v>
       </c>
-      <c r="F34" s="73"/>
+      <c r="F34" s="74"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
         <v>5300</v>
@@ -4468,10 +4468,10 @@
       <c r="D35" s="2">
         <v>50</v>
       </c>
-      <c r="E35" s="73">
+      <c r="E35" s="74">
         <v>2</v>
       </c>
-      <c r="F35" s="73"/>
+      <c r="F35" s="74"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4487,10 +4487,10 @@
       <c r="D36" s="2">
         <v>20</v>
       </c>
-      <c r="E36" s="73">
+      <c r="E36" s="74">
         <v>5</v>
       </c>
-      <c r="F36" s="73"/>
+      <c r="F36" s="74"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4506,8 +4506,8 @@
       <c r="D37" s="2">
         <v>10</v>
       </c>
-      <c r="E37" s="73"/>
-      <c r="F37" s="73"/>
+      <c r="E37" s="74"/>
+      <c r="F37" s="74"/>
       <c r="G37" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4520,10 +4520,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="72" t="s">
+      <c r="D38" s="73" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="72"/>
+      <c r="E38" s="73"/>
       <c r="F38" s="9"/>
       <c r="G38" s="9">
         <f>SUM(G32:G37)</f>
@@ -4570,76 +4570,76 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="50" t="s">
+      <c r="A42" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="50"/>
+      <c r="B42" s="41"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="50" t="s">
+      <c r="H42" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="50"/>
-      <c r="J42" s="50"/>
+      <c r="I42" s="41"/>
+      <c r="J42" s="41"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="43"/>
-      <c r="B43" s="43"/>
+      <c r="A43" s="42"/>
+      <c r="B43" s="42"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="43"/>
-      <c r="I43" s="43"/>
-      <c r="J43" s="43"/>
+      <c r="H43" s="42"/>
+      <c r="I43" s="42"/>
+      <c r="J43" s="42"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="43"/>
-      <c r="B44" s="43"/>
+      <c r="A44" s="42"/>
+      <c r="B44" s="42"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="43"/>
-      <c r="I44" s="43"/>
-      <c r="J44" s="43"/>
+      <c r="H44" s="42"/>
+      <c r="I44" s="42"/>
+      <c r="J44" s="42"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="43" t="s">
+      <c r="A45" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="B45" s="43"/>
+      <c r="B45" s="42"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="43" t="s">
+      <c r="H45" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="50"/>
-      <c r="J45" s="50"/>
+      <c r="I45" s="41"/>
+      <c r="J45" s="41"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="71" t="s">
+      <c r="A46" s="72" t="s">
         <v>14</v>
       </c>
-      <c r="B46" s="71"/>
+      <c r="B46" s="72"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="45" t="s">
+      <c r="H46" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="46"/>
-      <c r="J46" s="46"/>
+      <c r="I46" s="38"/>
+      <c r="J46" s="38"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -4667,30 +4667,6 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
     <mergeCell ref="H46:J46"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A46:B46"/>
@@ -4707,6 +4683,30 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -4738,63 +4738,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
-      <c r="J1" s="38"/>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="39"/>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="39"/>
+      <c r="B2" s="45"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="45"/>
+      <c r="I2" s="45"/>
+      <c r="J2" s="45"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="39"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
-      <c r="I3" s="39"/>
-      <c r="J3" s="39"/>
+      <c r="B3" s="45"/>
+      <c r="C3" s="45"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="45"/>
+      <c r="G3" s="45"/>
+      <c r="H3" s="45"/>
+      <c r="I3" s="45"/>
+      <c r="J3" s="45"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="40"/>
-      <c r="I4" s="40"/>
-      <c r="J4" s="40"/>
+      <c r="B4" s="47"/>
+      <c r="C4" s="47"/>
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="47"/>
+      <c r="G4" s="47"/>
+      <c r="H4" s="47"/>
+      <c r="I4" s="47"/>
+      <c r="J4" s="47"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -4804,10 +4804,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="37" t="s">
+      <c r="E5" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="37"/>
+      <c r="F5" s="48"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -4822,10 +4822,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="41">
+      <c r="E6" s="43">
         <v>44</v>
       </c>
-      <c r="F6" s="41"/>
+      <c r="F6" s="43"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>44000</v>
@@ -4841,10 +4841,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="41">
+      <c r="E7" s="43">
         <v>118</v>
       </c>
-      <c r="F7" s="41"/>
+      <c r="F7" s="43"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>59000</v>
@@ -4860,10 +4860,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="41">
+      <c r="E8" s="43">
         <v>510</v>
       </c>
-      <c r="F8" s="41"/>
+      <c r="F8" s="43"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>51000</v>
@@ -4879,8 +4879,8 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="41"/>
-      <c r="F9" s="41"/>
+      <c r="E9" s="43"/>
+      <c r="F9" s="43"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4896,8 +4896,8 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="41"/>
-      <c r="F10" s="41"/>
+      <c r="E10" s="43"/>
+      <c r="F10" s="43"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4913,8 +4913,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
+      <c r="E11" s="43"/>
+      <c r="F11" s="43"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4927,10 +4927,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="37" t="s">
+      <c r="D12" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="37"/>
+      <c r="E12" s="48"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -4977,72 +4977,72 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="42" t="s">
+      <c r="A16" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="42"/>
+      <c r="B16" s="49"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="42" t="s">
+      <c r="H16" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="42"/>
-      <c r="J16" s="42"/>
+      <c r="I16" s="49"/>
+      <c r="J16" s="49"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="42"/>
-      <c r="B17" s="42"/>
+      <c r="A17" s="49"/>
+      <c r="B17" s="49"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="42"/>
-      <c r="I17" s="42"/>
-      <c r="J17" s="42"/>
+      <c r="H17" s="49"/>
+      <c r="I17" s="49"/>
+      <c r="J17" s="49"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="42"/>
-      <c r="B18" s="42"/>
+      <c r="A18" s="49"/>
+      <c r="B18" s="49"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="42"/>
-      <c r="I18" s="42"/>
-      <c r="J18" s="42"/>
+      <c r="H18" s="49"/>
+      <c r="I18" s="49"/>
+      <c r="J18" s="49"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="43"/>
-      <c r="B19" s="43"/>
+      <c r="A19" s="42"/>
+      <c r="B19" s="42"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="44" t="s">
+      <c r="H19" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="44"/>
-      <c r="J19" s="44"/>
+      <c r="I19" s="50"/>
+      <c r="J19" s="50"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="76"/>
-      <c r="B20" s="76"/>
+      <c r="A20" s="75"/>
+      <c r="B20" s="75"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="45" t="s">
+      <c r="H20" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="46"/>
-      <c r="J20" s="46"/>
+      <c r="I20" s="38"/>
+      <c r="J20" s="38"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -5117,60 +5117,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="38" t="s">
+      <c r="A27" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="38"/>
-      <c r="C27" s="38"/>
-      <c r="D27" s="38"/>
-      <c r="E27" s="38"/>
-      <c r="F27" s="38"/>
-      <c r="G27" s="38"/>
-      <c r="H27" s="38"/>
-      <c r="I27" s="38"/>
-      <c r="J27" s="38"/>
+      <c r="B27" s="44"/>
+      <c r="C27" s="44"/>
+      <c r="D27" s="44"/>
+      <c r="E27" s="44"/>
+      <c r="F27" s="44"/>
+      <c r="G27" s="44"/>
+      <c r="H27" s="44"/>
+      <c r="I27" s="44"/>
+      <c r="J27" s="44"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="39" t="s">
+      <c r="A28" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="39"/>
-      <c r="C28" s="39"/>
-      <c r="D28" s="39"/>
-      <c r="E28" s="39"/>
-      <c r="F28" s="39"/>
-      <c r="G28" s="39"/>
-      <c r="H28" s="39"/>
-      <c r="I28" s="39"/>
-      <c r="J28" s="39"/>
+      <c r="B28" s="45"/>
+      <c r="C28" s="45"/>
+      <c r="D28" s="45"/>
+      <c r="E28" s="45"/>
+      <c r="F28" s="45"/>
+      <c r="G28" s="45"/>
+      <c r="H28" s="45"/>
+      <c r="I28" s="45"/>
+      <c r="J28" s="45"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="47" t="s">
+      <c r="A29" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="47"/>
-      <c r="C29" s="47"/>
-      <c r="D29" s="47"/>
-      <c r="E29" s="47"/>
-      <c r="F29" s="47"/>
-      <c r="G29" s="47"/>
-      <c r="H29" s="47"/>
-      <c r="I29" s="47"/>
-      <c r="J29" s="47"/>
+      <c r="B29" s="46"/>
+      <c r="C29" s="46"/>
+      <c r="D29" s="46"/>
+      <c r="E29" s="46"/>
+      <c r="F29" s="46"/>
+      <c r="G29" s="46"/>
+      <c r="H29" s="46"/>
+      <c r="I29" s="46"/>
+      <c r="J29" s="46"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="40" t="s">
+      <c r="A30" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="40"/>
-      <c r="C30" s="40"/>
-      <c r="D30" s="40"/>
-      <c r="E30" s="40"/>
-      <c r="F30" s="40"/>
-      <c r="G30" s="40"/>
-      <c r="H30" s="40"/>
-      <c r="I30" s="40"/>
-      <c r="J30" s="40"/>
+      <c r="B30" s="47"/>
+      <c r="C30" s="47"/>
+      <c r="D30" s="47"/>
+      <c r="E30" s="47"/>
+      <c r="F30" s="47"/>
+      <c r="G30" s="47"/>
+      <c r="H30" s="47"/>
+      <c r="I30" s="47"/>
+      <c r="J30" s="47"/>
     </row>
     <row r="31" spans="1:10" ht="23.25">
       <c r="A31" s="6"/>
@@ -5179,10 +5179,10 @@
       <c r="D31" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="37" t="s">
+      <c r="E31" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="37"/>
+      <c r="F31" s="48"/>
       <c r="G31" s="12" t="s">
         <v>5</v>
       </c>
@@ -5197,10 +5197,10 @@
       <c r="D32" s="11">
         <v>1000</v>
       </c>
-      <c r="E32" s="41">
+      <c r="E32" s="43">
         <v>44</v>
       </c>
-      <c r="F32" s="41"/>
+      <c r="F32" s="43"/>
       <c r="G32" s="11">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>44000</v>
@@ -5216,10 +5216,10 @@
       <c r="D33" s="11">
         <v>500</v>
       </c>
-      <c r="E33" s="41">
+      <c r="E33" s="43">
         <v>118</v>
       </c>
-      <c r="F33" s="41"/>
+      <c r="F33" s="43"/>
       <c r="G33" s="11">
         <f t="shared" si="1"/>
         <v>59000</v>
@@ -5235,10 +5235,10 @@
       <c r="D34" s="11">
         <v>100</v>
       </c>
-      <c r="E34" s="41">
+      <c r="E34" s="43">
         <v>510</v>
       </c>
-      <c r="F34" s="41"/>
+      <c r="F34" s="43"/>
       <c r="G34" s="11">
         <f t="shared" si="1"/>
         <v>51000</v>
@@ -5254,8 +5254,8 @@
       <c r="D35" s="11">
         <v>50</v>
       </c>
-      <c r="E35" s="41"/>
-      <c r="F35" s="41"/>
+      <c r="E35" s="43"/>
+      <c r="F35" s="43"/>
       <c r="G35" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -5271,8 +5271,8 @@
       <c r="D36" s="11">
         <v>20</v>
       </c>
-      <c r="E36" s="41"/>
-      <c r="F36" s="41"/>
+      <c r="E36" s="43"/>
+      <c r="F36" s="43"/>
       <c r="G36" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -5288,8 +5288,8 @@
       <c r="D37" s="11">
         <v>10</v>
       </c>
-      <c r="E37" s="41"/>
-      <c r="F37" s="41"/>
+      <c r="E37" s="43"/>
+      <c r="F37" s="43"/>
       <c r="G37" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -5302,10 +5302,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="75" t="s">
+      <c r="D38" s="76" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="75"/>
+      <c r="E38" s="76"/>
       <c r="F38" s="12"/>
       <c r="G38" s="12">
         <f>SUM(G32:G37)</f>
@@ -5352,72 +5352,72 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="50" t="s">
+      <c r="A42" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="50"/>
+      <c r="B42" s="41"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="50" t="s">
+      <c r="H42" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="50"/>
-      <c r="J42" s="50"/>
+      <c r="I42" s="41"/>
+      <c r="J42" s="41"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="43"/>
-      <c r="B43" s="43"/>
+      <c r="A43" s="42"/>
+      <c r="B43" s="42"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="43"/>
-      <c r="I43" s="43"/>
-      <c r="J43" s="43"/>
+      <c r="H43" s="42"/>
+      <c r="I43" s="42"/>
+      <c r="J43" s="42"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="43"/>
-      <c r="B44" s="43"/>
+      <c r="A44" s="42"/>
+      <c r="B44" s="42"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="43"/>
-      <c r="I44" s="43"/>
-      <c r="J44" s="43"/>
+      <c r="H44" s="42"/>
+      <c r="I44" s="42"/>
+      <c r="J44" s="42"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="43"/>
-      <c r="B45" s="43"/>
+      <c r="A45" s="42"/>
+      <c r="B45" s="42"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="43" t="s">
+      <c r="H45" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="50"/>
-      <c r="J45" s="50"/>
+      <c r="I45" s="41"/>
+      <c r="J45" s="41"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="71"/>
-      <c r="B46" s="71"/>
+      <c r="A46" s="72"/>
+      <c r="B46" s="72"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="45" t="s">
+      <c r="H46" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="46"/>
-      <c r="J46" s="46"/>
+      <c r="I46" s="38"/>
+      <c r="J46" s="38"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -5445,6 +5445,34 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -5457,34 +5485,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -5509,64 +5509,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
-      <c r="J1" s="38"/>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="39"/>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="39"/>
+      <c r="B2" s="45"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="45"/>
+      <c r="I2" s="45"/>
+      <c r="J2" s="45"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="39"/>
-      <c r="B3" s="39"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
-      <c r="I3" s="39"/>
-      <c r="J3" s="39"/>
+      <c r="A3" s="45"/>
+      <c r="B3" s="45"/>
+      <c r="C3" s="45"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="45"/>
+      <c r="G3" s="45"/>
+      <c r="H3" s="45"/>
+      <c r="I3" s="45"/>
+      <c r="J3" s="45"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="40"/>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="40"/>
-      <c r="I4" s="40"/>
-      <c r="J4" s="40"/>
+      <c r="A4" s="47"/>
+      <c r="B4" s="47"/>
+      <c r="C4" s="47"/>
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="47"/>
+      <c r="G4" s="47"/>
+      <c r="H4" s="47"/>
+      <c r="I4" s="47"/>
+      <c r="J4" s="47"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="D5" s="18"/>
-      <c r="E5" s="37"/>
-      <c r="F5" s="37"/>
+      <c r="E5" s="48"/>
+      <c r="F5" s="48"/>
       <c r="G5" s="18"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
@@ -5577,8 +5577,8 @@
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="17"/>
-      <c r="E6" s="41"/>
-      <c r="F6" s="41"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="43"/>
       <c r="G6" s="17"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -5589,8 +5589,8 @@
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
       <c r="D7" s="17"/>
-      <c r="E7" s="41"/>
-      <c r="F7" s="41"/>
+      <c r="E7" s="43"/>
+      <c r="F7" s="43"/>
       <c r="G7" s="17"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
@@ -5601,8 +5601,8 @@
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
       <c r="D8" s="17"/>
-      <c r="E8" s="41"/>
-      <c r="F8" s="41"/>
+      <c r="E8" s="43"/>
+      <c r="F8" s="43"/>
       <c r="G8" s="17"/>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -5613,8 +5613,8 @@
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="17"/>
-      <c r="E9" s="41"/>
-      <c r="F9" s="41"/>
+      <c r="E9" s="43"/>
+      <c r="F9" s="43"/>
       <c r="G9" s="17"/>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -5625,8 +5625,8 @@
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="17"/>
-      <c r="E10" s="41"/>
-      <c r="F10" s="41"/>
+      <c r="E10" s="43"/>
+      <c r="F10" s="43"/>
       <c r="G10" s="17"/>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
@@ -5637,8 +5637,8 @@
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="17"/>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
+      <c r="E11" s="43"/>
+      <c r="F11" s="43"/>
       <c r="G11" s="17"/>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
@@ -5648,8 +5648,8 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="37"/>
-      <c r="E12" s="37"/>
+      <c r="D12" s="48"/>
+      <c r="E12" s="48"/>
       <c r="F12" s="18"/>
       <c r="G12" s="18"/>
       <c r="H12" s="6"/>
@@ -5693,52 +5693,52 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="42"/>
-      <c r="B16" s="42"/>
+      <c r="A16" s="49"/>
+      <c r="B16" s="49"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="42"/>
-      <c r="I16" s="42"/>
-      <c r="J16" s="42"/>
+      <c r="H16" s="49"/>
+      <c r="I16" s="49"/>
+      <c r="J16" s="49"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="42"/>
-      <c r="B17" s="42"/>
+      <c r="A17" s="49"/>
+      <c r="B17" s="49"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="42"/>
-      <c r="I17" s="42"/>
-      <c r="J17" s="42"/>
+      <c r="H17" s="49"/>
+      <c r="I17" s="49"/>
+      <c r="J17" s="49"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="42"/>
-      <c r="B18" s="42"/>
+      <c r="A18" s="49"/>
+      <c r="B18" s="49"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="42"/>
-      <c r="I18" s="42"/>
-      <c r="J18" s="42"/>
+      <c r="H18" s="49"/>
+      <c r="I18" s="49"/>
+      <c r="J18" s="49"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="43"/>
-      <c r="B19" s="43"/>
+      <c r="A19" s="42"/>
+      <c r="B19" s="42"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="44"/>
-      <c r="I19" s="44"/>
-      <c r="J19" s="44"/>
+      <c r="H19" s="50"/>
+      <c r="I19" s="50"/>
+      <c r="J19" s="50"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -5748,9 +5748,9 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="45"/>
-      <c r="I20" s="46"/>
-      <c r="J20" s="46"/>
+      <c r="H20" s="37"/>
+      <c r="I20" s="38"/>
+      <c r="J20" s="38"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -5837,60 +5837,60 @@
       <c r="J27" s="6"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="38" t="s">
+      <c r="A28" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="38"/>
-      <c r="C28" s="38"/>
-      <c r="D28" s="38"/>
-      <c r="E28" s="38"/>
-      <c r="F28" s="38"/>
-      <c r="G28" s="38"/>
-      <c r="H28" s="38"/>
-      <c r="I28" s="38"/>
-      <c r="J28" s="38"/>
+      <c r="B28" s="44"/>
+      <c r="C28" s="44"/>
+      <c r="D28" s="44"/>
+      <c r="E28" s="44"/>
+      <c r="F28" s="44"/>
+      <c r="G28" s="44"/>
+      <c r="H28" s="44"/>
+      <c r="I28" s="44"/>
+      <c r="J28" s="44"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="39" t="s">
+      <c r="A29" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="39"/>
-      <c r="C29" s="39"/>
-      <c r="D29" s="39"/>
-      <c r="E29" s="39"/>
-      <c r="F29" s="39"/>
-      <c r="G29" s="39"/>
-      <c r="H29" s="39"/>
-      <c r="I29" s="39"/>
-      <c r="J29" s="39"/>
+      <c r="B29" s="45"/>
+      <c r="C29" s="45"/>
+      <c r="D29" s="45"/>
+      <c r="E29" s="45"/>
+      <c r="F29" s="45"/>
+      <c r="G29" s="45"/>
+      <c r="H29" s="45"/>
+      <c r="I29" s="45"/>
+      <c r="J29" s="45"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="47" t="s">
+      <c r="A30" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="47"/>
-      <c r="C30" s="47"/>
-      <c r="D30" s="47"/>
-      <c r="E30" s="47"/>
-      <c r="F30" s="47"/>
-      <c r="G30" s="47"/>
-      <c r="H30" s="47"/>
-      <c r="I30" s="47"/>
-      <c r="J30" s="47"/>
+      <c r="B30" s="46"/>
+      <c r="C30" s="46"/>
+      <c r="D30" s="46"/>
+      <c r="E30" s="46"/>
+      <c r="F30" s="46"/>
+      <c r="G30" s="46"/>
+      <c r="H30" s="46"/>
+      <c r="I30" s="46"/>
+      <c r="J30" s="46"/>
     </row>
     <row r="31" spans="1:10" ht="18.75">
-      <c r="A31" s="40" t="s">
+      <c r="A31" s="47" t="s">
         <v>19</v>
       </c>
-      <c r="B31" s="40"/>
-      <c r="C31" s="40"/>
-      <c r="D31" s="40"/>
-      <c r="E31" s="40"/>
-      <c r="F31" s="40"/>
-      <c r="G31" s="40"/>
-      <c r="H31" s="40"/>
-      <c r="I31" s="40"/>
-      <c r="J31" s="40"/>
+      <c r="B31" s="47"/>
+      <c r="C31" s="47"/>
+      <c r="D31" s="47"/>
+      <c r="E31" s="47"/>
+      <c r="F31" s="47"/>
+      <c r="G31" s="47"/>
+      <c r="H31" s="47"/>
+      <c r="I31" s="47"/>
+      <c r="J31" s="47"/>
     </row>
     <row r="32" spans="1:10" ht="20.25">
       <c r="A32" s="6" t="s">
@@ -5901,10 +5901,10 @@
       <c r="D32" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="74" t="s">
+      <c r="E32" s="70" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="74"/>
+      <c r="F32" s="70"/>
       <c r="G32" s="20" t="s">
         <v>5</v>
       </c>
@@ -5919,10 +5919,10 @@
       <c r="D33" s="19">
         <v>1000</v>
       </c>
-      <c r="E33" s="41">
+      <c r="E33" s="43">
         <v>30</v>
       </c>
-      <c r="F33" s="41"/>
+      <c r="F33" s="43"/>
       <c r="G33" s="19">
         <f t="shared" ref="G33:G38" si="0">SUM(D33*E33)</f>
         <v>30000</v>
@@ -5938,10 +5938,10 @@
       <c r="D34" s="19">
         <v>500</v>
       </c>
-      <c r="E34" s="41">
+      <c r="E34" s="43">
         <v>35</v>
       </c>
-      <c r="F34" s="41"/>
+      <c r="F34" s="43"/>
       <c r="G34" s="19">
         <f t="shared" si="0"/>
         <v>17500</v>
@@ -5957,10 +5957,10 @@
       <c r="D35" s="19">
         <v>100</v>
       </c>
-      <c r="E35" s="41">
+      <c r="E35" s="43">
         <v>425</v>
       </c>
-      <c r="F35" s="41"/>
+      <c r="F35" s="43"/>
       <c r="G35" s="19">
         <f t="shared" si="0"/>
         <v>42500</v>
@@ -5976,8 +5976,8 @@
       <c r="D36" s="19">
         <v>50</v>
       </c>
-      <c r="E36" s="41"/>
-      <c r="F36" s="41"/>
+      <c r="E36" s="43"/>
+      <c r="F36" s="43"/>
       <c r="G36" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -5993,8 +5993,8 @@
       <c r="D37" s="19">
         <v>20</v>
       </c>
-      <c r="E37" s="73"/>
-      <c r="F37" s="73"/>
+      <c r="E37" s="74"/>
+      <c r="F37" s="74"/>
       <c r="G37" s="19">
         <f>SUM(D37*E37)</f>
         <v>0</v>
@@ -6010,10 +6010,10 @@
       <c r="D38" s="19">
         <v>10</v>
       </c>
-      <c r="E38" s="73">
+      <c r="E38" s="74">
         <v>100</v>
       </c>
-      <c r="F38" s="73"/>
+      <c r="F38" s="74"/>
       <c r="G38" s="19">
         <f t="shared" si="0"/>
         <v>1000</v>
@@ -6076,58 +6076,58 @@
       <c r="J42" s="6"/>
     </row>
     <row r="43" spans="1:10" ht="15.75">
-      <c r="A43" s="50" t="s">
+      <c r="A43" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="50"/>
+      <c r="B43" s="41"/>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
-      <c r="H43" s="50" t="s">
+      <c r="H43" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="50"/>
-      <c r="J43" s="50"/>
+      <c r="I43" s="41"/>
+      <c r="J43" s="41"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="43"/>
-      <c r="B44" s="43"/>
+      <c r="A44" s="42"/>
+      <c r="B44" s="42"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="43"/>
-      <c r="I44" s="43"/>
-      <c r="J44" s="43"/>
+      <c r="H44" s="42"/>
+      <c r="I44" s="42"/>
+      <c r="J44" s="42"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="43"/>
-      <c r="B45" s="43"/>
+      <c r="A45" s="42"/>
+      <c r="B45" s="42"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="43"/>
-      <c r="I45" s="43"/>
-      <c r="J45" s="43"/>
+      <c r="H45" s="42"/>
+      <c r="I45" s="42"/>
+      <c r="J45" s="42"/>
     </row>
     <row r="46" spans="1:10" ht="15.75">
-      <c r="A46" s="43"/>
-      <c r="B46" s="43"/>
+      <c r="A46" s="42"/>
+      <c r="B46" s="42"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="43" t="s">
+      <c r="H46" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="50"/>
-      <c r="J46" s="50"/>
+      <c r="I46" s="41"/>
+      <c r="J46" s="41"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -6137,20 +6137,30 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="45"/>
-      <c r="I47" s="46"/>
-      <c r="J47" s="46"/>
+      <c r="H47" s="37"/>
+      <c r="I47" s="38"/>
+      <c r="J47" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="H47:J47"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="H43:J43"/>
-    <mergeCell ref="A44:B45"/>
-    <mergeCell ref="H44:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="E38:F38"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A28:J28"/>
@@ -6163,24 +6173,14 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="H47:J47"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="H43:J43"/>
+    <mergeCell ref="A44:B45"/>
+    <mergeCell ref="H44:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -6206,177 +6206,177 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
-      <c r="J1" s="38"/>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="39"/>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="39"/>
+      <c r="B2" s="45"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="45"/>
+      <c r="I2" s="45"/>
+      <c r="J2" s="45"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="87">
+      <c r="A5" s="88">
         <v>1</v>
       </c>
-      <c r="B5" s="79" t="s">
+      <c r="B5" s="81" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="79"/>
-      <c r="D5" s="79"/>
-      <c r="E5" s="79"/>
-      <c r="F5" s="79"/>
-      <c r="G5" s="86">
+      <c r="C5" s="81"/>
+      <c r="D5" s="81"/>
+      <c r="E5" s="81"/>
+      <c r="F5" s="81"/>
+      <c r="G5" s="79">
         <v>1650</v>
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="87"/>
-      <c r="B6" s="79"/>
-      <c r="C6" s="79"/>
-      <c r="D6" s="79"/>
-      <c r="E6" s="79"/>
-      <c r="F6" s="79"/>
-      <c r="G6" s="86"/>
+      <c r="A6" s="88"/>
+      <c r="B6" s="81"/>
+      <c r="C6" s="81"/>
+      <c r="D6" s="81"/>
+      <c r="E6" s="81"/>
+      <c r="F6" s="81"/>
+      <c r="G6" s="79"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="87">
+      <c r="A7" s="88">
         <v>2</v>
       </c>
-      <c r="B7" s="79" t="s">
+      <c r="B7" s="81" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="79"/>
-      <c r="D7" s="79"/>
-      <c r="E7" s="79"/>
-      <c r="F7" s="79"/>
-      <c r="G7" s="86">
+      <c r="C7" s="81"/>
+      <c r="D7" s="81"/>
+      <c r="E7" s="81"/>
+      <c r="F7" s="81"/>
+      <c r="G7" s="79">
         <v>1980</v>
       </c>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="87"/>
-      <c r="B8" s="79"/>
-      <c r="C8" s="79"/>
-      <c r="D8" s="79"/>
-      <c r="E8" s="79"/>
-      <c r="F8" s="79"/>
-      <c r="G8" s="86"/>
+      <c r="A8" s="88"/>
+      <c r="B8" s="81"/>
+      <c r="C8" s="81"/>
+      <c r="D8" s="81"/>
+      <c r="E8" s="81"/>
+      <c r="F8" s="81"/>
+      <c r="G8" s="79"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="87">
+      <c r="A9" s="88">
         <v>3</v>
       </c>
-      <c r="B9" s="79" t="s">
+      <c r="B9" s="81" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="79"/>
-      <c r="D9" s="79"/>
-      <c r="E9" s="79"/>
-      <c r="F9" s="79"/>
-      <c r="G9" s="86">
+      <c r="C9" s="81"/>
+      <c r="D9" s="81"/>
+      <c r="E9" s="81"/>
+      <c r="F9" s="81"/>
+      <c r="G9" s="79">
         <v>10538</v>
       </c>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="87"/>
-      <c r="B10" s="79"/>
-      <c r="C10" s="79"/>
-      <c r="D10" s="79"/>
-      <c r="E10" s="79"/>
-      <c r="F10" s="79"/>
-      <c r="G10" s="86"/>
+      <c r="A10" s="88"/>
+      <c r="B10" s="81"/>
+      <c r="C10" s="81"/>
+      <c r="D10" s="81"/>
+      <c r="E10" s="81"/>
+      <c r="F10" s="81"/>
+      <c r="G10" s="79"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="87">
+      <c r="A11" s="88">
         <v>4</v>
       </c>
-      <c r="B11" s="80" t="s">
+      <c r="B11" s="82" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="81"/>
-      <c r="D11" s="81"/>
-      <c r="E11" s="81"/>
-      <c r="F11" s="82"/>
-      <c r="G11" s="86">
+      <c r="C11" s="83"/>
+      <c r="D11" s="83"/>
+      <c r="E11" s="83"/>
+      <c r="F11" s="84"/>
+      <c r="G11" s="79">
         <v>1100</v>
       </c>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="87"/>
-      <c r="B12" s="83"/>
-      <c r="C12" s="84"/>
-      <c r="D12" s="84"/>
-      <c r="E12" s="84"/>
-      <c r="F12" s="85"/>
-      <c r="G12" s="86"/>
+      <c r="A12" s="88"/>
+      <c r="B12" s="85"/>
+      <c r="C12" s="86"/>
+      <c r="D12" s="86"/>
+      <c r="E12" s="86"/>
+      <c r="F12" s="87"/>
+      <c r="G12" s="79"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="88" t="s">
+      <c r="A13" s="80" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="88"/>
-      <c r="C13" s="88"/>
-      <c r="D13" s="88"/>
-      <c r="E13" s="88"/>
-      <c r="F13" s="88"/>
-      <c r="G13" s="86">
+      <c r="B13" s="80"/>
+      <c r="C13" s="80"/>
+      <c r="D13" s="80"/>
+      <c r="E13" s="80"/>
+      <c r="F13" s="80"/>
+      <c r="G13" s="79">
         <f>SUM(G5:G12)</f>
         <v>15268</v>
       </c>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="88"/>
-      <c r="B14" s="88"/>
-      <c r="C14" s="88"/>
-      <c r="D14" s="88"/>
-      <c r="E14" s="88"/>
-      <c r="F14" s="88"/>
-      <c r="G14" s="86"/>
+      <c r="A14" s="80"/>
+      <c r="B14" s="80"/>
+      <c r="C14" s="80"/>
+      <c r="D14" s="80"/>
+      <c r="E14" s="80"/>
+      <c r="F14" s="80"/>
+      <c r="G14" s="79"/>
     </row>
     <row r="23" spans="1:10" ht="18.75">
-      <c r="A23" s="47" t="s">
+      <c r="A23" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="47"/>
-      <c r="C23" s="47"/>
-      <c r="D23" s="47"/>
-      <c r="E23" s="47"/>
-      <c r="F23" s="47"/>
-      <c r="G23" s="47"/>
-      <c r="H23" s="47"/>
-      <c r="I23" s="47"/>
-      <c r="J23" s="47"/>
+      <c r="B23" s="46"/>
+      <c r="C23" s="46"/>
+      <c r="D23" s="46"/>
+      <c r="E23" s="46"/>
+      <c r="F23" s="46"/>
+      <c r="G23" s="46"/>
+      <c r="H23" s="46"/>
+      <c r="I23" s="46"/>
+      <c r="J23" s="46"/>
     </row>
     <row r="24" spans="1:10" ht="18.75">
-      <c r="A24" s="40"/>
-      <c r="B24" s="40"/>
-      <c r="C24" s="40"/>
-      <c r="D24" s="40"/>
-      <c r="E24" s="40"/>
-      <c r="F24" s="40"/>
-      <c r="G24" s="40"/>
-      <c r="H24" s="40"/>
-      <c r="I24" s="40"/>
-      <c r="J24" s="40"/>
+      <c r="A24" s="47"/>
+      <c r="B24" s="47"/>
+      <c r="C24" s="47"/>
+      <c r="D24" s="47"/>
+      <c r="E24" s="47"/>
+      <c r="F24" s="47"/>
+      <c r="G24" s="47"/>
+      <c r="H24" s="47"/>
+      <c r="I24" s="47"/>
+      <c r="J24" s="47"/>
     </row>
     <row r="25" spans="1:10" ht="20.25">
       <c r="A25" s="6" t="s">
@@ -6387,10 +6387,10 @@
       <c r="D25" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E25" s="74" t="s">
+      <c r="E25" s="70" t="s">
         <v>4</v>
       </c>
-      <c r="F25" s="74"/>
+      <c r="F25" s="70"/>
       <c r="G25" s="20" t="s">
         <v>5</v>
       </c>
@@ -6405,8 +6405,8 @@
       <c r="D26" s="19">
         <v>1000</v>
       </c>
-      <c r="E26" s="41"/>
-      <c r="F26" s="41"/>
+      <c r="E26" s="43"/>
+      <c r="F26" s="43"/>
       <c r="G26" s="19">
         <f t="shared" ref="G26:G31" si="0">SUM(D26*E26)</f>
         <v>0</v>
@@ -6422,10 +6422,10 @@
       <c r="D27" s="19">
         <v>500</v>
       </c>
-      <c r="E27" s="41">
+      <c r="E27" s="43">
         <v>30</v>
       </c>
-      <c r="F27" s="41"/>
+      <c r="F27" s="43"/>
       <c r="G27" s="19">
         <f t="shared" si="0"/>
         <v>15000</v>
@@ -6441,8 +6441,8 @@
       <c r="D28" s="19">
         <v>100</v>
       </c>
-      <c r="E28" s="41"/>
-      <c r="F28" s="41"/>
+      <c r="E28" s="43"/>
+      <c r="F28" s="43"/>
       <c r="G28" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -6458,10 +6458,10 @@
       <c r="D29" s="19">
         <v>50</v>
       </c>
-      <c r="E29" s="41">
+      <c r="E29" s="43">
         <v>5</v>
       </c>
-      <c r="F29" s="41"/>
+      <c r="F29" s="43"/>
       <c r="G29" s="19">
         <f t="shared" si="0"/>
         <v>250</v>
@@ -6477,8 +6477,8 @@
       <c r="D30" s="19">
         <v>20</v>
       </c>
-      <c r="E30" s="73"/>
-      <c r="F30" s="73"/>
+      <c r="E30" s="74"/>
+      <c r="F30" s="74"/>
       <c r="G30" s="19">
         <f>SUM(D30*E30)</f>
         <v>0</v>
@@ -6494,10 +6494,10 @@
       <c r="D31" s="19">
         <v>10</v>
       </c>
-      <c r="E31" s="73">
+      <c r="E31" s="74">
         <v>2</v>
       </c>
-      <c r="F31" s="73"/>
+      <c r="F31" s="74"/>
       <c r="G31" s="19">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -6560,58 +6560,58 @@
       <c r="J35" s="6"/>
     </row>
     <row r="36" spans="1:10" ht="15.75">
-      <c r="A36" s="50" t="s">
+      <c r="A36" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="50"/>
+      <c r="B36" s="41"/>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
       <c r="G36" s="7"/>
-      <c r="H36" s="50" t="s">
+      <c r="H36" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="I36" s="50"/>
-      <c r="J36" s="50"/>
+      <c r="I36" s="41"/>
+      <c r="J36" s="41"/>
     </row>
     <row r="37" spans="1:10">
-      <c r="A37" s="43"/>
-      <c r="B37" s="43"/>
+      <c r="A37" s="42"/>
+      <c r="B37" s="42"/>
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
       <c r="G37" s="6"/>
-      <c r="H37" s="43"/>
-      <c r="I37" s="43"/>
-      <c r="J37" s="43"/>
+      <c r="H37" s="42"/>
+      <c r="I37" s="42"/>
+      <c r="J37" s="42"/>
     </row>
     <row r="38" spans="1:10">
-      <c r="A38" s="43"/>
-      <c r="B38" s="43"/>
+      <c r="A38" s="42"/>
+      <c r="B38" s="42"/>
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
-      <c r="H38" s="43"/>
-      <c r="I38" s="43"/>
-      <c r="J38" s="43"/>
+      <c r="H38" s="42"/>
+      <c r="I38" s="42"/>
+      <c r="J38" s="42"/>
     </row>
     <row r="39" spans="1:10" ht="15.75">
-      <c r="A39" s="43"/>
-      <c r="B39" s="43"/>
+      <c r="A39" s="42"/>
+      <c r="B39" s="42"/>
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
       <c r="F39" s="6"/>
       <c r="G39" s="6"/>
-      <c r="H39" s="43" t="s">
+      <c r="H39" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="I39" s="50"/>
-      <c r="J39" s="50"/>
+      <c r="I39" s="41"/>
+      <c r="J39" s="41"/>
     </row>
     <row r="40" spans="1:10">
       <c r="A40" s="6"/>
@@ -6621,29 +6621,12 @@
       <c r="E40" s="6"/>
       <c r="F40" s="6"/>
       <c r="G40" s="6"/>
-      <c r="H40" s="45"/>
-      <c r="I40" s="46"/>
-      <c r="J40" s="46"/>
+      <c r="H40" s="37"/>
+      <c r="I40" s="38"/>
+      <c r="J40" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="H40:J40"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="H36:J36"/>
-    <mergeCell ref="A37:B38"/>
-    <mergeCell ref="H37:J38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="H39:J39"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="A13:F14"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="E30:F30"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="A23:J23"/>
@@ -6660,6 +6643,23 @@
     <mergeCell ref="B5:F6"/>
     <mergeCell ref="G5:G6"/>
     <mergeCell ref="B7:F8"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="A13:F14"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="H40:J40"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="H36:J36"/>
+    <mergeCell ref="A37:B38"/>
+    <mergeCell ref="H37:J38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="H39:J39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="71" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
09.07.2020 MC Sales Details
</commit_message>
<xml_diff>
--- a/2020/Others/Cash A.xlsx
+++ b/2020/Others/Cash A.xlsx
@@ -515,12 +515,39 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -529,57 +556,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -600,9 +576,21 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -612,27 +600,39 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -640,12 +640,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -667,6 +661,12 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -706,7 +706,7 @@
         <xdr:cNvPr id="2" name="Straight Connector 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -756,7 +756,7 @@
         <xdr:cNvPr id="3" name="Straight Connector 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -806,7 +806,7 @@
         <xdr:cNvPr id="4" name="Straight Connector 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -856,7 +856,7 @@
         <xdr:cNvPr id="5" name="Straight Connector 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000005000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -911,7 +911,7 @@
         <xdr:cNvPr id="12" name="Straight Connector 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00000C000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -961,7 +961,7 @@
         <xdr:cNvPr id="6" name="Straight Connector 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3F693EA6-49EB-42D1-B3CA-F15B26A03B41}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3F693EA6-49EB-42D1-B3CA-F15B26A03B41}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1011,7 +1011,7 @@
         <xdr:cNvPr id="8" name="Straight Connector 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{334CB43E-1331-4297-A64C-0895C28A3BBB}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{334CB43E-1331-4297-A64C-0895C28A3BBB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1061,7 +1061,7 @@
         <xdr:cNvPr id="9" name="Straight Connector 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A0D774EF-0DA8-4AF5-A477-477DFA29C2B2}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0D774EF-0DA8-4AF5-A477-477DFA29C2B2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1111,7 +1111,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0F2A810E-B364-491B-AB34-AE585B8D27E3}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0F2A810E-B364-491B-AB34-AE585B8D27E3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1123,7 +1123,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1161,7 +1161,7 @@
         <xdr:cNvPr id="13" name="Picture 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{BBEAD3A6-FB1B-45D2-BDBE-713A9FCBE3DE}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BBEAD3A6-FB1B-45D2-BDBE-713A9FCBE3DE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1173,7 +1173,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1216,7 +1216,7 @@
         <xdr:cNvPr id="2" name="Straight Connector 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1266,7 +1266,7 @@
         <xdr:cNvPr id="3" name="Straight Connector 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1316,7 +1316,7 @@
         <xdr:cNvPr id="4" name="Straight Connector 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1366,7 +1366,7 @@
         <xdr:cNvPr id="5" name="Straight Connector 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000005000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1416,7 +1416,7 @@
         <xdr:cNvPr id="6" name="Straight Connector 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000006000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1471,7 +1471,7 @@
         <xdr:cNvPr id="7" name="Straight Connector 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000007000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1521,7 +1521,7 @@
         <xdr:cNvPr id="8" name="Straight Connector 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000008000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1571,7 +1571,7 @@
         <xdr:cNvPr id="9" name="Straight Connector 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000009000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000009000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1621,7 +1621,7 @@
         <xdr:cNvPr id="10" name="Straight Connector 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-00000A000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1671,7 +1671,7 @@
         <xdr:cNvPr id="11" name="Straight Connector 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-00000B000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1721,7 +1721,7 @@
         <xdr:cNvPr id="12" name="Straight Connector 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-00000C000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1771,7 +1771,7 @@
         <xdr:cNvPr id="13" name="Straight Connector 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-00000D000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1826,7 +1826,7 @@
         <xdr:cNvPr id="2" name="Straight Connector 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1876,7 +1876,7 @@
         <xdr:cNvPr id="3" name="Straight Connector 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1926,7 +1926,7 @@
         <xdr:cNvPr id="4" name="Straight Connector 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1976,7 +1976,7 @@
         <xdr:cNvPr id="5" name="Straight Connector 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000005000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2031,7 +2031,7 @@
         <xdr:cNvPr id="4" name="Straight Connector 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2081,7 +2081,7 @@
         <xdr:cNvPr id="5" name="Straight Connector 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000005000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2371,7 +2371,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2393,60 +2393,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="44"/>
-      <c r="J1" s="44"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="45"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="45"/>
-      <c r="H2" s="45"/>
-      <c r="I2" s="45"/>
-      <c r="J2" s="45"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="39"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="45" t="s">
+      <c r="A3" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="45"/>
-      <c r="C3" s="45"/>
-      <c r="D3" s="45"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="45"/>
-      <c r="G3" s="45"/>
-      <c r="H3" s="45"/>
-      <c r="I3" s="45"/>
-      <c r="J3" s="45"/>
+      <c r="B3" s="39"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="39"/>
+      <c r="J3" s="39"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="47" t="s">
+      <c r="A4" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="47"/>
-      <c r="C4" s="47"/>
-      <c r="D4" s="47"/>
-      <c r="E4" s="47"/>
-      <c r="F4" s="47"/>
-      <c r="G4" s="47"/>
-      <c r="H4" s="47"/>
-      <c r="I4" s="47"/>
-      <c r="J4" s="47"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="40"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
@@ -2455,10 +2455,10 @@
       <c r="D5" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="48" t="s">
+      <c r="E5" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="48"/>
+      <c r="F5" s="37"/>
       <c r="G5" s="14" t="s">
         <v>5</v>
       </c>
@@ -2473,10 +2473,10 @@
       <c r="D6" s="13">
         <v>1000</v>
       </c>
-      <c r="E6" s="43">
+      <c r="E6" s="41">
         <v>50</v>
       </c>
-      <c r="F6" s="43"/>
+      <c r="F6" s="41"/>
       <c r="G6" s="13">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>50000</v>
@@ -2492,10 +2492,10 @@
       <c r="D7" s="13">
         <v>500</v>
       </c>
-      <c r="E7" s="43">
+      <c r="E7" s="41">
         <v>16</v>
       </c>
-      <c r="F7" s="43"/>
+      <c r="F7" s="41"/>
       <c r="G7" s="13">
         <f t="shared" si="0"/>
         <v>8000</v>
@@ -2511,10 +2511,10 @@
       <c r="D8" s="13">
         <v>100</v>
       </c>
-      <c r="E8" s="43">
+      <c r="E8" s="41">
         <v>151</v>
       </c>
-      <c r="F8" s="43"/>
+      <c r="F8" s="41"/>
       <c r="G8" s="13">
         <f t="shared" si="0"/>
         <v>15100</v>
@@ -2530,10 +2530,10 @@
       <c r="D9" s="13">
         <v>50</v>
       </c>
-      <c r="E9" s="43">
+      <c r="E9" s="41">
         <v>58</v>
       </c>
-      <c r="F9" s="43"/>
+      <c r="F9" s="41"/>
       <c r="G9" s="13">
         <f t="shared" si="0"/>
         <v>2900</v>
@@ -2549,8 +2549,8 @@
       <c r="D10" s="13">
         <v>20</v>
       </c>
-      <c r="E10" s="43"/>
-      <c r="F10" s="43"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="41"/>
       <c r="G10" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2566,8 +2566,8 @@
       <c r="D11" s="13">
         <v>10</v>
       </c>
-      <c r="E11" s="43"/>
-      <c r="F11" s="43"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="41"/>
       <c r="G11" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2580,10 +2580,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="48" t="s">
+      <c r="D12" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="48"/>
+      <c r="E12" s="37"/>
       <c r="F12" s="14"/>
       <c r="G12" s="14">
         <f>SUM(G6:G11)</f>
@@ -2630,58 +2630,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="49" t="s">
+      <c r="A16" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="49"/>
+      <c r="B16" s="42"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="49" t="s">
+      <c r="H16" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="49"/>
-      <c r="J16" s="49"/>
+      <c r="I16" s="42"/>
+      <c r="J16" s="42"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="49"/>
-      <c r="B17" s="49"/>
+      <c r="A17" s="42"/>
+      <c r="B17" s="42"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="49"/>
-      <c r="I17" s="49"/>
-      <c r="J17" s="49"/>
+      <c r="H17" s="42"/>
+      <c r="I17" s="42"/>
+      <c r="J17" s="42"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="49"/>
-      <c r="B18" s="49"/>
+      <c r="A18" s="42"/>
+      <c r="B18" s="42"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="49"/>
-      <c r="I18" s="49"/>
-      <c r="J18" s="49"/>
+      <c r="H18" s="42"/>
+      <c r="I18" s="42"/>
+      <c r="J18" s="42"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="42"/>
-      <c r="B19" s="42"/>
+      <c r="A19" s="43"/>
+      <c r="B19" s="43"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="50" t="s">
+      <c r="H19" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="50"/>
-      <c r="J19" s="50"/>
+      <c r="I19" s="44"/>
+      <c r="J19" s="44"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -2691,11 +2691,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="37" t="s">
+      <c r="H20" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="38"/>
-      <c r="J20" s="38"/>
+      <c r="I20" s="46"/>
+      <c r="J20" s="46"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -2770,60 +2770,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="44" t="s">
+      <c r="A27" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="44"/>
-      <c r="C27" s="44"/>
-      <c r="D27" s="44"/>
-      <c r="E27" s="44"/>
-      <c r="F27" s="44"/>
-      <c r="G27" s="44"/>
-      <c r="H27" s="44"/>
-      <c r="I27" s="44"/>
-      <c r="J27" s="44"/>
+      <c r="B27" s="38"/>
+      <c r="C27" s="38"/>
+      <c r="D27" s="38"/>
+      <c r="E27" s="38"/>
+      <c r="F27" s="38"/>
+      <c r="G27" s="38"/>
+      <c r="H27" s="38"/>
+      <c r="I27" s="38"/>
+      <c r="J27" s="38"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="45" t="s">
+      <c r="A28" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="45"/>
-      <c r="C28" s="45"/>
-      <c r="D28" s="45"/>
-      <c r="E28" s="45"/>
-      <c r="F28" s="45"/>
-      <c r="G28" s="45"/>
-      <c r="H28" s="45"/>
-      <c r="I28" s="45"/>
-      <c r="J28" s="45"/>
+      <c r="B28" s="39"/>
+      <c r="C28" s="39"/>
+      <c r="D28" s="39"/>
+      <c r="E28" s="39"/>
+      <c r="F28" s="39"/>
+      <c r="G28" s="39"/>
+      <c r="H28" s="39"/>
+      <c r="I28" s="39"/>
+      <c r="J28" s="39"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="46" t="s">
+      <c r="A29" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="46"/>
-      <c r="C29" s="46"/>
-      <c r="D29" s="46"/>
-      <c r="E29" s="46"/>
-      <c r="F29" s="46"/>
-      <c r="G29" s="46"/>
-      <c r="H29" s="46"/>
-      <c r="I29" s="46"/>
-      <c r="J29" s="46"/>
+      <c r="B29" s="47"/>
+      <c r="C29" s="47"/>
+      <c r="D29" s="47"/>
+      <c r="E29" s="47"/>
+      <c r="F29" s="47"/>
+      <c r="G29" s="47"/>
+      <c r="H29" s="47"/>
+      <c r="I29" s="47"/>
+      <c r="J29" s="47"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="47" t="s">
+      <c r="A30" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="47"/>
-      <c r="C30" s="47"/>
-      <c r="D30" s="47"/>
-      <c r="E30" s="47"/>
-      <c r="F30" s="47"/>
-      <c r="G30" s="47"/>
-      <c r="H30" s="47"/>
-      <c r="I30" s="47"/>
-      <c r="J30" s="47"/>
+      <c r="B30" s="40"/>
+      <c r="C30" s="40"/>
+      <c r="D30" s="40"/>
+      <c r="E30" s="40"/>
+      <c r="F30" s="40"/>
+      <c r="G30" s="40"/>
+      <c r="H30" s="40"/>
+      <c r="I30" s="40"/>
+      <c r="J30" s="40"/>
     </row>
     <row r="31" spans="1:10" ht="24.95" customHeight="1">
       <c r="A31" s="6"/>
@@ -2832,10 +2832,10 @@
       <c r="D31" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="48" t="s">
+      <c r="E31" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="48"/>
+      <c r="F31" s="37"/>
       <c r="G31" s="15" t="s">
         <v>5</v>
       </c>
@@ -2850,10 +2850,10 @@
       <c r="D32" s="16">
         <v>1000</v>
       </c>
-      <c r="E32" s="43">
+      <c r="E32" s="41">
         <v>50</v>
       </c>
-      <c r="F32" s="43"/>
+      <c r="F32" s="41"/>
       <c r="G32" s="16">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>50000</v>
@@ -2869,10 +2869,10 @@
       <c r="D33" s="16">
         <v>500</v>
       </c>
-      <c r="E33" s="43">
+      <c r="E33" s="41">
         <v>116</v>
       </c>
-      <c r="F33" s="43"/>
+      <c r="F33" s="41"/>
       <c r="G33" s="16">
         <f t="shared" si="1"/>
         <v>58000</v>
@@ -2888,10 +2888,10 @@
       <c r="D34" s="16">
         <v>100</v>
       </c>
-      <c r="E34" s="43">
+      <c r="E34" s="41">
         <v>151</v>
       </c>
-      <c r="F34" s="43"/>
+      <c r="F34" s="41"/>
       <c r="G34" s="16">
         <f t="shared" si="1"/>
         <v>15100</v>
@@ -2907,10 +2907,10 @@
       <c r="D35" s="16">
         <v>50</v>
       </c>
-      <c r="E35" s="43">
+      <c r="E35" s="41">
         <v>58</v>
       </c>
-      <c r="F35" s="43"/>
+      <c r="F35" s="41"/>
       <c r="G35" s="16">
         <f t="shared" si="1"/>
         <v>2900</v>
@@ -2926,8 +2926,8 @@
       <c r="D36" s="16">
         <v>20</v>
       </c>
-      <c r="E36" s="43"/>
-      <c r="F36" s="43"/>
+      <c r="E36" s="41"/>
+      <c r="F36" s="41"/>
       <c r="G36" s="16">
         <f>SUM(D36*E36)</f>
         <v>0</v>
@@ -2943,8 +2943,8 @@
       <c r="D37" s="16">
         <v>10</v>
       </c>
-      <c r="E37" s="43"/>
-      <c r="F37" s="43"/>
+      <c r="E37" s="41"/>
+      <c r="F37" s="41"/>
       <c r="G37" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2957,10 +2957,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="39" t="s">
+      <c r="D38" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="40"/>
+      <c r="E38" s="49"/>
       <c r="F38" s="15"/>
       <c r="G38" s="15">
         <f>SUM(G32:G37)</f>
@@ -3007,58 +3007,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" ht="15.75">
-      <c r="A42" s="41" t="s">
+      <c r="A42" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="41"/>
+      <c r="B42" s="50"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="41" t="s">
+      <c r="H42" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="41"/>
-      <c r="J42" s="41"/>
+      <c r="I42" s="50"/>
+      <c r="J42" s="50"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="42"/>
-      <c r="B43" s="42"/>
+      <c r="A43" s="43"/>
+      <c r="B43" s="43"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="42"/>
-      <c r="I43" s="42"/>
-      <c r="J43" s="42"/>
+      <c r="H43" s="43"/>
+      <c r="I43" s="43"/>
+      <c r="J43" s="43"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="42"/>
-      <c r="B44" s="42"/>
+      <c r="A44" s="43"/>
+      <c r="B44" s="43"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="42"/>
-      <c r="I44" s="42"/>
-      <c r="J44" s="42"/>
+      <c r="H44" s="43"/>
+      <c r="I44" s="43"/>
+      <c r="J44" s="43"/>
     </row>
     <row r="45" spans="1:10" ht="15.75">
-      <c r="A45" s="42"/>
-      <c r="B45" s="42"/>
+      <c r="A45" s="43"/>
+      <c r="B45" s="43"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="42" t="s">
+      <c r="H45" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="41"/>
-      <c r="J45" s="41"/>
+      <c r="I45" s="50"/>
+      <c r="J45" s="50"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="6"/>
@@ -3068,11 +3068,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="37" t="s">
+      <c r="H46" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="38"/>
-      <c r="J46" s="38"/>
+      <c r="I46" s="46"/>
+      <c r="J46" s="46"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -3100,6 +3100,32 @@
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -3112,32 +3138,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.25" footer="0"/>
   <pageSetup scale="85" orientation="portrait" r:id="rId1"/>
@@ -3149,8 +3149,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection sqref="A1:J46"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3169,64 +3169,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="58" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
-      <c r="G1" s="51"/>
-      <c r="H1" s="51"/>
-      <c r="I1" s="51"/>
-      <c r="J1" s="51"/>
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+      <c r="G1" s="58"/>
+      <c r="H1" s="58"/>
+      <c r="I1" s="58"/>
+      <c r="J1" s="58"/>
       <c r="K1" s="24"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="52" t="s">
+      <c r="A2" s="59" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="52"/>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="52"/>
-      <c r="I2" s="52"/>
-      <c r="J2" s="52"/>
+      <c r="B2" s="59"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="59"/>
+      <c r="H2" s="59"/>
+      <c r="I2" s="59"/>
+      <c r="J2" s="59"/>
       <c r="K2" s="24"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="52" t="s">
+      <c r="A3" s="59" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="52"/>
-      <c r="C3" s="52"/>
-      <c r="D3" s="52"/>
-      <c r="E3" s="52"/>
-      <c r="F3" s="52"/>
-      <c r="G3" s="52"/>
-      <c r="H3" s="52"/>
-      <c r="I3" s="52"/>
-      <c r="J3" s="52"/>
+      <c r="B3" s="59"/>
+      <c r="C3" s="59"/>
+      <c r="D3" s="59"/>
+      <c r="E3" s="59"/>
+      <c r="F3" s="59"/>
+      <c r="G3" s="59"/>
+      <c r="H3" s="59"/>
+      <c r="I3" s="59"/>
+      <c r="J3" s="59"/>
       <c r="K3" s="24"/>
     </row>
     <row r="4" spans="1:11" ht="26.25">
-      <c r="A4" s="55">
+      <c r="A4" s="66">
         <f ca="1">TODAY()</f>
-        <v>44014</v>
-      </c>
-      <c r="B4" s="55"/>
-      <c r="C4" s="55"/>
-      <c r="D4" s="55"/>
-      <c r="E4" s="55"/>
-      <c r="F4" s="55"/>
-      <c r="G4" s="55"/>
-      <c r="H4" s="55"/>
-      <c r="I4" s="55"/>
-      <c r="J4" s="55"/>
+        <v>44021</v>
+      </c>
+      <c r="B4" s="66"/>
+      <c r="C4" s="66"/>
+      <c r="D4" s="66"/>
+      <c r="E4" s="66"/>
+      <c r="F4" s="66"/>
+      <c r="G4" s="66"/>
+      <c r="H4" s="66"/>
+      <c r="I4" s="66"/>
+      <c r="J4" s="66"/>
       <c r="K4" s="24"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -3236,10 +3236,10 @@
       <c r="D5" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="53" t="s">
+      <c r="E5" s="61" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="53"/>
+      <c r="F5" s="61"/>
       <c r="G5" s="26" t="s">
         <v>5</v>
       </c>
@@ -3254,13 +3254,13 @@
       <c r="D6" s="27">
         <v>1000</v>
       </c>
-      <c r="E6" s="54">
-        <v>100</v>
-      </c>
-      <c r="F6" s="54"/>
+      <c r="E6" s="62">
+        <v>162</v>
+      </c>
+      <c r="F6" s="62"/>
       <c r="G6" s="27">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
-        <v>100000</v>
+        <v>162000</v>
       </c>
       <c r="H6" s="25"/>
       <c r="I6" s="25"/>
@@ -3273,13 +3273,13 @@
       <c r="D7" s="27">
         <v>500</v>
       </c>
-      <c r="E7" s="54">
-        <v>500</v>
-      </c>
-      <c r="F7" s="54"/>
+      <c r="E7" s="62">
+        <v>476</v>
+      </c>
+      <c r="F7" s="62"/>
       <c r="G7" s="27">
         <f t="shared" si="0"/>
-        <v>250000</v>
+        <v>238000</v>
       </c>
       <c r="H7" s="25"/>
       <c r="I7" s="25"/>
@@ -3292,10 +3292,10 @@
       <c r="D8" s="27">
         <v>100</v>
       </c>
-      <c r="E8" s="54">
+      <c r="E8" s="62">
         <v>500</v>
       </c>
-      <c r="F8" s="54"/>
+      <c r="F8" s="62"/>
       <c r="G8" s="27">
         <f t="shared" si="0"/>
         <v>50000</v>
@@ -3311,8 +3311,8 @@
       <c r="D9" s="27">
         <v>50</v>
       </c>
-      <c r="E9" s="54"/>
-      <c r="F9" s="54"/>
+      <c r="E9" s="62"/>
+      <c r="F9" s="62"/>
       <c r="G9" s="27">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3328,8 +3328,8 @@
       <c r="D10" s="27">
         <v>20</v>
       </c>
-      <c r="E10" s="54"/>
-      <c r="F10" s="54"/>
+      <c r="E10" s="62"/>
+      <c r="F10" s="62"/>
       <c r="G10" s="27">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3345,8 +3345,8 @@
       <c r="D11" s="27">
         <v>10</v>
       </c>
-      <c r="E11" s="54"/>
-      <c r="F11" s="54"/>
+      <c r="E11" s="62"/>
+      <c r="F11" s="62"/>
       <c r="G11" s="27">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3359,14 +3359,14 @@
       <c r="A12" s="25"/>
       <c r="B12" s="25"/>
       <c r="C12" s="25"/>
-      <c r="D12" s="54" t="s">
+      <c r="D12" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="54"/>
+      <c r="E12" s="62"/>
       <c r="F12" s="27"/>
       <c r="G12" s="22">
         <f>SUM(G6:G11)</f>
-        <v>400000</v>
+        <v>450000</v>
       </c>
       <c r="H12" s="25"/>
       <c r="I12" s="25"/>
@@ -3410,59 +3410,59 @@
     </row>
     <row r="16" spans="1:11">
       <c r="A16" s="28"/>
-      <c r="B16" s="57" t="s">
+      <c r="B16" s="69" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="57"/>
-      <c r="D16" s="57"/>
+      <c r="C16" s="69"/>
+      <c r="D16" s="69"/>
       <c r="E16" s="28"/>
       <c r="F16" s="29"/>
       <c r="G16" s="29"/>
-      <c r="H16" s="56" t="s">
+      <c r="H16" s="68" t="s">
         <v>7</v>
       </c>
-      <c r="I16" s="56"/>
-      <c r="J16" s="56"/>
+      <c r="I16" s="68"/>
+      <c r="J16" s="68"/>
     </row>
     <row r="17" spans="1:11">
-      <c r="A17" s="56"/>
-      <c r="B17" s="56"/>
-      <c r="C17" s="56"/>
-      <c r="D17" s="56"/>
+      <c r="A17" s="68"/>
+      <c r="B17" s="68"/>
+      <c r="C17" s="68"/>
+      <c r="D17" s="68"/>
       <c r="E17" s="29"/>
       <c r="F17" s="29"/>
       <c r="G17" s="29"/>
-      <c r="H17" s="56"/>
-      <c r="I17" s="56"/>
-      <c r="J17" s="56"/>
+      <c r="H17" s="68"/>
+      <c r="I17" s="68"/>
+      <c r="J17" s="68"/>
     </row>
     <row r="18" spans="1:11">
-      <c r="A18" s="56"/>
-      <c r="B18" s="56"/>
-      <c r="C18" s="56"/>
-      <c r="D18" s="56"/>
+      <c r="A18" s="68"/>
+      <c r="B18" s="68"/>
+      <c r="C18" s="68"/>
+      <c r="D18" s="68"/>
       <c r="E18" s="29"/>
       <c r="F18" s="29"/>
       <c r="G18" s="29"/>
-      <c r="H18" s="56"/>
-      <c r="I18" s="56"/>
-      <c r="J18" s="56"/>
+      <c r="H18" s="68"/>
+      <c r="I18" s="68"/>
+      <c r="J18" s="68"/>
     </row>
     <row r="19" spans="1:11" ht="17.25" customHeight="1">
       <c r="A19" s="33"/>
-      <c r="B19" s="58" t="s">
+      <c r="B19" s="67" t="s">
         <v>28</v>
       </c>
-      <c r="C19" s="58"/>
-      <c r="D19" s="58"/>
+      <c r="C19" s="67"/>
+      <c r="D19" s="67"/>
       <c r="E19" s="29"/>
       <c r="F19" s="29"/>
       <c r="G19" s="29"/>
-      <c r="H19" s="49" t="s">
+      <c r="H19" s="42" t="s">
         <v>30</v>
       </c>
-      <c r="I19" s="49"/>
-      <c r="J19" s="49"/>
+      <c r="I19" s="42"/>
+      <c r="J19" s="42"/>
     </row>
     <row r="20" spans="1:11">
       <c r="A20" s="25"/>
@@ -3472,9 +3472,9 @@
       <c r="E20" s="25"/>
       <c r="F20" s="25"/>
       <c r="G20" s="25"/>
-      <c r="H20" s="61"/>
-      <c r="I20" s="62"/>
-      <c r="J20" s="62"/>
+      <c r="H20" s="53"/>
+      <c r="I20" s="54"/>
+      <c r="J20" s="54"/>
     </row>
     <row r="21" spans="1:11">
       <c r="A21" s="25"/>
@@ -3561,66 +3561,66 @@
       <c r="J27" s="25"/>
     </row>
     <row r="28" spans="1:11" ht="31.5">
-      <c r="A28" s="51" t="s">
+      <c r="A28" s="58" t="s">
         <v>26</v>
       </c>
-      <c r="B28" s="51"/>
-      <c r="C28" s="51"/>
-      <c r="D28" s="51"/>
-      <c r="E28" s="51"/>
-      <c r="F28" s="51"/>
-      <c r="G28" s="51"/>
-      <c r="H28" s="51"/>
-      <c r="I28" s="51"/>
-      <c r="J28" s="51"/>
+      <c r="B28" s="58"/>
+      <c r="C28" s="58"/>
+      <c r="D28" s="58"/>
+      <c r="E28" s="58"/>
+      <c r="F28" s="58"/>
+      <c r="G28" s="58"/>
+      <c r="H28" s="58"/>
+      <c r="I28" s="58"/>
+      <c r="J28" s="58"/>
     </row>
     <row r="29" spans="1:11" ht="18">
-      <c r="A29" s="52" t="str">
+      <c r="A29" s="59" t="str">
         <f>A2</f>
         <v>Komola Super Market, Alaipur, Natore</v>
       </c>
-      <c r="B29" s="52"/>
-      <c r="C29" s="52"/>
-      <c r="D29" s="52"/>
-      <c r="E29" s="52"/>
-      <c r="F29" s="52"/>
-      <c r="G29" s="52"/>
-      <c r="H29" s="52"/>
-      <c r="I29" s="52"/>
-      <c r="J29" s="52"/>
+      <c r="B29" s="59"/>
+      <c r="C29" s="59"/>
+      <c r="D29" s="59"/>
+      <c r="E29" s="59"/>
+      <c r="F29" s="59"/>
+      <c r="G29" s="59"/>
+      <c r="H29" s="59"/>
+      <c r="I29" s="59"/>
+      <c r="J29" s="59"/>
     </row>
     <row r="30" spans="1:11" ht="18.75">
-      <c r="A30" s="66" t="str">
+      <c r="A30" s="60" t="str">
         <f>A3</f>
         <v>Cash Details As Per Below</v>
       </c>
-      <c r="B30" s="66"/>
-      <c r="C30" s="66"/>
-      <c r="D30" s="66"/>
-      <c r="E30" s="66"/>
-      <c r="F30" s="66"/>
-      <c r="G30" s="66"/>
-      <c r="H30" s="66"/>
-      <c r="I30" s="66"/>
-      <c r="J30" s="66"/>
+      <c r="B30" s="60"/>
+      <c r="C30" s="60"/>
+      <c r="D30" s="60"/>
+      <c r="E30" s="60"/>
+      <c r="F30" s="60"/>
+      <c r="G30" s="60"/>
+      <c r="H30" s="60"/>
+      <c r="I30" s="60"/>
+      <c r="J30" s="60"/>
       <c r="K30" s="6" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="26.25">
-      <c r="A31" s="55">
+      <c r="A31" s="66">
         <f ca="1">TODAY()</f>
-        <v>44014</v>
-      </c>
-      <c r="B31" s="55"/>
-      <c r="C31" s="55"/>
-      <c r="D31" s="55"/>
-      <c r="E31" s="55"/>
-      <c r="F31" s="55"/>
-      <c r="G31" s="55"/>
-      <c r="H31" s="55"/>
-      <c r="I31" s="55"/>
-      <c r="J31" s="55"/>
+        <v>44021</v>
+      </c>
+      <c r="B31" s="66"/>
+      <c r="C31" s="66"/>
+      <c r="D31" s="66"/>
+      <c r="E31" s="66"/>
+      <c r="F31" s="66"/>
+      <c r="G31" s="66"/>
+      <c r="H31" s="66"/>
+      <c r="I31" s="66"/>
+      <c r="J31" s="66"/>
     </row>
     <row r="32" spans="1:11" ht="27.95" customHeight="1">
       <c r="A32" s="25"/>
@@ -3629,10 +3629,10 @@
       <c r="D32" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="53" t="s">
+      <c r="E32" s="61" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="53"/>
+      <c r="F32" s="61"/>
       <c r="G32" s="26" t="s">
         <v>5</v>
       </c>
@@ -3647,14 +3647,14 @@
       <c r="D33" s="30">
         <v>1000</v>
       </c>
-      <c r="E33" s="54">
+      <c r="E33" s="62">
         <f>E6</f>
-        <v>100</v>
-      </c>
-      <c r="F33" s="54"/>
+        <v>162</v>
+      </c>
+      <c r="F33" s="62"/>
       <c r="G33" s="30">
         <f t="shared" ref="G33:G38" si="1">SUM(D33*E33)</f>
-        <v>100000</v>
+        <v>162000</v>
       </c>
       <c r="H33" s="25"/>
       <c r="I33" s="25"/>
@@ -3667,14 +3667,14 @@
       <c r="D34" s="30">
         <v>500</v>
       </c>
-      <c r="E34" s="54">
+      <c r="E34" s="62">
         <f>E7</f>
-        <v>500</v>
-      </c>
-      <c r="F34" s="54"/>
+        <v>476</v>
+      </c>
+      <c r="F34" s="62"/>
       <c r="G34" s="30">
         <f t="shared" si="1"/>
-        <v>250000</v>
+        <v>238000</v>
       </c>
       <c r="H34" s="25"/>
       <c r="I34" s="25"/>
@@ -3687,11 +3687,11 @@
       <c r="D35" s="30">
         <v>100</v>
       </c>
-      <c r="E35" s="54">
+      <c r="E35" s="62">
         <f>E8</f>
         <v>500</v>
       </c>
-      <c r="F35" s="54"/>
+      <c r="F35" s="62"/>
       <c r="G35" s="30">
         <f t="shared" si="1"/>
         <v>50000</v>
@@ -3707,8 +3707,8 @@
       <c r="D36" s="30">
         <v>50</v>
       </c>
-      <c r="E36" s="54"/>
-      <c r="F36" s="54"/>
+      <c r="E36" s="62"/>
+      <c r="F36" s="62"/>
       <c r="G36" s="30">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -3724,8 +3724,8 @@
       <c r="D37" s="30">
         <v>20</v>
       </c>
-      <c r="E37" s="54"/>
-      <c r="F37" s="54"/>
+      <c r="E37" s="62"/>
+      <c r="F37" s="62"/>
       <c r="G37" s="30">
         <f>SUM(D37*E37)</f>
         <v>0</v>
@@ -3741,8 +3741,8 @@
       <c r="D38" s="30">
         <v>10</v>
       </c>
-      <c r="E38" s="54"/>
-      <c r="F38" s="54"/>
+      <c r="E38" s="62"/>
+      <c r="F38" s="62"/>
       <c r="G38" s="30">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -3755,14 +3755,14 @@
       <c r="A39" s="25"/>
       <c r="B39" s="25"/>
       <c r="C39" s="25"/>
-      <c r="D39" s="67" t="s">
+      <c r="D39" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="68"/>
+      <c r="E39" s="64"/>
       <c r="F39" s="30"/>
       <c r="G39" s="23">
         <f>SUM(G33:G38)</f>
-        <v>400000</v>
+        <v>450000</v>
       </c>
       <c r="H39" s="25"/>
       <c r="I39" s="25"/>
@@ -3814,53 +3814,53 @@
       <c r="E43" s="29"/>
       <c r="F43" s="29"/>
       <c r="G43" s="29"/>
-      <c r="H43" s="63" t="s">
+      <c r="H43" s="55" t="s">
         <v>7</v>
       </c>
-      <c r="I43" s="63"/>
-      <c r="J43" s="63"/>
+      <c r="I43" s="55"/>
+      <c r="J43" s="55"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="64"/>
-      <c r="B44" s="64"/>
-      <c r="C44" s="64"/>
-      <c r="D44" s="64"/>
+      <c r="A44" s="56"/>
+      <c r="B44" s="56"/>
+      <c r="C44" s="56"/>
+      <c r="D44" s="56"/>
       <c r="E44" s="25"/>
       <c r="F44" s="25"/>
       <c r="G44" s="25"/>
-      <c r="H44" s="64"/>
-      <c r="I44" s="64"/>
-      <c r="J44" s="64"/>
+      <c r="H44" s="56"/>
+      <c r="I44" s="56"/>
+      <c r="J44" s="56"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="64"/>
-      <c r="B45" s="64"/>
-      <c r="C45" s="64"/>
-      <c r="D45" s="64"/>
+      <c r="A45" s="56"/>
+      <c r="B45" s="56"/>
+      <c r="C45" s="56"/>
+      <c r="D45" s="56"/>
       <c r="E45" s="25"/>
       <c r="F45" s="25"/>
       <c r="G45" s="25"/>
-      <c r="H45" s="64"/>
-      <c r="I45" s="64"/>
-      <c r="J45" s="64"/>
+      <c r="H45" s="56"/>
+      <c r="I45" s="56"/>
+      <c r="J45" s="56"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="31"/>
-      <c r="B46" s="69" t="str">
+      <c r="B46" s="65" t="str">
         <f>B19</f>
         <v>Rahinul Kabir</v>
       </c>
-      <c r="C46" s="69"/>
-      <c r="D46" s="69"/>
+      <c r="C46" s="65"/>
+      <c r="D46" s="65"/>
       <c r="E46" s="32"/>
       <c r="F46" s="32"/>
       <c r="G46" s="32"/>
-      <c r="H46" s="65" t="str">
+      <c r="H46" s="57" t="str">
         <f>H19</f>
         <v>Jafor Iqbal</v>
       </c>
-      <c r="I46" s="65"/>
-      <c r="J46" s="65"/>
+      <c r="I46" s="57"/>
+      <c r="J46" s="57"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="21"/>
@@ -3870,12 +3870,35 @@
       <c r="E47" s="21"/>
       <c r="F47" s="21"/>
       <c r="G47" s="21"/>
-      <c r="H47" s="59"/>
-      <c r="I47" s="60"/>
-      <c r="J47" s="60"/>
+      <c r="H47" s="51"/>
+      <c r="I47" s="52"/>
+      <c r="J47" s="52"/>
     </row>
   </sheetData>
   <mergeCells count="37">
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="A17:D18"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="A31:J31"/>
+    <mergeCell ref="B19:D19"/>
     <mergeCell ref="H47:J47"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="H43:J43"/>
@@ -3890,29 +3913,6 @@
     <mergeCell ref="D39:E39"/>
     <mergeCell ref="B46:D46"/>
     <mergeCell ref="A44:D45"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="A31:J31"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="A17:D18"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="A4:J4"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -3944,63 +3944,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="44"/>
-      <c r="J1" s="44"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="45"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="45"/>
-      <c r="H2" s="45"/>
-      <c r="I2" s="45"/>
-      <c r="J2" s="45"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="39"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="45" t="s">
+      <c r="A3" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="45"/>
-      <c r="C3" s="45"/>
-      <c r="D3" s="45"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="45"/>
-      <c r="G3" s="45"/>
-      <c r="H3" s="45"/>
-      <c r="I3" s="45"/>
-      <c r="J3" s="45"/>
+      <c r="B3" s="39"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="39"/>
+      <c r="J3" s="39"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="47" t="s">
+      <c r="A4" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="47"/>
-      <c r="C4" s="47"/>
-      <c r="D4" s="47"/>
-      <c r="E4" s="47"/>
-      <c r="F4" s="47"/>
-      <c r="G4" s="47"/>
-      <c r="H4" s="47"/>
-      <c r="I4" s="47"/>
-      <c r="J4" s="47"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="40"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -4010,10 +4010,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="48" t="s">
+      <c r="E5" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="48"/>
+      <c r="F5" s="37"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -4028,10 +4028,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="43">
+      <c r="E6" s="41">
         <v>68</v>
       </c>
-      <c r="F6" s="43"/>
+      <c r="F6" s="41"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>68000</v>
@@ -4047,10 +4047,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="43">
+      <c r="E7" s="41">
         <v>135</v>
       </c>
-      <c r="F7" s="43"/>
+      <c r="F7" s="41"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>67500</v>
@@ -4066,10 +4066,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="43">
+      <c r="E8" s="41">
         <v>53</v>
       </c>
-      <c r="F8" s="43"/>
+      <c r="F8" s="41"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>5300</v>
@@ -4085,10 +4085,10 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="43">
+      <c r="E9" s="41">
         <v>2</v>
       </c>
-      <c r="F9" s="43"/>
+      <c r="F9" s="41"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -4104,10 +4104,10 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="43">
+      <c r="E10" s="41">
         <v>5</v>
       </c>
-      <c r="F10" s="43"/>
+      <c r="F10" s="41"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -4123,8 +4123,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="43"/>
-      <c r="F11" s="43"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="41"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4137,10 +4137,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="48" t="s">
+      <c r="D12" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="48"/>
+      <c r="E12" s="37"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -4187,76 +4187,76 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="49" t="s">
+      <c r="A16" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="49"/>
+      <c r="B16" s="42"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="49" t="s">
+      <c r="H16" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="49"/>
-      <c r="J16" s="49"/>
+      <c r="I16" s="42"/>
+      <c r="J16" s="42"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="49"/>
-      <c r="B17" s="49"/>
+      <c r="A17" s="42"/>
+      <c r="B17" s="42"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="49"/>
-      <c r="I17" s="49"/>
-      <c r="J17" s="49"/>
+      <c r="H17" s="42"/>
+      <c r="I17" s="42"/>
+      <c r="J17" s="42"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="49"/>
-      <c r="B18" s="49"/>
+      <c r="A18" s="42"/>
+      <c r="B18" s="42"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="49"/>
-      <c r="I18" s="49"/>
-      <c r="J18" s="49"/>
+      <c r="H18" s="42"/>
+      <c r="I18" s="42"/>
+      <c r="J18" s="42"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="42" t="s">
+      <c r="A19" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="42"/>
+      <c r="B19" s="43"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="50" t="s">
+      <c r="H19" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="50"/>
-      <c r="J19" s="50"/>
+      <c r="I19" s="44"/>
+      <c r="J19" s="44"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="71" t="s">
+      <c r="A20" s="70" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="71"/>
+      <c r="B20" s="70"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="37" t="s">
+      <c r="H20" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="38"/>
-      <c r="J20" s="38"/>
+      <c r="I20" s="46"/>
+      <c r="J20" s="46"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4331,60 +4331,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="44" t="s">
+      <c r="A27" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="44"/>
-      <c r="C27" s="44"/>
-      <c r="D27" s="44"/>
-      <c r="E27" s="44"/>
-      <c r="F27" s="44"/>
-      <c r="G27" s="44"/>
-      <c r="H27" s="44"/>
-      <c r="I27" s="44"/>
-      <c r="J27" s="44"/>
+      <c r="B27" s="38"/>
+      <c r="C27" s="38"/>
+      <c r="D27" s="38"/>
+      <c r="E27" s="38"/>
+      <c r="F27" s="38"/>
+      <c r="G27" s="38"/>
+      <c r="H27" s="38"/>
+      <c r="I27" s="38"/>
+      <c r="J27" s="38"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="45" t="s">
+      <c r="A28" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="45"/>
-      <c r="C28" s="45"/>
-      <c r="D28" s="45"/>
-      <c r="E28" s="45"/>
-      <c r="F28" s="45"/>
-      <c r="G28" s="45"/>
-      <c r="H28" s="45"/>
-      <c r="I28" s="45"/>
-      <c r="J28" s="45"/>
+      <c r="B28" s="39"/>
+      <c r="C28" s="39"/>
+      <c r="D28" s="39"/>
+      <c r="E28" s="39"/>
+      <c r="F28" s="39"/>
+      <c r="G28" s="39"/>
+      <c r="H28" s="39"/>
+      <c r="I28" s="39"/>
+      <c r="J28" s="39"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="46" t="s">
+      <c r="A29" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="46"/>
-      <c r="C29" s="46"/>
-      <c r="D29" s="46"/>
-      <c r="E29" s="46"/>
-      <c r="F29" s="46"/>
-      <c r="G29" s="46"/>
-      <c r="H29" s="46"/>
-      <c r="I29" s="46"/>
-      <c r="J29" s="46"/>
+      <c r="B29" s="47"/>
+      <c r="C29" s="47"/>
+      <c r="D29" s="47"/>
+      <c r="E29" s="47"/>
+      <c r="F29" s="47"/>
+      <c r="G29" s="47"/>
+      <c r="H29" s="47"/>
+      <c r="I29" s="47"/>
+      <c r="J29" s="47"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="47" t="s">
+      <c r="A30" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="47"/>
-      <c r="C30" s="47"/>
-      <c r="D30" s="47"/>
-      <c r="E30" s="47"/>
-      <c r="F30" s="47"/>
-      <c r="G30" s="47"/>
-      <c r="H30" s="47"/>
-      <c r="I30" s="47"/>
-      <c r="J30" s="47"/>
+      <c r="B30" s="40"/>
+      <c r="C30" s="40"/>
+      <c r="D30" s="40"/>
+      <c r="E30" s="40"/>
+      <c r="F30" s="40"/>
+      <c r="G30" s="40"/>
+      <c r="H30" s="40"/>
+      <c r="I30" s="40"/>
+      <c r="J30" s="40"/>
     </row>
     <row r="31" spans="1:10" ht="20.25">
       <c r="A31" s="6"/>
@@ -4393,10 +4393,10 @@
       <c r="D31" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="70" t="s">
+      <c r="E31" s="74" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="70"/>
+      <c r="F31" s="74"/>
       <c r="G31" s="9" t="s">
         <v>5</v>
       </c>
@@ -4411,10 +4411,10 @@
       <c r="D32" s="2">
         <v>1000</v>
       </c>
-      <c r="E32" s="74">
+      <c r="E32" s="73">
         <v>68</v>
       </c>
-      <c r="F32" s="74"/>
+      <c r="F32" s="73"/>
       <c r="G32" s="2">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>68000</v>
@@ -4430,10 +4430,10 @@
       <c r="D33" s="2">
         <v>500</v>
       </c>
-      <c r="E33" s="74">
+      <c r="E33" s="73">
         <v>135</v>
       </c>
-      <c r="F33" s="74"/>
+      <c r="F33" s="73"/>
       <c r="G33" s="2">
         <f t="shared" si="1"/>
         <v>67500</v>
@@ -4449,10 +4449,10 @@
       <c r="D34" s="2">
         <v>100</v>
       </c>
-      <c r="E34" s="74">
+      <c r="E34" s="73">
         <v>53</v>
       </c>
-      <c r="F34" s="74"/>
+      <c r="F34" s="73"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
         <v>5300</v>
@@ -4468,10 +4468,10 @@
       <c r="D35" s="2">
         <v>50</v>
       </c>
-      <c r="E35" s="74">
+      <c r="E35" s="73">
         <v>2</v>
       </c>
-      <c r="F35" s="74"/>
+      <c r="F35" s="73"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4487,10 +4487,10 @@
       <c r="D36" s="2">
         <v>20</v>
       </c>
-      <c r="E36" s="74">
+      <c r="E36" s="73">
         <v>5</v>
       </c>
-      <c r="F36" s="74"/>
+      <c r="F36" s="73"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4506,8 +4506,8 @@
       <c r="D37" s="2">
         <v>10</v>
       </c>
-      <c r="E37" s="74"/>
-      <c r="F37" s="74"/>
+      <c r="E37" s="73"/>
+      <c r="F37" s="73"/>
       <c r="G37" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4520,10 +4520,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="73" t="s">
+      <c r="D38" s="72" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="73"/>
+      <c r="E38" s="72"/>
       <c r="F38" s="9"/>
       <c r="G38" s="9">
         <f>SUM(G32:G37)</f>
@@ -4570,76 +4570,76 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="41" t="s">
+      <c r="A42" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="41"/>
+      <c r="B42" s="50"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="41" t="s">
+      <c r="H42" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="41"/>
-      <c r="J42" s="41"/>
+      <c r="I42" s="50"/>
+      <c r="J42" s="50"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="42"/>
-      <c r="B43" s="42"/>
+      <c r="A43" s="43"/>
+      <c r="B43" s="43"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="42"/>
-      <c r="I43" s="42"/>
-      <c r="J43" s="42"/>
+      <c r="H43" s="43"/>
+      <c r="I43" s="43"/>
+      <c r="J43" s="43"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="42"/>
-      <c r="B44" s="42"/>
+      <c r="A44" s="43"/>
+      <c r="B44" s="43"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="42"/>
-      <c r="I44" s="42"/>
-      <c r="J44" s="42"/>
+      <c r="H44" s="43"/>
+      <c r="I44" s="43"/>
+      <c r="J44" s="43"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="42" t="s">
+      <c r="A45" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="B45" s="42"/>
+      <c r="B45" s="43"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="42" t="s">
+      <c r="H45" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="41"/>
-      <c r="J45" s="41"/>
+      <c r="I45" s="50"/>
+      <c r="J45" s="50"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="72" t="s">
+      <c r="A46" s="71" t="s">
         <v>14</v>
       </c>
-      <c r="B46" s="72"/>
+      <c r="B46" s="71"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="37" t="s">
+      <c r="H46" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="38"/>
-      <c r="J46" s="38"/>
+      <c r="I46" s="46"/>
+      <c r="J46" s="46"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -4667,6 +4667,30 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
     <mergeCell ref="H46:J46"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A46:B46"/>
@@ -4683,30 +4707,6 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -4738,63 +4738,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="44"/>
-      <c r="J1" s="44"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="45"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="45"/>
-      <c r="H2" s="45"/>
-      <c r="I2" s="45"/>
-      <c r="J2" s="45"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="39"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="45" t="s">
+      <c r="A3" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="45"/>
-      <c r="C3" s="45"/>
-      <c r="D3" s="45"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="45"/>
-      <c r="G3" s="45"/>
-      <c r="H3" s="45"/>
-      <c r="I3" s="45"/>
-      <c r="J3" s="45"/>
+      <c r="B3" s="39"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="39"/>
+      <c r="J3" s="39"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="47" t="s">
+      <c r="A4" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="47"/>
-      <c r="C4" s="47"/>
-      <c r="D4" s="47"/>
-      <c r="E4" s="47"/>
-      <c r="F4" s="47"/>
-      <c r="G4" s="47"/>
-      <c r="H4" s="47"/>
-      <c r="I4" s="47"/>
-      <c r="J4" s="47"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="40"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -4804,10 +4804,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="48" t="s">
+      <c r="E5" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="48"/>
+      <c r="F5" s="37"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -4822,10 +4822,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="43">
+      <c r="E6" s="41">
         <v>44</v>
       </c>
-      <c r="F6" s="43"/>
+      <c r="F6" s="41"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>44000</v>
@@ -4841,10 +4841,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="43">
+      <c r="E7" s="41">
         <v>118</v>
       </c>
-      <c r="F7" s="43"/>
+      <c r="F7" s="41"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>59000</v>
@@ -4860,10 +4860,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="43">
+      <c r="E8" s="41">
         <v>510</v>
       </c>
-      <c r="F8" s="43"/>
+      <c r="F8" s="41"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>51000</v>
@@ -4879,8 +4879,8 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="43"/>
-      <c r="F9" s="43"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="41"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4896,8 +4896,8 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="43"/>
-      <c r="F10" s="43"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="41"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4913,8 +4913,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="43"/>
-      <c r="F11" s="43"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="41"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4927,10 +4927,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="48" t="s">
+      <c r="D12" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="48"/>
+      <c r="E12" s="37"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -4977,72 +4977,72 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="49" t="s">
+      <c r="A16" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="49"/>
+      <c r="B16" s="42"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="49" t="s">
+      <c r="H16" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="49"/>
-      <c r="J16" s="49"/>
+      <c r="I16" s="42"/>
+      <c r="J16" s="42"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="49"/>
-      <c r="B17" s="49"/>
+      <c r="A17" s="42"/>
+      <c r="B17" s="42"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="49"/>
-      <c r="I17" s="49"/>
-      <c r="J17" s="49"/>
+      <c r="H17" s="42"/>
+      <c r="I17" s="42"/>
+      <c r="J17" s="42"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="49"/>
-      <c r="B18" s="49"/>
+      <c r="A18" s="42"/>
+      <c r="B18" s="42"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="49"/>
-      <c r="I18" s="49"/>
-      <c r="J18" s="49"/>
+      <c r="H18" s="42"/>
+      <c r="I18" s="42"/>
+      <c r="J18" s="42"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="42"/>
-      <c r="B19" s="42"/>
+      <c r="A19" s="43"/>
+      <c r="B19" s="43"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="50" t="s">
+      <c r="H19" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="50"/>
-      <c r="J19" s="50"/>
+      <c r="I19" s="44"/>
+      <c r="J19" s="44"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="75"/>
-      <c r="B20" s="75"/>
+      <c r="A20" s="76"/>
+      <c r="B20" s="76"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="37" t="s">
+      <c r="H20" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="38"/>
-      <c r="J20" s="38"/>
+      <c r="I20" s="46"/>
+      <c r="J20" s="46"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -5117,60 +5117,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="44" t="s">
+      <c r="A27" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="44"/>
-      <c r="C27" s="44"/>
-      <c r="D27" s="44"/>
-      <c r="E27" s="44"/>
-      <c r="F27" s="44"/>
-      <c r="G27" s="44"/>
-      <c r="H27" s="44"/>
-      <c r="I27" s="44"/>
-      <c r="J27" s="44"/>
+      <c r="B27" s="38"/>
+      <c r="C27" s="38"/>
+      <c r="D27" s="38"/>
+      <c r="E27" s="38"/>
+      <c r="F27" s="38"/>
+      <c r="G27" s="38"/>
+      <c r="H27" s="38"/>
+      <c r="I27" s="38"/>
+      <c r="J27" s="38"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="45" t="s">
+      <c r="A28" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="45"/>
-      <c r="C28" s="45"/>
-      <c r="D28" s="45"/>
-      <c r="E28" s="45"/>
-      <c r="F28" s="45"/>
-      <c r="G28" s="45"/>
-      <c r="H28" s="45"/>
-      <c r="I28" s="45"/>
-      <c r="J28" s="45"/>
+      <c r="B28" s="39"/>
+      <c r="C28" s="39"/>
+      <c r="D28" s="39"/>
+      <c r="E28" s="39"/>
+      <c r="F28" s="39"/>
+      <c r="G28" s="39"/>
+      <c r="H28" s="39"/>
+      <c r="I28" s="39"/>
+      <c r="J28" s="39"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="46" t="s">
+      <c r="A29" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="46"/>
-      <c r="C29" s="46"/>
-      <c r="D29" s="46"/>
-      <c r="E29" s="46"/>
-      <c r="F29" s="46"/>
-      <c r="G29" s="46"/>
-      <c r="H29" s="46"/>
-      <c r="I29" s="46"/>
-      <c r="J29" s="46"/>
+      <c r="B29" s="47"/>
+      <c r="C29" s="47"/>
+      <c r="D29" s="47"/>
+      <c r="E29" s="47"/>
+      <c r="F29" s="47"/>
+      <c r="G29" s="47"/>
+      <c r="H29" s="47"/>
+      <c r="I29" s="47"/>
+      <c r="J29" s="47"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="47" t="s">
+      <c r="A30" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="47"/>
-      <c r="C30" s="47"/>
-      <c r="D30" s="47"/>
-      <c r="E30" s="47"/>
-      <c r="F30" s="47"/>
-      <c r="G30" s="47"/>
-      <c r="H30" s="47"/>
-      <c r="I30" s="47"/>
-      <c r="J30" s="47"/>
+      <c r="B30" s="40"/>
+      <c r="C30" s="40"/>
+      <c r="D30" s="40"/>
+      <c r="E30" s="40"/>
+      <c r="F30" s="40"/>
+      <c r="G30" s="40"/>
+      <c r="H30" s="40"/>
+      <c r="I30" s="40"/>
+      <c r="J30" s="40"/>
     </row>
     <row r="31" spans="1:10" ht="23.25">
       <c r="A31" s="6"/>
@@ -5179,10 +5179,10 @@
       <c r="D31" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="48" t="s">
+      <c r="E31" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="48"/>
+      <c r="F31" s="37"/>
       <c r="G31" s="12" t="s">
         <v>5</v>
       </c>
@@ -5197,10 +5197,10 @@
       <c r="D32" s="11">
         <v>1000</v>
       </c>
-      <c r="E32" s="43">
+      <c r="E32" s="41">
         <v>44</v>
       </c>
-      <c r="F32" s="43"/>
+      <c r="F32" s="41"/>
       <c r="G32" s="11">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>44000</v>
@@ -5216,10 +5216,10 @@
       <c r="D33" s="11">
         <v>500</v>
       </c>
-      <c r="E33" s="43">
+      <c r="E33" s="41">
         <v>118</v>
       </c>
-      <c r="F33" s="43"/>
+      <c r="F33" s="41"/>
       <c r="G33" s="11">
         <f t="shared" si="1"/>
         <v>59000</v>
@@ -5235,10 +5235,10 @@
       <c r="D34" s="11">
         <v>100</v>
       </c>
-      <c r="E34" s="43">
+      <c r="E34" s="41">
         <v>510</v>
       </c>
-      <c r="F34" s="43"/>
+      <c r="F34" s="41"/>
       <c r="G34" s="11">
         <f t="shared" si="1"/>
         <v>51000</v>
@@ -5254,8 +5254,8 @@
       <c r="D35" s="11">
         <v>50</v>
       </c>
-      <c r="E35" s="43"/>
-      <c r="F35" s="43"/>
+      <c r="E35" s="41"/>
+      <c r="F35" s="41"/>
       <c r="G35" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -5271,8 +5271,8 @@
       <c r="D36" s="11">
         <v>20</v>
       </c>
-      <c r="E36" s="43"/>
-      <c r="F36" s="43"/>
+      <c r="E36" s="41"/>
+      <c r="F36" s="41"/>
       <c r="G36" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -5288,8 +5288,8 @@
       <c r="D37" s="11">
         <v>10</v>
       </c>
-      <c r="E37" s="43"/>
-      <c r="F37" s="43"/>
+      <c r="E37" s="41"/>
+      <c r="F37" s="41"/>
       <c r="G37" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -5302,10 +5302,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="76" t="s">
+      <c r="D38" s="75" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="76"/>
+      <c r="E38" s="75"/>
       <c r="F38" s="12"/>
       <c r="G38" s="12">
         <f>SUM(G32:G37)</f>
@@ -5352,72 +5352,72 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="41" t="s">
+      <c r="A42" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="41"/>
+      <c r="B42" s="50"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="41" t="s">
+      <c r="H42" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="41"/>
-      <c r="J42" s="41"/>
+      <c r="I42" s="50"/>
+      <c r="J42" s="50"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="42"/>
-      <c r="B43" s="42"/>
+      <c r="A43" s="43"/>
+      <c r="B43" s="43"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="42"/>
-      <c r="I43" s="42"/>
-      <c r="J43" s="42"/>
+      <c r="H43" s="43"/>
+      <c r="I43" s="43"/>
+      <c r="J43" s="43"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="42"/>
-      <c r="B44" s="42"/>
+      <c r="A44" s="43"/>
+      <c r="B44" s="43"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="42"/>
-      <c r="I44" s="42"/>
-      <c r="J44" s="42"/>
+      <c r="H44" s="43"/>
+      <c r="I44" s="43"/>
+      <c r="J44" s="43"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="42"/>
-      <c r="B45" s="42"/>
+      <c r="A45" s="43"/>
+      <c r="B45" s="43"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="42" t="s">
+      <c r="H45" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="41"/>
-      <c r="J45" s="41"/>
+      <c r="I45" s="50"/>
+      <c r="J45" s="50"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="72"/>
-      <c r="B46" s="72"/>
+      <c r="A46" s="71"/>
+      <c r="B46" s="71"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="37" t="s">
+      <c r="H46" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="38"/>
-      <c r="J46" s="38"/>
+      <c r="I46" s="46"/>
+      <c r="J46" s="46"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -5445,16 +5445,24 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="H20:J20"/>
@@ -5467,24 +5475,16 @@
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="E35:F35"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -5509,64 +5509,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="44"/>
-      <c r="J1" s="44"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="45"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="45"/>
-      <c r="H2" s="45"/>
-      <c r="I2" s="45"/>
-      <c r="J2" s="45"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="39"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="45"/>
-      <c r="B3" s="45"/>
-      <c r="C3" s="45"/>
-      <c r="D3" s="45"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="45"/>
-      <c r="G3" s="45"/>
-      <c r="H3" s="45"/>
-      <c r="I3" s="45"/>
-      <c r="J3" s="45"/>
+      <c r="A3" s="39"/>
+      <c r="B3" s="39"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="39"/>
+      <c r="J3" s="39"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="47"/>
-      <c r="B4" s="47"/>
-      <c r="C4" s="47"/>
-      <c r="D4" s="47"/>
-      <c r="E4" s="47"/>
-      <c r="F4" s="47"/>
-      <c r="G4" s="47"/>
-      <c r="H4" s="47"/>
-      <c r="I4" s="47"/>
-      <c r="J4" s="47"/>
+      <c r="A4" s="40"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="40"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="D5" s="18"/>
-      <c r="E5" s="48"/>
-      <c r="F5" s="48"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="37"/>
       <c r="G5" s="18"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
@@ -5577,8 +5577,8 @@
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="17"/>
-      <c r="E6" s="43"/>
-      <c r="F6" s="43"/>
+      <c r="E6" s="41"/>
+      <c r="F6" s="41"/>
       <c r="G6" s="17"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -5589,8 +5589,8 @@
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
       <c r="D7" s="17"/>
-      <c r="E7" s="43"/>
-      <c r="F7" s="43"/>
+      <c r="E7" s="41"/>
+      <c r="F7" s="41"/>
       <c r="G7" s="17"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
@@ -5601,8 +5601,8 @@
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
       <c r="D8" s="17"/>
-      <c r="E8" s="43"/>
-      <c r="F8" s="43"/>
+      <c r="E8" s="41"/>
+      <c r="F8" s="41"/>
       <c r="G8" s="17"/>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -5613,8 +5613,8 @@
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="17"/>
-      <c r="E9" s="43"/>
-      <c r="F9" s="43"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="41"/>
       <c r="G9" s="17"/>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -5625,8 +5625,8 @@
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="17"/>
-      <c r="E10" s="43"/>
-      <c r="F10" s="43"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="41"/>
       <c r="G10" s="17"/>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
@@ -5637,8 +5637,8 @@
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="17"/>
-      <c r="E11" s="43"/>
-      <c r="F11" s="43"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="41"/>
       <c r="G11" s="17"/>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
@@ -5648,8 +5648,8 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="48"/>
-      <c r="E12" s="48"/>
+      <c r="D12" s="37"/>
+      <c r="E12" s="37"/>
       <c r="F12" s="18"/>
       <c r="G12" s="18"/>
       <c r="H12" s="6"/>
@@ -5693,52 +5693,52 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="49"/>
-      <c r="B16" s="49"/>
+      <c r="A16" s="42"/>
+      <c r="B16" s="42"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="49"/>
-      <c r="I16" s="49"/>
-      <c r="J16" s="49"/>
+      <c r="H16" s="42"/>
+      <c r="I16" s="42"/>
+      <c r="J16" s="42"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="49"/>
-      <c r="B17" s="49"/>
+      <c r="A17" s="42"/>
+      <c r="B17" s="42"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="49"/>
-      <c r="I17" s="49"/>
-      <c r="J17" s="49"/>
+      <c r="H17" s="42"/>
+      <c r="I17" s="42"/>
+      <c r="J17" s="42"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="49"/>
-      <c r="B18" s="49"/>
+      <c r="A18" s="42"/>
+      <c r="B18" s="42"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="49"/>
-      <c r="I18" s="49"/>
-      <c r="J18" s="49"/>
+      <c r="H18" s="42"/>
+      <c r="I18" s="42"/>
+      <c r="J18" s="42"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="42"/>
-      <c r="B19" s="42"/>
+      <c r="A19" s="43"/>
+      <c r="B19" s="43"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="50"/>
-      <c r="I19" s="50"/>
-      <c r="J19" s="50"/>
+      <c r="H19" s="44"/>
+      <c r="I19" s="44"/>
+      <c r="J19" s="44"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -5748,9 +5748,9 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="37"/>
-      <c r="I20" s="38"/>
-      <c r="J20" s="38"/>
+      <c r="H20" s="45"/>
+      <c r="I20" s="46"/>
+      <c r="J20" s="46"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -5837,60 +5837,60 @@
       <c r="J27" s="6"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="44" t="s">
+      <c r="A28" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="44"/>
-      <c r="C28" s="44"/>
-      <c r="D28" s="44"/>
-      <c r="E28" s="44"/>
-      <c r="F28" s="44"/>
-      <c r="G28" s="44"/>
-      <c r="H28" s="44"/>
-      <c r="I28" s="44"/>
-      <c r="J28" s="44"/>
+      <c r="B28" s="38"/>
+      <c r="C28" s="38"/>
+      <c r="D28" s="38"/>
+      <c r="E28" s="38"/>
+      <c r="F28" s="38"/>
+      <c r="G28" s="38"/>
+      <c r="H28" s="38"/>
+      <c r="I28" s="38"/>
+      <c r="J28" s="38"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="45" t="s">
+      <c r="A29" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="45"/>
-      <c r="C29" s="45"/>
-      <c r="D29" s="45"/>
-      <c r="E29" s="45"/>
-      <c r="F29" s="45"/>
-      <c r="G29" s="45"/>
-      <c r="H29" s="45"/>
-      <c r="I29" s="45"/>
-      <c r="J29" s="45"/>
+      <c r="B29" s="39"/>
+      <c r="C29" s="39"/>
+      <c r="D29" s="39"/>
+      <c r="E29" s="39"/>
+      <c r="F29" s="39"/>
+      <c r="G29" s="39"/>
+      <c r="H29" s="39"/>
+      <c r="I29" s="39"/>
+      <c r="J29" s="39"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="46" t="s">
+      <c r="A30" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="46"/>
-      <c r="C30" s="46"/>
-      <c r="D30" s="46"/>
-      <c r="E30" s="46"/>
-      <c r="F30" s="46"/>
-      <c r="G30" s="46"/>
-      <c r="H30" s="46"/>
-      <c r="I30" s="46"/>
-      <c r="J30" s="46"/>
+      <c r="B30" s="47"/>
+      <c r="C30" s="47"/>
+      <c r="D30" s="47"/>
+      <c r="E30" s="47"/>
+      <c r="F30" s="47"/>
+      <c r="G30" s="47"/>
+      <c r="H30" s="47"/>
+      <c r="I30" s="47"/>
+      <c r="J30" s="47"/>
     </row>
     <row r="31" spans="1:10" ht="18.75">
-      <c r="A31" s="47" t="s">
+      <c r="A31" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="B31" s="47"/>
-      <c r="C31" s="47"/>
-      <c r="D31" s="47"/>
-      <c r="E31" s="47"/>
-      <c r="F31" s="47"/>
-      <c r="G31" s="47"/>
-      <c r="H31" s="47"/>
-      <c r="I31" s="47"/>
-      <c r="J31" s="47"/>
+      <c r="B31" s="40"/>
+      <c r="C31" s="40"/>
+      <c r="D31" s="40"/>
+      <c r="E31" s="40"/>
+      <c r="F31" s="40"/>
+      <c r="G31" s="40"/>
+      <c r="H31" s="40"/>
+      <c r="I31" s="40"/>
+      <c r="J31" s="40"/>
     </row>
     <row r="32" spans="1:10" ht="20.25">
       <c r="A32" s="6" t="s">
@@ -5901,10 +5901,10 @@
       <c r="D32" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="70" t="s">
+      <c r="E32" s="74" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="70"/>
+      <c r="F32" s="74"/>
       <c r="G32" s="20" t="s">
         <v>5</v>
       </c>
@@ -5919,10 +5919,10 @@
       <c r="D33" s="19">
         <v>1000</v>
       </c>
-      <c r="E33" s="43">
+      <c r="E33" s="41">
         <v>30</v>
       </c>
-      <c r="F33" s="43"/>
+      <c r="F33" s="41"/>
       <c r="G33" s="19">
         <f t="shared" ref="G33:G38" si="0">SUM(D33*E33)</f>
         <v>30000</v>
@@ -5938,10 +5938,10 @@
       <c r="D34" s="19">
         <v>500</v>
       </c>
-      <c r="E34" s="43">
+      <c r="E34" s="41">
         <v>35</v>
       </c>
-      <c r="F34" s="43"/>
+      <c r="F34" s="41"/>
       <c r="G34" s="19">
         <f t="shared" si="0"/>
         <v>17500</v>
@@ -5957,10 +5957,10 @@
       <c r="D35" s="19">
         <v>100</v>
       </c>
-      <c r="E35" s="43">
+      <c r="E35" s="41">
         <v>425</v>
       </c>
-      <c r="F35" s="43"/>
+      <c r="F35" s="41"/>
       <c r="G35" s="19">
         <f t="shared" si="0"/>
         <v>42500</v>
@@ -5976,8 +5976,8 @@
       <c r="D36" s="19">
         <v>50</v>
       </c>
-      <c r="E36" s="43"/>
-      <c r="F36" s="43"/>
+      <c r="E36" s="41"/>
+      <c r="F36" s="41"/>
       <c r="G36" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -5993,8 +5993,8 @@
       <c r="D37" s="19">
         <v>20</v>
       </c>
-      <c r="E37" s="74"/>
-      <c r="F37" s="74"/>
+      <c r="E37" s="73"/>
+      <c r="F37" s="73"/>
       <c r="G37" s="19">
         <f>SUM(D37*E37)</f>
         <v>0</v>
@@ -6010,10 +6010,10 @@
       <c r="D38" s="19">
         <v>10</v>
       </c>
-      <c r="E38" s="74">
+      <c r="E38" s="73">
         <v>100</v>
       </c>
-      <c r="F38" s="74"/>
+      <c r="F38" s="73"/>
       <c r="G38" s="19">
         <f t="shared" si="0"/>
         <v>1000</v>
@@ -6076,58 +6076,58 @@
       <c r="J42" s="6"/>
     </row>
     <row r="43" spans="1:10" ht="15.75">
-      <c r="A43" s="41" t="s">
+      <c r="A43" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="41"/>
+      <c r="B43" s="50"/>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
-      <c r="H43" s="41" t="s">
+      <c r="H43" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="41"/>
-      <c r="J43" s="41"/>
+      <c r="I43" s="50"/>
+      <c r="J43" s="50"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="42"/>
-      <c r="B44" s="42"/>
+      <c r="A44" s="43"/>
+      <c r="B44" s="43"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="42"/>
-      <c r="I44" s="42"/>
-      <c r="J44" s="42"/>
+      <c r="H44" s="43"/>
+      <c r="I44" s="43"/>
+      <c r="J44" s="43"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="42"/>
-      <c r="B45" s="42"/>
+      <c r="A45" s="43"/>
+      <c r="B45" s="43"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="42"/>
-      <c r="I45" s="42"/>
-      <c r="J45" s="42"/>
+      <c r="H45" s="43"/>
+      <c r="I45" s="43"/>
+      <c r="J45" s="43"/>
     </row>
     <row r="46" spans="1:10" ht="15.75">
-      <c r="A46" s="42"/>
-      <c r="B46" s="42"/>
+      <c r="A46" s="43"/>
+      <c r="B46" s="43"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="42" t="s">
+      <c r="H46" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="41"/>
-      <c r="J46" s="41"/>
+      <c r="I46" s="50"/>
+      <c r="J46" s="50"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -6137,12 +6137,38 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="37"/>
-      <c r="I47" s="38"/>
-      <c r="J47" s="38"/>
+      <c r="H47" s="45"/>
+      <c r="I47" s="46"/>
+      <c r="J47" s="46"/>
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="H47:J47"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="H43:J43"/>
+    <mergeCell ref="A44:B45"/>
+    <mergeCell ref="H44:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="A31:J31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -6155,32 +6181,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="A31:J31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="H47:J47"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="H43:J43"/>
-    <mergeCell ref="A44:B45"/>
-    <mergeCell ref="H44:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -6206,177 +6206,177 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="44"/>
-      <c r="J1" s="44"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="45"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="45"/>
-      <c r="H2" s="45"/>
-      <c r="I2" s="45"/>
-      <c r="J2" s="45"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="39"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="88">
+      <c r="A5" s="87">
         <v>1</v>
       </c>
-      <c r="B5" s="81" t="s">
+      <c r="B5" s="79" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="81"/>
-      <c r="D5" s="81"/>
-      <c r="E5" s="81"/>
-      <c r="F5" s="81"/>
-      <c r="G5" s="79">
+      <c r="C5" s="79"/>
+      <c r="D5" s="79"/>
+      <c r="E5" s="79"/>
+      <c r="F5" s="79"/>
+      <c r="G5" s="86">
         <v>1650</v>
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="88"/>
-      <c r="B6" s="81"/>
-      <c r="C6" s="81"/>
-      <c r="D6" s="81"/>
-      <c r="E6" s="81"/>
-      <c r="F6" s="81"/>
-      <c r="G6" s="79"/>
+      <c r="A6" s="87"/>
+      <c r="B6" s="79"/>
+      <c r="C6" s="79"/>
+      <c r="D6" s="79"/>
+      <c r="E6" s="79"/>
+      <c r="F6" s="79"/>
+      <c r="G6" s="86"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="88">
+      <c r="A7" s="87">
         <v>2</v>
       </c>
-      <c r="B7" s="81" t="s">
+      <c r="B7" s="79" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="81"/>
-      <c r="D7" s="81"/>
-      <c r="E7" s="81"/>
-      <c r="F7" s="81"/>
-      <c r="G7" s="79">
+      <c r="C7" s="79"/>
+      <c r="D7" s="79"/>
+      <c r="E7" s="79"/>
+      <c r="F7" s="79"/>
+      <c r="G7" s="86">
         <v>1980</v>
       </c>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="88"/>
-      <c r="B8" s="81"/>
-      <c r="C8" s="81"/>
-      <c r="D8" s="81"/>
-      <c r="E8" s="81"/>
-      <c r="F8" s="81"/>
-      <c r="G8" s="79"/>
+      <c r="A8" s="87"/>
+      <c r="B8" s="79"/>
+      <c r="C8" s="79"/>
+      <c r="D8" s="79"/>
+      <c r="E8" s="79"/>
+      <c r="F8" s="79"/>
+      <c r="G8" s="86"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="88">
+      <c r="A9" s="87">
         <v>3</v>
       </c>
-      <c r="B9" s="81" t="s">
+      <c r="B9" s="79" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="81"/>
-      <c r="D9" s="81"/>
-      <c r="E9" s="81"/>
-      <c r="F9" s="81"/>
-      <c r="G9" s="79">
+      <c r="C9" s="79"/>
+      <c r="D9" s="79"/>
+      <c r="E9" s="79"/>
+      <c r="F9" s="79"/>
+      <c r="G9" s="86">
         <v>10538</v>
       </c>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="88"/>
-      <c r="B10" s="81"/>
-      <c r="C10" s="81"/>
-      <c r="D10" s="81"/>
-      <c r="E10" s="81"/>
-      <c r="F10" s="81"/>
-      <c r="G10" s="79"/>
+      <c r="A10" s="87"/>
+      <c r="B10" s="79"/>
+      <c r="C10" s="79"/>
+      <c r="D10" s="79"/>
+      <c r="E10" s="79"/>
+      <c r="F10" s="79"/>
+      <c r="G10" s="86"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="88">
+      <c r="A11" s="87">
         <v>4</v>
       </c>
-      <c r="B11" s="82" t="s">
+      <c r="B11" s="80" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="83"/>
-      <c r="D11" s="83"/>
-      <c r="E11" s="83"/>
-      <c r="F11" s="84"/>
-      <c r="G11" s="79">
+      <c r="C11" s="81"/>
+      <c r="D11" s="81"/>
+      <c r="E11" s="81"/>
+      <c r="F11" s="82"/>
+      <c r="G11" s="86">
         <v>1100</v>
       </c>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="88"/>
-      <c r="B12" s="85"/>
-      <c r="C12" s="86"/>
-      <c r="D12" s="86"/>
-      <c r="E12" s="86"/>
-      <c r="F12" s="87"/>
-      <c r="G12" s="79"/>
+      <c r="A12" s="87"/>
+      <c r="B12" s="83"/>
+      <c r="C12" s="84"/>
+      <c r="D12" s="84"/>
+      <c r="E12" s="84"/>
+      <c r="F12" s="85"/>
+      <c r="G12" s="86"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="80" t="s">
+      <c r="A13" s="88" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="80"/>
-      <c r="C13" s="80"/>
-      <c r="D13" s="80"/>
-      <c r="E13" s="80"/>
-      <c r="F13" s="80"/>
-      <c r="G13" s="79">
+      <c r="B13" s="88"/>
+      <c r="C13" s="88"/>
+      <c r="D13" s="88"/>
+      <c r="E13" s="88"/>
+      <c r="F13" s="88"/>
+      <c r="G13" s="86">
         <f>SUM(G5:G12)</f>
         <v>15268</v>
       </c>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="80"/>
-      <c r="B14" s="80"/>
-      <c r="C14" s="80"/>
-      <c r="D14" s="80"/>
-      <c r="E14" s="80"/>
-      <c r="F14" s="80"/>
-      <c r="G14" s="79"/>
+      <c r="A14" s="88"/>
+      <c r="B14" s="88"/>
+      <c r="C14" s="88"/>
+      <c r="D14" s="88"/>
+      <c r="E14" s="88"/>
+      <c r="F14" s="88"/>
+      <c r="G14" s="86"/>
     </row>
     <row r="23" spans="1:10" ht="18.75">
-      <c r="A23" s="46" t="s">
+      <c r="A23" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="46"/>
-      <c r="C23" s="46"/>
-      <c r="D23" s="46"/>
-      <c r="E23" s="46"/>
-      <c r="F23" s="46"/>
-      <c r="G23" s="46"/>
-      <c r="H23" s="46"/>
-      <c r="I23" s="46"/>
-      <c r="J23" s="46"/>
+      <c r="B23" s="47"/>
+      <c r="C23" s="47"/>
+      <c r="D23" s="47"/>
+      <c r="E23" s="47"/>
+      <c r="F23" s="47"/>
+      <c r="G23" s="47"/>
+      <c r="H23" s="47"/>
+      <c r="I23" s="47"/>
+      <c r="J23" s="47"/>
     </row>
     <row r="24" spans="1:10" ht="18.75">
-      <c r="A24" s="47"/>
-      <c r="B24" s="47"/>
-      <c r="C24" s="47"/>
-      <c r="D24" s="47"/>
-      <c r="E24" s="47"/>
-      <c r="F24" s="47"/>
-      <c r="G24" s="47"/>
-      <c r="H24" s="47"/>
-      <c r="I24" s="47"/>
-      <c r="J24" s="47"/>
+      <c r="A24" s="40"/>
+      <c r="B24" s="40"/>
+      <c r="C24" s="40"/>
+      <c r="D24" s="40"/>
+      <c r="E24" s="40"/>
+      <c r="F24" s="40"/>
+      <c r="G24" s="40"/>
+      <c r="H24" s="40"/>
+      <c r="I24" s="40"/>
+      <c r="J24" s="40"/>
     </row>
     <row r="25" spans="1:10" ht="20.25">
       <c r="A25" s="6" t="s">
@@ -6387,10 +6387,10 @@
       <c r="D25" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E25" s="70" t="s">
+      <c r="E25" s="74" t="s">
         <v>4</v>
       </c>
-      <c r="F25" s="70"/>
+      <c r="F25" s="74"/>
       <c r="G25" s="20" t="s">
         <v>5</v>
       </c>
@@ -6405,8 +6405,8 @@
       <c r="D26" s="19">
         <v>1000</v>
       </c>
-      <c r="E26" s="43"/>
-      <c r="F26" s="43"/>
+      <c r="E26" s="41"/>
+      <c r="F26" s="41"/>
       <c r="G26" s="19">
         <f t="shared" ref="G26:G31" si="0">SUM(D26*E26)</f>
         <v>0</v>
@@ -6422,10 +6422,10 @@
       <c r="D27" s="19">
         <v>500</v>
       </c>
-      <c r="E27" s="43">
+      <c r="E27" s="41">
         <v>30</v>
       </c>
-      <c r="F27" s="43"/>
+      <c r="F27" s="41"/>
       <c r="G27" s="19">
         <f t="shared" si="0"/>
         <v>15000</v>
@@ -6441,8 +6441,8 @@
       <c r="D28" s="19">
         <v>100</v>
       </c>
-      <c r="E28" s="43"/>
-      <c r="F28" s="43"/>
+      <c r="E28" s="41"/>
+      <c r="F28" s="41"/>
       <c r="G28" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -6458,10 +6458,10 @@
       <c r="D29" s="19">
         <v>50</v>
       </c>
-      <c r="E29" s="43">
+      <c r="E29" s="41">
         <v>5</v>
       </c>
-      <c r="F29" s="43"/>
+      <c r="F29" s="41"/>
       <c r="G29" s="19">
         <f t="shared" si="0"/>
         <v>250</v>
@@ -6477,8 +6477,8 @@
       <c r="D30" s="19">
         <v>20</v>
       </c>
-      <c r="E30" s="74"/>
-      <c r="F30" s="74"/>
+      <c r="E30" s="73"/>
+      <c r="F30" s="73"/>
       <c r="G30" s="19">
         <f>SUM(D30*E30)</f>
         <v>0</v>
@@ -6494,10 +6494,10 @@
       <c r="D31" s="19">
         <v>10</v>
       </c>
-      <c r="E31" s="74">
+      <c r="E31" s="73">
         <v>2</v>
       </c>
-      <c r="F31" s="74"/>
+      <c r="F31" s="73"/>
       <c r="G31" s="19">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -6560,58 +6560,58 @@
       <c r="J35" s="6"/>
     </row>
     <row r="36" spans="1:10" ht="15.75">
-      <c r="A36" s="41" t="s">
+      <c r="A36" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="41"/>
+      <c r="B36" s="50"/>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
       <c r="G36" s="7"/>
-      <c r="H36" s="41" t="s">
+      <c r="H36" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="I36" s="41"/>
-      <c r="J36" s="41"/>
+      <c r="I36" s="50"/>
+      <c r="J36" s="50"/>
     </row>
     <row r="37" spans="1:10">
-      <c r="A37" s="42"/>
-      <c r="B37" s="42"/>
+      <c r="A37" s="43"/>
+      <c r="B37" s="43"/>
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
       <c r="G37" s="6"/>
-      <c r="H37" s="42"/>
-      <c r="I37" s="42"/>
-      <c r="J37" s="42"/>
+      <c r="H37" s="43"/>
+      <c r="I37" s="43"/>
+      <c r="J37" s="43"/>
     </row>
     <row r="38" spans="1:10">
-      <c r="A38" s="42"/>
-      <c r="B38" s="42"/>
+      <c r="A38" s="43"/>
+      <c r="B38" s="43"/>
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
-      <c r="H38" s="42"/>
-      <c r="I38" s="42"/>
-      <c r="J38" s="42"/>
+      <c r="H38" s="43"/>
+      <c r="I38" s="43"/>
+      <c r="J38" s="43"/>
     </row>
     <row r="39" spans="1:10" ht="15.75">
-      <c r="A39" s="42"/>
-      <c r="B39" s="42"/>
+      <c r="A39" s="43"/>
+      <c r="B39" s="43"/>
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
       <c r="F39" s="6"/>
       <c r="G39" s="6"/>
-      <c r="H39" s="42" t="s">
+      <c r="H39" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="I39" s="41"/>
-      <c r="J39" s="41"/>
+      <c r="I39" s="50"/>
+      <c r="J39" s="50"/>
     </row>
     <row r="40" spans="1:10">
       <c r="A40" s="6"/>
@@ -6621,12 +6621,29 @@
       <c r="E40" s="6"/>
       <c r="F40" s="6"/>
       <c r="G40" s="6"/>
-      <c r="H40" s="37"/>
-      <c r="I40" s="38"/>
-      <c r="J40" s="38"/>
+      <c r="H40" s="45"/>
+      <c r="I40" s="46"/>
+      <c r="J40" s="46"/>
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="H40:J40"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="H36:J36"/>
+    <mergeCell ref="A37:B38"/>
+    <mergeCell ref="H37:J38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="H39:J39"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="A13:F14"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="E30:F30"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="A23:J23"/>
@@ -6643,23 +6660,6 @@
     <mergeCell ref="B5:F6"/>
     <mergeCell ref="G5:G6"/>
     <mergeCell ref="B7:F8"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="A13:F14"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="H40:J40"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="H36:J36"/>
-    <mergeCell ref="A37:B38"/>
-    <mergeCell ref="H37:J38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="H39:J39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="71" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
16.07.2020 MC Sales Details
</commit_message>
<xml_diff>
--- a/2020/Others/Cash A.xlsx
+++ b/2020/Others/Cash A.xlsx
@@ -515,47 +515,71 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -576,21 +600,9 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -600,17 +612,8 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -624,15 +627,12 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -640,6 +640,12 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -661,12 +667,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -706,7 +706,7 @@
         <xdr:cNvPr id="2" name="Straight Connector 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -756,7 +756,7 @@
         <xdr:cNvPr id="3" name="Straight Connector 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -806,7 +806,7 @@
         <xdr:cNvPr id="4" name="Straight Connector 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -856,7 +856,7 @@
         <xdr:cNvPr id="5" name="Straight Connector 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -911,7 +911,7 @@
         <xdr:cNvPr id="12" name="Straight Connector 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000C000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00000C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -961,7 +961,7 @@
         <xdr:cNvPr id="6" name="Straight Connector 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3F693EA6-49EB-42D1-B3CA-F15B26A03B41}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3F693EA6-49EB-42D1-B3CA-F15B26A03B41}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1011,7 +1011,7 @@
         <xdr:cNvPr id="8" name="Straight Connector 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{334CB43E-1331-4297-A64C-0895C28A3BBB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{334CB43E-1331-4297-A64C-0895C28A3BBB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1061,7 +1061,7 @@
         <xdr:cNvPr id="9" name="Straight Connector 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0D774EF-0DA8-4AF5-A477-477DFA29C2B2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A0D774EF-0DA8-4AF5-A477-477DFA29C2B2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1111,7 +1111,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0F2A810E-B364-491B-AB34-AE585B8D27E3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0F2A810E-B364-491B-AB34-AE585B8D27E3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1123,7 +1123,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1161,7 +1161,7 @@
         <xdr:cNvPr id="13" name="Picture 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BBEAD3A6-FB1B-45D2-BDBE-713A9FCBE3DE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{BBEAD3A6-FB1B-45D2-BDBE-713A9FCBE3DE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1173,7 +1173,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1216,7 +1216,7 @@
         <xdr:cNvPr id="2" name="Straight Connector 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1266,7 +1266,7 @@
         <xdr:cNvPr id="3" name="Straight Connector 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1316,7 +1316,7 @@
         <xdr:cNvPr id="4" name="Straight Connector 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1366,7 +1366,7 @@
         <xdr:cNvPr id="5" name="Straight Connector 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1416,7 +1416,7 @@
         <xdr:cNvPr id="6" name="Straight Connector 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000006000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1471,7 +1471,7 @@
         <xdr:cNvPr id="7" name="Straight Connector 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000007000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1521,7 +1521,7 @@
         <xdr:cNvPr id="8" name="Straight Connector 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000008000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1571,7 +1571,7 @@
         <xdr:cNvPr id="9" name="Straight Connector 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000009000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000009000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1621,7 +1621,7 @@
         <xdr:cNvPr id="10" name="Straight Connector 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000A000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-00000A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1671,7 +1671,7 @@
         <xdr:cNvPr id="11" name="Straight Connector 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000B000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-00000B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1721,7 +1721,7 @@
         <xdr:cNvPr id="12" name="Straight Connector 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000C000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-00000C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1771,7 +1771,7 @@
         <xdr:cNvPr id="13" name="Straight Connector 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000D000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-00000D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1826,7 +1826,7 @@
         <xdr:cNvPr id="2" name="Straight Connector 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1876,7 +1876,7 @@
         <xdr:cNvPr id="3" name="Straight Connector 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1926,7 +1926,7 @@
         <xdr:cNvPr id="4" name="Straight Connector 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1976,7 +1976,7 @@
         <xdr:cNvPr id="5" name="Straight Connector 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2031,7 +2031,7 @@
         <xdr:cNvPr id="4" name="Straight Connector 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2081,7 +2081,7 @@
         <xdr:cNvPr id="5" name="Straight Connector 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2371,7 +2371,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2393,60 +2393,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
-      <c r="J1" s="38"/>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="39"/>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="39"/>
+      <c r="B2" s="45"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="45"/>
+      <c r="I2" s="45"/>
+      <c r="J2" s="45"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="39"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
-      <c r="I3" s="39"/>
-      <c r="J3" s="39"/>
+      <c r="B3" s="45"/>
+      <c r="C3" s="45"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="45"/>
+      <c r="G3" s="45"/>
+      <c r="H3" s="45"/>
+      <c r="I3" s="45"/>
+      <c r="J3" s="45"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="47" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="40"/>
-      <c r="I4" s="40"/>
-      <c r="J4" s="40"/>
+      <c r="B4" s="47"/>
+      <c r="C4" s="47"/>
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="47"/>
+      <c r="G4" s="47"/>
+      <c r="H4" s="47"/>
+      <c r="I4" s="47"/>
+      <c r="J4" s="47"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
@@ -2455,10 +2455,10 @@
       <c r="D5" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="37" t="s">
+      <c r="E5" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="37"/>
+      <c r="F5" s="48"/>
       <c r="G5" s="14" t="s">
         <v>5</v>
       </c>
@@ -2473,10 +2473,10 @@
       <c r="D6" s="13">
         <v>1000</v>
       </c>
-      <c r="E6" s="41">
+      <c r="E6" s="43">
         <v>50</v>
       </c>
-      <c r="F6" s="41"/>
+      <c r="F6" s="43"/>
       <c r="G6" s="13">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>50000</v>
@@ -2492,10 +2492,10 @@
       <c r="D7" s="13">
         <v>500</v>
       </c>
-      <c r="E7" s="41">
+      <c r="E7" s="43">
         <v>16</v>
       </c>
-      <c r="F7" s="41"/>
+      <c r="F7" s="43"/>
       <c r="G7" s="13">
         <f t="shared" si="0"/>
         <v>8000</v>
@@ -2511,10 +2511,10 @@
       <c r="D8" s="13">
         <v>100</v>
       </c>
-      <c r="E8" s="41">
+      <c r="E8" s="43">
         <v>151</v>
       </c>
-      <c r="F8" s="41"/>
+      <c r="F8" s="43"/>
       <c r="G8" s="13">
         <f t="shared" si="0"/>
         <v>15100</v>
@@ -2530,10 +2530,10 @@
       <c r="D9" s="13">
         <v>50</v>
       </c>
-      <c r="E9" s="41">
+      <c r="E9" s="43">
         <v>58</v>
       </c>
-      <c r="F9" s="41"/>
+      <c r="F9" s="43"/>
       <c r="G9" s="13">
         <f t="shared" si="0"/>
         <v>2900</v>
@@ -2549,8 +2549,8 @@
       <c r="D10" s="13">
         <v>20</v>
       </c>
-      <c r="E10" s="41"/>
-      <c r="F10" s="41"/>
+      <c r="E10" s="43"/>
+      <c r="F10" s="43"/>
       <c r="G10" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2566,8 +2566,8 @@
       <c r="D11" s="13">
         <v>10</v>
       </c>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
+      <c r="E11" s="43"/>
+      <c r="F11" s="43"/>
       <c r="G11" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2580,10 +2580,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="37" t="s">
+      <c r="D12" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="37"/>
+      <c r="E12" s="48"/>
       <c r="F12" s="14"/>
       <c r="G12" s="14">
         <f>SUM(G6:G11)</f>
@@ -2630,58 +2630,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="42" t="s">
+      <c r="A16" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="42"/>
+      <c r="B16" s="49"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="42" t="s">
+      <c r="H16" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="42"/>
-      <c r="J16" s="42"/>
+      <c r="I16" s="49"/>
+      <c r="J16" s="49"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="42"/>
-      <c r="B17" s="42"/>
+      <c r="A17" s="49"/>
+      <c r="B17" s="49"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="42"/>
-      <c r="I17" s="42"/>
-      <c r="J17" s="42"/>
+      <c r="H17" s="49"/>
+      <c r="I17" s="49"/>
+      <c r="J17" s="49"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="42"/>
-      <c r="B18" s="42"/>
+      <c r="A18" s="49"/>
+      <c r="B18" s="49"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="42"/>
-      <c r="I18" s="42"/>
-      <c r="J18" s="42"/>
+      <c r="H18" s="49"/>
+      <c r="I18" s="49"/>
+      <c r="J18" s="49"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="43"/>
-      <c r="B19" s="43"/>
+      <c r="A19" s="42"/>
+      <c r="B19" s="42"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="44" t="s">
+      <c r="H19" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="44"/>
-      <c r="J19" s="44"/>
+      <c r="I19" s="50"/>
+      <c r="J19" s="50"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -2691,11 +2691,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="45" t="s">
+      <c r="H20" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="46"/>
-      <c r="J20" s="46"/>
+      <c r="I20" s="38"/>
+      <c r="J20" s="38"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -2770,60 +2770,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="38" t="s">
+      <c r="A27" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="38"/>
-      <c r="C27" s="38"/>
-      <c r="D27" s="38"/>
-      <c r="E27" s="38"/>
-      <c r="F27" s="38"/>
-      <c r="G27" s="38"/>
-      <c r="H27" s="38"/>
-      <c r="I27" s="38"/>
-      <c r="J27" s="38"/>
+      <c r="B27" s="44"/>
+      <c r="C27" s="44"/>
+      <c r="D27" s="44"/>
+      <c r="E27" s="44"/>
+      <c r="F27" s="44"/>
+      <c r="G27" s="44"/>
+      <c r="H27" s="44"/>
+      <c r="I27" s="44"/>
+      <c r="J27" s="44"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="39" t="s">
+      <c r="A28" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="39"/>
-      <c r="C28" s="39"/>
-      <c r="D28" s="39"/>
-      <c r="E28" s="39"/>
-      <c r="F28" s="39"/>
-      <c r="G28" s="39"/>
-      <c r="H28" s="39"/>
-      <c r="I28" s="39"/>
-      <c r="J28" s="39"/>
+      <c r="B28" s="45"/>
+      <c r="C28" s="45"/>
+      <c r="D28" s="45"/>
+      <c r="E28" s="45"/>
+      <c r="F28" s="45"/>
+      <c r="G28" s="45"/>
+      <c r="H28" s="45"/>
+      <c r="I28" s="45"/>
+      <c r="J28" s="45"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="47" t="s">
+      <c r="A29" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="47"/>
-      <c r="C29" s="47"/>
-      <c r="D29" s="47"/>
-      <c r="E29" s="47"/>
-      <c r="F29" s="47"/>
-      <c r="G29" s="47"/>
-      <c r="H29" s="47"/>
-      <c r="I29" s="47"/>
-      <c r="J29" s="47"/>
+      <c r="B29" s="46"/>
+      <c r="C29" s="46"/>
+      <c r="D29" s="46"/>
+      <c r="E29" s="46"/>
+      <c r="F29" s="46"/>
+      <c r="G29" s="46"/>
+      <c r="H29" s="46"/>
+      <c r="I29" s="46"/>
+      <c r="J29" s="46"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="40" t="s">
+      <c r="A30" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="40"/>
-      <c r="C30" s="40"/>
-      <c r="D30" s="40"/>
-      <c r="E30" s="40"/>
-      <c r="F30" s="40"/>
-      <c r="G30" s="40"/>
-      <c r="H30" s="40"/>
-      <c r="I30" s="40"/>
-      <c r="J30" s="40"/>
+      <c r="B30" s="47"/>
+      <c r="C30" s="47"/>
+      <c r="D30" s="47"/>
+      <c r="E30" s="47"/>
+      <c r="F30" s="47"/>
+      <c r="G30" s="47"/>
+      <c r="H30" s="47"/>
+      <c r="I30" s="47"/>
+      <c r="J30" s="47"/>
     </row>
     <row r="31" spans="1:10" ht="24.95" customHeight="1">
       <c r="A31" s="6"/>
@@ -2832,10 +2832,10 @@
       <c r="D31" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="37" t="s">
+      <c r="E31" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="37"/>
+      <c r="F31" s="48"/>
       <c r="G31" s="15" t="s">
         <v>5</v>
       </c>
@@ -2850,10 +2850,10 @@
       <c r="D32" s="16">
         <v>1000</v>
       </c>
-      <c r="E32" s="41">
+      <c r="E32" s="43">
         <v>50</v>
       </c>
-      <c r="F32" s="41"/>
+      <c r="F32" s="43"/>
       <c r="G32" s="16">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>50000</v>
@@ -2869,10 +2869,10 @@
       <c r="D33" s="16">
         <v>500</v>
       </c>
-      <c r="E33" s="41">
+      <c r="E33" s="43">
         <v>116</v>
       </c>
-      <c r="F33" s="41"/>
+      <c r="F33" s="43"/>
       <c r="G33" s="16">
         <f t="shared" si="1"/>
         <v>58000</v>
@@ -2888,10 +2888,10 @@
       <c r="D34" s="16">
         <v>100</v>
       </c>
-      <c r="E34" s="41">
+      <c r="E34" s="43">
         <v>151</v>
       </c>
-      <c r="F34" s="41"/>
+      <c r="F34" s="43"/>
       <c r="G34" s="16">
         <f t="shared" si="1"/>
         <v>15100</v>
@@ -2907,10 +2907,10 @@
       <c r="D35" s="16">
         <v>50</v>
       </c>
-      <c r="E35" s="41">
+      <c r="E35" s="43">
         <v>58</v>
       </c>
-      <c r="F35" s="41"/>
+      <c r="F35" s="43"/>
       <c r="G35" s="16">
         <f t="shared" si="1"/>
         <v>2900</v>
@@ -2926,8 +2926,8 @@
       <c r="D36" s="16">
         <v>20</v>
       </c>
-      <c r="E36" s="41"/>
-      <c r="F36" s="41"/>
+      <c r="E36" s="43"/>
+      <c r="F36" s="43"/>
       <c r="G36" s="16">
         <f>SUM(D36*E36)</f>
         <v>0</v>
@@ -2943,8 +2943,8 @@
       <c r="D37" s="16">
         <v>10</v>
       </c>
-      <c r="E37" s="41"/>
-      <c r="F37" s="41"/>
+      <c r="E37" s="43"/>
+      <c r="F37" s="43"/>
       <c r="G37" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2957,10 +2957,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="48" t="s">
+      <c r="D38" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="49"/>
+      <c r="E38" s="40"/>
       <c r="F38" s="15"/>
       <c r="G38" s="15">
         <f>SUM(G32:G37)</f>
@@ -3007,58 +3007,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" ht="15.75">
-      <c r="A42" s="50" t="s">
+      <c r="A42" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="50"/>
+      <c r="B42" s="41"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="50" t="s">
+      <c r="H42" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="50"/>
-      <c r="J42" s="50"/>
+      <c r="I42" s="41"/>
+      <c r="J42" s="41"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="43"/>
-      <c r="B43" s="43"/>
+      <c r="A43" s="42"/>
+      <c r="B43" s="42"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="43"/>
-      <c r="I43" s="43"/>
-      <c r="J43" s="43"/>
+      <c r="H43" s="42"/>
+      <c r="I43" s="42"/>
+      <c r="J43" s="42"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="43"/>
-      <c r="B44" s="43"/>
+      <c r="A44" s="42"/>
+      <c r="B44" s="42"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="43"/>
-      <c r="I44" s="43"/>
-      <c r="J44" s="43"/>
+      <c r="H44" s="42"/>
+      <c r="I44" s="42"/>
+      <c r="J44" s="42"/>
     </row>
     <row r="45" spans="1:10" ht="15.75">
-      <c r="A45" s="43"/>
-      <c r="B45" s="43"/>
+      <c r="A45" s="42"/>
+      <c r="B45" s="42"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="43" t="s">
+      <c r="H45" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="50"/>
-      <c r="J45" s="50"/>
+      <c r="I45" s="41"/>
+      <c r="J45" s="41"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="6"/>
@@ -3068,11 +3068,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="45" t="s">
+      <c r="H46" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="46"/>
-      <c r="J46" s="46"/>
+      <c r="I46" s="38"/>
+      <c r="J46" s="38"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -3100,14 +3100,24 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="E37:F37"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A27:J27"/>
@@ -3120,24 +3130,14 @@
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.25" footer="0"/>
   <pageSetup scale="85" orientation="portrait" r:id="rId1"/>
@@ -3150,7 +3150,7 @@
   <dimension ref="A1:K47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3169,64 +3169,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="51" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
-      <c r="F1" s="58"/>
-      <c r="G1" s="58"/>
-      <c r="H1" s="58"/>
-      <c r="I1" s="58"/>
-      <c r="J1" s="58"/>
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
+      <c r="G1" s="51"/>
+      <c r="H1" s="51"/>
+      <c r="I1" s="51"/>
+      <c r="J1" s="51"/>
       <c r="K1" s="24"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="59" t="s">
+      <c r="A2" s="52" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="59"/>
-      <c r="C2" s="59"/>
-      <c r="D2" s="59"/>
-      <c r="E2" s="59"/>
-      <c r="F2" s="59"/>
-      <c r="G2" s="59"/>
-      <c r="H2" s="59"/>
-      <c r="I2" s="59"/>
-      <c r="J2" s="59"/>
+      <c r="B2" s="52"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="52"/>
+      <c r="I2" s="52"/>
+      <c r="J2" s="52"/>
       <c r="K2" s="24"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="59" t="s">
+      <c r="A3" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="59"/>
-      <c r="C3" s="59"/>
-      <c r="D3" s="59"/>
-      <c r="E3" s="59"/>
-      <c r="F3" s="59"/>
-      <c r="G3" s="59"/>
-      <c r="H3" s="59"/>
-      <c r="I3" s="59"/>
-      <c r="J3" s="59"/>
+      <c r="B3" s="52"/>
+      <c r="C3" s="52"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="52"/>
+      <c r="F3" s="52"/>
+      <c r="G3" s="52"/>
+      <c r="H3" s="52"/>
+      <c r="I3" s="52"/>
+      <c r="J3" s="52"/>
       <c r="K3" s="24"/>
     </row>
     <row r="4" spans="1:11" ht="26.25">
-      <c r="A4" s="66">
+      <c r="A4" s="55">
         <f ca="1">TODAY()</f>
-        <v>44021</v>
-      </c>
-      <c r="B4" s="66"/>
-      <c r="C4" s="66"/>
-      <c r="D4" s="66"/>
-      <c r="E4" s="66"/>
-      <c r="F4" s="66"/>
-      <c r="G4" s="66"/>
-      <c r="H4" s="66"/>
-      <c r="I4" s="66"/>
-      <c r="J4" s="66"/>
+        <v>44028</v>
+      </c>
+      <c r="B4" s="55"/>
+      <c r="C4" s="55"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="55"/>
+      <c r="F4" s="55"/>
+      <c r="G4" s="55"/>
+      <c r="H4" s="55"/>
+      <c r="I4" s="55"/>
+      <c r="J4" s="55"/>
       <c r="K4" s="24"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -3236,10 +3236,10 @@
       <c r="D5" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="61" t="s">
+      <c r="E5" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="61"/>
+      <c r="F5" s="53"/>
       <c r="G5" s="26" t="s">
         <v>5</v>
       </c>
@@ -3254,13 +3254,13 @@
       <c r="D6" s="27">
         <v>1000</v>
       </c>
-      <c r="E6" s="62">
-        <v>162</v>
-      </c>
-      <c r="F6" s="62"/>
+      <c r="E6" s="54">
+        <v>130</v>
+      </c>
+      <c r="F6" s="54"/>
       <c r="G6" s="27">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
-        <v>162000</v>
+        <v>130000</v>
       </c>
       <c r="H6" s="25"/>
       <c r="I6" s="25"/>
@@ -3273,13 +3273,13 @@
       <c r="D7" s="27">
         <v>500</v>
       </c>
-      <c r="E7" s="62">
-        <v>476</v>
-      </c>
-      <c r="F7" s="62"/>
+      <c r="E7" s="54">
+        <v>800</v>
+      </c>
+      <c r="F7" s="54"/>
       <c r="G7" s="27">
         <f t="shared" si="0"/>
-        <v>238000</v>
+        <v>400000</v>
       </c>
       <c r="H7" s="25"/>
       <c r="I7" s="25"/>
@@ -3292,13 +3292,13 @@
       <c r="D8" s="27">
         <v>100</v>
       </c>
-      <c r="E8" s="62">
-        <v>500</v>
-      </c>
-      <c r="F8" s="62"/>
+      <c r="E8" s="54">
+        <v>700</v>
+      </c>
+      <c r="F8" s="54"/>
       <c r="G8" s="27">
         <f t="shared" si="0"/>
-        <v>50000</v>
+        <v>70000</v>
       </c>
       <c r="H8" s="25"/>
       <c r="I8" s="25"/>
@@ -3311,8 +3311,8 @@
       <c r="D9" s="27">
         <v>50</v>
       </c>
-      <c r="E9" s="62"/>
-      <c r="F9" s="62"/>
+      <c r="E9" s="54"/>
+      <c r="F9" s="54"/>
       <c r="G9" s="27">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3328,8 +3328,8 @@
       <c r="D10" s="27">
         <v>20</v>
       </c>
-      <c r="E10" s="62"/>
-      <c r="F10" s="62"/>
+      <c r="E10" s="54"/>
+      <c r="F10" s="54"/>
       <c r="G10" s="27">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3345,8 +3345,8 @@
       <c r="D11" s="27">
         <v>10</v>
       </c>
-      <c r="E11" s="62"/>
-      <c r="F11" s="62"/>
+      <c r="E11" s="54"/>
+      <c r="F11" s="54"/>
       <c r="G11" s="27">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3359,14 +3359,14 @@
       <c r="A12" s="25"/>
       <c r="B12" s="25"/>
       <c r="C12" s="25"/>
-      <c r="D12" s="62" t="s">
+      <c r="D12" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="62"/>
+      <c r="E12" s="54"/>
       <c r="F12" s="27"/>
       <c r="G12" s="22">
         <f>SUM(G6:G11)</f>
-        <v>450000</v>
+        <v>600000</v>
       </c>
       <c r="H12" s="25"/>
       <c r="I12" s="25"/>
@@ -3410,59 +3410,59 @@
     </row>
     <row r="16" spans="1:11">
       <c r="A16" s="28"/>
-      <c r="B16" s="69" t="s">
+      <c r="B16" s="57" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="69"/>
-      <c r="D16" s="69"/>
+      <c r="C16" s="57"/>
+      <c r="D16" s="57"/>
       <c r="E16" s="28"/>
       <c r="F16" s="29"/>
       <c r="G16" s="29"/>
-      <c r="H16" s="68" t="s">
+      <c r="H16" s="56" t="s">
         <v>7</v>
       </c>
-      <c r="I16" s="68"/>
-      <c r="J16" s="68"/>
+      <c r="I16" s="56"/>
+      <c r="J16" s="56"/>
     </row>
     <row r="17" spans="1:11">
-      <c r="A17" s="68"/>
-      <c r="B17" s="68"/>
-      <c r="C17" s="68"/>
-      <c r="D17" s="68"/>
+      <c r="A17" s="56"/>
+      <c r="B17" s="56"/>
+      <c r="C17" s="56"/>
+      <c r="D17" s="56"/>
       <c r="E17" s="29"/>
       <c r="F17" s="29"/>
       <c r="G17" s="29"/>
-      <c r="H17" s="68"/>
-      <c r="I17" s="68"/>
-      <c r="J17" s="68"/>
+      <c r="H17" s="56"/>
+      <c r="I17" s="56"/>
+      <c r="J17" s="56"/>
     </row>
     <row r="18" spans="1:11">
-      <c r="A18" s="68"/>
-      <c r="B18" s="68"/>
-      <c r="C18" s="68"/>
-      <c r="D18" s="68"/>
+      <c r="A18" s="56"/>
+      <c r="B18" s="56"/>
+      <c r="C18" s="56"/>
+      <c r="D18" s="56"/>
       <c r="E18" s="29"/>
       <c r="F18" s="29"/>
       <c r="G18" s="29"/>
-      <c r="H18" s="68"/>
-      <c r="I18" s="68"/>
-      <c r="J18" s="68"/>
+      <c r="H18" s="56"/>
+      <c r="I18" s="56"/>
+      <c r="J18" s="56"/>
     </row>
     <row r="19" spans="1:11" ht="17.25" customHeight="1">
       <c r="A19" s="33"/>
-      <c r="B19" s="67" t="s">
+      <c r="B19" s="58" t="s">
         <v>28</v>
       </c>
-      <c r="C19" s="67"/>
-      <c r="D19" s="67"/>
+      <c r="C19" s="58"/>
+      <c r="D19" s="58"/>
       <c r="E19" s="29"/>
       <c r="F19" s="29"/>
       <c r="G19" s="29"/>
-      <c r="H19" s="42" t="s">
+      <c r="H19" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="I19" s="42"/>
-      <c r="J19" s="42"/>
+      <c r="I19" s="49"/>
+      <c r="J19" s="49"/>
     </row>
     <row r="20" spans="1:11">
       <c r="A20" s="25"/>
@@ -3472,9 +3472,9 @@
       <c r="E20" s="25"/>
       <c r="F20" s="25"/>
       <c r="G20" s="25"/>
-      <c r="H20" s="53"/>
-      <c r="I20" s="54"/>
-      <c r="J20" s="54"/>
+      <c r="H20" s="61"/>
+      <c r="I20" s="62"/>
+      <c r="J20" s="62"/>
     </row>
     <row r="21" spans="1:11">
       <c r="A21" s="25"/>
@@ -3561,66 +3561,66 @@
       <c r="J27" s="25"/>
     </row>
     <row r="28" spans="1:11" ht="31.5">
-      <c r="A28" s="58" t="s">
+      <c r="A28" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="B28" s="58"/>
-      <c r="C28" s="58"/>
-      <c r="D28" s="58"/>
-      <c r="E28" s="58"/>
-      <c r="F28" s="58"/>
-      <c r="G28" s="58"/>
-      <c r="H28" s="58"/>
-      <c r="I28" s="58"/>
-      <c r="J28" s="58"/>
+      <c r="B28" s="51"/>
+      <c r="C28" s="51"/>
+      <c r="D28" s="51"/>
+      <c r="E28" s="51"/>
+      <c r="F28" s="51"/>
+      <c r="G28" s="51"/>
+      <c r="H28" s="51"/>
+      <c r="I28" s="51"/>
+      <c r="J28" s="51"/>
     </row>
     <row r="29" spans="1:11" ht="18">
-      <c r="A29" s="59" t="str">
+      <c r="A29" s="52" t="str">
         <f>A2</f>
         <v>Komola Super Market, Alaipur, Natore</v>
       </c>
-      <c r="B29" s="59"/>
-      <c r="C29" s="59"/>
-      <c r="D29" s="59"/>
-      <c r="E29" s="59"/>
-      <c r="F29" s="59"/>
-      <c r="G29" s="59"/>
-      <c r="H29" s="59"/>
-      <c r="I29" s="59"/>
-      <c r="J29" s="59"/>
+      <c r="B29" s="52"/>
+      <c r="C29" s="52"/>
+      <c r="D29" s="52"/>
+      <c r="E29" s="52"/>
+      <c r="F29" s="52"/>
+      <c r="G29" s="52"/>
+      <c r="H29" s="52"/>
+      <c r="I29" s="52"/>
+      <c r="J29" s="52"/>
     </row>
     <row r="30" spans="1:11" ht="18.75">
-      <c r="A30" s="60" t="str">
+      <c r="A30" s="66" t="str">
         <f>A3</f>
         <v>Cash Details As Per Below</v>
       </c>
-      <c r="B30" s="60"/>
-      <c r="C30" s="60"/>
-      <c r="D30" s="60"/>
-      <c r="E30" s="60"/>
-      <c r="F30" s="60"/>
-      <c r="G30" s="60"/>
-      <c r="H30" s="60"/>
-      <c r="I30" s="60"/>
-      <c r="J30" s="60"/>
+      <c r="B30" s="66"/>
+      <c r="C30" s="66"/>
+      <c r="D30" s="66"/>
+      <c r="E30" s="66"/>
+      <c r="F30" s="66"/>
+      <c r="G30" s="66"/>
+      <c r="H30" s="66"/>
+      <c r="I30" s="66"/>
+      <c r="J30" s="66"/>
       <c r="K30" s="6" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="26.25">
-      <c r="A31" s="66">
+      <c r="A31" s="55">
         <f ca="1">TODAY()</f>
-        <v>44021</v>
-      </c>
-      <c r="B31" s="66"/>
-      <c r="C31" s="66"/>
-      <c r="D31" s="66"/>
-      <c r="E31" s="66"/>
-      <c r="F31" s="66"/>
-      <c r="G31" s="66"/>
-      <c r="H31" s="66"/>
-      <c r="I31" s="66"/>
-      <c r="J31" s="66"/>
+        <v>44028</v>
+      </c>
+      <c r="B31" s="55"/>
+      <c r="C31" s="55"/>
+      <c r="D31" s="55"/>
+      <c r="E31" s="55"/>
+      <c r="F31" s="55"/>
+      <c r="G31" s="55"/>
+      <c r="H31" s="55"/>
+      <c r="I31" s="55"/>
+      <c r="J31" s="55"/>
     </row>
     <row r="32" spans="1:11" ht="27.95" customHeight="1">
       <c r="A32" s="25"/>
@@ -3629,10 +3629,10 @@
       <c r="D32" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="61" t="s">
+      <c r="E32" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="61"/>
+      <c r="F32" s="53"/>
       <c r="G32" s="26" t="s">
         <v>5</v>
       </c>
@@ -3647,14 +3647,14 @@
       <c r="D33" s="30">
         <v>1000</v>
       </c>
-      <c r="E33" s="62">
+      <c r="E33" s="54">
         <f>E6</f>
-        <v>162</v>
-      </c>
-      <c r="F33" s="62"/>
+        <v>130</v>
+      </c>
+      <c r="F33" s="54"/>
       <c r="G33" s="30">
         <f t="shared" ref="G33:G38" si="1">SUM(D33*E33)</f>
-        <v>162000</v>
+        <v>130000</v>
       </c>
       <c r="H33" s="25"/>
       <c r="I33" s="25"/>
@@ -3667,14 +3667,14 @@
       <c r="D34" s="30">
         <v>500</v>
       </c>
-      <c r="E34" s="62">
+      <c r="E34" s="54">
         <f>E7</f>
-        <v>476</v>
-      </c>
-      <c r="F34" s="62"/>
+        <v>800</v>
+      </c>
+      <c r="F34" s="54"/>
       <c r="G34" s="30">
         <f t="shared" si="1"/>
-        <v>238000</v>
+        <v>400000</v>
       </c>
       <c r="H34" s="25"/>
       <c r="I34" s="25"/>
@@ -3687,14 +3687,14 @@
       <c r="D35" s="30">
         <v>100</v>
       </c>
-      <c r="E35" s="62">
+      <c r="E35" s="54">
         <f>E8</f>
-        <v>500</v>
-      </c>
-      <c r="F35" s="62"/>
+        <v>700</v>
+      </c>
+      <c r="F35" s="54"/>
       <c r="G35" s="30">
         <f t="shared" si="1"/>
-        <v>50000</v>
+        <v>70000</v>
       </c>
       <c r="H35" s="25"/>
       <c r="I35" s="25"/>
@@ -3707,8 +3707,8 @@
       <c r="D36" s="30">
         <v>50</v>
       </c>
-      <c r="E36" s="62"/>
-      <c r="F36" s="62"/>
+      <c r="E36" s="54"/>
+      <c r="F36" s="54"/>
       <c r="G36" s="30">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -3724,8 +3724,8 @@
       <c r="D37" s="30">
         <v>20</v>
       </c>
-      <c r="E37" s="62"/>
-      <c r="F37" s="62"/>
+      <c r="E37" s="54"/>
+      <c r="F37" s="54"/>
       <c r="G37" s="30">
         <f>SUM(D37*E37)</f>
         <v>0</v>
@@ -3741,8 +3741,8 @@
       <c r="D38" s="30">
         <v>10</v>
       </c>
-      <c r="E38" s="62"/>
-      <c r="F38" s="62"/>
+      <c r="E38" s="54"/>
+      <c r="F38" s="54"/>
       <c r="G38" s="30">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -3755,14 +3755,14 @@
       <c r="A39" s="25"/>
       <c r="B39" s="25"/>
       <c r="C39" s="25"/>
-      <c r="D39" s="63" t="s">
+      <c r="D39" s="67" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="64"/>
+      <c r="E39" s="68"/>
       <c r="F39" s="30"/>
       <c r="G39" s="23">
         <f>SUM(G33:G38)</f>
-        <v>450000</v>
+        <v>600000</v>
       </c>
       <c r="H39" s="25"/>
       <c r="I39" s="25"/>
@@ -3814,53 +3814,53 @@
       <c r="E43" s="29"/>
       <c r="F43" s="29"/>
       <c r="G43" s="29"/>
-      <c r="H43" s="55" t="s">
+      <c r="H43" s="63" t="s">
         <v>7</v>
       </c>
-      <c r="I43" s="55"/>
-      <c r="J43" s="55"/>
+      <c r="I43" s="63"/>
+      <c r="J43" s="63"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="56"/>
-      <c r="B44" s="56"/>
-      <c r="C44" s="56"/>
-      <c r="D44" s="56"/>
+      <c r="A44" s="64"/>
+      <c r="B44" s="64"/>
+      <c r="C44" s="64"/>
+      <c r="D44" s="64"/>
       <c r="E44" s="25"/>
       <c r="F44" s="25"/>
       <c r="G44" s="25"/>
-      <c r="H44" s="56"/>
-      <c r="I44" s="56"/>
-      <c r="J44" s="56"/>
+      <c r="H44" s="64"/>
+      <c r="I44" s="64"/>
+      <c r="J44" s="64"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="56"/>
-      <c r="B45" s="56"/>
-      <c r="C45" s="56"/>
-      <c r="D45" s="56"/>
+      <c r="A45" s="64"/>
+      <c r="B45" s="64"/>
+      <c r="C45" s="64"/>
+      <c r="D45" s="64"/>
       <c r="E45" s="25"/>
       <c r="F45" s="25"/>
       <c r="G45" s="25"/>
-      <c r="H45" s="56"/>
-      <c r="I45" s="56"/>
-      <c r="J45" s="56"/>
+      <c r="H45" s="64"/>
+      <c r="I45" s="64"/>
+      <c r="J45" s="64"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="31"/>
-      <c r="B46" s="65" t="str">
+      <c r="B46" s="69" t="str">
         <f>B19</f>
         <v>Rahinul Kabir</v>
       </c>
-      <c r="C46" s="65"/>
-      <c r="D46" s="65"/>
+      <c r="C46" s="69"/>
+      <c r="D46" s="69"/>
       <c r="E46" s="32"/>
       <c r="F46" s="32"/>
       <c r="G46" s="32"/>
-      <c r="H46" s="57" t="str">
+      <c r="H46" s="65" t="str">
         <f>H19</f>
         <v>Jafor Iqbal</v>
       </c>
-      <c r="I46" s="57"/>
-      <c r="J46" s="57"/>
+      <c r="I46" s="65"/>
+      <c r="J46" s="65"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="21"/>
@@ -3870,35 +3870,12 @@
       <c r="E47" s="21"/>
       <c r="F47" s="21"/>
       <c r="G47" s="21"/>
-      <c r="H47" s="51"/>
-      <c r="I47" s="52"/>
-      <c r="J47" s="52"/>
+      <c r="H47" s="59"/>
+      <c r="I47" s="60"/>
+      <c r="J47" s="60"/>
     </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="A17:D18"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="A31:J31"/>
-    <mergeCell ref="B19:D19"/>
     <mergeCell ref="H47:J47"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="H43:J43"/>
@@ -3913,6 +3890,29 @@
     <mergeCell ref="D39:E39"/>
     <mergeCell ref="B46:D46"/>
     <mergeCell ref="A44:D45"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="A31:J31"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="A17:D18"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="A4:J4"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -3944,63 +3944,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
-      <c r="J1" s="38"/>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="39"/>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="39"/>
+      <c r="B2" s="45"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="45"/>
+      <c r="I2" s="45"/>
+      <c r="J2" s="45"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="39"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
-      <c r="I3" s="39"/>
-      <c r="J3" s="39"/>
+      <c r="B3" s="45"/>
+      <c r="C3" s="45"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="45"/>
+      <c r="G3" s="45"/>
+      <c r="H3" s="45"/>
+      <c r="I3" s="45"/>
+      <c r="J3" s="45"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="40"/>
-      <c r="I4" s="40"/>
-      <c r="J4" s="40"/>
+      <c r="B4" s="47"/>
+      <c r="C4" s="47"/>
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="47"/>
+      <c r="G4" s="47"/>
+      <c r="H4" s="47"/>
+      <c r="I4" s="47"/>
+      <c r="J4" s="47"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -4010,10 +4010,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="37" t="s">
+      <c r="E5" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="37"/>
+      <c r="F5" s="48"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -4028,10 +4028,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="41">
+      <c r="E6" s="43">
         <v>68</v>
       </c>
-      <c r="F6" s="41"/>
+      <c r="F6" s="43"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>68000</v>
@@ -4047,10 +4047,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="41">
+      <c r="E7" s="43">
         <v>135</v>
       </c>
-      <c r="F7" s="41"/>
+      <c r="F7" s="43"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>67500</v>
@@ -4066,10 +4066,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="41">
+      <c r="E8" s="43">
         <v>53</v>
       </c>
-      <c r="F8" s="41"/>
+      <c r="F8" s="43"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>5300</v>
@@ -4085,10 +4085,10 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="41">
+      <c r="E9" s="43">
         <v>2</v>
       </c>
-      <c r="F9" s="41"/>
+      <c r="F9" s="43"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -4104,10 +4104,10 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="41">
+      <c r="E10" s="43">
         <v>5</v>
       </c>
-      <c r="F10" s="41"/>
+      <c r="F10" s="43"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -4123,8 +4123,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
+      <c r="E11" s="43"/>
+      <c r="F11" s="43"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4137,10 +4137,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="37" t="s">
+      <c r="D12" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="37"/>
+      <c r="E12" s="48"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -4187,76 +4187,76 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="42" t="s">
+      <c r="A16" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="42"/>
+      <c r="B16" s="49"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="42" t="s">
+      <c r="H16" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="42"/>
-      <c r="J16" s="42"/>
+      <c r="I16" s="49"/>
+      <c r="J16" s="49"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="42"/>
-      <c r="B17" s="42"/>
+      <c r="A17" s="49"/>
+      <c r="B17" s="49"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="42"/>
-      <c r="I17" s="42"/>
-      <c r="J17" s="42"/>
+      <c r="H17" s="49"/>
+      <c r="I17" s="49"/>
+      <c r="J17" s="49"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="42"/>
-      <c r="B18" s="42"/>
+      <c r="A18" s="49"/>
+      <c r="B18" s="49"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="42"/>
-      <c r="I18" s="42"/>
-      <c r="J18" s="42"/>
+      <c r="H18" s="49"/>
+      <c r="I18" s="49"/>
+      <c r="J18" s="49"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="43" t="s">
+      <c r="A19" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="43"/>
+      <c r="B19" s="42"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="44" t="s">
+      <c r="H19" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="44"/>
-      <c r="J19" s="44"/>
+      <c r="I19" s="50"/>
+      <c r="J19" s="50"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="70" t="s">
+      <c r="A20" s="71" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="70"/>
+      <c r="B20" s="71"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="45" t="s">
+      <c r="H20" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="46"/>
-      <c r="J20" s="46"/>
+      <c r="I20" s="38"/>
+      <c r="J20" s="38"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4331,60 +4331,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="38" t="s">
+      <c r="A27" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="38"/>
-      <c r="C27" s="38"/>
-      <c r="D27" s="38"/>
-      <c r="E27" s="38"/>
-      <c r="F27" s="38"/>
-      <c r="G27" s="38"/>
-      <c r="H27" s="38"/>
-      <c r="I27" s="38"/>
-      <c r="J27" s="38"/>
+      <c r="B27" s="44"/>
+      <c r="C27" s="44"/>
+      <c r="D27" s="44"/>
+      <c r="E27" s="44"/>
+      <c r="F27" s="44"/>
+      <c r="G27" s="44"/>
+      <c r="H27" s="44"/>
+      <c r="I27" s="44"/>
+      <c r="J27" s="44"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="39" t="s">
+      <c r="A28" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="39"/>
-      <c r="C28" s="39"/>
-      <c r="D28" s="39"/>
-      <c r="E28" s="39"/>
-      <c r="F28" s="39"/>
-      <c r="G28" s="39"/>
-      <c r="H28" s="39"/>
-      <c r="I28" s="39"/>
-      <c r="J28" s="39"/>
+      <c r="B28" s="45"/>
+      <c r="C28" s="45"/>
+      <c r="D28" s="45"/>
+      <c r="E28" s="45"/>
+      <c r="F28" s="45"/>
+      <c r="G28" s="45"/>
+      <c r="H28" s="45"/>
+      <c r="I28" s="45"/>
+      <c r="J28" s="45"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="47" t="s">
+      <c r="A29" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="47"/>
-      <c r="C29" s="47"/>
-      <c r="D29" s="47"/>
-      <c r="E29" s="47"/>
-      <c r="F29" s="47"/>
-      <c r="G29" s="47"/>
-      <c r="H29" s="47"/>
-      <c r="I29" s="47"/>
-      <c r="J29" s="47"/>
+      <c r="B29" s="46"/>
+      <c r="C29" s="46"/>
+      <c r="D29" s="46"/>
+      <c r="E29" s="46"/>
+      <c r="F29" s="46"/>
+      <c r="G29" s="46"/>
+      <c r="H29" s="46"/>
+      <c r="I29" s="46"/>
+      <c r="J29" s="46"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="40" t="s">
+      <c r="A30" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="40"/>
-      <c r="C30" s="40"/>
-      <c r="D30" s="40"/>
-      <c r="E30" s="40"/>
-      <c r="F30" s="40"/>
-      <c r="G30" s="40"/>
-      <c r="H30" s="40"/>
-      <c r="I30" s="40"/>
-      <c r="J30" s="40"/>
+      <c r="B30" s="47"/>
+      <c r="C30" s="47"/>
+      <c r="D30" s="47"/>
+      <c r="E30" s="47"/>
+      <c r="F30" s="47"/>
+      <c r="G30" s="47"/>
+      <c r="H30" s="47"/>
+      <c r="I30" s="47"/>
+      <c r="J30" s="47"/>
     </row>
     <row r="31" spans="1:10" ht="20.25">
       <c r="A31" s="6"/>
@@ -4393,10 +4393,10 @@
       <c r="D31" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="74" t="s">
+      <c r="E31" s="70" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="74"/>
+      <c r="F31" s="70"/>
       <c r="G31" s="9" t="s">
         <v>5</v>
       </c>
@@ -4411,10 +4411,10 @@
       <c r="D32" s="2">
         <v>1000</v>
       </c>
-      <c r="E32" s="73">
+      <c r="E32" s="74">
         <v>68</v>
       </c>
-      <c r="F32" s="73"/>
+      <c r="F32" s="74"/>
       <c r="G32" s="2">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>68000</v>
@@ -4430,10 +4430,10 @@
       <c r="D33" s="2">
         <v>500</v>
       </c>
-      <c r="E33" s="73">
+      <c r="E33" s="74">
         <v>135</v>
       </c>
-      <c r="F33" s="73"/>
+      <c r="F33" s="74"/>
       <c r="G33" s="2">
         <f t="shared" si="1"/>
         <v>67500</v>
@@ -4449,10 +4449,10 @@
       <c r="D34" s="2">
         <v>100</v>
       </c>
-      <c r="E34" s="73">
+      <c r="E34" s="74">
         <v>53</v>
       </c>
-      <c r="F34" s="73"/>
+      <c r="F34" s="74"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
         <v>5300</v>
@@ -4468,10 +4468,10 @@
       <c r="D35" s="2">
         <v>50</v>
       </c>
-      <c r="E35" s="73">
+      <c r="E35" s="74">
         <v>2</v>
       </c>
-      <c r="F35" s="73"/>
+      <c r="F35" s="74"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4487,10 +4487,10 @@
       <c r="D36" s="2">
         <v>20</v>
       </c>
-      <c r="E36" s="73">
+      <c r="E36" s="74">
         <v>5</v>
       </c>
-      <c r="F36" s="73"/>
+      <c r="F36" s="74"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4506,8 +4506,8 @@
       <c r="D37" s="2">
         <v>10</v>
       </c>
-      <c r="E37" s="73"/>
-      <c r="F37" s="73"/>
+      <c r="E37" s="74"/>
+      <c r="F37" s="74"/>
       <c r="G37" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4520,10 +4520,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="72" t="s">
+      <c r="D38" s="73" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="72"/>
+      <c r="E38" s="73"/>
       <c r="F38" s="9"/>
       <c r="G38" s="9">
         <f>SUM(G32:G37)</f>
@@ -4570,76 +4570,76 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="50" t="s">
+      <c r="A42" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="50"/>
+      <c r="B42" s="41"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="50" t="s">
+      <c r="H42" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="50"/>
-      <c r="J42" s="50"/>
+      <c r="I42" s="41"/>
+      <c r="J42" s="41"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="43"/>
-      <c r="B43" s="43"/>
+      <c r="A43" s="42"/>
+      <c r="B43" s="42"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="43"/>
-      <c r="I43" s="43"/>
-      <c r="J43" s="43"/>
+      <c r="H43" s="42"/>
+      <c r="I43" s="42"/>
+      <c r="J43" s="42"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="43"/>
-      <c r="B44" s="43"/>
+      <c r="A44" s="42"/>
+      <c r="B44" s="42"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="43"/>
-      <c r="I44" s="43"/>
-      <c r="J44" s="43"/>
+      <c r="H44" s="42"/>
+      <c r="I44" s="42"/>
+      <c r="J44" s="42"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="43" t="s">
+      <c r="A45" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="B45" s="43"/>
+      <c r="B45" s="42"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="43" t="s">
+      <c r="H45" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="50"/>
-      <c r="J45" s="50"/>
+      <c r="I45" s="41"/>
+      <c r="J45" s="41"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="71" t="s">
+      <c r="A46" s="72" t="s">
         <v>14</v>
       </c>
-      <c r="B46" s="71"/>
+      <c r="B46" s="72"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="45" t="s">
+      <c r="H46" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="46"/>
-      <c r="J46" s="46"/>
+      <c r="I46" s="38"/>
+      <c r="J46" s="38"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -4667,30 +4667,6 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
     <mergeCell ref="H46:J46"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A46:B46"/>
@@ -4707,6 +4683,30 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -4738,63 +4738,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
-      <c r="J1" s="38"/>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="39"/>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="39"/>
+      <c r="B2" s="45"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="45"/>
+      <c r="I2" s="45"/>
+      <c r="J2" s="45"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="39"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
-      <c r="I3" s="39"/>
-      <c r="J3" s="39"/>
+      <c r="B3" s="45"/>
+      <c r="C3" s="45"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="45"/>
+      <c r="G3" s="45"/>
+      <c r="H3" s="45"/>
+      <c r="I3" s="45"/>
+      <c r="J3" s="45"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="40"/>
-      <c r="I4" s="40"/>
-      <c r="J4" s="40"/>
+      <c r="B4" s="47"/>
+      <c r="C4" s="47"/>
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="47"/>
+      <c r="G4" s="47"/>
+      <c r="H4" s="47"/>
+      <c r="I4" s="47"/>
+      <c r="J4" s="47"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -4804,10 +4804,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="37" t="s">
+      <c r="E5" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="37"/>
+      <c r="F5" s="48"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -4822,10 +4822,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="41">
+      <c r="E6" s="43">
         <v>44</v>
       </c>
-      <c r="F6" s="41"/>
+      <c r="F6" s="43"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>44000</v>
@@ -4841,10 +4841,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="41">
+      <c r="E7" s="43">
         <v>118</v>
       </c>
-      <c r="F7" s="41"/>
+      <c r="F7" s="43"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>59000</v>
@@ -4860,10 +4860,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="41">
+      <c r="E8" s="43">
         <v>510</v>
       </c>
-      <c r="F8" s="41"/>
+      <c r="F8" s="43"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>51000</v>
@@ -4879,8 +4879,8 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="41"/>
-      <c r="F9" s="41"/>
+      <c r="E9" s="43"/>
+      <c r="F9" s="43"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4896,8 +4896,8 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="41"/>
-      <c r="F10" s="41"/>
+      <c r="E10" s="43"/>
+      <c r="F10" s="43"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4913,8 +4913,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
+      <c r="E11" s="43"/>
+      <c r="F11" s="43"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4927,10 +4927,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="37" t="s">
+      <c r="D12" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="37"/>
+      <c r="E12" s="48"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -4977,72 +4977,72 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="42" t="s">
+      <c r="A16" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="42"/>
+      <c r="B16" s="49"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="42" t="s">
+      <c r="H16" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="42"/>
-      <c r="J16" s="42"/>
+      <c r="I16" s="49"/>
+      <c r="J16" s="49"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="42"/>
-      <c r="B17" s="42"/>
+      <c r="A17" s="49"/>
+      <c r="B17" s="49"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="42"/>
-      <c r="I17" s="42"/>
-      <c r="J17" s="42"/>
+      <c r="H17" s="49"/>
+      <c r="I17" s="49"/>
+      <c r="J17" s="49"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="42"/>
-      <c r="B18" s="42"/>
+      <c r="A18" s="49"/>
+      <c r="B18" s="49"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="42"/>
-      <c r="I18" s="42"/>
-      <c r="J18" s="42"/>
+      <c r="H18" s="49"/>
+      <c r="I18" s="49"/>
+      <c r="J18" s="49"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="43"/>
-      <c r="B19" s="43"/>
+      <c r="A19" s="42"/>
+      <c r="B19" s="42"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="44" t="s">
+      <c r="H19" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="44"/>
-      <c r="J19" s="44"/>
+      <c r="I19" s="50"/>
+      <c r="J19" s="50"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="76"/>
-      <c r="B20" s="76"/>
+      <c r="A20" s="75"/>
+      <c r="B20" s="75"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="45" t="s">
+      <c r="H20" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="46"/>
-      <c r="J20" s="46"/>
+      <c r="I20" s="38"/>
+      <c r="J20" s="38"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -5117,60 +5117,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="38" t="s">
+      <c r="A27" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="38"/>
-      <c r="C27" s="38"/>
-      <c r="D27" s="38"/>
-      <c r="E27" s="38"/>
-      <c r="F27" s="38"/>
-      <c r="G27" s="38"/>
-      <c r="H27" s="38"/>
-      <c r="I27" s="38"/>
-      <c r="J27" s="38"/>
+      <c r="B27" s="44"/>
+      <c r="C27" s="44"/>
+      <c r="D27" s="44"/>
+      <c r="E27" s="44"/>
+      <c r="F27" s="44"/>
+      <c r="G27" s="44"/>
+      <c r="H27" s="44"/>
+      <c r="I27" s="44"/>
+      <c r="J27" s="44"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="39" t="s">
+      <c r="A28" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="39"/>
-      <c r="C28" s="39"/>
-      <c r="D28" s="39"/>
-      <c r="E28" s="39"/>
-      <c r="F28" s="39"/>
-      <c r="G28" s="39"/>
-      <c r="H28" s="39"/>
-      <c r="I28" s="39"/>
-      <c r="J28" s="39"/>
+      <c r="B28" s="45"/>
+      <c r="C28" s="45"/>
+      <c r="D28" s="45"/>
+      <c r="E28" s="45"/>
+      <c r="F28" s="45"/>
+      <c r="G28" s="45"/>
+      <c r="H28" s="45"/>
+      <c r="I28" s="45"/>
+      <c r="J28" s="45"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="47" t="s">
+      <c r="A29" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="47"/>
-      <c r="C29" s="47"/>
-      <c r="D29" s="47"/>
-      <c r="E29" s="47"/>
-      <c r="F29" s="47"/>
-      <c r="G29" s="47"/>
-      <c r="H29" s="47"/>
-      <c r="I29" s="47"/>
-      <c r="J29" s="47"/>
+      <c r="B29" s="46"/>
+      <c r="C29" s="46"/>
+      <c r="D29" s="46"/>
+      <c r="E29" s="46"/>
+      <c r="F29" s="46"/>
+      <c r="G29" s="46"/>
+      <c r="H29" s="46"/>
+      <c r="I29" s="46"/>
+      <c r="J29" s="46"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="40" t="s">
+      <c r="A30" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="40"/>
-      <c r="C30" s="40"/>
-      <c r="D30" s="40"/>
-      <c r="E30" s="40"/>
-      <c r="F30" s="40"/>
-      <c r="G30" s="40"/>
-      <c r="H30" s="40"/>
-      <c r="I30" s="40"/>
-      <c r="J30" s="40"/>
+      <c r="B30" s="47"/>
+      <c r="C30" s="47"/>
+      <c r="D30" s="47"/>
+      <c r="E30" s="47"/>
+      <c r="F30" s="47"/>
+      <c r="G30" s="47"/>
+      <c r="H30" s="47"/>
+      <c r="I30" s="47"/>
+      <c r="J30" s="47"/>
     </row>
     <row r="31" spans="1:10" ht="23.25">
       <c r="A31" s="6"/>
@@ -5179,10 +5179,10 @@
       <c r="D31" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="37" t="s">
+      <c r="E31" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="37"/>
+      <c r="F31" s="48"/>
       <c r="G31" s="12" t="s">
         <v>5</v>
       </c>
@@ -5197,10 +5197,10 @@
       <c r="D32" s="11">
         <v>1000</v>
       </c>
-      <c r="E32" s="41">
+      <c r="E32" s="43">
         <v>44</v>
       </c>
-      <c r="F32" s="41"/>
+      <c r="F32" s="43"/>
       <c r="G32" s="11">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>44000</v>
@@ -5216,10 +5216,10 @@
       <c r="D33" s="11">
         <v>500</v>
       </c>
-      <c r="E33" s="41">
+      <c r="E33" s="43">
         <v>118</v>
       </c>
-      <c r="F33" s="41"/>
+      <c r="F33" s="43"/>
       <c r="G33" s="11">
         <f t="shared" si="1"/>
         <v>59000</v>
@@ -5235,10 +5235,10 @@
       <c r="D34" s="11">
         <v>100</v>
       </c>
-      <c r="E34" s="41">
+      <c r="E34" s="43">
         <v>510</v>
       </c>
-      <c r="F34" s="41"/>
+      <c r="F34" s="43"/>
       <c r="G34" s="11">
         <f t="shared" si="1"/>
         <v>51000</v>
@@ -5254,8 +5254,8 @@
       <c r="D35" s="11">
         <v>50</v>
       </c>
-      <c r="E35" s="41"/>
-      <c r="F35" s="41"/>
+      <c r="E35" s="43"/>
+      <c r="F35" s="43"/>
       <c r="G35" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -5271,8 +5271,8 @@
       <c r="D36" s="11">
         <v>20</v>
       </c>
-      <c r="E36" s="41"/>
-      <c r="F36" s="41"/>
+      <c r="E36" s="43"/>
+      <c r="F36" s="43"/>
       <c r="G36" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -5288,8 +5288,8 @@
       <c r="D37" s="11">
         <v>10</v>
       </c>
-      <c r="E37" s="41"/>
-      <c r="F37" s="41"/>
+      <c r="E37" s="43"/>
+      <c r="F37" s="43"/>
       <c r="G37" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -5302,10 +5302,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="75" t="s">
+      <c r="D38" s="76" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="75"/>
+      <c r="E38" s="76"/>
       <c r="F38" s="12"/>
       <c r="G38" s="12">
         <f>SUM(G32:G37)</f>
@@ -5352,72 +5352,72 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="50" t="s">
+      <c r="A42" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="50"/>
+      <c r="B42" s="41"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="50" t="s">
+      <c r="H42" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="50"/>
-      <c r="J42" s="50"/>
+      <c r="I42" s="41"/>
+      <c r="J42" s="41"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="43"/>
-      <c r="B43" s="43"/>
+      <c r="A43" s="42"/>
+      <c r="B43" s="42"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="43"/>
-      <c r="I43" s="43"/>
-      <c r="J43" s="43"/>
+      <c r="H43" s="42"/>
+      <c r="I43" s="42"/>
+      <c r="J43" s="42"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="43"/>
-      <c r="B44" s="43"/>
+      <c r="A44" s="42"/>
+      <c r="B44" s="42"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="43"/>
-      <c r="I44" s="43"/>
-      <c r="J44" s="43"/>
+      <c r="H44" s="42"/>
+      <c r="I44" s="42"/>
+      <c r="J44" s="42"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="43"/>
-      <c r="B45" s="43"/>
+      <c r="A45" s="42"/>
+      <c r="B45" s="42"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="43" t="s">
+      <c r="H45" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="50"/>
-      <c r="J45" s="50"/>
+      <c r="I45" s="41"/>
+      <c r="J45" s="41"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="71"/>
-      <c r="B46" s="71"/>
+      <c r="A46" s="72"/>
+      <c r="B46" s="72"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="45" t="s">
+      <c r="H46" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="46"/>
-      <c r="J46" s="46"/>
+      <c r="I46" s="38"/>
+      <c r="J46" s="38"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -5445,6 +5445,34 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -5457,34 +5485,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -5509,64 +5509,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
-      <c r="J1" s="38"/>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="39"/>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="39"/>
+      <c r="B2" s="45"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="45"/>
+      <c r="I2" s="45"/>
+      <c r="J2" s="45"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="39"/>
-      <c r="B3" s="39"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
-      <c r="I3" s="39"/>
-      <c r="J3" s="39"/>
+      <c r="A3" s="45"/>
+      <c r="B3" s="45"/>
+      <c r="C3" s="45"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="45"/>
+      <c r="G3" s="45"/>
+      <c r="H3" s="45"/>
+      <c r="I3" s="45"/>
+      <c r="J3" s="45"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="40"/>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="40"/>
-      <c r="I4" s="40"/>
-      <c r="J4" s="40"/>
+      <c r="A4" s="47"/>
+      <c r="B4" s="47"/>
+      <c r="C4" s="47"/>
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="47"/>
+      <c r="G4" s="47"/>
+      <c r="H4" s="47"/>
+      <c r="I4" s="47"/>
+      <c r="J4" s="47"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="D5" s="18"/>
-      <c r="E5" s="37"/>
-      <c r="F5" s="37"/>
+      <c r="E5" s="48"/>
+      <c r="F5" s="48"/>
       <c r="G5" s="18"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
@@ -5577,8 +5577,8 @@
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="17"/>
-      <c r="E6" s="41"/>
-      <c r="F6" s="41"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="43"/>
       <c r="G6" s="17"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -5589,8 +5589,8 @@
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
       <c r="D7" s="17"/>
-      <c r="E7" s="41"/>
-      <c r="F7" s="41"/>
+      <c r="E7" s="43"/>
+      <c r="F7" s="43"/>
       <c r="G7" s="17"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
@@ -5601,8 +5601,8 @@
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
       <c r="D8" s="17"/>
-      <c r="E8" s="41"/>
-      <c r="F8" s="41"/>
+      <c r="E8" s="43"/>
+      <c r="F8" s="43"/>
       <c r="G8" s="17"/>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -5613,8 +5613,8 @@
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="17"/>
-      <c r="E9" s="41"/>
-      <c r="F9" s="41"/>
+      <c r="E9" s="43"/>
+      <c r="F9" s="43"/>
       <c r="G9" s="17"/>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -5625,8 +5625,8 @@
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="17"/>
-      <c r="E10" s="41"/>
-      <c r="F10" s="41"/>
+      <c r="E10" s="43"/>
+      <c r="F10" s="43"/>
       <c r="G10" s="17"/>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
@@ -5637,8 +5637,8 @@
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="17"/>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
+      <c r="E11" s="43"/>
+      <c r="F11" s="43"/>
       <c r="G11" s="17"/>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
@@ -5648,8 +5648,8 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="37"/>
-      <c r="E12" s="37"/>
+      <c r="D12" s="48"/>
+      <c r="E12" s="48"/>
       <c r="F12" s="18"/>
       <c r="G12" s="18"/>
       <c r="H12" s="6"/>
@@ -5693,52 +5693,52 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="42"/>
-      <c r="B16" s="42"/>
+      <c r="A16" s="49"/>
+      <c r="B16" s="49"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="42"/>
-      <c r="I16" s="42"/>
-      <c r="J16" s="42"/>
+      <c r="H16" s="49"/>
+      <c r="I16" s="49"/>
+      <c r="J16" s="49"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="42"/>
-      <c r="B17" s="42"/>
+      <c r="A17" s="49"/>
+      <c r="B17" s="49"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="42"/>
-      <c r="I17" s="42"/>
-      <c r="J17" s="42"/>
+      <c r="H17" s="49"/>
+      <c r="I17" s="49"/>
+      <c r="J17" s="49"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="42"/>
-      <c r="B18" s="42"/>
+      <c r="A18" s="49"/>
+      <c r="B18" s="49"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="42"/>
-      <c r="I18" s="42"/>
-      <c r="J18" s="42"/>
+      <c r="H18" s="49"/>
+      <c r="I18" s="49"/>
+      <c r="J18" s="49"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="43"/>
-      <c r="B19" s="43"/>
+      <c r="A19" s="42"/>
+      <c r="B19" s="42"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="44"/>
-      <c r="I19" s="44"/>
-      <c r="J19" s="44"/>
+      <c r="H19" s="50"/>
+      <c r="I19" s="50"/>
+      <c r="J19" s="50"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -5748,9 +5748,9 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="45"/>
-      <c r="I20" s="46"/>
-      <c r="J20" s="46"/>
+      <c r="H20" s="37"/>
+      <c r="I20" s="38"/>
+      <c r="J20" s="38"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -5837,60 +5837,60 @@
       <c r="J27" s="6"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="38" t="s">
+      <c r="A28" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="38"/>
-      <c r="C28" s="38"/>
-      <c r="D28" s="38"/>
-      <c r="E28" s="38"/>
-      <c r="F28" s="38"/>
-      <c r="G28" s="38"/>
-      <c r="H28" s="38"/>
-      <c r="I28" s="38"/>
-      <c r="J28" s="38"/>
+      <c r="B28" s="44"/>
+      <c r="C28" s="44"/>
+      <c r="D28" s="44"/>
+      <c r="E28" s="44"/>
+      <c r="F28" s="44"/>
+      <c r="G28" s="44"/>
+      <c r="H28" s="44"/>
+      <c r="I28" s="44"/>
+      <c r="J28" s="44"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="39" t="s">
+      <c r="A29" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="39"/>
-      <c r="C29" s="39"/>
-      <c r="D29" s="39"/>
-      <c r="E29" s="39"/>
-      <c r="F29" s="39"/>
-      <c r="G29" s="39"/>
-      <c r="H29" s="39"/>
-      <c r="I29" s="39"/>
-      <c r="J29" s="39"/>
+      <c r="B29" s="45"/>
+      <c r="C29" s="45"/>
+      <c r="D29" s="45"/>
+      <c r="E29" s="45"/>
+      <c r="F29" s="45"/>
+      <c r="G29" s="45"/>
+      <c r="H29" s="45"/>
+      <c r="I29" s="45"/>
+      <c r="J29" s="45"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="47" t="s">
+      <c r="A30" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="47"/>
-      <c r="C30" s="47"/>
-      <c r="D30" s="47"/>
-      <c r="E30" s="47"/>
-      <c r="F30" s="47"/>
-      <c r="G30" s="47"/>
-      <c r="H30" s="47"/>
-      <c r="I30" s="47"/>
-      <c r="J30" s="47"/>
+      <c r="B30" s="46"/>
+      <c r="C30" s="46"/>
+      <c r="D30" s="46"/>
+      <c r="E30" s="46"/>
+      <c r="F30" s="46"/>
+      <c r="G30" s="46"/>
+      <c r="H30" s="46"/>
+      <c r="I30" s="46"/>
+      <c r="J30" s="46"/>
     </row>
     <row r="31" spans="1:10" ht="18.75">
-      <c r="A31" s="40" t="s">
+      <c r="A31" s="47" t="s">
         <v>19</v>
       </c>
-      <c r="B31" s="40"/>
-      <c r="C31" s="40"/>
-      <c r="D31" s="40"/>
-      <c r="E31" s="40"/>
-      <c r="F31" s="40"/>
-      <c r="G31" s="40"/>
-      <c r="H31" s="40"/>
-      <c r="I31" s="40"/>
-      <c r="J31" s="40"/>
+      <c r="B31" s="47"/>
+      <c r="C31" s="47"/>
+      <c r="D31" s="47"/>
+      <c r="E31" s="47"/>
+      <c r="F31" s="47"/>
+      <c r="G31" s="47"/>
+      <c r="H31" s="47"/>
+      <c r="I31" s="47"/>
+      <c r="J31" s="47"/>
     </row>
     <row r="32" spans="1:10" ht="20.25">
       <c r="A32" s="6" t="s">
@@ -5901,10 +5901,10 @@
       <c r="D32" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="74" t="s">
+      <c r="E32" s="70" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="74"/>
+      <c r="F32" s="70"/>
       <c r="G32" s="20" t="s">
         <v>5</v>
       </c>
@@ -5919,10 +5919,10 @@
       <c r="D33" s="19">
         <v>1000</v>
       </c>
-      <c r="E33" s="41">
+      <c r="E33" s="43">
         <v>30</v>
       </c>
-      <c r="F33" s="41"/>
+      <c r="F33" s="43"/>
       <c r="G33" s="19">
         <f t="shared" ref="G33:G38" si="0">SUM(D33*E33)</f>
         <v>30000</v>
@@ -5938,10 +5938,10 @@
       <c r="D34" s="19">
         <v>500</v>
       </c>
-      <c r="E34" s="41">
+      <c r="E34" s="43">
         <v>35</v>
       </c>
-      <c r="F34" s="41"/>
+      <c r="F34" s="43"/>
       <c r="G34" s="19">
         <f t="shared" si="0"/>
         <v>17500</v>
@@ -5957,10 +5957,10 @@
       <c r="D35" s="19">
         <v>100</v>
       </c>
-      <c r="E35" s="41">
+      <c r="E35" s="43">
         <v>425</v>
       </c>
-      <c r="F35" s="41"/>
+      <c r="F35" s="43"/>
       <c r="G35" s="19">
         <f t="shared" si="0"/>
         <v>42500</v>
@@ -5976,8 +5976,8 @@
       <c r="D36" s="19">
         <v>50</v>
       </c>
-      <c r="E36" s="41"/>
-      <c r="F36" s="41"/>
+      <c r="E36" s="43"/>
+      <c r="F36" s="43"/>
       <c r="G36" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -5993,8 +5993,8 @@
       <c r="D37" s="19">
         <v>20</v>
       </c>
-      <c r="E37" s="73"/>
-      <c r="F37" s="73"/>
+      <c r="E37" s="74"/>
+      <c r="F37" s="74"/>
       <c r="G37" s="19">
         <f>SUM(D37*E37)</f>
         <v>0</v>
@@ -6010,10 +6010,10 @@
       <c r="D38" s="19">
         <v>10</v>
       </c>
-      <c r="E38" s="73">
+      <c r="E38" s="74">
         <v>100</v>
       </c>
-      <c r="F38" s="73"/>
+      <c r="F38" s="74"/>
       <c r="G38" s="19">
         <f t="shared" si="0"/>
         <v>1000</v>
@@ -6076,58 +6076,58 @@
       <c r="J42" s="6"/>
     </row>
     <row r="43" spans="1:10" ht="15.75">
-      <c r="A43" s="50" t="s">
+      <c r="A43" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="50"/>
+      <c r="B43" s="41"/>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
-      <c r="H43" s="50" t="s">
+      <c r="H43" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="50"/>
-      <c r="J43" s="50"/>
+      <c r="I43" s="41"/>
+      <c r="J43" s="41"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="43"/>
-      <c r="B44" s="43"/>
+      <c r="A44" s="42"/>
+      <c r="B44" s="42"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="43"/>
-      <c r="I44" s="43"/>
-      <c r="J44" s="43"/>
+      <c r="H44" s="42"/>
+      <c r="I44" s="42"/>
+      <c r="J44" s="42"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="43"/>
-      <c r="B45" s="43"/>
+      <c r="A45" s="42"/>
+      <c r="B45" s="42"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="43"/>
-      <c r="I45" s="43"/>
-      <c r="J45" s="43"/>
+      <c r="H45" s="42"/>
+      <c r="I45" s="42"/>
+      <c r="J45" s="42"/>
     </row>
     <row r="46" spans="1:10" ht="15.75">
-      <c r="A46" s="43"/>
-      <c r="B46" s="43"/>
+      <c r="A46" s="42"/>
+      <c r="B46" s="42"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="43" t="s">
+      <c r="H46" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="50"/>
-      <c r="J46" s="50"/>
+      <c r="I46" s="41"/>
+      <c r="J46" s="41"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -6137,20 +6137,30 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="45"/>
-      <c r="I47" s="46"/>
-      <c r="J47" s="46"/>
+      <c r="H47" s="37"/>
+      <c r="I47" s="38"/>
+      <c r="J47" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="H47:J47"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="H43:J43"/>
-    <mergeCell ref="A44:B45"/>
-    <mergeCell ref="H44:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="E38:F38"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A28:J28"/>
@@ -6163,24 +6173,14 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="H47:J47"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="H43:J43"/>
+    <mergeCell ref="A44:B45"/>
+    <mergeCell ref="H44:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -6206,177 +6206,177 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
-      <c r="J1" s="38"/>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="39"/>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="39"/>
+      <c r="B2" s="45"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="45"/>
+      <c r="I2" s="45"/>
+      <c r="J2" s="45"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="87">
+      <c r="A5" s="88">
         <v>1</v>
       </c>
-      <c r="B5" s="79" t="s">
+      <c r="B5" s="81" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="79"/>
-      <c r="D5" s="79"/>
-      <c r="E5" s="79"/>
-      <c r="F5" s="79"/>
-      <c r="G5" s="86">
+      <c r="C5" s="81"/>
+      <c r="D5" s="81"/>
+      <c r="E5" s="81"/>
+      <c r="F5" s="81"/>
+      <c r="G5" s="79">
         <v>1650</v>
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="87"/>
-      <c r="B6" s="79"/>
-      <c r="C6" s="79"/>
-      <c r="D6" s="79"/>
-      <c r="E6" s="79"/>
-      <c r="F6" s="79"/>
-      <c r="G6" s="86"/>
+      <c r="A6" s="88"/>
+      <c r="B6" s="81"/>
+      <c r="C6" s="81"/>
+      <c r="D6" s="81"/>
+      <c r="E6" s="81"/>
+      <c r="F6" s="81"/>
+      <c r="G6" s="79"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="87">
+      <c r="A7" s="88">
         <v>2</v>
       </c>
-      <c r="B7" s="79" t="s">
+      <c r="B7" s="81" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="79"/>
-      <c r="D7" s="79"/>
-      <c r="E7" s="79"/>
-      <c r="F7" s="79"/>
-      <c r="G7" s="86">
+      <c r="C7" s="81"/>
+      <c r="D7" s="81"/>
+      <c r="E7" s="81"/>
+      <c r="F7" s="81"/>
+      <c r="G7" s="79">
         <v>1980</v>
       </c>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="87"/>
-      <c r="B8" s="79"/>
-      <c r="C8" s="79"/>
-      <c r="D8" s="79"/>
-      <c r="E8" s="79"/>
-      <c r="F8" s="79"/>
-      <c r="G8" s="86"/>
+      <c r="A8" s="88"/>
+      <c r="B8" s="81"/>
+      <c r="C8" s="81"/>
+      <c r="D8" s="81"/>
+      <c r="E8" s="81"/>
+      <c r="F8" s="81"/>
+      <c r="G8" s="79"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="87">
+      <c r="A9" s="88">
         <v>3</v>
       </c>
-      <c r="B9" s="79" t="s">
+      <c r="B9" s="81" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="79"/>
-      <c r="D9" s="79"/>
-      <c r="E9" s="79"/>
-      <c r="F9" s="79"/>
-      <c r="G9" s="86">
+      <c r="C9" s="81"/>
+      <c r="D9" s="81"/>
+      <c r="E9" s="81"/>
+      <c r="F9" s="81"/>
+      <c r="G9" s="79">
         <v>10538</v>
       </c>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="87"/>
-      <c r="B10" s="79"/>
-      <c r="C10" s="79"/>
-      <c r="D10" s="79"/>
-      <c r="E10" s="79"/>
-      <c r="F10" s="79"/>
-      <c r="G10" s="86"/>
+      <c r="A10" s="88"/>
+      <c r="B10" s="81"/>
+      <c r="C10" s="81"/>
+      <c r="D10" s="81"/>
+      <c r="E10" s="81"/>
+      <c r="F10" s="81"/>
+      <c r="G10" s="79"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="87">
+      <c r="A11" s="88">
         <v>4</v>
       </c>
-      <c r="B11" s="80" t="s">
+      <c r="B11" s="82" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="81"/>
-      <c r="D11" s="81"/>
-      <c r="E11" s="81"/>
-      <c r="F11" s="82"/>
-      <c r="G11" s="86">
+      <c r="C11" s="83"/>
+      <c r="D11" s="83"/>
+      <c r="E11" s="83"/>
+      <c r="F11" s="84"/>
+      <c r="G11" s="79">
         <v>1100</v>
       </c>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="87"/>
-      <c r="B12" s="83"/>
-      <c r="C12" s="84"/>
-      <c r="D12" s="84"/>
-      <c r="E12" s="84"/>
-      <c r="F12" s="85"/>
-      <c r="G12" s="86"/>
+      <c r="A12" s="88"/>
+      <c r="B12" s="85"/>
+      <c r="C12" s="86"/>
+      <c r="D12" s="86"/>
+      <c r="E12" s="86"/>
+      <c r="F12" s="87"/>
+      <c r="G12" s="79"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="88" t="s">
+      <c r="A13" s="80" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="88"/>
-      <c r="C13" s="88"/>
-      <c r="D13" s="88"/>
-      <c r="E13" s="88"/>
-      <c r="F13" s="88"/>
-      <c r="G13" s="86">
+      <c r="B13" s="80"/>
+      <c r="C13" s="80"/>
+      <c r="D13" s="80"/>
+      <c r="E13" s="80"/>
+      <c r="F13" s="80"/>
+      <c r="G13" s="79">
         <f>SUM(G5:G12)</f>
         <v>15268</v>
       </c>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="88"/>
-      <c r="B14" s="88"/>
-      <c r="C14" s="88"/>
-      <c r="D14" s="88"/>
-      <c r="E14" s="88"/>
-      <c r="F14" s="88"/>
-      <c r="G14" s="86"/>
+      <c r="A14" s="80"/>
+      <c r="B14" s="80"/>
+      <c r="C14" s="80"/>
+      <c r="D14" s="80"/>
+      <c r="E14" s="80"/>
+      <c r="F14" s="80"/>
+      <c r="G14" s="79"/>
     </row>
     <row r="23" spans="1:10" ht="18.75">
-      <c r="A23" s="47" t="s">
+      <c r="A23" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="47"/>
-      <c r="C23" s="47"/>
-      <c r="D23" s="47"/>
-      <c r="E23" s="47"/>
-      <c r="F23" s="47"/>
-      <c r="G23" s="47"/>
-      <c r="H23" s="47"/>
-      <c r="I23" s="47"/>
-      <c r="J23" s="47"/>
+      <c r="B23" s="46"/>
+      <c r="C23" s="46"/>
+      <c r="D23" s="46"/>
+      <c r="E23" s="46"/>
+      <c r="F23" s="46"/>
+      <c r="G23" s="46"/>
+      <c r="H23" s="46"/>
+      <c r="I23" s="46"/>
+      <c r="J23" s="46"/>
     </row>
     <row r="24" spans="1:10" ht="18.75">
-      <c r="A24" s="40"/>
-      <c r="B24" s="40"/>
-      <c r="C24" s="40"/>
-      <c r="D24" s="40"/>
-      <c r="E24" s="40"/>
-      <c r="F24" s="40"/>
-      <c r="G24" s="40"/>
-      <c r="H24" s="40"/>
-      <c r="I24" s="40"/>
-      <c r="J24" s="40"/>
+      <c r="A24" s="47"/>
+      <c r="B24" s="47"/>
+      <c r="C24" s="47"/>
+      <c r="D24" s="47"/>
+      <c r="E24" s="47"/>
+      <c r="F24" s="47"/>
+      <c r="G24" s="47"/>
+      <c r="H24" s="47"/>
+      <c r="I24" s="47"/>
+      <c r="J24" s="47"/>
     </row>
     <row r="25" spans="1:10" ht="20.25">
       <c r="A25" s="6" t="s">
@@ -6387,10 +6387,10 @@
       <c r="D25" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E25" s="74" t="s">
+      <c r="E25" s="70" t="s">
         <v>4</v>
       </c>
-      <c r="F25" s="74"/>
+      <c r="F25" s="70"/>
       <c r="G25" s="20" t="s">
         <v>5</v>
       </c>
@@ -6405,8 +6405,8 @@
       <c r="D26" s="19">
         <v>1000</v>
       </c>
-      <c r="E26" s="41"/>
-      <c r="F26" s="41"/>
+      <c r="E26" s="43"/>
+      <c r="F26" s="43"/>
       <c r="G26" s="19">
         <f t="shared" ref="G26:G31" si="0">SUM(D26*E26)</f>
         <v>0</v>
@@ -6422,10 +6422,10 @@
       <c r="D27" s="19">
         <v>500</v>
       </c>
-      <c r="E27" s="41">
+      <c r="E27" s="43">
         <v>30</v>
       </c>
-      <c r="F27" s="41"/>
+      <c r="F27" s="43"/>
       <c r="G27" s="19">
         <f t="shared" si="0"/>
         <v>15000</v>
@@ -6441,8 +6441,8 @@
       <c r="D28" s="19">
         <v>100</v>
       </c>
-      <c r="E28" s="41"/>
-      <c r="F28" s="41"/>
+      <c r="E28" s="43"/>
+      <c r="F28" s="43"/>
       <c r="G28" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -6458,10 +6458,10 @@
       <c r="D29" s="19">
         <v>50</v>
       </c>
-      <c r="E29" s="41">
+      <c r="E29" s="43">
         <v>5</v>
       </c>
-      <c r="F29" s="41"/>
+      <c r="F29" s="43"/>
       <c r="G29" s="19">
         <f t="shared" si="0"/>
         <v>250</v>
@@ -6477,8 +6477,8 @@
       <c r="D30" s="19">
         <v>20</v>
       </c>
-      <c r="E30" s="73"/>
-      <c r="F30" s="73"/>
+      <c r="E30" s="74"/>
+      <c r="F30" s="74"/>
       <c r="G30" s="19">
         <f>SUM(D30*E30)</f>
         <v>0</v>
@@ -6494,10 +6494,10 @@
       <c r="D31" s="19">
         <v>10</v>
       </c>
-      <c r="E31" s="73">
+      <c r="E31" s="74">
         <v>2</v>
       </c>
-      <c r="F31" s="73"/>
+      <c r="F31" s="74"/>
       <c r="G31" s="19">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -6560,58 +6560,58 @@
       <c r="J35" s="6"/>
     </row>
     <row r="36" spans="1:10" ht="15.75">
-      <c r="A36" s="50" t="s">
+      <c r="A36" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="50"/>
+      <c r="B36" s="41"/>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
       <c r="G36" s="7"/>
-      <c r="H36" s="50" t="s">
+      <c r="H36" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="I36" s="50"/>
-      <c r="J36" s="50"/>
+      <c r="I36" s="41"/>
+      <c r="J36" s="41"/>
     </row>
     <row r="37" spans="1:10">
-      <c r="A37" s="43"/>
-      <c r="B37" s="43"/>
+      <c r="A37" s="42"/>
+      <c r="B37" s="42"/>
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
       <c r="G37" s="6"/>
-      <c r="H37" s="43"/>
-      <c r="I37" s="43"/>
-      <c r="J37" s="43"/>
+      <c r="H37" s="42"/>
+      <c r="I37" s="42"/>
+      <c r="J37" s="42"/>
     </row>
     <row r="38" spans="1:10">
-      <c r="A38" s="43"/>
-      <c r="B38" s="43"/>
+      <c r="A38" s="42"/>
+      <c r="B38" s="42"/>
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
-      <c r="H38" s="43"/>
-      <c r="I38" s="43"/>
-      <c r="J38" s="43"/>
+      <c r="H38" s="42"/>
+      <c r="I38" s="42"/>
+      <c r="J38" s="42"/>
     </row>
     <row r="39" spans="1:10" ht="15.75">
-      <c r="A39" s="43"/>
-      <c r="B39" s="43"/>
+      <c r="A39" s="42"/>
+      <c r="B39" s="42"/>
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
       <c r="F39" s="6"/>
       <c r="G39" s="6"/>
-      <c r="H39" s="43" t="s">
+      <c r="H39" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="I39" s="50"/>
-      <c r="J39" s="50"/>
+      <c r="I39" s="41"/>
+      <c r="J39" s="41"/>
     </row>
     <row r="40" spans="1:10">
       <c r="A40" s="6"/>
@@ -6621,29 +6621,12 @@
       <c r="E40" s="6"/>
       <c r="F40" s="6"/>
       <c r="G40" s="6"/>
-      <c r="H40" s="45"/>
-      <c r="I40" s="46"/>
-      <c r="J40" s="46"/>
+      <c r="H40" s="37"/>
+      <c r="I40" s="38"/>
+      <c r="J40" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="H40:J40"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="H36:J36"/>
-    <mergeCell ref="A37:B38"/>
-    <mergeCell ref="H37:J38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="H39:J39"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="A13:F14"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="E30:F30"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="A23:J23"/>
@@ -6660,6 +6643,23 @@
     <mergeCell ref="B5:F6"/>
     <mergeCell ref="G5:G6"/>
     <mergeCell ref="B7:F8"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="A13:F14"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="H40:J40"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="H36:J36"/>
+    <mergeCell ref="A37:B38"/>
+    <mergeCell ref="H37:J38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="H39:J39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="71" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
23.07.2020 MC Sales Details
</commit_message>
<xml_diff>
--- a/2020/Others/Cash A.xlsx
+++ b/2020/Others/Cash A.xlsx
@@ -122,7 +122,7 @@
     <t>Komola Super Market, Alaipur, Natore</t>
   </si>
   <si>
-    <t>Jafor Iqbal</t>
+    <t>Tanjib</t>
   </si>
 </sst>
 </file>
@@ -515,12 +515,39 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -529,57 +556,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -600,9 +576,21 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -612,27 +600,39 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -640,12 +640,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -667,6 +661,12 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -706,7 +706,7 @@
         <xdr:cNvPr id="2" name="Straight Connector 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -756,7 +756,7 @@
         <xdr:cNvPr id="3" name="Straight Connector 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -806,7 +806,7 @@
         <xdr:cNvPr id="4" name="Straight Connector 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -856,7 +856,7 @@
         <xdr:cNvPr id="5" name="Straight Connector 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000005000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -911,7 +911,7 @@
         <xdr:cNvPr id="12" name="Straight Connector 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00000C000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -961,7 +961,7 @@
         <xdr:cNvPr id="6" name="Straight Connector 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3F693EA6-49EB-42D1-B3CA-F15B26A03B41}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3F693EA6-49EB-42D1-B3CA-F15B26A03B41}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1011,7 +1011,7 @@
         <xdr:cNvPr id="8" name="Straight Connector 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{334CB43E-1331-4297-A64C-0895C28A3BBB}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{334CB43E-1331-4297-A64C-0895C28A3BBB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1061,7 +1061,7 @@
         <xdr:cNvPr id="9" name="Straight Connector 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A0D774EF-0DA8-4AF5-A477-477DFA29C2B2}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0D774EF-0DA8-4AF5-A477-477DFA29C2B2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1111,7 +1111,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0F2A810E-B364-491B-AB34-AE585B8D27E3}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0F2A810E-B364-491B-AB34-AE585B8D27E3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1123,7 +1123,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1161,7 +1161,7 @@
         <xdr:cNvPr id="13" name="Picture 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{BBEAD3A6-FB1B-45D2-BDBE-713A9FCBE3DE}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BBEAD3A6-FB1B-45D2-BDBE-713A9FCBE3DE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1173,7 +1173,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1216,7 +1216,7 @@
         <xdr:cNvPr id="2" name="Straight Connector 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1266,7 +1266,7 @@
         <xdr:cNvPr id="3" name="Straight Connector 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1316,7 +1316,7 @@
         <xdr:cNvPr id="4" name="Straight Connector 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1366,7 +1366,7 @@
         <xdr:cNvPr id="5" name="Straight Connector 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000005000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1416,7 +1416,7 @@
         <xdr:cNvPr id="6" name="Straight Connector 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000006000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1471,7 +1471,7 @@
         <xdr:cNvPr id="7" name="Straight Connector 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000007000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1521,7 +1521,7 @@
         <xdr:cNvPr id="8" name="Straight Connector 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000008000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1571,7 +1571,7 @@
         <xdr:cNvPr id="9" name="Straight Connector 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000009000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000009000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1621,7 +1621,7 @@
         <xdr:cNvPr id="10" name="Straight Connector 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-00000A000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1671,7 +1671,7 @@
         <xdr:cNvPr id="11" name="Straight Connector 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-00000B000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1721,7 +1721,7 @@
         <xdr:cNvPr id="12" name="Straight Connector 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-00000C000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1771,7 +1771,7 @@
         <xdr:cNvPr id="13" name="Straight Connector 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-00000D000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1826,7 +1826,7 @@
         <xdr:cNvPr id="2" name="Straight Connector 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1876,7 +1876,7 @@
         <xdr:cNvPr id="3" name="Straight Connector 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1926,7 +1926,7 @@
         <xdr:cNvPr id="4" name="Straight Connector 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1976,7 +1976,7 @@
         <xdr:cNvPr id="5" name="Straight Connector 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000005000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2031,7 +2031,7 @@
         <xdr:cNvPr id="4" name="Straight Connector 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2081,7 +2081,7 @@
         <xdr:cNvPr id="5" name="Straight Connector 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000005000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2371,7 +2371,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2393,60 +2393,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="44"/>
-      <c r="J1" s="44"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="45"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="45"/>
-      <c r="H2" s="45"/>
-      <c r="I2" s="45"/>
-      <c r="J2" s="45"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="39"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="45" t="s">
+      <c r="A3" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="45"/>
-      <c r="C3" s="45"/>
-      <c r="D3" s="45"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="45"/>
-      <c r="G3" s="45"/>
-      <c r="H3" s="45"/>
-      <c r="I3" s="45"/>
-      <c r="J3" s="45"/>
+      <c r="B3" s="39"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="39"/>
+      <c r="J3" s="39"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="47" t="s">
+      <c r="A4" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="47"/>
-      <c r="C4" s="47"/>
-      <c r="D4" s="47"/>
-      <c r="E4" s="47"/>
-      <c r="F4" s="47"/>
-      <c r="G4" s="47"/>
-      <c r="H4" s="47"/>
-      <c r="I4" s="47"/>
-      <c r="J4" s="47"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="40"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
@@ -2455,10 +2455,10 @@
       <c r="D5" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="48" t="s">
+      <c r="E5" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="48"/>
+      <c r="F5" s="37"/>
       <c r="G5" s="14" t="s">
         <v>5</v>
       </c>
@@ -2473,10 +2473,10 @@
       <c r="D6" s="13">
         <v>1000</v>
       </c>
-      <c r="E6" s="43">
+      <c r="E6" s="41">
         <v>50</v>
       </c>
-      <c r="F6" s="43"/>
+      <c r="F6" s="41"/>
       <c r="G6" s="13">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>50000</v>
@@ -2492,10 +2492,10 @@
       <c r="D7" s="13">
         <v>500</v>
       </c>
-      <c r="E7" s="43">
+      <c r="E7" s="41">
         <v>16</v>
       </c>
-      <c r="F7" s="43"/>
+      <c r="F7" s="41"/>
       <c r="G7" s="13">
         <f t="shared" si="0"/>
         <v>8000</v>
@@ -2511,10 +2511,10 @@
       <c r="D8" s="13">
         <v>100</v>
       </c>
-      <c r="E8" s="43">
+      <c r="E8" s="41">
         <v>151</v>
       </c>
-      <c r="F8" s="43"/>
+      <c r="F8" s="41"/>
       <c r="G8" s="13">
         <f t="shared" si="0"/>
         <v>15100</v>
@@ -2530,10 +2530,10 @@
       <c r="D9" s="13">
         <v>50</v>
       </c>
-      <c r="E9" s="43">
+      <c r="E9" s="41">
         <v>58</v>
       </c>
-      <c r="F9" s="43"/>
+      <c r="F9" s="41"/>
       <c r="G9" s="13">
         <f t="shared" si="0"/>
         <v>2900</v>
@@ -2549,8 +2549,8 @@
       <c r="D10" s="13">
         <v>20</v>
       </c>
-      <c r="E10" s="43"/>
-      <c r="F10" s="43"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="41"/>
       <c r="G10" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2566,8 +2566,8 @@
       <c r="D11" s="13">
         <v>10</v>
       </c>
-      <c r="E11" s="43"/>
-      <c r="F11" s="43"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="41"/>
       <c r="G11" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2580,10 +2580,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="48" t="s">
+      <c r="D12" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="48"/>
+      <c r="E12" s="37"/>
       <c r="F12" s="14"/>
       <c r="G12" s="14">
         <f>SUM(G6:G11)</f>
@@ -2630,58 +2630,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="49" t="s">
+      <c r="A16" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="49"/>
+      <c r="B16" s="42"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="49" t="s">
+      <c r="H16" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="49"/>
-      <c r="J16" s="49"/>
+      <c r="I16" s="42"/>
+      <c r="J16" s="42"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="49"/>
-      <c r="B17" s="49"/>
+      <c r="A17" s="42"/>
+      <c r="B17" s="42"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="49"/>
-      <c r="I17" s="49"/>
-      <c r="J17" s="49"/>
+      <c r="H17" s="42"/>
+      <c r="I17" s="42"/>
+      <c r="J17" s="42"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="49"/>
-      <c r="B18" s="49"/>
+      <c r="A18" s="42"/>
+      <c r="B18" s="42"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="49"/>
-      <c r="I18" s="49"/>
-      <c r="J18" s="49"/>
+      <c r="H18" s="42"/>
+      <c r="I18" s="42"/>
+      <c r="J18" s="42"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="42"/>
-      <c r="B19" s="42"/>
+      <c r="A19" s="43"/>
+      <c r="B19" s="43"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="50" t="s">
+      <c r="H19" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="50"/>
-      <c r="J19" s="50"/>
+      <c r="I19" s="44"/>
+      <c r="J19" s="44"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -2691,11 +2691,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="37" t="s">
+      <c r="H20" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="38"/>
-      <c r="J20" s="38"/>
+      <c r="I20" s="46"/>
+      <c r="J20" s="46"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -2770,60 +2770,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="44" t="s">
+      <c r="A27" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="44"/>
-      <c r="C27" s="44"/>
-      <c r="D27" s="44"/>
-      <c r="E27" s="44"/>
-      <c r="F27" s="44"/>
-      <c r="G27" s="44"/>
-      <c r="H27" s="44"/>
-      <c r="I27" s="44"/>
-      <c r="J27" s="44"/>
+      <c r="B27" s="38"/>
+      <c r="C27" s="38"/>
+      <c r="D27" s="38"/>
+      <c r="E27" s="38"/>
+      <c r="F27" s="38"/>
+      <c r="G27" s="38"/>
+      <c r="H27" s="38"/>
+      <c r="I27" s="38"/>
+      <c r="J27" s="38"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="45" t="s">
+      <c r="A28" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="45"/>
-      <c r="C28" s="45"/>
-      <c r="D28" s="45"/>
-      <c r="E28" s="45"/>
-      <c r="F28" s="45"/>
-      <c r="G28" s="45"/>
-      <c r="H28" s="45"/>
-      <c r="I28" s="45"/>
-      <c r="J28" s="45"/>
+      <c r="B28" s="39"/>
+      <c r="C28" s="39"/>
+      <c r="D28" s="39"/>
+      <c r="E28" s="39"/>
+      <c r="F28" s="39"/>
+      <c r="G28" s="39"/>
+      <c r="H28" s="39"/>
+      <c r="I28" s="39"/>
+      <c r="J28" s="39"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="46" t="s">
+      <c r="A29" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="46"/>
-      <c r="C29" s="46"/>
-      <c r="D29" s="46"/>
-      <c r="E29" s="46"/>
-      <c r="F29" s="46"/>
-      <c r="G29" s="46"/>
-      <c r="H29" s="46"/>
-      <c r="I29" s="46"/>
-      <c r="J29" s="46"/>
+      <c r="B29" s="47"/>
+      <c r="C29" s="47"/>
+      <c r="D29" s="47"/>
+      <c r="E29" s="47"/>
+      <c r="F29" s="47"/>
+      <c r="G29" s="47"/>
+      <c r="H29" s="47"/>
+      <c r="I29" s="47"/>
+      <c r="J29" s="47"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="47" t="s">
+      <c r="A30" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="47"/>
-      <c r="C30" s="47"/>
-      <c r="D30" s="47"/>
-      <c r="E30" s="47"/>
-      <c r="F30" s="47"/>
-      <c r="G30" s="47"/>
-      <c r="H30" s="47"/>
-      <c r="I30" s="47"/>
-      <c r="J30" s="47"/>
+      <c r="B30" s="40"/>
+      <c r="C30" s="40"/>
+      <c r="D30" s="40"/>
+      <c r="E30" s="40"/>
+      <c r="F30" s="40"/>
+      <c r="G30" s="40"/>
+      <c r="H30" s="40"/>
+      <c r="I30" s="40"/>
+      <c r="J30" s="40"/>
     </row>
     <row r="31" spans="1:10" ht="24.95" customHeight="1">
       <c r="A31" s="6"/>
@@ -2832,10 +2832,10 @@
       <c r="D31" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="48" t="s">
+      <c r="E31" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="48"/>
+      <c r="F31" s="37"/>
       <c r="G31" s="15" t="s">
         <v>5</v>
       </c>
@@ -2850,10 +2850,10 @@
       <c r="D32" s="16">
         <v>1000</v>
       </c>
-      <c r="E32" s="43">
+      <c r="E32" s="41">
         <v>50</v>
       </c>
-      <c r="F32" s="43"/>
+      <c r="F32" s="41"/>
       <c r="G32" s="16">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>50000</v>
@@ -2869,10 +2869,10 @@
       <c r="D33" s="16">
         <v>500</v>
       </c>
-      <c r="E33" s="43">
+      <c r="E33" s="41">
         <v>116</v>
       </c>
-      <c r="F33" s="43"/>
+      <c r="F33" s="41"/>
       <c r="G33" s="16">
         <f t="shared" si="1"/>
         <v>58000</v>
@@ -2888,10 +2888,10 @@
       <c r="D34" s="16">
         <v>100</v>
       </c>
-      <c r="E34" s="43">
+      <c r="E34" s="41">
         <v>151</v>
       </c>
-      <c r="F34" s="43"/>
+      <c r="F34" s="41"/>
       <c r="G34" s="16">
         <f t="shared" si="1"/>
         <v>15100</v>
@@ -2907,10 +2907,10 @@
       <c r="D35" s="16">
         <v>50</v>
       </c>
-      <c r="E35" s="43">
+      <c r="E35" s="41">
         <v>58</v>
       </c>
-      <c r="F35" s="43"/>
+      <c r="F35" s="41"/>
       <c r="G35" s="16">
         <f t="shared" si="1"/>
         <v>2900</v>
@@ -2926,8 +2926,8 @@
       <c r="D36" s="16">
         <v>20</v>
       </c>
-      <c r="E36" s="43"/>
-      <c r="F36" s="43"/>
+      <c r="E36" s="41"/>
+      <c r="F36" s="41"/>
       <c r="G36" s="16">
         <f>SUM(D36*E36)</f>
         <v>0</v>
@@ -2943,8 +2943,8 @@
       <c r="D37" s="16">
         <v>10</v>
       </c>
-      <c r="E37" s="43"/>
-      <c r="F37" s="43"/>
+      <c r="E37" s="41"/>
+      <c r="F37" s="41"/>
       <c r="G37" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2957,10 +2957,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="39" t="s">
+      <c r="D38" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="40"/>
+      <c r="E38" s="49"/>
       <c r="F38" s="15"/>
       <c r="G38" s="15">
         <f>SUM(G32:G37)</f>
@@ -3007,58 +3007,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" ht="15.75">
-      <c r="A42" s="41" t="s">
+      <c r="A42" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="41"/>
+      <c r="B42" s="50"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="41" t="s">
+      <c r="H42" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="41"/>
-      <c r="J42" s="41"/>
+      <c r="I42" s="50"/>
+      <c r="J42" s="50"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="42"/>
-      <c r="B43" s="42"/>
+      <c r="A43" s="43"/>
+      <c r="B43" s="43"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="42"/>
-      <c r="I43" s="42"/>
-      <c r="J43" s="42"/>
+      <c r="H43" s="43"/>
+      <c r="I43" s="43"/>
+      <c r="J43" s="43"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="42"/>
-      <c r="B44" s="42"/>
+      <c r="A44" s="43"/>
+      <c r="B44" s="43"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="42"/>
-      <c r="I44" s="42"/>
-      <c r="J44" s="42"/>
+      <c r="H44" s="43"/>
+      <c r="I44" s="43"/>
+      <c r="J44" s="43"/>
     </row>
     <row r="45" spans="1:10" ht="15.75">
-      <c r="A45" s="42"/>
-      <c r="B45" s="42"/>
+      <c r="A45" s="43"/>
+      <c r="B45" s="43"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="42" t="s">
+      <c r="H45" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="41"/>
-      <c r="J45" s="41"/>
+      <c r="I45" s="50"/>
+      <c r="J45" s="50"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="6"/>
@@ -3068,11 +3068,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="37" t="s">
+      <c r="H46" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="38"/>
-      <c r="J46" s="38"/>
+      <c r="I46" s="46"/>
+      <c r="J46" s="46"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -3100,6 +3100,32 @@
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -3112,32 +3138,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.25" footer="0"/>
   <pageSetup scale="85" orientation="portrait" r:id="rId1"/>
@@ -3150,7 +3150,7 @@
   <dimension ref="A1:K47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="M39" sqref="M39:N39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3169,64 +3169,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="58" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
-      <c r="G1" s="51"/>
-      <c r="H1" s="51"/>
-      <c r="I1" s="51"/>
-      <c r="J1" s="51"/>
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+      <c r="G1" s="58"/>
+      <c r="H1" s="58"/>
+      <c r="I1" s="58"/>
+      <c r="J1" s="58"/>
       <c r="K1" s="24"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="52" t="s">
+      <c r="A2" s="59" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="52"/>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="52"/>
-      <c r="I2" s="52"/>
-      <c r="J2" s="52"/>
+      <c r="B2" s="59"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="59"/>
+      <c r="H2" s="59"/>
+      <c r="I2" s="59"/>
+      <c r="J2" s="59"/>
       <c r="K2" s="24"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="52" t="s">
+      <c r="A3" s="59" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="52"/>
-      <c r="C3" s="52"/>
-      <c r="D3" s="52"/>
-      <c r="E3" s="52"/>
-      <c r="F3" s="52"/>
-      <c r="G3" s="52"/>
-      <c r="H3" s="52"/>
-      <c r="I3" s="52"/>
-      <c r="J3" s="52"/>
+      <c r="B3" s="59"/>
+      <c r="C3" s="59"/>
+      <c r="D3" s="59"/>
+      <c r="E3" s="59"/>
+      <c r="F3" s="59"/>
+      <c r="G3" s="59"/>
+      <c r="H3" s="59"/>
+      <c r="I3" s="59"/>
+      <c r="J3" s="59"/>
       <c r="K3" s="24"/>
     </row>
     <row r="4" spans="1:11" ht="26.25">
-      <c r="A4" s="55">
+      <c r="A4" s="66">
         <f ca="1">TODAY()</f>
-        <v>44028</v>
-      </c>
-      <c r="B4" s="55"/>
-      <c r="C4" s="55"/>
-      <c r="D4" s="55"/>
-      <c r="E4" s="55"/>
-      <c r="F4" s="55"/>
-      <c r="G4" s="55"/>
-      <c r="H4" s="55"/>
-      <c r="I4" s="55"/>
-      <c r="J4" s="55"/>
+        <v>44035</v>
+      </c>
+      <c r="B4" s="66"/>
+      <c r="C4" s="66"/>
+      <c r="D4" s="66"/>
+      <c r="E4" s="66"/>
+      <c r="F4" s="66"/>
+      <c r="G4" s="66"/>
+      <c r="H4" s="66"/>
+      <c r="I4" s="66"/>
+      <c r="J4" s="66"/>
       <c r="K4" s="24"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -3236,10 +3236,10 @@
       <c r="D5" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="53" t="s">
+      <c r="E5" s="61" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="53"/>
+      <c r="F5" s="61"/>
       <c r="G5" s="26" t="s">
         <v>5</v>
       </c>
@@ -3254,13 +3254,13 @@
       <c r="D6" s="27">
         <v>1000</v>
       </c>
-      <c r="E6" s="54">
-        <v>130</v>
-      </c>
-      <c r="F6" s="54"/>
+      <c r="E6" s="62">
+        <v>450</v>
+      </c>
+      <c r="F6" s="62"/>
       <c r="G6" s="27">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
-        <v>130000</v>
+        <v>450000</v>
       </c>
       <c r="H6" s="25"/>
       <c r="I6" s="25"/>
@@ -3273,13 +3273,13 @@
       <c r="D7" s="27">
         <v>500</v>
       </c>
-      <c r="E7" s="54">
-        <v>800</v>
-      </c>
-      <c r="F7" s="54"/>
+      <c r="E7" s="62">
+        <v>600</v>
+      </c>
+      <c r="F7" s="62"/>
       <c r="G7" s="27">
         <f t="shared" si="0"/>
-        <v>400000</v>
+        <v>300000</v>
       </c>
       <c r="H7" s="25"/>
       <c r="I7" s="25"/>
@@ -3292,13 +3292,13 @@
       <c r="D8" s="27">
         <v>100</v>
       </c>
-      <c r="E8" s="54">
-        <v>700</v>
-      </c>
-      <c r="F8" s="54"/>
+      <c r="E8" s="62">
+        <v>500</v>
+      </c>
+      <c r="F8" s="62"/>
       <c r="G8" s="27">
         <f t="shared" si="0"/>
-        <v>70000</v>
+        <v>50000</v>
       </c>
       <c r="H8" s="25"/>
       <c r="I8" s="25"/>
@@ -3311,8 +3311,8 @@
       <c r="D9" s="27">
         <v>50</v>
       </c>
-      <c r="E9" s="54"/>
-      <c r="F9" s="54"/>
+      <c r="E9" s="62"/>
+      <c r="F9" s="62"/>
       <c r="G9" s="27">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3328,8 +3328,8 @@
       <c r="D10" s="27">
         <v>20</v>
       </c>
-      <c r="E10" s="54"/>
-      <c r="F10" s="54"/>
+      <c r="E10" s="62"/>
+      <c r="F10" s="62"/>
       <c r="G10" s="27">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3345,8 +3345,8 @@
       <c r="D11" s="27">
         <v>10</v>
       </c>
-      <c r="E11" s="54"/>
-      <c r="F11" s="54"/>
+      <c r="E11" s="62"/>
+      <c r="F11" s="62"/>
       <c r="G11" s="27">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3359,14 +3359,14 @@
       <c r="A12" s="25"/>
       <c r="B12" s="25"/>
       <c r="C12" s="25"/>
-      <c r="D12" s="54" t="s">
+      <c r="D12" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="54"/>
+      <c r="E12" s="62"/>
       <c r="F12" s="27"/>
       <c r="G12" s="22">
         <f>SUM(G6:G11)</f>
-        <v>600000</v>
+        <v>800000</v>
       </c>
       <c r="H12" s="25"/>
       <c r="I12" s="25"/>
@@ -3410,59 +3410,59 @@
     </row>
     <row r="16" spans="1:11">
       <c r="A16" s="28"/>
-      <c r="B16" s="57" t="s">
+      <c r="B16" s="69" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="57"/>
-      <c r="D16" s="57"/>
+      <c r="C16" s="69"/>
+      <c r="D16" s="69"/>
       <c r="E16" s="28"/>
       <c r="F16" s="29"/>
       <c r="G16" s="29"/>
-      <c r="H16" s="56" t="s">
+      <c r="H16" s="68" t="s">
         <v>7</v>
       </c>
-      <c r="I16" s="56"/>
-      <c r="J16" s="56"/>
+      <c r="I16" s="68"/>
+      <c r="J16" s="68"/>
     </row>
     <row r="17" spans="1:11">
-      <c r="A17" s="56"/>
-      <c r="B17" s="56"/>
-      <c r="C17" s="56"/>
-      <c r="D17" s="56"/>
+      <c r="A17" s="68"/>
+      <c r="B17" s="68"/>
+      <c r="C17" s="68"/>
+      <c r="D17" s="68"/>
       <c r="E17" s="29"/>
       <c r="F17" s="29"/>
       <c r="G17" s="29"/>
-      <c r="H17" s="56"/>
-      <c r="I17" s="56"/>
-      <c r="J17" s="56"/>
+      <c r="H17" s="68"/>
+      <c r="I17" s="68"/>
+      <c r="J17" s="68"/>
     </row>
     <row r="18" spans="1:11">
-      <c r="A18" s="56"/>
-      <c r="B18" s="56"/>
-      <c r="C18" s="56"/>
-      <c r="D18" s="56"/>
+      <c r="A18" s="68"/>
+      <c r="B18" s="68"/>
+      <c r="C18" s="68"/>
+      <c r="D18" s="68"/>
       <c r="E18" s="29"/>
       <c r="F18" s="29"/>
       <c r="G18" s="29"/>
-      <c r="H18" s="56"/>
-      <c r="I18" s="56"/>
-      <c r="J18" s="56"/>
+      <c r="H18" s="68"/>
+      <c r="I18" s="68"/>
+      <c r="J18" s="68"/>
     </row>
     <row r="19" spans="1:11" ht="17.25" customHeight="1">
       <c r="A19" s="33"/>
-      <c r="B19" s="58" t="s">
+      <c r="B19" s="67" t="s">
         <v>28</v>
       </c>
-      <c r="C19" s="58"/>
-      <c r="D19" s="58"/>
+      <c r="C19" s="67"/>
+      <c r="D19" s="67"/>
       <c r="E19" s="29"/>
       <c r="F19" s="29"/>
       <c r="G19" s="29"/>
-      <c r="H19" s="49" t="s">
+      <c r="H19" s="42" t="s">
         <v>30</v>
       </c>
-      <c r="I19" s="49"/>
-      <c r="J19" s="49"/>
+      <c r="I19" s="42"/>
+      <c r="J19" s="42"/>
     </row>
     <row r="20" spans="1:11">
       <c r="A20" s="25"/>
@@ -3472,9 +3472,9 @@
       <c r="E20" s="25"/>
       <c r="F20" s="25"/>
       <c r="G20" s="25"/>
-      <c r="H20" s="61"/>
-      <c r="I20" s="62"/>
-      <c r="J20" s="62"/>
+      <c r="H20" s="53"/>
+      <c r="I20" s="54"/>
+      <c r="J20" s="54"/>
     </row>
     <row r="21" spans="1:11">
       <c r="A21" s="25"/>
@@ -3561,66 +3561,66 @@
       <c r="J27" s="25"/>
     </row>
     <row r="28" spans="1:11" ht="31.5">
-      <c r="A28" s="51" t="s">
+      <c r="A28" s="58" t="s">
         <v>26</v>
       </c>
-      <c r="B28" s="51"/>
-      <c r="C28" s="51"/>
-      <c r="D28" s="51"/>
-      <c r="E28" s="51"/>
-      <c r="F28" s="51"/>
-      <c r="G28" s="51"/>
-      <c r="H28" s="51"/>
-      <c r="I28" s="51"/>
-      <c r="J28" s="51"/>
+      <c r="B28" s="58"/>
+      <c r="C28" s="58"/>
+      <c r="D28" s="58"/>
+      <c r="E28" s="58"/>
+      <c r="F28" s="58"/>
+      <c r="G28" s="58"/>
+      <c r="H28" s="58"/>
+      <c r="I28" s="58"/>
+      <c r="J28" s="58"/>
     </row>
     <row r="29" spans="1:11" ht="18">
-      <c r="A29" s="52" t="str">
+      <c r="A29" s="59" t="str">
         <f>A2</f>
         <v>Komola Super Market, Alaipur, Natore</v>
       </c>
-      <c r="B29" s="52"/>
-      <c r="C29" s="52"/>
-      <c r="D29" s="52"/>
-      <c r="E29" s="52"/>
-      <c r="F29" s="52"/>
-      <c r="G29" s="52"/>
-      <c r="H29" s="52"/>
-      <c r="I29" s="52"/>
-      <c r="J29" s="52"/>
+      <c r="B29" s="59"/>
+      <c r="C29" s="59"/>
+      <c r="D29" s="59"/>
+      <c r="E29" s="59"/>
+      <c r="F29" s="59"/>
+      <c r="G29" s="59"/>
+      <c r="H29" s="59"/>
+      <c r="I29" s="59"/>
+      <c r="J29" s="59"/>
     </row>
     <row r="30" spans="1:11" ht="18.75">
-      <c r="A30" s="66" t="str">
+      <c r="A30" s="60" t="str">
         <f>A3</f>
         <v>Cash Details As Per Below</v>
       </c>
-      <c r="B30" s="66"/>
-      <c r="C30" s="66"/>
-      <c r="D30" s="66"/>
-      <c r="E30" s="66"/>
-      <c r="F30" s="66"/>
-      <c r="G30" s="66"/>
-      <c r="H30" s="66"/>
-      <c r="I30" s="66"/>
-      <c r="J30" s="66"/>
+      <c r="B30" s="60"/>
+      <c r="C30" s="60"/>
+      <c r="D30" s="60"/>
+      <c r="E30" s="60"/>
+      <c r="F30" s="60"/>
+      <c r="G30" s="60"/>
+      <c r="H30" s="60"/>
+      <c r="I30" s="60"/>
+      <c r="J30" s="60"/>
       <c r="K30" s="6" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="26.25">
-      <c r="A31" s="55">
+      <c r="A31" s="66">
         <f ca="1">TODAY()</f>
-        <v>44028</v>
-      </c>
-      <c r="B31" s="55"/>
-      <c r="C31" s="55"/>
-      <c r="D31" s="55"/>
-      <c r="E31" s="55"/>
-      <c r="F31" s="55"/>
-      <c r="G31" s="55"/>
-      <c r="H31" s="55"/>
-      <c r="I31" s="55"/>
-      <c r="J31" s="55"/>
+        <v>44035</v>
+      </c>
+      <c r="B31" s="66"/>
+      <c r="C31" s="66"/>
+      <c r="D31" s="66"/>
+      <c r="E31" s="66"/>
+      <c r="F31" s="66"/>
+      <c r="G31" s="66"/>
+      <c r="H31" s="66"/>
+      <c r="I31" s="66"/>
+      <c r="J31" s="66"/>
     </row>
     <row r="32" spans="1:11" ht="27.95" customHeight="1">
       <c r="A32" s="25"/>
@@ -3629,10 +3629,10 @@
       <c r="D32" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="53" t="s">
+      <c r="E32" s="61" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="53"/>
+      <c r="F32" s="61"/>
       <c r="G32" s="26" t="s">
         <v>5</v>
       </c>
@@ -3647,14 +3647,14 @@
       <c r="D33" s="30">
         <v>1000</v>
       </c>
-      <c r="E33" s="54">
+      <c r="E33" s="62">
         <f>E6</f>
-        <v>130</v>
-      </c>
-      <c r="F33" s="54"/>
+        <v>450</v>
+      </c>
+      <c r="F33" s="62"/>
       <c r="G33" s="30">
         <f t="shared" ref="G33:G38" si="1">SUM(D33*E33)</f>
-        <v>130000</v>
+        <v>450000</v>
       </c>
       <c r="H33" s="25"/>
       <c r="I33" s="25"/>
@@ -3667,14 +3667,14 @@
       <c r="D34" s="30">
         <v>500</v>
       </c>
-      <c r="E34" s="54">
+      <c r="E34" s="62">
         <f>E7</f>
-        <v>800</v>
-      </c>
-      <c r="F34" s="54"/>
+        <v>600</v>
+      </c>
+      <c r="F34" s="62"/>
       <c r="G34" s="30">
         <f t="shared" si="1"/>
-        <v>400000</v>
+        <v>300000</v>
       </c>
       <c r="H34" s="25"/>
       <c r="I34" s="25"/>
@@ -3687,14 +3687,14 @@
       <c r="D35" s="30">
         <v>100</v>
       </c>
-      <c r="E35" s="54">
+      <c r="E35" s="62">
         <f>E8</f>
-        <v>700</v>
-      </c>
-      <c r="F35" s="54"/>
+        <v>500</v>
+      </c>
+      <c r="F35" s="62"/>
       <c r="G35" s="30">
         <f t="shared" si="1"/>
-        <v>70000</v>
+        <v>50000</v>
       </c>
       <c r="H35" s="25"/>
       <c r="I35" s="25"/>
@@ -3707,8 +3707,8 @@
       <c r="D36" s="30">
         <v>50</v>
       </c>
-      <c r="E36" s="54"/>
-      <c r="F36" s="54"/>
+      <c r="E36" s="62"/>
+      <c r="F36" s="62"/>
       <c r="G36" s="30">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -3724,8 +3724,8 @@
       <c r="D37" s="30">
         <v>20</v>
       </c>
-      <c r="E37" s="54"/>
-      <c r="F37" s="54"/>
+      <c r="E37" s="62"/>
+      <c r="F37" s="62"/>
       <c r="G37" s="30">
         <f>SUM(D37*E37)</f>
         <v>0</v>
@@ -3741,8 +3741,8 @@
       <c r="D38" s="30">
         <v>10</v>
       </c>
-      <c r="E38" s="54"/>
-      <c r="F38" s="54"/>
+      <c r="E38" s="62"/>
+      <c r="F38" s="62"/>
       <c r="G38" s="30">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -3755,14 +3755,14 @@
       <c r="A39" s="25"/>
       <c r="B39" s="25"/>
       <c r="C39" s="25"/>
-      <c r="D39" s="67" t="s">
+      <c r="D39" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="68"/>
+      <c r="E39" s="64"/>
       <c r="F39" s="30"/>
       <c r="G39" s="23">
         <f>SUM(G33:G38)</f>
-        <v>600000</v>
+        <v>800000</v>
       </c>
       <c r="H39" s="25"/>
       <c r="I39" s="25"/>
@@ -3814,53 +3814,53 @@
       <c r="E43" s="29"/>
       <c r="F43" s="29"/>
       <c r="G43" s="29"/>
-      <c r="H43" s="63" t="s">
+      <c r="H43" s="55" t="s">
         <v>7</v>
       </c>
-      <c r="I43" s="63"/>
-      <c r="J43" s="63"/>
+      <c r="I43" s="55"/>
+      <c r="J43" s="55"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="64"/>
-      <c r="B44" s="64"/>
-      <c r="C44" s="64"/>
-      <c r="D44" s="64"/>
+      <c r="A44" s="56"/>
+      <c r="B44" s="56"/>
+      <c r="C44" s="56"/>
+      <c r="D44" s="56"/>
       <c r="E44" s="25"/>
       <c r="F44" s="25"/>
       <c r="G44" s="25"/>
-      <c r="H44" s="64"/>
-      <c r="I44" s="64"/>
-      <c r="J44" s="64"/>
+      <c r="H44" s="56"/>
+      <c r="I44" s="56"/>
+      <c r="J44" s="56"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="64"/>
-      <c r="B45" s="64"/>
-      <c r="C45" s="64"/>
-      <c r="D45" s="64"/>
+      <c r="A45" s="56"/>
+      <c r="B45" s="56"/>
+      <c r="C45" s="56"/>
+      <c r="D45" s="56"/>
       <c r="E45" s="25"/>
       <c r="F45" s="25"/>
       <c r="G45" s="25"/>
-      <c r="H45" s="64"/>
-      <c r="I45" s="64"/>
-      <c r="J45" s="64"/>
+      <c r="H45" s="56"/>
+      <c r="I45" s="56"/>
+      <c r="J45" s="56"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="31"/>
-      <c r="B46" s="69" t="str">
+      <c r="B46" s="65" t="str">
         <f>B19</f>
         <v>Rahinul Kabir</v>
       </c>
-      <c r="C46" s="69"/>
-      <c r="D46" s="69"/>
+      <c r="C46" s="65"/>
+      <c r="D46" s="65"/>
       <c r="E46" s="32"/>
       <c r="F46" s="32"/>
       <c r="G46" s="32"/>
-      <c r="H46" s="65" t="str">
+      <c r="H46" s="57" t="str">
         <f>H19</f>
-        <v>Jafor Iqbal</v>
-      </c>
-      <c r="I46" s="65"/>
-      <c r="J46" s="65"/>
+        <v>Tanjib</v>
+      </c>
+      <c r="I46" s="57"/>
+      <c r="J46" s="57"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="21"/>
@@ -3870,12 +3870,35 @@
       <c r="E47" s="21"/>
       <c r="F47" s="21"/>
       <c r="G47" s="21"/>
-      <c r="H47" s="59"/>
-      <c r="I47" s="60"/>
-      <c r="J47" s="60"/>
+      <c r="H47" s="51"/>
+      <c r="I47" s="52"/>
+      <c r="J47" s="52"/>
     </row>
   </sheetData>
   <mergeCells count="37">
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="A17:D18"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="A31:J31"/>
+    <mergeCell ref="B19:D19"/>
     <mergeCell ref="H47:J47"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="H43:J43"/>
@@ -3890,29 +3913,6 @@
     <mergeCell ref="D39:E39"/>
     <mergeCell ref="B46:D46"/>
     <mergeCell ref="A44:D45"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="A31:J31"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="A17:D18"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="A4:J4"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -3944,63 +3944,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="44"/>
-      <c r="J1" s="44"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="45"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="45"/>
-      <c r="H2" s="45"/>
-      <c r="I2" s="45"/>
-      <c r="J2" s="45"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="39"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="45" t="s">
+      <c r="A3" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="45"/>
-      <c r="C3" s="45"/>
-      <c r="D3" s="45"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="45"/>
-      <c r="G3" s="45"/>
-      <c r="H3" s="45"/>
-      <c r="I3" s="45"/>
-      <c r="J3" s="45"/>
+      <c r="B3" s="39"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="39"/>
+      <c r="J3" s="39"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="47" t="s">
+      <c r="A4" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="47"/>
-      <c r="C4" s="47"/>
-      <c r="D4" s="47"/>
-      <c r="E4" s="47"/>
-      <c r="F4" s="47"/>
-      <c r="G4" s="47"/>
-      <c r="H4" s="47"/>
-      <c r="I4" s="47"/>
-      <c r="J4" s="47"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="40"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -4010,10 +4010,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="48" t="s">
+      <c r="E5" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="48"/>
+      <c r="F5" s="37"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -4028,10 +4028,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="43">
+      <c r="E6" s="41">
         <v>68</v>
       </c>
-      <c r="F6" s="43"/>
+      <c r="F6" s="41"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>68000</v>
@@ -4047,10 +4047,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="43">
+      <c r="E7" s="41">
         <v>135</v>
       </c>
-      <c r="F7" s="43"/>
+      <c r="F7" s="41"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>67500</v>
@@ -4066,10 +4066,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="43">
+      <c r="E8" s="41">
         <v>53</v>
       </c>
-      <c r="F8" s="43"/>
+      <c r="F8" s="41"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>5300</v>
@@ -4085,10 +4085,10 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="43">
+      <c r="E9" s="41">
         <v>2</v>
       </c>
-      <c r="F9" s="43"/>
+      <c r="F9" s="41"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -4104,10 +4104,10 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="43">
+      <c r="E10" s="41">
         <v>5</v>
       </c>
-      <c r="F10" s="43"/>
+      <c r="F10" s="41"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -4123,8 +4123,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="43"/>
-      <c r="F11" s="43"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="41"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4137,10 +4137,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="48" t="s">
+      <c r="D12" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="48"/>
+      <c r="E12" s="37"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -4187,76 +4187,76 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="49" t="s">
+      <c r="A16" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="49"/>
+      <c r="B16" s="42"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="49" t="s">
+      <c r="H16" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="49"/>
-      <c r="J16" s="49"/>
+      <c r="I16" s="42"/>
+      <c r="J16" s="42"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="49"/>
-      <c r="B17" s="49"/>
+      <c r="A17" s="42"/>
+      <c r="B17" s="42"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="49"/>
-      <c r="I17" s="49"/>
-      <c r="J17" s="49"/>
+      <c r="H17" s="42"/>
+      <c r="I17" s="42"/>
+      <c r="J17" s="42"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="49"/>
-      <c r="B18" s="49"/>
+      <c r="A18" s="42"/>
+      <c r="B18" s="42"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="49"/>
-      <c r="I18" s="49"/>
-      <c r="J18" s="49"/>
+      <c r="H18" s="42"/>
+      <c r="I18" s="42"/>
+      <c r="J18" s="42"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="42" t="s">
+      <c r="A19" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="42"/>
+      <c r="B19" s="43"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="50" t="s">
+      <c r="H19" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="50"/>
-      <c r="J19" s="50"/>
+      <c r="I19" s="44"/>
+      <c r="J19" s="44"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="71" t="s">
+      <c r="A20" s="70" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="71"/>
+      <c r="B20" s="70"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="37" t="s">
+      <c r="H20" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="38"/>
-      <c r="J20" s="38"/>
+      <c r="I20" s="46"/>
+      <c r="J20" s="46"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4331,60 +4331,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="44" t="s">
+      <c r="A27" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="44"/>
-      <c r="C27" s="44"/>
-      <c r="D27" s="44"/>
-      <c r="E27" s="44"/>
-      <c r="F27" s="44"/>
-      <c r="G27" s="44"/>
-      <c r="H27" s="44"/>
-      <c r="I27" s="44"/>
-      <c r="J27" s="44"/>
+      <c r="B27" s="38"/>
+      <c r="C27" s="38"/>
+      <c r="D27" s="38"/>
+      <c r="E27" s="38"/>
+      <c r="F27" s="38"/>
+      <c r="G27" s="38"/>
+      <c r="H27" s="38"/>
+      <c r="I27" s="38"/>
+      <c r="J27" s="38"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="45" t="s">
+      <c r="A28" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="45"/>
-      <c r="C28" s="45"/>
-      <c r="D28" s="45"/>
-      <c r="E28" s="45"/>
-      <c r="F28" s="45"/>
-      <c r="G28" s="45"/>
-      <c r="H28" s="45"/>
-      <c r="I28" s="45"/>
-      <c r="J28" s="45"/>
+      <c r="B28" s="39"/>
+      <c r="C28" s="39"/>
+      <c r="D28" s="39"/>
+      <c r="E28" s="39"/>
+      <c r="F28" s="39"/>
+      <c r="G28" s="39"/>
+      <c r="H28" s="39"/>
+      <c r="I28" s="39"/>
+      <c r="J28" s="39"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="46" t="s">
+      <c r="A29" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="46"/>
-      <c r="C29" s="46"/>
-      <c r="D29" s="46"/>
-      <c r="E29" s="46"/>
-      <c r="F29" s="46"/>
-      <c r="G29" s="46"/>
-      <c r="H29" s="46"/>
-      <c r="I29" s="46"/>
-      <c r="J29" s="46"/>
+      <c r="B29" s="47"/>
+      <c r="C29" s="47"/>
+      <c r="D29" s="47"/>
+      <c r="E29" s="47"/>
+      <c r="F29" s="47"/>
+      <c r="G29" s="47"/>
+      <c r="H29" s="47"/>
+      <c r="I29" s="47"/>
+      <c r="J29" s="47"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="47" t="s">
+      <c r="A30" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="47"/>
-      <c r="C30" s="47"/>
-      <c r="D30" s="47"/>
-      <c r="E30" s="47"/>
-      <c r="F30" s="47"/>
-      <c r="G30" s="47"/>
-      <c r="H30" s="47"/>
-      <c r="I30" s="47"/>
-      <c r="J30" s="47"/>
+      <c r="B30" s="40"/>
+      <c r="C30" s="40"/>
+      <c r="D30" s="40"/>
+      <c r="E30" s="40"/>
+      <c r="F30" s="40"/>
+      <c r="G30" s="40"/>
+      <c r="H30" s="40"/>
+      <c r="I30" s="40"/>
+      <c r="J30" s="40"/>
     </row>
     <row r="31" spans="1:10" ht="20.25">
       <c r="A31" s="6"/>
@@ -4393,10 +4393,10 @@
       <c r="D31" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="70" t="s">
+      <c r="E31" s="74" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="70"/>
+      <c r="F31" s="74"/>
       <c r="G31" s="9" t="s">
         <v>5</v>
       </c>
@@ -4411,10 +4411,10 @@
       <c r="D32" s="2">
         <v>1000</v>
       </c>
-      <c r="E32" s="74">
+      <c r="E32" s="73">
         <v>68</v>
       </c>
-      <c r="F32" s="74"/>
+      <c r="F32" s="73"/>
       <c r="G32" s="2">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>68000</v>
@@ -4430,10 +4430,10 @@
       <c r="D33" s="2">
         <v>500</v>
       </c>
-      <c r="E33" s="74">
+      <c r="E33" s="73">
         <v>135</v>
       </c>
-      <c r="F33" s="74"/>
+      <c r="F33" s="73"/>
       <c r="G33" s="2">
         <f t="shared" si="1"/>
         <v>67500</v>
@@ -4449,10 +4449,10 @@
       <c r="D34" s="2">
         <v>100</v>
       </c>
-      <c r="E34" s="74">
+      <c r="E34" s="73">
         <v>53</v>
       </c>
-      <c r="F34" s="74"/>
+      <c r="F34" s="73"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
         <v>5300</v>
@@ -4468,10 +4468,10 @@
       <c r="D35" s="2">
         <v>50</v>
       </c>
-      <c r="E35" s="74">
+      <c r="E35" s="73">
         <v>2</v>
       </c>
-      <c r="F35" s="74"/>
+      <c r="F35" s="73"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4487,10 +4487,10 @@
       <c r="D36" s="2">
         <v>20</v>
       </c>
-      <c r="E36" s="74">
+      <c r="E36" s="73">
         <v>5</v>
       </c>
-      <c r="F36" s="74"/>
+      <c r="F36" s="73"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4506,8 +4506,8 @@
       <c r="D37" s="2">
         <v>10</v>
       </c>
-      <c r="E37" s="74"/>
-      <c r="F37" s="74"/>
+      <c r="E37" s="73"/>
+      <c r="F37" s="73"/>
       <c r="G37" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4520,10 +4520,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="73" t="s">
+      <c r="D38" s="72" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="73"/>
+      <c r="E38" s="72"/>
       <c r="F38" s="9"/>
       <c r="G38" s="9">
         <f>SUM(G32:G37)</f>
@@ -4570,76 +4570,76 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="41" t="s">
+      <c r="A42" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="41"/>
+      <c r="B42" s="50"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="41" t="s">
+      <c r="H42" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="41"/>
-      <c r="J42" s="41"/>
+      <c r="I42" s="50"/>
+      <c r="J42" s="50"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="42"/>
-      <c r="B43" s="42"/>
+      <c r="A43" s="43"/>
+      <c r="B43" s="43"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="42"/>
-      <c r="I43" s="42"/>
-      <c r="J43" s="42"/>
+      <c r="H43" s="43"/>
+      <c r="I43" s="43"/>
+      <c r="J43" s="43"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="42"/>
-      <c r="B44" s="42"/>
+      <c r="A44" s="43"/>
+      <c r="B44" s="43"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="42"/>
-      <c r="I44" s="42"/>
-      <c r="J44" s="42"/>
+      <c r="H44" s="43"/>
+      <c r="I44" s="43"/>
+      <c r="J44" s="43"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="42" t="s">
+      <c r="A45" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="B45" s="42"/>
+      <c r="B45" s="43"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="42" t="s">
+      <c r="H45" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="41"/>
-      <c r="J45" s="41"/>
+      <c r="I45" s="50"/>
+      <c r="J45" s="50"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="72" t="s">
+      <c r="A46" s="71" t="s">
         <v>14</v>
       </c>
-      <c r="B46" s="72"/>
+      <c r="B46" s="71"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="37" t="s">
+      <c r="H46" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="38"/>
-      <c r="J46" s="38"/>
+      <c r="I46" s="46"/>
+      <c r="J46" s="46"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -4667,6 +4667,30 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
     <mergeCell ref="H46:J46"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A46:B46"/>
@@ -4683,30 +4707,6 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -4738,63 +4738,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="44"/>
-      <c r="J1" s="44"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="45"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="45"/>
-      <c r="H2" s="45"/>
-      <c r="I2" s="45"/>
-      <c r="J2" s="45"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="39"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="45" t="s">
+      <c r="A3" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="45"/>
-      <c r="C3" s="45"/>
-      <c r="D3" s="45"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="45"/>
-      <c r="G3" s="45"/>
-      <c r="H3" s="45"/>
-      <c r="I3" s="45"/>
-      <c r="J3" s="45"/>
+      <c r="B3" s="39"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="39"/>
+      <c r="J3" s="39"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="47" t="s">
+      <c r="A4" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="47"/>
-      <c r="C4" s="47"/>
-      <c r="D4" s="47"/>
-      <c r="E4" s="47"/>
-      <c r="F4" s="47"/>
-      <c r="G4" s="47"/>
-      <c r="H4" s="47"/>
-      <c r="I4" s="47"/>
-      <c r="J4" s="47"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="40"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -4804,10 +4804,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="48" t="s">
+      <c r="E5" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="48"/>
+      <c r="F5" s="37"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -4822,10 +4822,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="43">
+      <c r="E6" s="41">
         <v>44</v>
       </c>
-      <c r="F6" s="43"/>
+      <c r="F6" s="41"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>44000</v>
@@ -4841,10 +4841,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="43">
+      <c r="E7" s="41">
         <v>118</v>
       </c>
-      <c r="F7" s="43"/>
+      <c r="F7" s="41"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>59000</v>
@@ -4860,10 +4860,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="43">
+      <c r="E8" s="41">
         <v>510</v>
       </c>
-      <c r="F8" s="43"/>
+      <c r="F8" s="41"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>51000</v>
@@ -4879,8 +4879,8 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="43"/>
-      <c r="F9" s="43"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="41"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4896,8 +4896,8 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="43"/>
-      <c r="F10" s="43"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="41"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4913,8 +4913,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="43"/>
-      <c r="F11" s="43"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="41"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4927,10 +4927,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="48" t="s">
+      <c r="D12" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="48"/>
+      <c r="E12" s="37"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -4977,72 +4977,72 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="49" t="s">
+      <c r="A16" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="49"/>
+      <c r="B16" s="42"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="49" t="s">
+      <c r="H16" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="49"/>
-      <c r="J16" s="49"/>
+      <c r="I16" s="42"/>
+      <c r="J16" s="42"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="49"/>
-      <c r="B17" s="49"/>
+      <c r="A17" s="42"/>
+      <c r="B17" s="42"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="49"/>
-      <c r="I17" s="49"/>
-      <c r="J17" s="49"/>
+      <c r="H17" s="42"/>
+      <c r="I17" s="42"/>
+      <c r="J17" s="42"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="49"/>
-      <c r="B18" s="49"/>
+      <c r="A18" s="42"/>
+      <c r="B18" s="42"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="49"/>
-      <c r="I18" s="49"/>
-      <c r="J18" s="49"/>
+      <c r="H18" s="42"/>
+      <c r="I18" s="42"/>
+      <c r="J18" s="42"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="42"/>
-      <c r="B19" s="42"/>
+      <c r="A19" s="43"/>
+      <c r="B19" s="43"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="50" t="s">
+      <c r="H19" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="50"/>
-      <c r="J19" s="50"/>
+      <c r="I19" s="44"/>
+      <c r="J19" s="44"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="75"/>
-      <c r="B20" s="75"/>
+      <c r="A20" s="76"/>
+      <c r="B20" s="76"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="37" t="s">
+      <c r="H20" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="38"/>
-      <c r="J20" s="38"/>
+      <c r="I20" s="46"/>
+      <c r="J20" s="46"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -5117,60 +5117,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="44" t="s">
+      <c r="A27" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="44"/>
-      <c r="C27" s="44"/>
-      <c r="D27" s="44"/>
-      <c r="E27" s="44"/>
-      <c r="F27" s="44"/>
-      <c r="G27" s="44"/>
-      <c r="H27" s="44"/>
-      <c r="I27" s="44"/>
-      <c r="J27" s="44"/>
+      <c r="B27" s="38"/>
+      <c r="C27" s="38"/>
+      <c r="D27" s="38"/>
+      <c r="E27" s="38"/>
+      <c r="F27" s="38"/>
+      <c r="G27" s="38"/>
+      <c r="H27" s="38"/>
+      <c r="I27" s="38"/>
+      <c r="J27" s="38"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="45" t="s">
+      <c r="A28" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="45"/>
-      <c r="C28" s="45"/>
-      <c r="D28" s="45"/>
-      <c r="E28" s="45"/>
-      <c r="F28" s="45"/>
-      <c r="G28" s="45"/>
-      <c r="H28" s="45"/>
-      <c r="I28" s="45"/>
-      <c r="J28" s="45"/>
+      <c r="B28" s="39"/>
+      <c r="C28" s="39"/>
+      <c r="D28" s="39"/>
+      <c r="E28" s="39"/>
+      <c r="F28" s="39"/>
+      <c r="G28" s="39"/>
+      <c r="H28" s="39"/>
+      <c r="I28" s="39"/>
+      <c r="J28" s="39"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="46" t="s">
+      <c r="A29" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="46"/>
-      <c r="C29" s="46"/>
-      <c r="D29" s="46"/>
-      <c r="E29" s="46"/>
-      <c r="F29" s="46"/>
-      <c r="G29" s="46"/>
-      <c r="H29" s="46"/>
-      <c r="I29" s="46"/>
-      <c r="J29" s="46"/>
+      <c r="B29" s="47"/>
+      <c r="C29" s="47"/>
+      <c r="D29" s="47"/>
+      <c r="E29" s="47"/>
+      <c r="F29" s="47"/>
+      <c r="G29" s="47"/>
+      <c r="H29" s="47"/>
+      <c r="I29" s="47"/>
+      <c r="J29" s="47"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="47" t="s">
+      <c r="A30" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="47"/>
-      <c r="C30" s="47"/>
-      <c r="D30" s="47"/>
-      <c r="E30" s="47"/>
-      <c r="F30" s="47"/>
-      <c r="G30" s="47"/>
-      <c r="H30" s="47"/>
-      <c r="I30" s="47"/>
-      <c r="J30" s="47"/>
+      <c r="B30" s="40"/>
+      <c r="C30" s="40"/>
+      <c r="D30" s="40"/>
+      <c r="E30" s="40"/>
+      <c r="F30" s="40"/>
+      <c r="G30" s="40"/>
+      <c r="H30" s="40"/>
+      <c r="I30" s="40"/>
+      <c r="J30" s="40"/>
     </row>
     <row r="31" spans="1:10" ht="23.25">
       <c r="A31" s="6"/>
@@ -5179,10 +5179,10 @@
       <c r="D31" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="48" t="s">
+      <c r="E31" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="48"/>
+      <c r="F31" s="37"/>
       <c r="G31" s="12" t="s">
         <v>5</v>
       </c>
@@ -5197,10 +5197,10 @@
       <c r="D32" s="11">
         <v>1000</v>
       </c>
-      <c r="E32" s="43">
+      <c r="E32" s="41">
         <v>44</v>
       </c>
-      <c r="F32" s="43"/>
+      <c r="F32" s="41"/>
       <c r="G32" s="11">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>44000</v>
@@ -5216,10 +5216,10 @@
       <c r="D33" s="11">
         <v>500</v>
       </c>
-      <c r="E33" s="43">
+      <c r="E33" s="41">
         <v>118</v>
       </c>
-      <c r="F33" s="43"/>
+      <c r="F33" s="41"/>
       <c r="G33" s="11">
         <f t="shared" si="1"/>
         <v>59000</v>
@@ -5235,10 +5235,10 @@
       <c r="D34" s="11">
         <v>100</v>
       </c>
-      <c r="E34" s="43">
+      <c r="E34" s="41">
         <v>510</v>
       </c>
-      <c r="F34" s="43"/>
+      <c r="F34" s="41"/>
       <c r="G34" s="11">
         <f t="shared" si="1"/>
         <v>51000</v>
@@ -5254,8 +5254,8 @@
       <c r="D35" s="11">
         <v>50</v>
       </c>
-      <c r="E35" s="43"/>
-      <c r="F35" s="43"/>
+      <c r="E35" s="41"/>
+      <c r="F35" s="41"/>
       <c r="G35" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -5271,8 +5271,8 @@
       <c r="D36" s="11">
         <v>20</v>
       </c>
-      <c r="E36" s="43"/>
-      <c r="F36" s="43"/>
+      <c r="E36" s="41"/>
+      <c r="F36" s="41"/>
       <c r="G36" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -5288,8 +5288,8 @@
       <c r="D37" s="11">
         <v>10</v>
       </c>
-      <c r="E37" s="43"/>
-      <c r="F37" s="43"/>
+      <c r="E37" s="41"/>
+      <c r="F37" s="41"/>
       <c r="G37" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -5302,10 +5302,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="76" t="s">
+      <c r="D38" s="75" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="76"/>
+      <c r="E38" s="75"/>
       <c r="F38" s="12"/>
       <c r="G38" s="12">
         <f>SUM(G32:G37)</f>
@@ -5352,72 +5352,72 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="41" t="s">
+      <c r="A42" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="41"/>
+      <c r="B42" s="50"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="41" t="s">
+      <c r="H42" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="41"/>
-      <c r="J42" s="41"/>
+      <c r="I42" s="50"/>
+      <c r="J42" s="50"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="42"/>
-      <c r="B43" s="42"/>
+      <c r="A43" s="43"/>
+      <c r="B43" s="43"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="42"/>
-      <c r="I43" s="42"/>
-      <c r="J43" s="42"/>
+      <c r="H43" s="43"/>
+      <c r="I43" s="43"/>
+      <c r="J43" s="43"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="42"/>
-      <c r="B44" s="42"/>
+      <c r="A44" s="43"/>
+      <c r="B44" s="43"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="42"/>
-      <c r="I44" s="42"/>
-      <c r="J44" s="42"/>
+      <c r="H44" s="43"/>
+      <c r="I44" s="43"/>
+      <c r="J44" s="43"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="42"/>
-      <c r="B45" s="42"/>
+      <c r="A45" s="43"/>
+      <c r="B45" s="43"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="42" t="s">
+      <c r="H45" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="41"/>
-      <c r="J45" s="41"/>
+      <c r="I45" s="50"/>
+      <c r="J45" s="50"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="72"/>
-      <c r="B46" s="72"/>
+      <c r="A46" s="71"/>
+      <c r="B46" s="71"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="37" t="s">
+      <c r="H46" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="38"/>
-      <c r="J46" s="38"/>
+      <c r="I46" s="46"/>
+      <c r="J46" s="46"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -5445,16 +5445,24 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="H20:J20"/>
@@ -5467,24 +5475,16 @@
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="E35:F35"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -5509,64 +5509,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="44"/>
-      <c r="J1" s="44"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="45"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="45"/>
-      <c r="H2" s="45"/>
-      <c r="I2" s="45"/>
-      <c r="J2" s="45"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="39"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="45"/>
-      <c r="B3" s="45"/>
-      <c r="C3" s="45"/>
-      <c r="D3" s="45"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="45"/>
-      <c r="G3" s="45"/>
-      <c r="H3" s="45"/>
-      <c r="I3" s="45"/>
-      <c r="J3" s="45"/>
+      <c r="A3" s="39"/>
+      <c r="B3" s="39"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="39"/>
+      <c r="J3" s="39"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="47"/>
-      <c r="B4" s="47"/>
-      <c r="C4" s="47"/>
-      <c r="D4" s="47"/>
-      <c r="E4" s="47"/>
-      <c r="F4" s="47"/>
-      <c r="G4" s="47"/>
-      <c r="H4" s="47"/>
-      <c r="I4" s="47"/>
-      <c r="J4" s="47"/>
+      <c r="A4" s="40"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="40"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="D5" s="18"/>
-      <c r="E5" s="48"/>
-      <c r="F5" s="48"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="37"/>
       <c r="G5" s="18"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
@@ -5577,8 +5577,8 @@
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="17"/>
-      <c r="E6" s="43"/>
-      <c r="F6" s="43"/>
+      <c r="E6" s="41"/>
+      <c r="F6" s="41"/>
       <c r="G6" s="17"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -5589,8 +5589,8 @@
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
       <c r="D7" s="17"/>
-      <c r="E7" s="43"/>
-      <c r="F7" s="43"/>
+      <c r="E7" s="41"/>
+      <c r="F7" s="41"/>
       <c r="G7" s="17"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
@@ -5601,8 +5601,8 @@
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
       <c r="D8" s="17"/>
-      <c r="E8" s="43"/>
-      <c r="F8" s="43"/>
+      <c r="E8" s="41"/>
+      <c r="F8" s="41"/>
       <c r="G8" s="17"/>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -5613,8 +5613,8 @@
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="17"/>
-      <c r="E9" s="43"/>
-      <c r="F9" s="43"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="41"/>
       <c r="G9" s="17"/>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -5625,8 +5625,8 @@
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="17"/>
-      <c r="E10" s="43"/>
-      <c r="F10" s="43"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="41"/>
       <c r="G10" s="17"/>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
@@ -5637,8 +5637,8 @@
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="17"/>
-      <c r="E11" s="43"/>
-      <c r="F11" s="43"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="41"/>
       <c r="G11" s="17"/>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
@@ -5648,8 +5648,8 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="48"/>
-      <c r="E12" s="48"/>
+      <c r="D12" s="37"/>
+      <c r="E12" s="37"/>
       <c r="F12" s="18"/>
       <c r="G12" s="18"/>
       <c r="H12" s="6"/>
@@ -5693,52 +5693,52 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="49"/>
-      <c r="B16" s="49"/>
+      <c r="A16" s="42"/>
+      <c r="B16" s="42"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="49"/>
-      <c r="I16" s="49"/>
-      <c r="J16" s="49"/>
+      <c r="H16" s="42"/>
+      <c r="I16" s="42"/>
+      <c r="J16" s="42"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="49"/>
-      <c r="B17" s="49"/>
+      <c r="A17" s="42"/>
+      <c r="B17" s="42"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="49"/>
-      <c r="I17" s="49"/>
-      <c r="J17" s="49"/>
+      <c r="H17" s="42"/>
+      <c r="I17" s="42"/>
+      <c r="J17" s="42"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="49"/>
-      <c r="B18" s="49"/>
+      <c r="A18" s="42"/>
+      <c r="B18" s="42"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="49"/>
-      <c r="I18" s="49"/>
-      <c r="J18" s="49"/>
+      <c r="H18" s="42"/>
+      <c r="I18" s="42"/>
+      <c r="J18" s="42"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="42"/>
-      <c r="B19" s="42"/>
+      <c r="A19" s="43"/>
+      <c r="B19" s="43"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="50"/>
-      <c r="I19" s="50"/>
-      <c r="J19" s="50"/>
+      <c r="H19" s="44"/>
+      <c r="I19" s="44"/>
+      <c r="J19" s="44"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -5748,9 +5748,9 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="37"/>
-      <c r="I20" s="38"/>
-      <c r="J20" s="38"/>
+      <c r="H20" s="45"/>
+      <c r="I20" s="46"/>
+      <c r="J20" s="46"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -5837,60 +5837,60 @@
       <c r="J27" s="6"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="44" t="s">
+      <c r="A28" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="44"/>
-      <c r="C28" s="44"/>
-      <c r="D28" s="44"/>
-      <c r="E28" s="44"/>
-      <c r="F28" s="44"/>
-      <c r="G28" s="44"/>
-      <c r="H28" s="44"/>
-      <c r="I28" s="44"/>
-      <c r="J28" s="44"/>
+      <c r="B28" s="38"/>
+      <c r="C28" s="38"/>
+      <c r="D28" s="38"/>
+      <c r="E28" s="38"/>
+      <c r="F28" s="38"/>
+      <c r="G28" s="38"/>
+      <c r="H28" s="38"/>
+      <c r="I28" s="38"/>
+      <c r="J28" s="38"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="45" t="s">
+      <c r="A29" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="45"/>
-      <c r="C29" s="45"/>
-      <c r="D29" s="45"/>
-      <c r="E29" s="45"/>
-      <c r="F29" s="45"/>
-      <c r="G29" s="45"/>
-      <c r="H29" s="45"/>
-      <c r="I29" s="45"/>
-      <c r="J29" s="45"/>
+      <c r="B29" s="39"/>
+      <c r="C29" s="39"/>
+      <c r="D29" s="39"/>
+      <c r="E29" s="39"/>
+      <c r="F29" s="39"/>
+      <c r="G29" s="39"/>
+      <c r="H29" s="39"/>
+      <c r="I29" s="39"/>
+      <c r="J29" s="39"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="46" t="s">
+      <c r="A30" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="46"/>
-      <c r="C30" s="46"/>
-      <c r="D30" s="46"/>
-      <c r="E30" s="46"/>
-      <c r="F30" s="46"/>
-      <c r="G30" s="46"/>
-      <c r="H30" s="46"/>
-      <c r="I30" s="46"/>
-      <c r="J30" s="46"/>
+      <c r="B30" s="47"/>
+      <c r="C30" s="47"/>
+      <c r="D30" s="47"/>
+      <c r="E30" s="47"/>
+      <c r="F30" s="47"/>
+      <c r="G30" s="47"/>
+      <c r="H30" s="47"/>
+      <c r="I30" s="47"/>
+      <c r="J30" s="47"/>
     </row>
     <row r="31" spans="1:10" ht="18.75">
-      <c r="A31" s="47" t="s">
+      <c r="A31" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="B31" s="47"/>
-      <c r="C31" s="47"/>
-      <c r="D31" s="47"/>
-      <c r="E31" s="47"/>
-      <c r="F31" s="47"/>
-      <c r="G31" s="47"/>
-      <c r="H31" s="47"/>
-      <c r="I31" s="47"/>
-      <c r="J31" s="47"/>
+      <c r="B31" s="40"/>
+      <c r="C31" s="40"/>
+      <c r="D31" s="40"/>
+      <c r="E31" s="40"/>
+      <c r="F31" s="40"/>
+      <c r="G31" s="40"/>
+      <c r="H31" s="40"/>
+      <c r="I31" s="40"/>
+      <c r="J31" s="40"/>
     </row>
     <row r="32" spans="1:10" ht="20.25">
       <c r="A32" s="6" t="s">
@@ -5901,10 +5901,10 @@
       <c r="D32" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="70" t="s">
+      <c r="E32" s="74" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="70"/>
+      <c r="F32" s="74"/>
       <c r="G32" s="20" t="s">
         <v>5</v>
       </c>
@@ -5919,10 +5919,10 @@
       <c r="D33" s="19">
         <v>1000</v>
       </c>
-      <c r="E33" s="43">
+      <c r="E33" s="41">
         <v>30</v>
       </c>
-      <c r="F33" s="43"/>
+      <c r="F33" s="41"/>
       <c r="G33" s="19">
         <f t="shared" ref="G33:G38" si="0">SUM(D33*E33)</f>
         <v>30000</v>
@@ -5938,10 +5938,10 @@
       <c r="D34" s="19">
         <v>500</v>
       </c>
-      <c r="E34" s="43">
+      <c r="E34" s="41">
         <v>35</v>
       </c>
-      <c r="F34" s="43"/>
+      <c r="F34" s="41"/>
       <c r="G34" s="19">
         <f t="shared" si="0"/>
         <v>17500</v>
@@ -5957,10 +5957,10 @@
       <c r="D35" s="19">
         <v>100</v>
       </c>
-      <c r="E35" s="43">
+      <c r="E35" s="41">
         <v>425</v>
       </c>
-      <c r="F35" s="43"/>
+      <c r="F35" s="41"/>
       <c r="G35" s="19">
         <f t="shared" si="0"/>
         <v>42500</v>
@@ -5976,8 +5976,8 @@
       <c r="D36" s="19">
         <v>50</v>
       </c>
-      <c r="E36" s="43"/>
-      <c r="F36" s="43"/>
+      <c r="E36" s="41"/>
+      <c r="F36" s="41"/>
       <c r="G36" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -5993,8 +5993,8 @@
       <c r="D37" s="19">
         <v>20</v>
       </c>
-      <c r="E37" s="74"/>
-      <c r="F37" s="74"/>
+      <c r="E37" s="73"/>
+      <c r="F37" s="73"/>
       <c r="G37" s="19">
         <f>SUM(D37*E37)</f>
         <v>0</v>
@@ -6010,10 +6010,10 @@
       <c r="D38" s="19">
         <v>10</v>
       </c>
-      <c r="E38" s="74">
+      <c r="E38" s="73">
         <v>100</v>
       </c>
-      <c r="F38" s="74"/>
+      <c r="F38" s="73"/>
       <c r="G38" s="19">
         <f t="shared" si="0"/>
         <v>1000</v>
@@ -6076,58 +6076,58 @@
       <c r="J42" s="6"/>
     </row>
     <row r="43" spans="1:10" ht="15.75">
-      <c r="A43" s="41" t="s">
+      <c r="A43" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="41"/>
+      <c r="B43" s="50"/>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
-      <c r="H43" s="41" t="s">
+      <c r="H43" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="41"/>
-      <c r="J43" s="41"/>
+      <c r="I43" s="50"/>
+      <c r="J43" s="50"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="42"/>
-      <c r="B44" s="42"/>
+      <c r="A44" s="43"/>
+      <c r="B44" s="43"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="42"/>
-      <c r="I44" s="42"/>
-      <c r="J44" s="42"/>
+      <c r="H44" s="43"/>
+      <c r="I44" s="43"/>
+      <c r="J44" s="43"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="42"/>
-      <c r="B45" s="42"/>
+      <c r="A45" s="43"/>
+      <c r="B45" s="43"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="42"/>
-      <c r="I45" s="42"/>
-      <c r="J45" s="42"/>
+      <c r="H45" s="43"/>
+      <c r="I45" s="43"/>
+      <c r="J45" s="43"/>
     </row>
     <row r="46" spans="1:10" ht="15.75">
-      <c r="A46" s="42"/>
-      <c r="B46" s="42"/>
+      <c r="A46" s="43"/>
+      <c r="B46" s="43"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="42" t="s">
+      <c r="H46" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="41"/>
-      <c r="J46" s="41"/>
+      <c r="I46" s="50"/>
+      <c r="J46" s="50"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -6137,12 +6137,38 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="37"/>
-      <c r="I47" s="38"/>
-      <c r="J47" s="38"/>
+      <c r="H47" s="45"/>
+      <c r="I47" s="46"/>
+      <c r="J47" s="46"/>
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="H47:J47"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="H43:J43"/>
+    <mergeCell ref="A44:B45"/>
+    <mergeCell ref="H44:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="A31:J31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -6155,32 +6181,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="A31:J31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="H47:J47"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="H43:J43"/>
-    <mergeCell ref="A44:B45"/>
-    <mergeCell ref="H44:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -6206,177 +6206,177 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="44"/>
-      <c r="J1" s="44"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="45"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="45"/>
-      <c r="H2" s="45"/>
-      <c r="I2" s="45"/>
-      <c r="J2" s="45"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="39"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="88">
+      <c r="A5" s="87">
         <v>1</v>
       </c>
-      <c r="B5" s="81" t="s">
+      <c r="B5" s="79" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="81"/>
-      <c r="D5" s="81"/>
-      <c r="E5" s="81"/>
-      <c r="F5" s="81"/>
-      <c r="G5" s="79">
+      <c r="C5" s="79"/>
+      <c r="D5" s="79"/>
+      <c r="E5" s="79"/>
+      <c r="F5" s="79"/>
+      <c r="G5" s="86">
         <v>1650</v>
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="88"/>
-      <c r="B6" s="81"/>
-      <c r="C6" s="81"/>
-      <c r="D6" s="81"/>
-      <c r="E6" s="81"/>
-      <c r="F6" s="81"/>
-      <c r="G6" s="79"/>
+      <c r="A6" s="87"/>
+      <c r="B6" s="79"/>
+      <c r="C6" s="79"/>
+      <c r="D6" s="79"/>
+      <c r="E6" s="79"/>
+      <c r="F6" s="79"/>
+      <c r="G6" s="86"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="88">
+      <c r="A7" s="87">
         <v>2</v>
       </c>
-      <c r="B7" s="81" t="s">
+      <c r="B7" s="79" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="81"/>
-      <c r="D7" s="81"/>
-      <c r="E7" s="81"/>
-      <c r="F7" s="81"/>
-      <c r="G7" s="79">
+      <c r="C7" s="79"/>
+      <c r="D7" s="79"/>
+      <c r="E7" s="79"/>
+      <c r="F7" s="79"/>
+      <c r="G7" s="86">
         <v>1980</v>
       </c>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="88"/>
-      <c r="B8" s="81"/>
-      <c r="C8" s="81"/>
-      <c r="D8" s="81"/>
-      <c r="E8" s="81"/>
-      <c r="F8" s="81"/>
-      <c r="G8" s="79"/>
+      <c r="A8" s="87"/>
+      <c r="B8" s="79"/>
+      <c r="C8" s="79"/>
+      <c r="D8" s="79"/>
+      <c r="E8" s="79"/>
+      <c r="F8" s="79"/>
+      <c r="G8" s="86"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="88">
+      <c r="A9" s="87">
         <v>3</v>
       </c>
-      <c r="B9" s="81" t="s">
+      <c r="B9" s="79" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="81"/>
-      <c r="D9" s="81"/>
-      <c r="E9" s="81"/>
-      <c r="F9" s="81"/>
-      <c r="G9" s="79">
+      <c r="C9" s="79"/>
+      <c r="D9" s="79"/>
+      <c r="E9" s="79"/>
+      <c r="F9" s="79"/>
+      <c r="G9" s="86">
         <v>10538</v>
       </c>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="88"/>
-      <c r="B10" s="81"/>
-      <c r="C10" s="81"/>
-      <c r="D10" s="81"/>
-      <c r="E10" s="81"/>
-      <c r="F10" s="81"/>
-      <c r="G10" s="79"/>
+      <c r="A10" s="87"/>
+      <c r="B10" s="79"/>
+      <c r="C10" s="79"/>
+      <c r="D10" s="79"/>
+      <c r="E10" s="79"/>
+      <c r="F10" s="79"/>
+      <c r="G10" s="86"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="88">
+      <c r="A11" s="87">
         <v>4</v>
       </c>
-      <c r="B11" s="82" t="s">
+      <c r="B11" s="80" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="83"/>
-      <c r="D11" s="83"/>
-      <c r="E11" s="83"/>
-      <c r="F11" s="84"/>
-      <c r="G11" s="79">
+      <c r="C11" s="81"/>
+      <c r="D11" s="81"/>
+      <c r="E11" s="81"/>
+      <c r="F11" s="82"/>
+      <c r="G11" s="86">
         <v>1100</v>
       </c>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="88"/>
-      <c r="B12" s="85"/>
-      <c r="C12" s="86"/>
-      <c r="D12" s="86"/>
-      <c r="E12" s="86"/>
-      <c r="F12" s="87"/>
-      <c r="G12" s="79"/>
+      <c r="A12" s="87"/>
+      <c r="B12" s="83"/>
+      <c r="C12" s="84"/>
+      <c r="D12" s="84"/>
+      <c r="E12" s="84"/>
+      <c r="F12" s="85"/>
+      <c r="G12" s="86"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="80" t="s">
+      <c r="A13" s="88" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="80"/>
-      <c r="C13" s="80"/>
-      <c r="D13" s="80"/>
-      <c r="E13" s="80"/>
-      <c r="F13" s="80"/>
-      <c r="G13" s="79">
+      <c r="B13" s="88"/>
+      <c r="C13" s="88"/>
+      <c r="D13" s="88"/>
+      <c r="E13" s="88"/>
+      <c r="F13" s="88"/>
+      <c r="G13" s="86">
         <f>SUM(G5:G12)</f>
         <v>15268</v>
       </c>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="80"/>
-      <c r="B14" s="80"/>
-      <c r="C14" s="80"/>
-      <c r="D14" s="80"/>
-      <c r="E14" s="80"/>
-      <c r="F14" s="80"/>
-      <c r="G14" s="79"/>
+      <c r="A14" s="88"/>
+      <c r="B14" s="88"/>
+      <c r="C14" s="88"/>
+      <c r="D14" s="88"/>
+      <c r="E14" s="88"/>
+      <c r="F14" s="88"/>
+      <c r="G14" s="86"/>
     </row>
     <row r="23" spans="1:10" ht="18.75">
-      <c r="A23" s="46" t="s">
+      <c r="A23" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="46"/>
-      <c r="C23" s="46"/>
-      <c r="D23" s="46"/>
-      <c r="E23" s="46"/>
-      <c r="F23" s="46"/>
-      <c r="G23" s="46"/>
-      <c r="H23" s="46"/>
-      <c r="I23" s="46"/>
-      <c r="J23" s="46"/>
+      <c r="B23" s="47"/>
+      <c r="C23" s="47"/>
+      <c r="D23" s="47"/>
+      <c r="E23" s="47"/>
+      <c r="F23" s="47"/>
+      <c r="G23" s="47"/>
+      <c r="H23" s="47"/>
+      <c r="I23" s="47"/>
+      <c r="J23" s="47"/>
     </row>
     <row r="24" spans="1:10" ht="18.75">
-      <c r="A24" s="47"/>
-      <c r="B24" s="47"/>
-      <c r="C24" s="47"/>
-      <c r="D24" s="47"/>
-      <c r="E24" s="47"/>
-      <c r="F24" s="47"/>
-      <c r="G24" s="47"/>
-      <c r="H24" s="47"/>
-      <c r="I24" s="47"/>
-      <c r="J24" s="47"/>
+      <c r="A24" s="40"/>
+      <c r="B24" s="40"/>
+      <c r="C24" s="40"/>
+      <c r="D24" s="40"/>
+      <c r="E24" s="40"/>
+      <c r="F24" s="40"/>
+      <c r="G24" s="40"/>
+      <c r="H24" s="40"/>
+      <c r="I24" s="40"/>
+      <c r="J24" s="40"/>
     </row>
     <row r="25" spans="1:10" ht="20.25">
       <c r="A25" s="6" t="s">
@@ -6387,10 +6387,10 @@
       <c r="D25" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E25" s="70" t="s">
+      <c r="E25" s="74" t="s">
         <v>4</v>
       </c>
-      <c r="F25" s="70"/>
+      <c r="F25" s="74"/>
       <c r="G25" s="20" t="s">
         <v>5</v>
       </c>
@@ -6405,8 +6405,8 @@
       <c r="D26" s="19">
         <v>1000</v>
       </c>
-      <c r="E26" s="43"/>
-      <c r="F26" s="43"/>
+      <c r="E26" s="41"/>
+      <c r="F26" s="41"/>
       <c r="G26" s="19">
         <f t="shared" ref="G26:G31" si="0">SUM(D26*E26)</f>
         <v>0</v>
@@ -6422,10 +6422,10 @@
       <c r="D27" s="19">
         <v>500</v>
       </c>
-      <c r="E27" s="43">
+      <c r="E27" s="41">
         <v>30</v>
       </c>
-      <c r="F27" s="43"/>
+      <c r="F27" s="41"/>
       <c r="G27" s="19">
         <f t="shared" si="0"/>
         <v>15000</v>
@@ -6441,8 +6441,8 @@
       <c r="D28" s="19">
         <v>100</v>
       </c>
-      <c r="E28" s="43"/>
-      <c r="F28" s="43"/>
+      <c r="E28" s="41"/>
+      <c r="F28" s="41"/>
       <c r="G28" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -6458,10 +6458,10 @@
       <c r="D29" s="19">
         <v>50</v>
       </c>
-      <c r="E29" s="43">
+      <c r="E29" s="41">
         <v>5</v>
       </c>
-      <c r="F29" s="43"/>
+      <c r="F29" s="41"/>
       <c r="G29" s="19">
         <f t="shared" si="0"/>
         <v>250</v>
@@ -6477,8 +6477,8 @@
       <c r="D30" s="19">
         <v>20</v>
       </c>
-      <c r="E30" s="74"/>
-      <c r="F30" s="74"/>
+      <c r="E30" s="73"/>
+      <c r="F30" s="73"/>
       <c r="G30" s="19">
         <f>SUM(D30*E30)</f>
         <v>0</v>
@@ -6494,10 +6494,10 @@
       <c r="D31" s="19">
         <v>10</v>
       </c>
-      <c r="E31" s="74">
+      <c r="E31" s="73">
         <v>2</v>
       </c>
-      <c r="F31" s="74"/>
+      <c r="F31" s="73"/>
       <c r="G31" s="19">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -6560,58 +6560,58 @@
       <c r="J35" s="6"/>
     </row>
     <row r="36" spans="1:10" ht="15.75">
-      <c r="A36" s="41" t="s">
+      <c r="A36" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="41"/>
+      <c r="B36" s="50"/>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
       <c r="G36" s="7"/>
-      <c r="H36" s="41" t="s">
+      <c r="H36" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="I36" s="41"/>
-      <c r="J36" s="41"/>
+      <c r="I36" s="50"/>
+      <c r="J36" s="50"/>
     </row>
     <row r="37" spans="1:10">
-      <c r="A37" s="42"/>
-      <c r="B37" s="42"/>
+      <c r="A37" s="43"/>
+      <c r="B37" s="43"/>
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
       <c r="G37" s="6"/>
-      <c r="H37" s="42"/>
-      <c r="I37" s="42"/>
-      <c r="J37" s="42"/>
+      <c r="H37" s="43"/>
+      <c r="I37" s="43"/>
+      <c r="J37" s="43"/>
     </row>
     <row r="38" spans="1:10">
-      <c r="A38" s="42"/>
-      <c r="B38" s="42"/>
+      <c r="A38" s="43"/>
+      <c r="B38" s="43"/>
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
-      <c r="H38" s="42"/>
-      <c r="I38" s="42"/>
-      <c r="J38" s="42"/>
+      <c r="H38" s="43"/>
+      <c r="I38" s="43"/>
+      <c r="J38" s="43"/>
     </row>
     <row r="39" spans="1:10" ht="15.75">
-      <c r="A39" s="42"/>
-      <c r="B39" s="42"/>
+      <c r="A39" s="43"/>
+      <c r="B39" s="43"/>
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
       <c r="F39" s="6"/>
       <c r="G39" s="6"/>
-      <c r="H39" s="42" t="s">
+      <c r="H39" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="I39" s="41"/>
-      <c r="J39" s="41"/>
+      <c r="I39" s="50"/>
+      <c r="J39" s="50"/>
     </row>
     <row r="40" spans="1:10">
       <c r="A40" s="6"/>
@@ -6621,12 +6621,29 @@
       <c r="E40" s="6"/>
       <c r="F40" s="6"/>
       <c r="G40" s="6"/>
-      <c r="H40" s="37"/>
-      <c r="I40" s="38"/>
-      <c r="J40" s="38"/>
+      <c r="H40" s="45"/>
+      <c r="I40" s="46"/>
+      <c r="J40" s="46"/>
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="H40:J40"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="H36:J36"/>
+    <mergeCell ref="A37:B38"/>
+    <mergeCell ref="H37:J38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="H39:J39"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="A13:F14"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="E30:F30"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="A23:J23"/>
@@ -6643,23 +6660,6 @@
     <mergeCell ref="B5:F6"/>
     <mergeCell ref="G5:G6"/>
     <mergeCell ref="B7:F8"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="A13:F14"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="H40:J40"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="H36:J36"/>
-    <mergeCell ref="A37:B38"/>
-    <mergeCell ref="H37:J38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="H39:J39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="71" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
06.08.2020 MC Sales Details
</commit_message>
<xml_diff>
--- a/2020/Others/Cash A.xlsx
+++ b/2020/Others/Cash A.xlsx
@@ -122,7 +122,7 @@
     <t>Komola Super Market, Alaipur, Natore</t>
   </si>
   <si>
-    <t>Tanjib</t>
+    <t>Jafor Iqbal</t>
   </si>
 </sst>
 </file>
@@ -515,47 +515,71 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -576,21 +600,9 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -600,17 +612,8 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -624,15 +627,12 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -640,6 +640,12 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -661,12 +667,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -706,7 +706,7 @@
         <xdr:cNvPr id="2" name="Straight Connector 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -756,7 +756,7 @@
         <xdr:cNvPr id="3" name="Straight Connector 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -806,7 +806,7 @@
         <xdr:cNvPr id="4" name="Straight Connector 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -856,7 +856,7 @@
         <xdr:cNvPr id="5" name="Straight Connector 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -911,7 +911,7 @@
         <xdr:cNvPr id="12" name="Straight Connector 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000C000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00000C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -961,7 +961,7 @@
         <xdr:cNvPr id="6" name="Straight Connector 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3F693EA6-49EB-42D1-B3CA-F15B26A03B41}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3F693EA6-49EB-42D1-B3CA-F15B26A03B41}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1011,7 +1011,7 @@
         <xdr:cNvPr id="8" name="Straight Connector 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{334CB43E-1331-4297-A64C-0895C28A3BBB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{334CB43E-1331-4297-A64C-0895C28A3BBB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1061,7 +1061,7 @@
         <xdr:cNvPr id="9" name="Straight Connector 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0D774EF-0DA8-4AF5-A477-477DFA29C2B2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A0D774EF-0DA8-4AF5-A477-477DFA29C2B2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1111,7 +1111,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0F2A810E-B364-491B-AB34-AE585B8D27E3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0F2A810E-B364-491B-AB34-AE585B8D27E3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1123,7 +1123,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1161,7 +1161,7 @@
         <xdr:cNvPr id="13" name="Picture 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BBEAD3A6-FB1B-45D2-BDBE-713A9FCBE3DE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{BBEAD3A6-FB1B-45D2-BDBE-713A9FCBE3DE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1173,7 +1173,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1216,7 +1216,7 @@
         <xdr:cNvPr id="2" name="Straight Connector 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1266,7 +1266,7 @@
         <xdr:cNvPr id="3" name="Straight Connector 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1316,7 +1316,7 @@
         <xdr:cNvPr id="4" name="Straight Connector 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1366,7 +1366,7 @@
         <xdr:cNvPr id="5" name="Straight Connector 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1416,7 +1416,7 @@
         <xdr:cNvPr id="6" name="Straight Connector 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000006000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1471,7 +1471,7 @@
         <xdr:cNvPr id="7" name="Straight Connector 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000007000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1521,7 +1521,7 @@
         <xdr:cNvPr id="8" name="Straight Connector 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000008000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1571,7 +1571,7 @@
         <xdr:cNvPr id="9" name="Straight Connector 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000009000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000009000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1621,7 +1621,7 @@
         <xdr:cNvPr id="10" name="Straight Connector 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000A000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-00000A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1671,7 +1671,7 @@
         <xdr:cNvPr id="11" name="Straight Connector 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000B000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-00000B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1721,7 +1721,7 @@
         <xdr:cNvPr id="12" name="Straight Connector 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000C000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-00000C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1771,7 +1771,7 @@
         <xdr:cNvPr id="13" name="Straight Connector 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000D000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-00000D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1826,7 +1826,7 @@
         <xdr:cNvPr id="2" name="Straight Connector 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1876,7 +1876,7 @@
         <xdr:cNvPr id="3" name="Straight Connector 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1926,7 +1926,7 @@
         <xdr:cNvPr id="4" name="Straight Connector 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1976,7 +1976,7 @@
         <xdr:cNvPr id="5" name="Straight Connector 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2031,7 +2031,7 @@
         <xdr:cNvPr id="4" name="Straight Connector 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2081,7 +2081,7 @@
         <xdr:cNvPr id="5" name="Straight Connector 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2371,7 +2371,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2393,60 +2393,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
-      <c r="J1" s="38"/>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="39"/>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="39"/>
+      <c r="B2" s="45"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="45"/>
+      <c r="I2" s="45"/>
+      <c r="J2" s="45"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="39"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
-      <c r="I3" s="39"/>
-      <c r="J3" s="39"/>
+      <c r="B3" s="45"/>
+      <c r="C3" s="45"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="45"/>
+      <c r="G3" s="45"/>
+      <c r="H3" s="45"/>
+      <c r="I3" s="45"/>
+      <c r="J3" s="45"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="47" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="40"/>
-      <c r="I4" s="40"/>
-      <c r="J4" s="40"/>
+      <c r="B4" s="47"/>
+      <c r="C4" s="47"/>
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="47"/>
+      <c r="G4" s="47"/>
+      <c r="H4" s="47"/>
+      <c r="I4" s="47"/>
+      <c r="J4" s="47"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
@@ -2455,10 +2455,10 @@
       <c r="D5" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="37" t="s">
+      <c r="E5" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="37"/>
+      <c r="F5" s="48"/>
       <c r="G5" s="14" t="s">
         <v>5</v>
       </c>
@@ -2473,10 +2473,10 @@
       <c r="D6" s="13">
         <v>1000</v>
       </c>
-      <c r="E6" s="41">
+      <c r="E6" s="43">
         <v>50</v>
       </c>
-      <c r="F6" s="41"/>
+      <c r="F6" s="43"/>
       <c r="G6" s="13">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>50000</v>
@@ -2492,10 +2492,10 @@
       <c r="D7" s="13">
         <v>500</v>
       </c>
-      <c r="E7" s="41">
+      <c r="E7" s="43">
         <v>16</v>
       </c>
-      <c r="F7" s="41"/>
+      <c r="F7" s="43"/>
       <c r="G7" s="13">
         <f t="shared" si="0"/>
         <v>8000</v>
@@ -2511,10 +2511,10 @@
       <c r="D8" s="13">
         <v>100</v>
       </c>
-      <c r="E8" s="41">
+      <c r="E8" s="43">
         <v>151</v>
       </c>
-      <c r="F8" s="41"/>
+      <c r="F8" s="43"/>
       <c r="G8" s="13">
         <f t="shared" si="0"/>
         <v>15100</v>
@@ -2530,10 +2530,10 @@
       <c r="D9" s="13">
         <v>50</v>
       </c>
-      <c r="E9" s="41">
+      <c r="E9" s="43">
         <v>58</v>
       </c>
-      <c r="F9" s="41"/>
+      <c r="F9" s="43"/>
       <c r="G9" s="13">
         <f t="shared" si="0"/>
         <v>2900</v>
@@ -2549,8 +2549,8 @@
       <c r="D10" s="13">
         <v>20</v>
       </c>
-      <c r="E10" s="41"/>
-      <c r="F10" s="41"/>
+      <c r="E10" s="43"/>
+      <c r="F10" s="43"/>
       <c r="G10" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2566,8 +2566,8 @@
       <c r="D11" s="13">
         <v>10</v>
       </c>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
+      <c r="E11" s="43"/>
+      <c r="F11" s="43"/>
       <c r="G11" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2580,10 +2580,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="37" t="s">
+      <c r="D12" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="37"/>
+      <c r="E12" s="48"/>
       <c r="F12" s="14"/>
       <c r="G12" s="14">
         <f>SUM(G6:G11)</f>
@@ -2630,58 +2630,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="42" t="s">
+      <c r="A16" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="42"/>
+      <c r="B16" s="49"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="42" t="s">
+      <c r="H16" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="42"/>
-      <c r="J16" s="42"/>
+      <c r="I16" s="49"/>
+      <c r="J16" s="49"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="42"/>
-      <c r="B17" s="42"/>
+      <c r="A17" s="49"/>
+      <c r="B17" s="49"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="42"/>
-      <c r="I17" s="42"/>
-      <c r="J17" s="42"/>
+      <c r="H17" s="49"/>
+      <c r="I17" s="49"/>
+      <c r="J17" s="49"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="42"/>
-      <c r="B18" s="42"/>
+      <c r="A18" s="49"/>
+      <c r="B18" s="49"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="42"/>
-      <c r="I18" s="42"/>
-      <c r="J18" s="42"/>
+      <c r="H18" s="49"/>
+      <c r="I18" s="49"/>
+      <c r="J18" s="49"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="43"/>
-      <c r="B19" s="43"/>
+      <c r="A19" s="42"/>
+      <c r="B19" s="42"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="44" t="s">
+      <c r="H19" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="44"/>
-      <c r="J19" s="44"/>
+      <c r="I19" s="50"/>
+      <c r="J19" s="50"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -2691,11 +2691,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="45" t="s">
+      <c r="H20" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="46"/>
-      <c r="J20" s="46"/>
+      <c r="I20" s="38"/>
+      <c r="J20" s="38"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -2770,60 +2770,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="38" t="s">
+      <c r="A27" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="38"/>
-      <c r="C27" s="38"/>
-      <c r="D27" s="38"/>
-      <c r="E27" s="38"/>
-      <c r="F27" s="38"/>
-      <c r="G27" s="38"/>
-      <c r="H27" s="38"/>
-      <c r="I27" s="38"/>
-      <c r="J27" s="38"/>
+      <c r="B27" s="44"/>
+      <c r="C27" s="44"/>
+      <c r="D27" s="44"/>
+      <c r="E27" s="44"/>
+      <c r="F27" s="44"/>
+      <c r="G27" s="44"/>
+      <c r="H27" s="44"/>
+      <c r="I27" s="44"/>
+      <c r="J27" s="44"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="39" t="s">
+      <c r="A28" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="39"/>
-      <c r="C28" s="39"/>
-      <c r="D28" s="39"/>
-      <c r="E28" s="39"/>
-      <c r="F28" s="39"/>
-      <c r="G28" s="39"/>
-      <c r="H28" s="39"/>
-      <c r="I28" s="39"/>
-      <c r="J28" s="39"/>
+      <c r="B28" s="45"/>
+      <c r="C28" s="45"/>
+      <c r="D28" s="45"/>
+      <c r="E28" s="45"/>
+      <c r="F28" s="45"/>
+      <c r="G28" s="45"/>
+      <c r="H28" s="45"/>
+      <c r="I28" s="45"/>
+      <c r="J28" s="45"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="47" t="s">
+      <c r="A29" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="47"/>
-      <c r="C29" s="47"/>
-      <c r="D29" s="47"/>
-      <c r="E29" s="47"/>
-      <c r="F29" s="47"/>
-      <c r="G29" s="47"/>
-      <c r="H29" s="47"/>
-      <c r="I29" s="47"/>
-      <c r="J29" s="47"/>
+      <c r="B29" s="46"/>
+      <c r="C29" s="46"/>
+      <c r="D29" s="46"/>
+      <c r="E29" s="46"/>
+      <c r="F29" s="46"/>
+      <c r="G29" s="46"/>
+      <c r="H29" s="46"/>
+      <c r="I29" s="46"/>
+      <c r="J29" s="46"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="40" t="s">
+      <c r="A30" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="40"/>
-      <c r="C30" s="40"/>
-      <c r="D30" s="40"/>
-      <c r="E30" s="40"/>
-      <c r="F30" s="40"/>
-      <c r="G30" s="40"/>
-      <c r="H30" s="40"/>
-      <c r="I30" s="40"/>
-      <c r="J30" s="40"/>
+      <c r="B30" s="47"/>
+      <c r="C30" s="47"/>
+      <c r="D30" s="47"/>
+      <c r="E30" s="47"/>
+      <c r="F30" s="47"/>
+      <c r="G30" s="47"/>
+      <c r="H30" s="47"/>
+      <c r="I30" s="47"/>
+      <c r="J30" s="47"/>
     </row>
     <row r="31" spans="1:10" ht="24.95" customHeight="1">
       <c r="A31" s="6"/>
@@ -2832,10 +2832,10 @@
       <c r="D31" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="37" t="s">
+      <c r="E31" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="37"/>
+      <c r="F31" s="48"/>
       <c r="G31" s="15" t="s">
         <v>5</v>
       </c>
@@ -2850,10 +2850,10 @@
       <c r="D32" s="16">
         <v>1000</v>
       </c>
-      <c r="E32" s="41">
+      <c r="E32" s="43">
         <v>50</v>
       </c>
-      <c r="F32" s="41"/>
+      <c r="F32" s="43"/>
       <c r="G32" s="16">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>50000</v>
@@ -2869,10 +2869,10 @@
       <c r="D33" s="16">
         <v>500</v>
       </c>
-      <c r="E33" s="41">
+      <c r="E33" s="43">
         <v>116</v>
       </c>
-      <c r="F33" s="41"/>
+      <c r="F33" s="43"/>
       <c r="G33" s="16">
         <f t="shared" si="1"/>
         <v>58000</v>
@@ -2888,10 +2888,10 @@
       <c r="D34" s="16">
         <v>100</v>
       </c>
-      <c r="E34" s="41">
+      <c r="E34" s="43">
         <v>151</v>
       </c>
-      <c r="F34" s="41"/>
+      <c r="F34" s="43"/>
       <c r="G34" s="16">
         <f t="shared" si="1"/>
         <v>15100</v>
@@ -2907,10 +2907,10 @@
       <c r="D35" s="16">
         <v>50</v>
       </c>
-      <c r="E35" s="41">
+      <c r="E35" s="43">
         <v>58</v>
       </c>
-      <c r="F35" s="41"/>
+      <c r="F35" s="43"/>
       <c r="G35" s="16">
         <f t="shared" si="1"/>
         <v>2900</v>
@@ -2926,8 +2926,8 @@
       <c r="D36" s="16">
         <v>20</v>
       </c>
-      <c r="E36" s="41"/>
-      <c r="F36" s="41"/>
+      <c r="E36" s="43"/>
+      <c r="F36" s="43"/>
       <c r="G36" s="16">
         <f>SUM(D36*E36)</f>
         <v>0</v>
@@ -2943,8 +2943,8 @@
       <c r="D37" s="16">
         <v>10</v>
       </c>
-      <c r="E37" s="41"/>
-      <c r="F37" s="41"/>
+      <c r="E37" s="43"/>
+      <c r="F37" s="43"/>
       <c r="G37" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2957,10 +2957,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="48" t="s">
+      <c r="D38" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="49"/>
+      <c r="E38" s="40"/>
       <c r="F38" s="15"/>
       <c r="G38" s="15">
         <f>SUM(G32:G37)</f>
@@ -3007,58 +3007,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" ht="15.75">
-      <c r="A42" s="50" t="s">
+      <c r="A42" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="50"/>
+      <c r="B42" s="41"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="50" t="s">
+      <c r="H42" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="50"/>
-      <c r="J42" s="50"/>
+      <c r="I42" s="41"/>
+      <c r="J42" s="41"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="43"/>
-      <c r="B43" s="43"/>
+      <c r="A43" s="42"/>
+      <c r="B43" s="42"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="43"/>
-      <c r="I43" s="43"/>
-      <c r="J43" s="43"/>
+      <c r="H43" s="42"/>
+      <c r="I43" s="42"/>
+      <c r="J43" s="42"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="43"/>
-      <c r="B44" s="43"/>
+      <c r="A44" s="42"/>
+      <c r="B44" s="42"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="43"/>
-      <c r="I44" s="43"/>
-      <c r="J44" s="43"/>
+      <c r="H44" s="42"/>
+      <c r="I44" s="42"/>
+      <c r="J44" s="42"/>
     </row>
     <row r="45" spans="1:10" ht="15.75">
-      <c r="A45" s="43"/>
-      <c r="B45" s="43"/>
+      <c r="A45" s="42"/>
+      <c r="B45" s="42"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="43" t="s">
+      <c r="H45" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="50"/>
-      <c r="J45" s="50"/>
+      <c r="I45" s="41"/>
+      <c r="J45" s="41"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="6"/>
@@ -3068,11 +3068,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="45" t="s">
+      <c r="H46" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="46"/>
-      <c r="J46" s="46"/>
+      <c r="I46" s="38"/>
+      <c r="J46" s="38"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -3100,14 +3100,24 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="E37:F37"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A27:J27"/>
@@ -3120,24 +3130,14 @@
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.25" footer="0"/>
   <pageSetup scale="85" orientation="portrait" r:id="rId1"/>
@@ -3149,8 +3149,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M39" sqref="M39:N39"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="N64" sqref="N64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3169,64 +3169,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="51" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
-      <c r="F1" s="58"/>
-      <c r="G1" s="58"/>
-      <c r="H1" s="58"/>
-      <c r="I1" s="58"/>
-      <c r="J1" s="58"/>
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
+      <c r="G1" s="51"/>
+      <c r="H1" s="51"/>
+      <c r="I1" s="51"/>
+      <c r="J1" s="51"/>
       <c r="K1" s="24"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="59" t="s">
+      <c r="A2" s="52" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="59"/>
-      <c r="C2" s="59"/>
-      <c r="D2" s="59"/>
-      <c r="E2" s="59"/>
-      <c r="F2" s="59"/>
-      <c r="G2" s="59"/>
-      <c r="H2" s="59"/>
-      <c r="I2" s="59"/>
-      <c r="J2" s="59"/>
+      <c r="B2" s="52"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="52"/>
+      <c r="I2" s="52"/>
+      <c r="J2" s="52"/>
       <c r="K2" s="24"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="59" t="s">
+      <c r="A3" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="59"/>
-      <c r="C3" s="59"/>
-      <c r="D3" s="59"/>
-      <c r="E3" s="59"/>
-      <c r="F3" s="59"/>
-      <c r="G3" s="59"/>
-      <c r="H3" s="59"/>
-      <c r="I3" s="59"/>
-      <c r="J3" s="59"/>
+      <c r="B3" s="52"/>
+      <c r="C3" s="52"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="52"/>
+      <c r="F3" s="52"/>
+      <c r="G3" s="52"/>
+      <c r="H3" s="52"/>
+      <c r="I3" s="52"/>
+      <c r="J3" s="52"/>
       <c r="K3" s="24"/>
     </row>
     <row r="4" spans="1:11" ht="26.25">
-      <c r="A4" s="66">
+      <c r="A4" s="55">
         <f ca="1">TODAY()</f>
-        <v>44035</v>
-      </c>
-      <c r="B4" s="66"/>
-      <c r="C4" s="66"/>
-      <c r="D4" s="66"/>
-      <c r="E4" s="66"/>
-      <c r="F4" s="66"/>
-      <c r="G4" s="66"/>
-      <c r="H4" s="66"/>
-      <c r="I4" s="66"/>
-      <c r="J4" s="66"/>
+        <v>44049</v>
+      </c>
+      <c r="B4" s="55"/>
+      <c r="C4" s="55"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="55"/>
+      <c r="F4" s="55"/>
+      <c r="G4" s="55"/>
+      <c r="H4" s="55"/>
+      <c r="I4" s="55"/>
+      <c r="J4" s="55"/>
       <c r="K4" s="24"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -3236,10 +3236,10 @@
       <c r="D5" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="61" t="s">
+      <c r="E5" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="61"/>
+      <c r="F5" s="53"/>
       <c r="G5" s="26" t="s">
         <v>5</v>
       </c>
@@ -3254,13 +3254,13 @@
       <c r="D6" s="27">
         <v>1000</v>
       </c>
-      <c r="E6" s="62">
-        <v>450</v>
-      </c>
-      <c r="F6" s="62"/>
+      <c r="E6" s="54">
+        <v>238</v>
+      </c>
+      <c r="F6" s="54"/>
       <c r="G6" s="27">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
-        <v>450000</v>
+        <v>238000</v>
       </c>
       <c r="H6" s="25"/>
       <c r="I6" s="25"/>
@@ -3273,13 +3273,13 @@
       <c r="D7" s="27">
         <v>500</v>
       </c>
-      <c r="E7" s="62">
-        <v>600</v>
-      </c>
-      <c r="F7" s="62"/>
+      <c r="E7" s="54">
+        <v>504</v>
+      </c>
+      <c r="F7" s="54"/>
       <c r="G7" s="27">
         <f t="shared" si="0"/>
-        <v>300000</v>
+        <v>252000</v>
       </c>
       <c r="H7" s="25"/>
       <c r="I7" s="25"/>
@@ -3292,13 +3292,13 @@
       <c r="D8" s="27">
         <v>100</v>
       </c>
-      <c r="E8" s="62">
-        <v>500</v>
-      </c>
-      <c r="F8" s="62"/>
+      <c r="E8" s="54">
+        <v>1100</v>
+      </c>
+      <c r="F8" s="54"/>
       <c r="G8" s="27">
         <f t="shared" si="0"/>
-        <v>50000</v>
+        <v>110000</v>
       </c>
       <c r="H8" s="25"/>
       <c r="I8" s="25"/>
@@ -3311,8 +3311,8 @@
       <c r="D9" s="27">
         <v>50</v>
       </c>
-      <c r="E9" s="62"/>
-      <c r="F9" s="62"/>
+      <c r="E9" s="54"/>
+      <c r="F9" s="54"/>
       <c r="G9" s="27">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3328,8 +3328,8 @@
       <c r="D10" s="27">
         <v>20</v>
       </c>
-      <c r="E10" s="62"/>
-      <c r="F10" s="62"/>
+      <c r="E10" s="54"/>
+      <c r="F10" s="54"/>
       <c r="G10" s="27">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3345,8 +3345,8 @@
       <c r="D11" s="27">
         <v>10</v>
       </c>
-      <c r="E11" s="62"/>
-      <c r="F11" s="62"/>
+      <c r="E11" s="54"/>
+      <c r="F11" s="54"/>
       <c r="G11" s="27">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3359,14 +3359,14 @@
       <c r="A12" s="25"/>
       <c r="B12" s="25"/>
       <c r="C12" s="25"/>
-      <c r="D12" s="62" t="s">
+      <c r="D12" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="62"/>
+      <c r="E12" s="54"/>
       <c r="F12" s="27"/>
       <c r="G12" s="22">
         <f>SUM(G6:G11)</f>
-        <v>800000</v>
+        <v>600000</v>
       </c>
       <c r="H12" s="25"/>
       <c r="I12" s="25"/>
@@ -3410,59 +3410,59 @@
     </row>
     <row r="16" spans="1:11">
       <c r="A16" s="28"/>
-      <c r="B16" s="69" t="s">
+      <c r="B16" s="57" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="69"/>
-      <c r="D16" s="69"/>
+      <c r="C16" s="57"/>
+      <c r="D16" s="57"/>
       <c r="E16" s="28"/>
       <c r="F16" s="29"/>
       <c r="G16" s="29"/>
-      <c r="H16" s="68" t="s">
+      <c r="H16" s="56" t="s">
         <v>7</v>
       </c>
-      <c r="I16" s="68"/>
-      <c r="J16" s="68"/>
+      <c r="I16" s="56"/>
+      <c r="J16" s="56"/>
     </row>
     <row r="17" spans="1:11">
-      <c r="A17" s="68"/>
-      <c r="B17" s="68"/>
-      <c r="C17" s="68"/>
-      <c r="D17" s="68"/>
+      <c r="A17" s="56"/>
+      <c r="B17" s="56"/>
+      <c r="C17" s="56"/>
+      <c r="D17" s="56"/>
       <c r="E17" s="29"/>
       <c r="F17" s="29"/>
       <c r="G17" s="29"/>
-      <c r="H17" s="68"/>
-      <c r="I17" s="68"/>
-      <c r="J17" s="68"/>
+      <c r="H17" s="56"/>
+      <c r="I17" s="56"/>
+      <c r="J17" s="56"/>
     </row>
     <row r="18" spans="1:11">
-      <c r="A18" s="68"/>
-      <c r="B18" s="68"/>
-      <c r="C18" s="68"/>
-      <c r="D18" s="68"/>
+      <c r="A18" s="56"/>
+      <c r="B18" s="56"/>
+      <c r="C18" s="56"/>
+      <c r="D18" s="56"/>
       <c r="E18" s="29"/>
       <c r="F18" s="29"/>
       <c r="G18" s="29"/>
-      <c r="H18" s="68"/>
-      <c r="I18" s="68"/>
-      <c r="J18" s="68"/>
+      <c r="H18" s="56"/>
+      <c r="I18" s="56"/>
+      <c r="J18" s="56"/>
     </row>
     <row r="19" spans="1:11" ht="17.25" customHeight="1">
       <c r="A19" s="33"/>
-      <c r="B19" s="67" t="s">
+      <c r="B19" s="58" t="s">
         <v>28</v>
       </c>
-      <c r="C19" s="67"/>
-      <c r="D19" s="67"/>
+      <c r="C19" s="58"/>
+      <c r="D19" s="58"/>
       <c r="E19" s="29"/>
       <c r="F19" s="29"/>
       <c r="G19" s="29"/>
-      <c r="H19" s="42" t="s">
+      <c r="H19" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="I19" s="42"/>
-      <c r="J19" s="42"/>
+      <c r="I19" s="49"/>
+      <c r="J19" s="49"/>
     </row>
     <row r="20" spans="1:11">
       <c r="A20" s="25"/>
@@ -3472,9 +3472,9 @@
       <c r="E20" s="25"/>
       <c r="F20" s="25"/>
       <c r="G20" s="25"/>
-      <c r="H20" s="53"/>
-      <c r="I20" s="54"/>
-      <c r="J20" s="54"/>
+      <c r="H20" s="61"/>
+      <c r="I20" s="62"/>
+      <c r="J20" s="62"/>
     </row>
     <row r="21" spans="1:11">
       <c r="A21" s="25"/>
@@ -3561,66 +3561,66 @@
       <c r="J27" s="25"/>
     </row>
     <row r="28" spans="1:11" ht="31.5">
-      <c r="A28" s="58" t="s">
+      <c r="A28" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="B28" s="58"/>
-      <c r="C28" s="58"/>
-      <c r="D28" s="58"/>
-      <c r="E28" s="58"/>
-      <c r="F28" s="58"/>
-      <c r="G28" s="58"/>
-      <c r="H28" s="58"/>
-      <c r="I28" s="58"/>
-      <c r="J28" s="58"/>
+      <c r="B28" s="51"/>
+      <c r="C28" s="51"/>
+      <c r="D28" s="51"/>
+      <c r="E28" s="51"/>
+      <c r="F28" s="51"/>
+      <c r="G28" s="51"/>
+      <c r="H28" s="51"/>
+      <c r="I28" s="51"/>
+      <c r="J28" s="51"/>
     </row>
     <row r="29" spans="1:11" ht="18">
-      <c r="A29" s="59" t="str">
+      <c r="A29" s="52" t="str">
         <f>A2</f>
         <v>Komola Super Market, Alaipur, Natore</v>
       </c>
-      <c r="B29" s="59"/>
-      <c r="C29" s="59"/>
-      <c r="D29" s="59"/>
-      <c r="E29" s="59"/>
-      <c r="F29" s="59"/>
-      <c r="G29" s="59"/>
-      <c r="H29" s="59"/>
-      <c r="I29" s="59"/>
-      <c r="J29" s="59"/>
+      <c r="B29" s="52"/>
+      <c r="C29" s="52"/>
+      <c r="D29" s="52"/>
+      <c r="E29" s="52"/>
+      <c r="F29" s="52"/>
+      <c r="G29" s="52"/>
+      <c r="H29" s="52"/>
+      <c r="I29" s="52"/>
+      <c r="J29" s="52"/>
     </row>
     <row r="30" spans="1:11" ht="18.75">
-      <c r="A30" s="60" t="str">
+      <c r="A30" s="66" t="str">
         <f>A3</f>
         <v>Cash Details As Per Below</v>
       </c>
-      <c r="B30" s="60"/>
-      <c r="C30" s="60"/>
-      <c r="D30" s="60"/>
-      <c r="E30" s="60"/>
-      <c r="F30" s="60"/>
-      <c r="G30" s="60"/>
-      <c r="H30" s="60"/>
-      <c r="I30" s="60"/>
-      <c r="J30" s="60"/>
+      <c r="B30" s="66"/>
+      <c r="C30" s="66"/>
+      <c r="D30" s="66"/>
+      <c r="E30" s="66"/>
+      <c r="F30" s="66"/>
+      <c r="G30" s="66"/>
+      <c r="H30" s="66"/>
+      <c r="I30" s="66"/>
+      <c r="J30" s="66"/>
       <c r="K30" s="6" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="26.25">
-      <c r="A31" s="66">
+      <c r="A31" s="55">
         <f ca="1">TODAY()</f>
-        <v>44035</v>
-      </c>
-      <c r="B31" s="66"/>
-      <c r="C31" s="66"/>
-      <c r="D31" s="66"/>
-      <c r="E31" s="66"/>
-      <c r="F31" s="66"/>
-      <c r="G31" s="66"/>
-      <c r="H31" s="66"/>
-      <c r="I31" s="66"/>
-      <c r="J31" s="66"/>
+        <v>44049</v>
+      </c>
+      <c r="B31" s="55"/>
+      <c r="C31" s="55"/>
+      <c r="D31" s="55"/>
+      <c r="E31" s="55"/>
+      <c r="F31" s="55"/>
+      <c r="G31" s="55"/>
+      <c r="H31" s="55"/>
+      <c r="I31" s="55"/>
+      <c r="J31" s="55"/>
     </row>
     <row r="32" spans="1:11" ht="27.95" customHeight="1">
       <c r="A32" s="25"/>
@@ -3629,10 +3629,10 @@
       <c r="D32" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="61" t="s">
+      <c r="E32" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="61"/>
+      <c r="F32" s="53"/>
       <c r="G32" s="26" t="s">
         <v>5</v>
       </c>
@@ -3647,14 +3647,14 @@
       <c r="D33" s="30">
         <v>1000</v>
       </c>
-      <c r="E33" s="62">
+      <c r="E33" s="54">
         <f>E6</f>
-        <v>450</v>
-      </c>
-      <c r="F33" s="62"/>
+        <v>238</v>
+      </c>
+      <c r="F33" s="54"/>
       <c r="G33" s="30">
         <f t="shared" ref="G33:G38" si="1">SUM(D33*E33)</f>
-        <v>450000</v>
+        <v>238000</v>
       </c>
       <c r="H33" s="25"/>
       <c r="I33" s="25"/>
@@ -3667,14 +3667,14 @@
       <c r="D34" s="30">
         <v>500</v>
       </c>
-      <c r="E34" s="62">
+      <c r="E34" s="54">
         <f>E7</f>
-        <v>600</v>
-      </c>
-      <c r="F34" s="62"/>
+        <v>504</v>
+      </c>
+      <c r="F34" s="54"/>
       <c r="G34" s="30">
         <f t="shared" si="1"/>
-        <v>300000</v>
+        <v>252000</v>
       </c>
       <c r="H34" s="25"/>
       <c r="I34" s="25"/>
@@ -3687,14 +3687,14 @@
       <c r="D35" s="30">
         <v>100</v>
       </c>
-      <c r="E35" s="62">
+      <c r="E35" s="54">
         <f>E8</f>
-        <v>500</v>
-      </c>
-      <c r="F35" s="62"/>
+        <v>1100</v>
+      </c>
+      <c r="F35" s="54"/>
       <c r="G35" s="30">
         <f t="shared" si="1"/>
-        <v>50000</v>
+        <v>110000</v>
       </c>
       <c r="H35" s="25"/>
       <c r="I35" s="25"/>
@@ -3707,8 +3707,8 @@
       <c r="D36" s="30">
         <v>50</v>
       </c>
-      <c r="E36" s="62"/>
-      <c r="F36" s="62"/>
+      <c r="E36" s="54"/>
+      <c r="F36" s="54"/>
       <c r="G36" s="30">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -3724,8 +3724,8 @@
       <c r="D37" s="30">
         <v>20</v>
       </c>
-      <c r="E37" s="62"/>
-      <c r="F37" s="62"/>
+      <c r="E37" s="54"/>
+      <c r="F37" s="54"/>
       <c r="G37" s="30">
         <f>SUM(D37*E37)</f>
         <v>0</v>
@@ -3741,8 +3741,8 @@
       <c r="D38" s="30">
         <v>10</v>
       </c>
-      <c r="E38" s="62"/>
-      <c r="F38" s="62"/>
+      <c r="E38" s="54"/>
+      <c r="F38" s="54"/>
       <c r="G38" s="30">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -3755,14 +3755,14 @@
       <c r="A39" s="25"/>
       <c r="B39" s="25"/>
       <c r="C39" s="25"/>
-      <c r="D39" s="63" t="s">
+      <c r="D39" s="67" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="64"/>
+      <c r="E39" s="68"/>
       <c r="F39" s="30"/>
       <c r="G39" s="23">
         <f>SUM(G33:G38)</f>
-        <v>800000</v>
+        <v>600000</v>
       </c>
       <c r="H39" s="25"/>
       <c r="I39" s="25"/>
@@ -3814,53 +3814,53 @@
       <c r="E43" s="29"/>
       <c r="F43" s="29"/>
       <c r="G43" s="29"/>
-      <c r="H43" s="55" t="s">
+      <c r="H43" s="63" t="s">
         <v>7</v>
       </c>
-      <c r="I43" s="55"/>
-      <c r="J43" s="55"/>
+      <c r="I43" s="63"/>
+      <c r="J43" s="63"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="56"/>
-      <c r="B44" s="56"/>
-      <c r="C44" s="56"/>
-      <c r="D44" s="56"/>
+      <c r="A44" s="64"/>
+      <c r="B44" s="64"/>
+      <c r="C44" s="64"/>
+      <c r="D44" s="64"/>
       <c r="E44" s="25"/>
       <c r="F44" s="25"/>
       <c r="G44" s="25"/>
-      <c r="H44" s="56"/>
-      <c r="I44" s="56"/>
-      <c r="J44" s="56"/>
+      <c r="H44" s="64"/>
+      <c r="I44" s="64"/>
+      <c r="J44" s="64"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="56"/>
-      <c r="B45" s="56"/>
-      <c r="C45" s="56"/>
-      <c r="D45" s="56"/>
+      <c r="A45" s="64"/>
+      <c r="B45" s="64"/>
+      <c r="C45" s="64"/>
+      <c r="D45" s="64"/>
       <c r="E45" s="25"/>
       <c r="F45" s="25"/>
       <c r="G45" s="25"/>
-      <c r="H45" s="56"/>
-      <c r="I45" s="56"/>
-      <c r="J45" s="56"/>
+      <c r="H45" s="64"/>
+      <c r="I45" s="64"/>
+      <c r="J45" s="64"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="31"/>
-      <c r="B46" s="65" t="str">
+      <c r="B46" s="69" t="str">
         <f>B19</f>
         <v>Rahinul Kabir</v>
       </c>
-      <c r="C46" s="65"/>
-      <c r="D46" s="65"/>
+      <c r="C46" s="69"/>
+      <c r="D46" s="69"/>
       <c r="E46" s="32"/>
       <c r="F46" s="32"/>
       <c r="G46" s="32"/>
-      <c r="H46" s="57" t="str">
+      <c r="H46" s="65" t="str">
         <f>H19</f>
-        <v>Tanjib</v>
-      </c>
-      <c r="I46" s="57"/>
-      <c r="J46" s="57"/>
+        <v>Jafor Iqbal</v>
+      </c>
+      <c r="I46" s="65"/>
+      <c r="J46" s="65"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="21"/>
@@ -3870,35 +3870,12 @@
       <c r="E47" s="21"/>
       <c r="F47" s="21"/>
       <c r="G47" s="21"/>
-      <c r="H47" s="51"/>
-      <c r="I47" s="52"/>
-      <c r="J47" s="52"/>
+      <c r="H47" s="59"/>
+      <c r="I47" s="60"/>
+      <c r="J47" s="60"/>
     </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="A17:D18"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="A31:J31"/>
-    <mergeCell ref="B19:D19"/>
     <mergeCell ref="H47:J47"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="H43:J43"/>
@@ -3913,6 +3890,29 @@
     <mergeCell ref="D39:E39"/>
     <mergeCell ref="B46:D46"/>
     <mergeCell ref="A44:D45"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="A31:J31"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="A17:D18"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="A4:J4"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -3944,63 +3944,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
-      <c r="J1" s="38"/>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="39"/>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="39"/>
+      <c r="B2" s="45"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="45"/>
+      <c r="I2" s="45"/>
+      <c r="J2" s="45"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="39"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
-      <c r="I3" s="39"/>
-      <c r="J3" s="39"/>
+      <c r="B3" s="45"/>
+      <c r="C3" s="45"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="45"/>
+      <c r="G3" s="45"/>
+      <c r="H3" s="45"/>
+      <c r="I3" s="45"/>
+      <c r="J3" s="45"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="40"/>
-      <c r="I4" s="40"/>
-      <c r="J4" s="40"/>
+      <c r="B4" s="47"/>
+      <c r="C4" s="47"/>
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="47"/>
+      <c r="G4" s="47"/>
+      <c r="H4" s="47"/>
+      <c r="I4" s="47"/>
+      <c r="J4" s="47"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -4010,10 +4010,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="37" t="s">
+      <c r="E5" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="37"/>
+      <c r="F5" s="48"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -4028,10 +4028,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="41">
+      <c r="E6" s="43">
         <v>68</v>
       </c>
-      <c r="F6" s="41"/>
+      <c r="F6" s="43"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>68000</v>
@@ -4047,10 +4047,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="41">
+      <c r="E7" s="43">
         <v>135</v>
       </c>
-      <c r="F7" s="41"/>
+      <c r="F7" s="43"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>67500</v>
@@ -4066,10 +4066,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="41">
+      <c r="E8" s="43">
         <v>53</v>
       </c>
-      <c r="F8" s="41"/>
+      <c r="F8" s="43"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>5300</v>
@@ -4085,10 +4085,10 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="41">
+      <c r="E9" s="43">
         <v>2</v>
       </c>
-      <c r="F9" s="41"/>
+      <c r="F9" s="43"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -4104,10 +4104,10 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="41">
+      <c r="E10" s="43">
         <v>5</v>
       </c>
-      <c r="F10" s="41"/>
+      <c r="F10" s="43"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -4123,8 +4123,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
+      <c r="E11" s="43"/>
+      <c r="F11" s="43"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4137,10 +4137,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="37" t="s">
+      <c r="D12" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="37"/>
+      <c r="E12" s="48"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -4187,76 +4187,76 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="42" t="s">
+      <c r="A16" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="42"/>
+      <c r="B16" s="49"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="42" t="s">
+      <c r="H16" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="42"/>
-      <c r="J16" s="42"/>
+      <c r="I16" s="49"/>
+      <c r="J16" s="49"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="42"/>
-      <c r="B17" s="42"/>
+      <c r="A17" s="49"/>
+      <c r="B17" s="49"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="42"/>
-      <c r="I17" s="42"/>
-      <c r="J17" s="42"/>
+      <c r="H17" s="49"/>
+      <c r="I17" s="49"/>
+      <c r="J17" s="49"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="42"/>
-      <c r="B18" s="42"/>
+      <c r="A18" s="49"/>
+      <c r="B18" s="49"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="42"/>
-      <c r="I18" s="42"/>
-      <c r="J18" s="42"/>
+      <c r="H18" s="49"/>
+      <c r="I18" s="49"/>
+      <c r="J18" s="49"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="43" t="s">
+      <c r="A19" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="43"/>
+      <c r="B19" s="42"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="44" t="s">
+      <c r="H19" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="44"/>
-      <c r="J19" s="44"/>
+      <c r="I19" s="50"/>
+      <c r="J19" s="50"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="70" t="s">
+      <c r="A20" s="71" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="70"/>
+      <c r="B20" s="71"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="45" t="s">
+      <c r="H20" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="46"/>
-      <c r="J20" s="46"/>
+      <c r="I20" s="38"/>
+      <c r="J20" s="38"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4331,60 +4331,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="38" t="s">
+      <c r="A27" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="38"/>
-      <c r="C27" s="38"/>
-      <c r="D27" s="38"/>
-      <c r="E27" s="38"/>
-      <c r="F27" s="38"/>
-      <c r="G27" s="38"/>
-      <c r="H27" s="38"/>
-      <c r="I27" s="38"/>
-      <c r="J27" s="38"/>
+      <c r="B27" s="44"/>
+      <c r="C27" s="44"/>
+      <c r="D27" s="44"/>
+      <c r="E27" s="44"/>
+      <c r="F27" s="44"/>
+      <c r="G27" s="44"/>
+      <c r="H27" s="44"/>
+      <c r="I27" s="44"/>
+      <c r="J27" s="44"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="39" t="s">
+      <c r="A28" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="39"/>
-      <c r="C28" s="39"/>
-      <c r="D28" s="39"/>
-      <c r="E28" s="39"/>
-      <c r="F28" s="39"/>
-      <c r="G28" s="39"/>
-      <c r="H28" s="39"/>
-      <c r="I28" s="39"/>
-      <c r="J28" s="39"/>
+      <c r="B28" s="45"/>
+      <c r="C28" s="45"/>
+      <c r="D28" s="45"/>
+      <c r="E28" s="45"/>
+      <c r="F28" s="45"/>
+      <c r="G28" s="45"/>
+      <c r="H28" s="45"/>
+      <c r="I28" s="45"/>
+      <c r="J28" s="45"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="47" t="s">
+      <c r="A29" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="47"/>
-      <c r="C29" s="47"/>
-      <c r="D29" s="47"/>
-      <c r="E29" s="47"/>
-      <c r="F29" s="47"/>
-      <c r="G29" s="47"/>
-      <c r="H29" s="47"/>
-      <c r="I29" s="47"/>
-      <c r="J29" s="47"/>
+      <c r="B29" s="46"/>
+      <c r="C29" s="46"/>
+      <c r="D29" s="46"/>
+      <c r="E29" s="46"/>
+      <c r="F29" s="46"/>
+      <c r="G29" s="46"/>
+      <c r="H29" s="46"/>
+      <c r="I29" s="46"/>
+      <c r="J29" s="46"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="40" t="s">
+      <c r="A30" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="40"/>
-      <c r="C30" s="40"/>
-      <c r="D30" s="40"/>
-      <c r="E30" s="40"/>
-      <c r="F30" s="40"/>
-      <c r="G30" s="40"/>
-      <c r="H30" s="40"/>
-      <c r="I30" s="40"/>
-      <c r="J30" s="40"/>
+      <c r="B30" s="47"/>
+      <c r="C30" s="47"/>
+      <c r="D30" s="47"/>
+      <c r="E30" s="47"/>
+      <c r="F30" s="47"/>
+      <c r="G30" s="47"/>
+      <c r="H30" s="47"/>
+      <c r="I30" s="47"/>
+      <c r="J30" s="47"/>
     </row>
     <row r="31" spans="1:10" ht="20.25">
       <c r="A31" s="6"/>
@@ -4393,10 +4393,10 @@
       <c r="D31" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="74" t="s">
+      <c r="E31" s="70" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="74"/>
+      <c r="F31" s="70"/>
       <c r="G31" s="9" t="s">
         <v>5</v>
       </c>
@@ -4411,10 +4411,10 @@
       <c r="D32" s="2">
         <v>1000</v>
       </c>
-      <c r="E32" s="73">
+      <c r="E32" s="74">
         <v>68</v>
       </c>
-      <c r="F32" s="73"/>
+      <c r="F32" s="74"/>
       <c r="G32" s="2">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>68000</v>
@@ -4430,10 +4430,10 @@
       <c r="D33" s="2">
         <v>500</v>
       </c>
-      <c r="E33" s="73">
+      <c r="E33" s="74">
         <v>135</v>
       </c>
-      <c r="F33" s="73"/>
+      <c r="F33" s="74"/>
       <c r="G33" s="2">
         <f t="shared" si="1"/>
         <v>67500</v>
@@ -4449,10 +4449,10 @@
       <c r="D34" s="2">
         <v>100</v>
       </c>
-      <c r="E34" s="73">
+      <c r="E34" s="74">
         <v>53</v>
       </c>
-      <c r="F34" s="73"/>
+      <c r="F34" s="74"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
         <v>5300</v>
@@ -4468,10 +4468,10 @@
       <c r="D35" s="2">
         <v>50</v>
       </c>
-      <c r="E35" s="73">
+      <c r="E35" s="74">
         <v>2</v>
       </c>
-      <c r="F35" s="73"/>
+      <c r="F35" s="74"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4487,10 +4487,10 @@
       <c r="D36" s="2">
         <v>20</v>
       </c>
-      <c r="E36" s="73">
+      <c r="E36" s="74">
         <v>5</v>
       </c>
-      <c r="F36" s="73"/>
+      <c r="F36" s="74"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4506,8 +4506,8 @@
       <c r="D37" s="2">
         <v>10</v>
       </c>
-      <c r="E37" s="73"/>
-      <c r="F37" s="73"/>
+      <c r="E37" s="74"/>
+      <c r="F37" s="74"/>
       <c r="G37" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4520,10 +4520,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="72" t="s">
+      <c r="D38" s="73" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="72"/>
+      <c r="E38" s="73"/>
       <c r="F38" s="9"/>
       <c r="G38" s="9">
         <f>SUM(G32:G37)</f>
@@ -4570,76 +4570,76 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="50" t="s">
+      <c r="A42" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="50"/>
+      <c r="B42" s="41"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="50" t="s">
+      <c r="H42" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="50"/>
-      <c r="J42" s="50"/>
+      <c r="I42" s="41"/>
+      <c r="J42" s="41"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="43"/>
-      <c r="B43" s="43"/>
+      <c r="A43" s="42"/>
+      <c r="B43" s="42"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="43"/>
-      <c r="I43" s="43"/>
-      <c r="J43" s="43"/>
+      <c r="H43" s="42"/>
+      <c r="I43" s="42"/>
+      <c r="J43" s="42"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="43"/>
-      <c r="B44" s="43"/>
+      <c r="A44" s="42"/>
+      <c r="B44" s="42"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="43"/>
-      <c r="I44" s="43"/>
-      <c r="J44" s="43"/>
+      <c r="H44" s="42"/>
+      <c r="I44" s="42"/>
+      <c r="J44" s="42"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="43" t="s">
+      <c r="A45" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="B45" s="43"/>
+      <c r="B45" s="42"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="43" t="s">
+      <c r="H45" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="50"/>
-      <c r="J45" s="50"/>
+      <c r="I45" s="41"/>
+      <c r="J45" s="41"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="71" t="s">
+      <c r="A46" s="72" t="s">
         <v>14</v>
       </c>
-      <c r="B46" s="71"/>
+      <c r="B46" s="72"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="45" t="s">
+      <c r="H46" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="46"/>
-      <c r="J46" s="46"/>
+      <c r="I46" s="38"/>
+      <c r="J46" s="38"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -4667,30 +4667,6 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
     <mergeCell ref="H46:J46"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A46:B46"/>
@@ -4707,6 +4683,30 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -4738,63 +4738,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
-      <c r="J1" s="38"/>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="39"/>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="39"/>
+      <c r="B2" s="45"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="45"/>
+      <c r="I2" s="45"/>
+      <c r="J2" s="45"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="39"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
-      <c r="I3" s="39"/>
-      <c r="J3" s="39"/>
+      <c r="B3" s="45"/>
+      <c r="C3" s="45"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="45"/>
+      <c r="G3" s="45"/>
+      <c r="H3" s="45"/>
+      <c r="I3" s="45"/>
+      <c r="J3" s="45"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="40"/>
-      <c r="I4" s="40"/>
-      <c r="J4" s="40"/>
+      <c r="B4" s="47"/>
+      <c r="C4" s="47"/>
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="47"/>
+      <c r="G4" s="47"/>
+      <c r="H4" s="47"/>
+      <c r="I4" s="47"/>
+      <c r="J4" s="47"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -4804,10 +4804,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="37" t="s">
+      <c r="E5" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="37"/>
+      <c r="F5" s="48"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -4822,10 +4822,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="41">
+      <c r="E6" s="43">
         <v>44</v>
       </c>
-      <c r="F6" s="41"/>
+      <c r="F6" s="43"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>44000</v>
@@ -4841,10 +4841,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="41">
+      <c r="E7" s="43">
         <v>118</v>
       </c>
-      <c r="F7" s="41"/>
+      <c r="F7" s="43"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>59000</v>
@@ -4860,10 +4860,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="41">
+      <c r="E8" s="43">
         <v>510</v>
       </c>
-      <c r="F8" s="41"/>
+      <c r="F8" s="43"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>51000</v>
@@ -4879,8 +4879,8 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="41"/>
-      <c r="F9" s="41"/>
+      <c r="E9" s="43"/>
+      <c r="F9" s="43"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4896,8 +4896,8 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="41"/>
-      <c r="F10" s="41"/>
+      <c r="E10" s="43"/>
+      <c r="F10" s="43"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4913,8 +4913,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
+      <c r="E11" s="43"/>
+      <c r="F11" s="43"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4927,10 +4927,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="37" t="s">
+      <c r="D12" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="37"/>
+      <c r="E12" s="48"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -4977,72 +4977,72 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="42" t="s">
+      <c r="A16" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="42"/>
+      <c r="B16" s="49"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="42" t="s">
+      <c r="H16" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="42"/>
-      <c r="J16" s="42"/>
+      <c r="I16" s="49"/>
+      <c r="J16" s="49"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="42"/>
-      <c r="B17" s="42"/>
+      <c r="A17" s="49"/>
+      <c r="B17" s="49"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="42"/>
-      <c r="I17" s="42"/>
-      <c r="J17" s="42"/>
+      <c r="H17" s="49"/>
+      <c r="I17" s="49"/>
+      <c r="J17" s="49"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="42"/>
-      <c r="B18" s="42"/>
+      <c r="A18" s="49"/>
+      <c r="B18" s="49"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="42"/>
-      <c r="I18" s="42"/>
-      <c r="J18" s="42"/>
+      <c r="H18" s="49"/>
+      <c r="I18" s="49"/>
+      <c r="J18" s="49"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="43"/>
-      <c r="B19" s="43"/>
+      <c r="A19" s="42"/>
+      <c r="B19" s="42"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="44" t="s">
+      <c r="H19" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="44"/>
-      <c r="J19" s="44"/>
+      <c r="I19" s="50"/>
+      <c r="J19" s="50"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="76"/>
-      <c r="B20" s="76"/>
+      <c r="A20" s="75"/>
+      <c r="B20" s="75"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="45" t="s">
+      <c r="H20" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="46"/>
-      <c r="J20" s="46"/>
+      <c r="I20" s="38"/>
+      <c r="J20" s="38"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -5117,60 +5117,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="38" t="s">
+      <c r="A27" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="38"/>
-      <c r="C27" s="38"/>
-      <c r="D27" s="38"/>
-      <c r="E27" s="38"/>
-      <c r="F27" s="38"/>
-      <c r="G27" s="38"/>
-      <c r="H27" s="38"/>
-      <c r="I27" s="38"/>
-      <c r="J27" s="38"/>
+      <c r="B27" s="44"/>
+      <c r="C27" s="44"/>
+      <c r="D27" s="44"/>
+      <c r="E27" s="44"/>
+      <c r="F27" s="44"/>
+      <c r="G27" s="44"/>
+      <c r="H27" s="44"/>
+      <c r="I27" s="44"/>
+      <c r="J27" s="44"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="39" t="s">
+      <c r="A28" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="39"/>
-      <c r="C28" s="39"/>
-      <c r="D28" s="39"/>
-      <c r="E28" s="39"/>
-      <c r="F28" s="39"/>
-      <c r="G28" s="39"/>
-      <c r="H28" s="39"/>
-      <c r="I28" s="39"/>
-      <c r="J28" s="39"/>
+      <c r="B28" s="45"/>
+      <c r="C28" s="45"/>
+      <c r="D28" s="45"/>
+      <c r="E28" s="45"/>
+      <c r="F28" s="45"/>
+      <c r="G28" s="45"/>
+      <c r="H28" s="45"/>
+      <c r="I28" s="45"/>
+      <c r="J28" s="45"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="47" t="s">
+      <c r="A29" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="47"/>
-      <c r="C29" s="47"/>
-      <c r="D29" s="47"/>
-      <c r="E29" s="47"/>
-      <c r="F29" s="47"/>
-      <c r="G29" s="47"/>
-      <c r="H29" s="47"/>
-      <c r="I29" s="47"/>
-      <c r="J29" s="47"/>
+      <c r="B29" s="46"/>
+      <c r="C29" s="46"/>
+      <c r="D29" s="46"/>
+      <c r="E29" s="46"/>
+      <c r="F29" s="46"/>
+      <c r="G29" s="46"/>
+      <c r="H29" s="46"/>
+      <c r="I29" s="46"/>
+      <c r="J29" s="46"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="40" t="s">
+      <c r="A30" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="40"/>
-      <c r="C30" s="40"/>
-      <c r="D30" s="40"/>
-      <c r="E30" s="40"/>
-      <c r="F30" s="40"/>
-      <c r="G30" s="40"/>
-      <c r="H30" s="40"/>
-      <c r="I30" s="40"/>
-      <c r="J30" s="40"/>
+      <c r="B30" s="47"/>
+      <c r="C30" s="47"/>
+      <c r="D30" s="47"/>
+      <c r="E30" s="47"/>
+      <c r="F30" s="47"/>
+      <c r="G30" s="47"/>
+      <c r="H30" s="47"/>
+      <c r="I30" s="47"/>
+      <c r="J30" s="47"/>
     </row>
     <row r="31" spans="1:10" ht="23.25">
       <c r="A31" s="6"/>
@@ -5179,10 +5179,10 @@
       <c r="D31" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="37" t="s">
+      <c r="E31" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="37"/>
+      <c r="F31" s="48"/>
       <c r="G31" s="12" t="s">
         <v>5</v>
       </c>
@@ -5197,10 +5197,10 @@
       <c r="D32" s="11">
         <v>1000</v>
       </c>
-      <c r="E32" s="41">
+      <c r="E32" s="43">
         <v>44</v>
       </c>
-      <c r="F32" s="41"/>
+      <c r="F32" s="43"/>
       <c r="G32" s="11">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>44000</v>
@@ -5216,10 +5216,10 @@
       <c r="D33" s="11">
         <v>500</v>
       </c>
-      <c r="E33" s="41">
+      <c r="E33" s="43">
         <v>118</v>
       </c>
-      <c r="F33" s="41"/>
+      <c r="F33" s="43"/>
       <c r="G33" s="11">
         <f t="shared" si="1"/>
         <v>59000</v>
@@ -5235,10 +5235,10 @@
       <c r="D34" s="11">
         <v>100</v>
       </c>
-      <c r="E34" s="41">
+      <c r="E34" s="43">
         <v>510</v>
       </c>
-      <c r="F34" s="41"/>
+      <c r="F34" s="43"/>
       <c r="G34" s="11">
         <f t="shared" si="1"/>
         <v>51000</v>
@@ -5254,8 +5254,8 @@
       <c r="D35" s="11">
         <v>50</v>
       </c>
-      <c r="E35" s="41"/>
-      <c r="F35" s="41"/>
+      <c r="E35" s="43"/>
+      <c r="F35" s="43"/>
       <c r="G35" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -5271,8 +5271,8 @@
       <c r="D36" s="11">
         <v>20</v>
       </c>
-      <c r="E36" s="41"/>
-      <c r="F36" s="41"/>
+      <c r="E36" s="43"/>
+      <c r="F36" s="43"/>
       <c r="G36" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -5288,8 +5288,8 @@
       <c r="D37" s="11">
         <v>10</v>
       </c>
-      <c r="E37" s="41"/>
-      <c r="F37" s="41"/>
+      <c r="E37" s="43"/>
+      <c r="F37" s="43"/>
       <c r="G37" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -5302,10 +5302,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="75" t="s">
+      <c r="D38" s="76" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="75"/>
+      <c r="E38" s="76"/>
       <c r="F38" s="12"/>
       <c r="G38" s="12">
         <f>SUM(G32:G37)</f>
@@ -5352,72 +5352,72 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="50" t="s">
+      <c r="A42" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="50"/>
+      <c r="B42" s="41"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="50" t="s">
+      <c r="H42" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="50"/>
-      <c r="J42" s="50"/>
+      <c r="I42" s="41"/>
+      <c r="J42" s="41"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="43"/>
-      <c r="B43" s="43"/>
+      <c r="A43" s="42"/>
+      <c r="B43" s="42"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="43"/>
-      <c r="I43" s="43"/>
-      <c r="J43" s="43"/>
+      <c r="H43" s="42"/>
+      <c r="I43" s="42"/>
+      <c r="J43" s="42"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="43"/>
-      <c r="B44" s="43"/>
+      <c r="A44" s="42"/>
+      <c r="B44" s="42"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="43"/>
-      <c r="I44" s="43"/>
-      <c r="J44" s="43"/>
+      <c r="H44" s="42"/>
+      <c r="I44" s="42"/>
+      <c r="J44" s="42"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="43"/>
-      <c r="B45" s="43"/>
+      <c r="A45" s="42"/>
+      <c r="B45" s="42"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="43" t="s">
+      <c r="H45" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="50"/>
-      <c r="J45" s="50"/>
+      <c r="I45" s="41"/>
+      <c r="J45" s="41"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="71"/>
-      <c r="B46" s="71"/>
+      <c r="A46" s="72"/>
+      <c r="B46" s="72"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="45" t="s">
+      <c r="H46" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="46"/>
-      <c r="J46" s="46"/>
+      <c r="I46" s="38"/>
+      <c r="J46" s="38"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -5445,6 +5445,34 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -5457,34 +5485,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -5509,64 +5509,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
-      <c r="J1" s="38"/>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="39"/>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="39"/>
+      <c r="B2" s="45"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="45"/>
+      <c r="I2" s="45"/>
+      <c r="J2" s="45"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="39"/>
-      <c r="B3" s="39"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
-      <c r="I3" s="39"/>
-      <c r="J3" s="39"/>
+      <c r="A3" s="45"/>
+      <c r="B3" s="45"/>
+      <c r="C3" s="45"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="45"/>
+      <c r="G3" s="45"/>
+      <c r="H3" s="45"/>
+      <c r="I3" s="45"/>
+      <c r="J3" s="45"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="40"/>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="40"/>
-      <c r="I4" s="40"/>
-      <c r="J4" s="40"/>
+      <c r="A4" s="47"/>
+      <c r="B4" s="47"/>
+      <c r="C4" s="47"/>
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="47"/>
+      <c r="G4" s="47"/>
+      <c r="H4" s="47"/>
+      <c r="I4" s="47"/>
+      <c r="J4" s="47"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="D5" s="18"/>
-      <c r="E5" s="37"/>
-      <c r="F5" s="37"/>
+      <c r="E5" s="48"/>
+      <c r="F5" s="48"/>
       <c r="G5" s="18"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
@@ -5577,8 +5577,8 @@
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="17"/>
-      <c r="E6" s="41"/>
-      <c r="F6" s="41"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="43"/>
       <c r="G6" s="17"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -5589,8 +5589,8 @@
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
       <c r="D7" s="17"/>
-      <c r="E7" s="41"/>
-      <c r="F7" s="41"/>
+      <c r="E7" s="43"/>
+      <c r="F7" s="43"/>
       <c r="G7" s="17"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
@@ -5601,8 +5601,8 @@
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
       <c r="D8" s="17"/>
-      <c r="E8" s="41"/>
-      <c r="F8" s="41"/>
+      <c r="E8" s="43"/>
+      <c r="F8" s="43"/>
       <c r="G8" s="17"/>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -5613,8 +5613,8 @@
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="17"/>
-      <c r="E9" s="41"/>
-      <c r="F9" s="41"/>
+      <c r="E9" s="43"/>
+      <c r="F9" s="43"/>
       <c r="G9" s="17"/>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -5625,8 +5625,8 @@
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="17"/>
-      <c r="E10" s="41"/>
-      <c r="F10" s="41"/>
+      <c r="E10" s="43"/>
+      <c r="F10" s="43"/>
       <c r="G10" s="17"/>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
@@ -5637,8 +5637,8 @@
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="17"/>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
+      <c r="E11" s="43"/>
+      <c r="F11" s="43"/>
       <c r="G11" s="17"/>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
@@ -5648,8 +5648,8 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="37"/>
-      <c r="E12" s="37"/>
+      <c r="D12" s="48"/>
+      <c r="E12" s="48"/>
       <c r="F12" s="18"/>
       <c r="G12" s="18"/>
       <c r="H12" s="6"/>
@@ -5693,52 +5693,52 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="42"/>
-      <c r="B16" s="42"/>
+      <c r="A16" s="49"/>
+      <c r="B16" s="49"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="42"/>
-      <c r="I16" s="42"/>
-      <c r="J16" s="42"/>
+      <c r="H16" s="49"/>
+      <c r="I16" s="49"/>
+      <c r="J16" s="49"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="42"/>
-      <c r="B17" s="42"/>
+      <c r="A17" s="49"/>
+      <c r="B17" s="49"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="42"/>
-      <c r="I17" s="42"/>
-      <c r="J17" s="42"/>
+      <c r="H17" s="49"/>
+      <c r="I17" s="49"/>
+      <c r="J17" s="49"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="42"/>
-      <c r="B18" s="42"/>
+      <c r="A18" s="49"/>
+      <c r="B18" s="49"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="42"/>
-      <c r="I18" s="42"/>
-      <c r="J18" s="42"/>
+      <c r="H18" s="49"/>
+      <c r="I18" s="49"/>
+      <c r="J18" s="49"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="43"/>
-      <c r="B19" s="43"/>
+      <c r="A19" s="42"/>
+      <c r="B19" s="42"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="44"/>
-      <c r="I19" s="44"/>
-      <c r="J19" s="44"/>
+      <c r="H19" s="50"/>
+      <c r="I19" s="50"/>
+      <c r="J19" s="50"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -5748,9 +5748,9 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="45"/>
-      <c r="I20" s="46"/>
-      <c r="J20" s="46"/>
+      <c r="H20" s="37"/>
+      <c r="I20" s="38"/>
+      <c r="J20" s="38"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -5837,60 +5837,60 @@
       <c r="J27" s="6"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="38" t="s">
+      <c r="A28" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="38"/>
-      <c r="C28" s="38"/>
-      <c r="D28" s="38"/>
-      <c r="E28" s="38"/>
-      <c r="F28" s="38"/>
-      <c r="G28" s="38"/>
-      <c r="H28" s="38"/>
-      <c r="I28" s="38"/>
-      <c r="J28" s="38"/>
+      <c r="B28" s="44"/>
+      <c r="C28" s="44"/>
+      <c r="D28" s="44"/>
+      <c r="E28" s="44"/>
+      <c r="F28" s="44"/>
+      <c r="G28" s="44"/>
+      <c r="H28" s="44"/>
+      <c r="I28" s="44"/>
+      <c r="J28" s="44"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="39" t="s">
+      <c r="A29" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="39"/>
-      <c r="C29" s="39"/>
-      <c r="D29" s="39"/>
-      <c r="E29" s="39"/>
-      <c r="F29" s="39"/>
-      <c r="G29" s="39"/>
-      <c r="H29" s="39"/>
-      <c r="I29" s="39"/>
-      <c r="J29" s="39"/>
+      <c r="B29" s="45"/>
+      <c r="C29" s="45"/>
+      <c r="D29" s="45"/>
+      <c r="E29" s="45"/>
+      <c r="F29" s="45"/>
+      <c r="G29" s="45"/>
+      <c r="H29" s="45"/>
+      <c r="I29" s="45"/>
+      <c r="J29" s="45"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="47" t="s">
+      <c r="A30" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="47"/>
-      <c r="C30" s="47"/>
-      <c r="D30" s="47"/>
-      <c r="E30" s="47"/>
-      <c r="F30" s="47"/>
-      <c r="G30" s="47"/>
-      <c r="H30" s="47"/>
-      <c r="I30" s="47"/>
-      <c r="J30" s="47"/>
+      <c r="B30" s="46"/>
+      <c r="C30" s="46"/>
+      <c r="D30" s="46"/>
+      <c r="E30" s="46"/>
+      <c r="F30" s="46"/>
+      <c r="G30" s="46"/>
+      <c r="H30" s="46"/>
+      <c r="I30" s="46"/>
+      <c r="J30" s="46"/>
     </row>
     <row r="31" spans="1:10" ht="18.75">
-      <c r="A31" s="40" t="s">
+      <c r="A31" s="47" t="s">
         <v>19</v>
       </c>
-      <c r="B31" s="40"/>
-      <c r="C31" s="40"/>
-      <c r="D31" s="40"/>
-      <c r="E31" s="40"/>
-      <c r="F31" s="40"/>
-      <c r="G31" s="40"/>
-      <c r="H31" s="40"/>
-      <c r="I31" s="40"/>
-      <c r="J31" s="40"/>
+      <c r="B31" s="47"/>
+      <c r="C31" s="47"/>
+      <c r="D31" s="47"/>
+      <c r="E31" s="47"/>
+      <c r="F31" s="47"/>
+      <c r="G31" s="47"/>
+      <c r="H31" s="47"/>
+      <c r="I31" s="47"/>
+      <c r="J31" s="47"/>
     </row>
     <row r="32" spans="1:10" ht="20.25">
       <c r="A32" s="6" t="s">
@@ -5901,10 +5901,10 @@
       <c r="D32" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="74" t="s">
+      <c r="E32" s="70" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="74"/>
+      <c r="F32" s="70"/>
       <c r="G32" s="20" t="s">
         <v>5</v>
       </c>
@@ -5919,10 +5919,10 @@
       <c r="D33" s="19">
         <v>1000</v>
       </c>
-      <c r="E33" s="41">
+      <c r="E33" s="43">
         <v>30</v>
       </c>
-      <c r="F33" s="41"/>
+      <c r="F33" s="43"/>
       <c r="G33" s="19">
         <f t="shared" ref="G33:G38" si="0">SUM(D33*E33)</f>
         <v>30000</v>
@@ -5938,10 +5938,10 @@
       <c r="D34" s="19">
         <v>500</v>
       </c>
-      <c r="E34" s="41">
+      <c r="E34" s="43">
         <v>35</v>
       </c>
-      <c r="F34" s="41"/>
+      <c r="F34" s="43"/>
       <c r="G34" s="19">
         <f t="shared" si="0"/>
         <v>17500</v>
@@ -5957,10 +5957,10 @@
       <c r="D35" s="19">
         <v>100</v>
       </c>
-      <c r="E35" s="41">
+      <c r="E35" s="43">
         <v>425</v>
       </c>
-      <c r="F35" s="41"/>
+      <c r="F35" s="43"/>
       <c r="G35" s="19">
         <f t="shared" si="0"/>
         <v>42500</v>
@@ -5976,8 +5976,8 @@
       <c r="D36" s="19">
         <v>50</v>
       </c>
-      <c r="E36" s="41"/>
-      <c r="F36" s="41"/>
+      <c r="E36" s="43"/>
+      <c r="F36" s="43"/>
       <c r="G36" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -5993,8 +5993,8 @@
       <c r="D37" s="19">
         <v>20</v>
       </c>
-      <c r="E37" s="73"/>
-      <c r="F37" s="73"/>
+      <c r="E37" s="74"/>
+      <c r="F37" s="74"/>
       <c r="G37" s="19">
         <f>SUM(D37*E37)</f>
         <v>0</v>
@@ -6010,10 +6010,10 @@
       <c r="D38" s="19">
         <v>10</v>
       </c>
-      <c r="E38" s="73">
+      <c r="E38" s="74">
         <v>100</v>
       </c>
-      <c r="F38" s="73"/>
+      <c r="F38" s="74"/>
       <c r="G38" s="19">
         <f t="shared" si="0"/>
         <v>1000</v>
@@ -6076,58 +6076,58 @@
       <c r="J42" s="6"/>
     </row>
     <row r="43" spans="1:10" ht="15.75">
-      <c r="A43" s="50" t="s">
+      <c r="A43" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="50"/>
+      <c r="B43" s="41"/>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
-      <c r="H43" s="50" t="s">
+      <c r="H43" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="50"/>
-      <c r="J43" s="50"/>
+      <c r="I43" s="41"/>
+      <c r="J43" s="41"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="43"/>
-      <c r="B44" s="43"/>
+      <c r="A44" s="42"/>
+      <c r="B44" s="42"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="43"/>
-      <c r="I44" s="43"/>
-      <c r="J44" s="43"/>
+      <c r="H44" s="42"/>
+      <c r="I44" s="42"/>
+      <c r="J44" s="42"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="43"/>
-      <c r="B45" s="43"/>
+      <c r="A45" s="42"/>
+      <c r="B45" s="42"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="43"/>
-      <c r="I45" s="43"/>
-      <c r="J45" s="43"/>
+      <c r="H45" s="42"/>
+      <c r="I45" s="42"/>
+      <c r="J45" s="42"/>
     </row>
     <row r="46" spans="1:10" ht="15.75">
-      <c r="A46" s="43"/>
-      <c r="B46" s="43"/>
+      <c r="A46" s="42"/>
+      <c r="B46" s="42"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="43" t="s">
+      <c r="H46" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="50"/>
-      <c r="J46" s="50"/>
+      <c r="I46" s="41"/>
+      <c r="J46" s="41"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -6137,20 +6137,30 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="45"/>
-      <c r="I47" s="46"/>
-      <c r="J47" s="46"/>
+      <c r="H47" s="37"/>
+      <c r="I47" s="38"/>
+      <c r="J47" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="H47:J47"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="H43:J43"/>
-    <mergeCell ref="A44:B45"/>
-    <mergeCell ref="H44:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="E38:F38"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A28:J28"/>
@@ -6163,24 +6173,14 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="H47:J47"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="H43:J43"/>
+    <mergeCell ref="A44:B45"/>
+    <mergeCell ref="H44:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -6206,177 +6206,177 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
-      <c r="J1" s="38"/>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="39"/>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="39"/>
+      <c r="B2" s="45"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="45"/>
+      <c r="I2" s="45"/>
+      <c r="J2" s="45"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="87">
+      <c r="A5" s="88">
         <v>1</v>
       </c>
-      <c r="B5" s="79" t="s">
+      <c r="B5" s="81" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="79"/>
-      <c r="D5" s="79"/>
-      <c r="E5" s="79"/>
-      <c r="F5" s="79"/>
-      <c r="G5" s="86">
+      <c r="C5" s="81"/>
+      <c r="D5" s="81"/>
+      <c r="E5" s="81"/>
+      <c r="F5" s="81"/>
+      <c r="G5" s="79">
         <v>1650</v>
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="87"/>
-      <c r="B6" s="79"/>
-      <c r="C6" s="79"/>
-      <c r="D6" s="79"/>
-      <c r="E6" s="79"/>
-      <c r="F6" s="79"/>
-      <c r="G6" s="86"/>
+      <c r="A6" s="88"/>
+      <c r="B6" s="81"/>
+      <c r="C6" s="81"/>
+      <c r="D6" s="81"/>
+      <c r="E6" s="81"/>
+      <c r="F6" s="81"/>
+      <c r="G6" s="79"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="87">
+      <c r="A7" s="88">
         <v>2</v>
       </c>
-      <c r="B7" s="79" t="s">
+      <c r="B7" s="81" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="79"/>
-      <c r="D7" s="79"/>
-      <c r="E7" s="79"/>
-      <c r="F7" s="79"/>
-      <c r="G7" s="86">
+      <c r="C7" s="81"/>
+      <c r="D7" s="81"/>
+      <c r="E7" s="81"/>
+      <c r="F7" s="81"/>
+      <c r="G7" s="79">
         <v>1980</v>
       </c>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="87"/>
-      <c r="B8" s="79"/>
-      <c r="C8" s="79"/>
-      <c r="D8" s="79"/>
-      <c r="E8" s="79"/>
-      <c r="F8" s="79"/>
-      <c r="G8" s="86"/>
+      <c r="A8" s="88"/>
+      <c r="B8" s="81"/>
+      <c r="C8" s="81"/>
+      <c r="D8" s="81"/>
+      <c r="E8" s="81"/>
+      <c r="F8" s="81"/>
+      <c r="G8" s="79"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="87">
+      <c r="A9" s="88">
         <v>3</v>
       </c>
-      <c r="B9" s="79" t="s">
+      <c r="B9" s="81" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="79"/>
-      <c r="D9" s="79"/>
-      <c r="E9" s="79"/>
-      <c r="F9" s="79"/>
-      <c r="G9" s="86">
+      <c r="C9" s="81"/>
+      <c r="D9" s="81"/>
+      <c r="E9" s="81"/>
+      <c r="F9" s="81"/>
+      <c r="G9" s="79">
         <v>10538</v>
       </c>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="87"/>
-      <c r="B10" s="79"/>
-      <c r="C10" s="79"/>
-      <c r="D10" s="79"/>
-      <c r="E10" s="79"/>
-      <c r="F10" s="79"/>
-      <c r="G10" s="86"/>
+      <c r="A10" s="88"/>
+      <c r="B10" s="81"/>
+      <c r="C10" s="81"/>
+      <c r="D10" s="81"/>
+      <c r="E10" s="81"/>
+      <c r="F10" s="81"/>
+      <c r="G10" s="79"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="87">
+      <c r="A11" s="88">
         <v>4</v>
       </c>
-      <c r="B11" s="80" t="s">
+      <c r="B11" s="82" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="81"/>
-      <c r="D11" s="81"/>
-      <c r="E11" s="81"/>
-      <c r="F11" s="82"/>
-      <c r="G11" s="86">
+      <c r="C11" s="83"/>
+      <c r="D11" s="83"/>
+      <c r="E11" s="83"/>
+      <c r="F11" s="84"/>
+      <c r="G11" s="79">
         <v>1100</v>
       </c>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="87"/>
-      <c r="B12" s="83"/>
-      <c r="C12" s="84"/>
-      <c r="D12" s="84"/>
-      <c r="E12" s="84"/>
-      <c r="F12" s="85"/>
-      <c r="G12" s="86"/>
+      <c r="A12" s="88"/>
+      <c r="B12" s="85"/>
+      <c r="C12" s="86"/>
+      <c r="D12" s="86"/>
+      <c r="E12" s="86"/>
+      <c r="F12" s="87"/>
+      <c r="G12" s="79"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="88" t="s">
+      <c r="A13" s="80" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="88"/>
-      <c r="C13" s="88"/>
-      <c r="D13" s="88"/>
-      <c r="E13" s="88"/>
-      <c r="F13" s="88"/>
-      <c r="G13" s="86">
+      <c r="B13" s="80"/>
+      <c r="C13" s="80"/>
+      <c r="D13" s="80"/>
+      <c r="E13" s="80"/>
+      <c r="F13" s="80"/>
+      <c r="G13" s="79">
         <f>SUM(G5:G12)</f>
         <v>15268</v>
       </c>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="88"/>
-      <c r="B14" s="88"/>
-      <c r="C14" s="88"/>
-      <c r="D14" s="88"/>
-      <c r="E14" s="88"/>
-      <c r="F14" s="88"/>
-      <c r="G14" s="86"/>
+      <c r="A14" s="80"/>
+      <c r="B14" s="80"/>
+      <c r="C14" s="80"/>
+      <c r="D14" s="80"/>
+      <c r="E14" s="80"/>
+      <c r="F14" s="80"/>
+      <c r="G14" s="79"/>
     </row>
     <row r="23" spans="1:10" ht="18.75">
-      <c r="A23" s="47" t="s">
+      <c r="A23" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="47"/>
-      <c r="C23" s="47"/>
-      <c r="D23" s="47"/>
-      <c r="E23" s="47"/>
-      <c r="F23" s="47"/>
-      <c r="G23" s="47"/>
-      <c r="H23" s="47"/>
-      <c r="I23" s="47"/>
-      <c r="J23" s="47"/>
+      <c r="B23" s="46"/>
+      <c r="C23" s="46"/>
+      <c r="D23" s="46"/>
+      <c r="E23" s="46"/>
+      <c r="F23" s="46"/>
+      <c r="G23" s="46"/>
+      <c r="H23" s="46"/>
+      <c r="I23" s="46"/>
+      <c r="J23" s="46"/>
     </row>
     <row r="24" spans="1:10" ht="18.75">
-      <c r="A24" s="40"/>
-      <c r="B24" s="40"/>
-      <c r="C24" s="40"/>
-      <c r="D24" s="40"/>
-      <c r="E24" s="40"/>
-      <c r="F24" s="40"/>
-      <c r="G24" s="40"/>
-      <c r="H24" s="40"/>
-      <c r="I24" s="40"/>
-      <c r="J24" s="40"/>
+      <c r="A24" s="47"/>
+      <c r="B24" s="47"/>
+      <c r="C24" s="47"/>
+      <c r="D24" s="47"/>
+      <c r="E24" s="47"/>
+      <c r="F24" s="47"/>
+      <c r="G24" s="47"/>
+      <c r="H24" s="47"/>
+      <c r="I24" s="47"/>
+      <c r="J24" s="47"/>
     </row>
     <row r="25" spans="1:10" ht="20.25">
       <c r="A25" s="6" t="s">
@@ -6387,10 +6387,10 @@
       <c r="D25" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E25" s="74" t="s">
+      <c r="E25" s="70" t="s">
         <v>4</v>
       </c>
-      <c r="F25" s="74"/>
+      <c r="F25" s="70"/>
       <c r="G25" s="20" t="s">
         <v>5</v>
       </c>
@@ -6405,8 +6405,8 @@
       <c r="D26" s="19">
         <v>1000</v>
       </c>
-      <c r="E26" s="41"/>
-      <c r="F26" s="41"/>
+      <c r="E26" s="43"/>
+      <c r="F26" s="43"/>
       <c r="G26" s="19">
         <f t="shared" ref="G26:G31" si="0">SUM(D26*E26)</f>
         <v>0</v>
@@ -6422,10 +6422,10 @@
       <c r="D27" s="19">
         <v>500</v>
       </c>
-      <c r="E27" s="41">
+      <c r="E27" s="43">
         <v>30</v>
       </c>
-      <c r="F27" s="41"/>
+      <c r="F27" s="43"/>
       <c r="G27" s="19">
         <f t="shared" si="0"/>
         <v>15000</v>
@@ -6441,8 +6441,8 @@
       <c r="D28" s="19">
         <v>100</v>
       </c>
-      <c r="E28" s="41"/>
-      <c r="F28" s="41"/>
+      <c r="E28" s="43"/>
+      <c r="F28" s="43"/>
       <c r="G28" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -6458,10 +6458,10 @@
       <c r="D29" s="19">
         <v>50</v>
       </c>
-      <c r="E29" s="41">
+      <c r="E29" s="43">
         <v>5</v>
       </c>
-      <c r="F29" s="41"/>
+      <c r="F29" s="43"/>
       <c r="G29" s="19">
         <f t="shared" si="0"/>
         <v>250</v>
@@ -6477,8 +6477,8 @@
       <c r="D30" s="19">
         <v>20</v>
       </c>
-      <c r="E30" s="73"/>
-      <c r="F30" s="73"/>
+      <c r="E30" s="74"/>
+      <c r="F30" s="74"/>
       <c r="G30" s="19">
         <f>SUM(D30*E30)</f>
         <v>0</v>
@@ -6494,10 +6494,10 @@
       <c r="D31" s="19">
         <v>10</v>
       </c>
-      <c r="E31" s="73">
+      <c r="E31" s="74">
         <v>2</v>
       </c>
-      <c r="F31" s="73"/>
+      <c r="F31" s="74"/>
       <c r="G31" s="19">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -6560,58 +6560,58 @@
       <c r="J35" s="6"/>
     </row>
     <row r="36" spans="1:10" ht="15.75">
-      <c r="A36" s="50" t="s">
+      <c r="A36" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="50"/>
+      <c r="B36" s="41"/>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
       <c r="G36" s="7"/>
-      <c r="H36" s="50" t="s">
+      <c r="H36" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="I36" s="50"/>
-      <c r="J36" s="50"/>
+      <c r="I36" s="41"/>
+      <c r="J36" s="41"/>
     </row>
     <row r="37" spans="1:10">
-      <c r="A37" s="43"/>
-      <c r="B37" s="43"/>
+      <c r="A37" s="42"/>
+      <c r="B37" s="42"/>
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
       <c r="G37" s="6"/>
-      <c r="H37" s="43"/>
-      <c r="I37" s="43"/>
-      <c r="J37" s="43"/>
+      <c r="H37" s="42"/>
+      <c r="I37" s="42"/>
+      <c r="J37" s="42"/>
     </row>
     <row r="38" spans="1:10">
-      <c r="A38" s="43"/>
-      <c r="B38" s="43"/>
+      <c r="A38" s="42"/>
+      <c r="B38" s="42"/>
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
-      <c r="H38" s="43"/>
-      <c r="I38" s="43"/>
-      <c r="J38" s="43"/>
+      <c r="H38" s="42"/>
+      <c r="I38" s="42"/>
+      <c r="J38" s="42"/>
     </row>
     <row r="39" spans="1:10" ht="15.75">
-      <c r="A39" s="43"/>
-      <c r="B39" s="43"/>
+      <c r="A39" s="42"/>
+      <c r="B39" s="42"/>
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
       <c r="F39" s="6"/>
       <c r="G39" s="6"/>
-      <c r="H39" s="43" t="s">
+      <c r="H39" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="I39" s="50"/>
-      <c r="J39" s="50"/>
+      <c r="I39" s="41"/>
+      <c r="J39" s="41"/>
     </row>
     <row r="40" spans="1:10">
       <c r="A40" s="6"/>
@@ -6621,29 +6621,12 @@
       <c r="E40" s="6"/>
       <c r="F40" s="6"/>
       <c r="G40" s="6"/>
-      <c r="H40" s="45"/>
-      <c r="I40" s="46"/>
-      <c r="J40" s="46"/>
+      <c r="H40" s="37"/>
+      <c r="I40" s="38"/>
+      <c r="J40" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="H40:J40"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="H36:J36"/>
-    <mergeCell ref="A37:B38"/>
-    <mergeCell ref="H37:J38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="H39:J39"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="A13:F14"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="E30:F30"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="A23:J23"/>
@@ -6660,6 +6643,23 @@
     <mergeCell ref="B5:F6"/>
     <mergeCell ref="G5:G6"/>
     <mergeCell ref="B7:F8"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="A13:F14"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="H40:J40"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="H36:J36"/>
+    <mergeCell ref="A37:B38"/>
+    <mergeCell ref="H37:J38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="H39:J39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="71" orientation="portrait" r:id="rId1"/>

</xml_diff>